<commit_message>
add subject alias search criterion
</commit_message>
<xml_diff>
--- a/criterion_property_definitions.xlsx
+++ b/criterion_property_definitions.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1692" uniqueCount="402">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1702" uniqueCount="404">
   <si>
     <t>property</t>
   </si>
@@ -1223,6 +1223,12 @@
   </si>
   <si>
     <t>inputField.category</t>
+  </si>
+  <si>
+    <t>proband.personParticulars.alias</t>
+  </si>
+  <si>
+    <t>proband.animalParticulars.alias</t>
   </si>
 </sst>
 </file>
@@ -1555,10 +1561,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:L263"/>
+  <dimension ref="A1:L265"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A97" workbookViewId="0">
-      <selection activeCell="B120" sqref="B120"/>
+      <selection activeCell="B135" sqref="B135"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="15.7109375" defaultRowHeight="16.5" customHeight="1"/>
@@ -4306,13 +4312,13 @@
         <v>84</v>
       </c>
       <c r="B131" t="s">
-        <v>397</v>
+        <v>402</v>
       </c>
       <c r="C131" t="s">
         <v>17</v>
       </c>
       <c r="K131" t="s">
-        <v>397</v>
+        <v>402</v>
       </c>
       <c r="L131" t="s">
         <v>133</v>
@@ -4323,16 +4329,16 @@
         <v>84</v>
       </c>
       <c r="B132" t="s">
-        <v>395</v>
+        <v>397</v>
       </c>
       <c r="C132" t="s">
-        <v>36</v>
+        <v>17</v>
       </c>
       <c r="K132" t="s">
-        <v>395</v>
+        <v>397</v>
       </c>
       <c r="L132" t="s">
-        <v>138</v>
+        <v>133</v>
       </c>
     </row>
     <row r="133" spans="1:12" ht="16.5" customHeight="1">
@@ -4340,42 +4346,42 @@
         <v>84</v>
       </c>
       <c r="B133" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="C133" t="s">
-        <v>17</v>
-      </c>
-      <c r="D133" t="s">
-        <v>350</v>
-      </c>
-      <c r="E133" t="s">
-        <v>91</v>
-      </c>
-      <c r="F133" t="s">
-        <v>12</v>
-      </c>
-      <c r="G133" t="s">
-        <v>92</v>
+        <v>36</v>
       </c>
       <c r="K133" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="L133" t="s">
-        <v>132</v>
+        <v>138</v>
       </c>
     </row>
     <row r="134" spans="1:12" ht="16.5" customHeight="1">
       <c r="A134" t="s">
-        <v>198</v>
+        <v>84</v>
       </c>
       <c r="B134" t="s">
-        <v>93</v>
+        <v>396</v>
       </c>
       <c r="C134" t="s">
-        <v>19</v>
+        <v>17</v>
+      </c>
+      <c r="D134" t="s">
+        <v>350</v>
+      </c>
+      <c r="E134" t="s">
+        <v>91</v>
+      </c>
+      <c r="F134" t="s">
+        <v>12</v>
+      </c>
+      <c r="G134" t="s">
+        <v>92</v>
       </c>
       <c r="K134" t="s">
-        <v>93</v>
+        <v>396</v>
       </c>
       <c r="L134" t="s">
         <v>132</v>
@@ -4386,30 +4392,30 @@
         <v>84</v>
       </c>
       <c r="B135" t="s">
-        <v>398</v>
+        <v>403</v>
       </c>
       <c r="C135" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="K135" t="s">
-        <v>398</v>
+        <v>403</v>
       </c>
       <c r="L135" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
     </row>
     <row r="136" spans="1:12" ht="16.5" customHeight="1">
       <c r="A136" t="s">
-        <v>84</v>
+        <v>198</v>
       </c>
       <c r="B136" t="s">
-        <v>399</v>
+        <v>93</v>
       </c>
       <c r="C136" t="s">
         <v>19</v>
       </c>
       <c r="K136" t="s">
-        <v>399</v>
+        <v>93</v>
       </c>
       <c r="L136" t="s">
         <v>132</v>
@@ -4420,19 +4426,16 @@
         <v>84</v>
       </c>
       <c r="B137" t="s">
-        <v>400</v>
+        <v>398</v>
       </c>
       <c r="C137" t="s">
-        <v>9</v>
-      </c>
-      <c r="J137" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="K137" t="s">
-        <v>400</v>
+        <v>398</v>
       </c>
       <c r="L137" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
     </row>
     <row r="138" spans="1:12" ht="16.5" customHeight="1">
@@ -4440,13 +4443,13 @@
         <v>84</v>
       </c>
       <c r="B138" t="s">
-        <v>293</v>
+        <v>399</v>
       </c>
       <c r="C138" t="s">
         <v>19</v>
       </c>
       <c r="K138" t="s">
-        <v>293</v>
+        <v>399</v>
       </c>
       <c r="L138" t="s">
         <v>132</v>
@@ -4457,30 +4460,33 @@
         <v>84</v>
       </c>
       <c r="B139" t="s">
-        <v>287</v>
+        <v>400</v>
       </c>
       <c r="C139" t="s">
-        <v>19</v>
+        <v>9</v>
+      </c>
+      <c r="J139" t="s">
+        <v>22</v>
       </c>
       <c r="K139" t="s">
-        <v>287</v>
+        <v>400</v>
       </c>
       <c r="L139" t="s">
-        <v>132</v>
+        <v>135</v>
       </c>
     </row>
     <row r="140" spans="1:12" ht="16.5" customHeight="1">
       <c r="A140" t="s">
-        <v>198</v>
+        <v>84</v>
       </c>
       <c r="B140" t="s">
-        <v>94</v>
+        <v>293</v>
       </c>
       <c r="C140" t="s">
         <v>19</v>
       </c>
       <c r="K140" t="s">
-        <v>94</v>
+        <v>293</v>
       </c>
       <c r="L140" t="s">
         <v>132</v>
@@ -4491,25 +4497,13 @@
         <v>84</v>
       </c>
       <c r="B141" t="s">
-        <v>151</v>
+        <v>287</v>
       </c>
       <c r="C141" t="s">
-        <v>9</v>
-      </c>
-      <c r="D141" t="s">
-        <v>359</v>
-      </c>
-      <c r="E141" t="s">
-        <v>152</v>
-      </c>
-      <c r="F141" t="s">
-        <v>12</v>
-      </c>
-      <c r="G141" t="s">
-        <v>13</v>
+        <v>19</v>
       </c>
       <c r="K141" t="s">
-        <v>151</v>
+        <v>287</v>
       </c>
       <c r="L141" t="s">
         <v>132</v>
@@ -4517,16 +4511,16 @@
     </row>
     <row r="142" spans="1:12" ht="16.5" customHeight="1">
       <c r="A142" t="s">
-        <v>84</v>
+        <v>198</v>
       </c>
       <c r="B142" t="s">
-        <v>150</v>
+        <v>94</v>
       </c>
       <c r="C142" t="s">
         <v>19</v>
       </c>
       <c r="K142" t="s">
-        <v>150</v>
+        <v>94</v>
       </c>
       <c r="L142" t="s">
         <v>132</v>
@@ -4537,16 +4531,28 @@
         <v>84</v>
       </c>
       <c r="B143" t="s">
-        <v>95</v>
+        <v>151</v>
       </c>
       <c r="C143" t="s">
-        <v>36</v>
+        <v>9</v>
+      </c>
+      <c r="D143" t="s">
+        <v>359</v>
+      </c>
+      <c r="E143" t="s">
+        <v>152</v>
+      </c>
+      <c r="F143" t="s">
+        <v>12</v>
+      </c>
+      <c r="G143" t="s">
+        <v>13</v>
       </c>
       <c r="K143" t="s">
-        <v>95</v>
+        <v>151</v>
       </c>
       <c r="L143" t="s">
-        <v>138</v>
+        <v>132</v>
       </c>
     </row>
     <row r="144" spans="1:12" ht="16.5" customHeight="1">
@@ -4554,28 +4560,16 @@
         <v>84</v>
       </c>
       <c r="B144" t="s">
-        <v>95</v>
+        <v>150</v>
       </c>
       <c r="C144" t="s">
-        <v>17</v>
-      </c>
-      <c r="D144" t="s">
-        <v>335</v>
-      </c>
-      <c r="E144" t="s">
-        <v>271</v>
-      </c>
-      <c r="F144" t="s">
-        <v>12</v>
-      </c>
-      <c r="G144" t="s">
-        <v>61</v>
+        <v>19</v>
       </c>
       <c r="K144" t="s">
-        <v>262</v>
-      </c>
-      <c r="L144" s="1" t="s">
-        <v>269</v>
+        <v>150</v>
+      </c>
+      <c r="L144" t="s">
+        <v>132</v>
       </c>
     </row>
     <row r="145" spans="1:12" ht="16.5" customHeight="1">
@@ -4583,19 +4577,16 @@
         <v>84</v>
       </c>
       <c r="B145" t="s">
-        <v>181</v>
+        <v>95</v>
       </c>
       <c r="C145" t="s">
-        <v>17</v>
-      </c>
-      <c r="H145" t="s">
-        <v>175</v>
+        <v>36</v>
       </c>
       <c r="K145" t="s">
-        <v>181</v>
+        <v>95</v>
       </c>
       <c r="L145" t="s">
-        <v>133</v>
+        <v>138</v>
       </c>
     </row>
     <row r="146" spans="1:12" ht="16.5" customHeight="1">
@@ -4603,19 +4594,28 @@
         <v>84</v>
       </c>
       <c r="B146" t="s">
-        <v>182</v>
+        <v>95</v>
       </c>
       <c r="C146" t="s">
         <v>17</v>
       </c>
-      <c r="H146" t="s">
-        <v>176</v>
+      <c r="D146" t="s">
+        <v>335</v>
+      </c>
+      <c r="E146" t="s">
+        <v>271</v>
+      </c>
+      <c r="F146" t="s">
+        <v>12</v>
+      </c>
+      <c r="G146" t="s">
+        <v>61</v>
       </c>
       <c r="K146" t="s">
-        <v>182</v>
-      </c>
-      <c r="L146" t="s">
-        <v>133</v>
+        <v>262</v>
+      </c>
+      <c r="L146" s="1" t="s">
+        <v>269</v>
       </c>
     </row>
     <row r="147" spans="1:12" ht="16.5" customHeight="1">
@@ -4623,16 +4623,16 @@
         <v>84</v>
       </c>
       <c r="B147" t="s">
-        <v>199</v>
+        <v>181</v>
       </c>
       <c r="C147" t="s">
         <v>17</v>
       </c>
       <c r="H147" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="K147" t="s">
-        <v>199</v>
+        <v>181</v>
       </c>
       <c r="L147" t="s">
         <v>133</v>
@@ -4643,19 +4643,19 @@
         <v>84</v>
       </c>
       <c r="B148" t="s">
-        <v>242</v>
+        <v>182</v>
       </c>
       <c r="C148" t="s">
         <v>17</v>
       </c>
       <c r="H148" t="s">
-        <v>244</v>
+        <v>176</v>
       </c>
       <c r="K148" t="s">
-        <v>242</v>
+        <v>182</v>
       </c>
       <c r="L148" t="s">
-        <v>243</v>
+        <v>133</v>
       </c>
     </row>
     <row r="149" spans="1:12" ht="16.5" customHeight="1">
@@ -4663,16 +4663,19 @@
         <v>84</v>
       </c>
       <c r="B149" t="s">
-        <v>185</v>
+        <v>199</v>
       </c>
       <c r="C149" t="s">
-        <v>36</v>
+        <v>17</v>
+      </c>
+      <c r="H149" t="s">
+        <v>174</v>
       </c>
       <c r="K149" t="s">
-        <v>185</v>
+        <v>199</v>
       </c>
       <c r="L149" t="s">
-        <v>272</v>
+        <v>133</v>
       </c>
     </row>
     <row r="150" spans="1:12" ht="16.5" customHeight="1">
@@ -4680,28 +4683,19 @@
         <v>84</v>
       </c>
       <c r="B150" t="s">
-        <v>185</v>
+        <v>242</v>
       </c>
       <c r="C150" t="s">
         <v>17</v>
       </c>
-      <c r="D150" t="s">
-        <v>335</v>
-      </c>
-      <c r="E150" t="s">
-        <v>271</v>
-      </c>
-      <c r="F150" t="s">
-        <v>12</v>
-      </c>
-      <c r="G150" t="s">
-        <v>61</v>
+      <c r="H150" t="s">
+        <v>244</v>
       </c>
       <c r="K150" t="s">
-        <v>261</v>
-      </c>
-      <c r="L150" s="1" t="s">
-        <v>269</v>
+        <v>242</v>
+      </c>
+      <c r="L150" t="s">
+        <v>243</v>
       </c>
     </row>
     <row r="151" spans="1:12" ht="16.5" customHeight="1">
@@ -4709,13 +4703,13 @@
         <v>84</v>
       </c>
       <c r="B151" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="C151" t="s">
         <v>36</v>
       </c>
       <c r="K151" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="L151" t="s">
         <v>272</v>
@@ -4726,7 +4720,7 @@
         <v>84</v>
       </c>
       <c r="B152" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="C152" t="s">
         <v>17</v>
@@ -4744,7 +4738,7 @@
         <v>61</v>
       </c>
       <c r="K152" t="s">
-        <v>260</v>
+        <v>261</v>
       </c>
       <c r="L152" s="1" t="s">
         <v>269</v>
@@ -4755,16 +4749,16 @@
         <v>84</v>
       </c>
       <c r="B153" t="s">
-        <v>173</v>
+        <v>186</v>
       </c>
       <c r="C153" t="s">
-        <v>9</v>
+        <v>36</v>
       </c>
       <c r="K153" t="s">
-        <v>173</v>
+        <v>186</v>
       </c>
       <c r="L153" t="s">
-        <v>136</v>
+        <v>272</v>
       </c>
     </row>
     <row r="154" spans="1:12" ht="16.5" customHeight="1">
@@ -4772,19 +4766,28 @@
         <v>84</v>
       </c>
       <c r="B154" t="s">
-        <v>320</v>
+        <v>186</v>
       </c>
       <c r="C154" t="s">
         <v>17</v>
       </c>
-      <c r="H154" t="s">
-        <v>322</v>
+      <c r="D154" t="s">
+        <v>335</v>
+      </c>
+      <c r="E154" t="s">
+        <v>271</v>
+      </c>
+      <c r="F154" t="s">
+        <v>12</v>
+      </c>
+      <c r="G154" t="s">
+        <v>61</v>
       </c>
       <c r="K154" t="s">
-        <v>320</v>
-      </c>
-      <c r="L154" t="s">
-        <v>243</v>
+        <v>260</v>
+      </c>
+      <c r="L154" s="1" t="s">
+        <v>269</v>
       </c>
     </row>
     <row r="155" spans="1:12" ht="16.5" customHeight="1">
@@ -4792,19 +4795,16 @@
         <v>84</v>
       </c>
       <c r="B155" t="s">
-        <v>321</v>
+        <v>173</v>
       </c>
       <c r="C155" t="s">
-        <v>17</v>
-      </c>
-      <c r="H155" t="s">
-        <v>323</v>
+        <v>9</v>
       </c>
       <c r="K155" t="s">
-        <v>321</v>
+        <v>173</v>
       </c>
       <c r="L155" t="s">
-        <v>243</v>
+        <v>136</v>
       </c>
     </row>
     <row r="156" spans="1:12" ht="16.5" customHeight="1">
@@ -4812,16 +4812,16 @@
         <v>84</v>
       </c>
       <c r="B156" t="s">
-        <v>324</v>
+        <v>320</v>
       </c>
       <c r="C156" t="s">
         <v>17</v>
       </c>
       <c r="H156" t="s">
-        <v>325</v>
+        <v>322</v>
       </c>
       <c r="K156" t="s">
-        <v>324</v>
+        <v>320</v>
       </c>
       <c r="L156" t="s">
         <v>243</v>
@@ -4832,16 +4832,19 @@
         <v>84</v>
       </c>
       <c r="B157" t="s">
-        <v>326</v>
+        <v>321</v>
       </c>
       <c r="C157" t="s">
-        <v>36</v>
+        <v>17</v>
+      </c>
+      <c r="H157" t="s">
+        <v>323</v>
       </c>
       <c r="K157" t="s">
-        <v>326</v>
+        <v>321</v>
       </c>
       <c r="L157" t="s">
-        <v>272</v>
+        <v>243</v>
       </c>
     </row>
     <row r="158" spans="1:12" ht="16.5" customHeight="1">
@@ -4849,28 +4852,19 @@
         <v>84</v>
       </c>
       <c r="B158" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
       <c r="C158" t="s">
         <v>17</v>
       </c>
-      <c r="D158" t="s">
-        <v>335</v>
-      </c>
-      <c r="E158" t="s">
-        <v>271</v>
-      </c>
-      <c r="F158" t="s">
-        <v>12</v>
-      </c>
-      <c r="G158" t="s">
-        <v>61</v>
+      <c r="H158" t="s">
+        <v>325</v>
       </c>
       <c r="K158" t="s">
-        <v>329</v>
-      </c>
-      <c r="L158" s="1" t="s">
-        <v>269</v>
+        <v>324</v>
+      </c>
+      <c r="L158" t="s">
+        <v>243</v>
       </c>
     </row>
     <row r="159" spans="1:12" ht="16.5" customHeight="1">
@@ -4878,13 +4872,13 @@
         <v>84</v>
       </c>
       <c r="B159" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="C159" t="s">
         <v>36</v>
       </c>
       <c r="K159" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="L159" t="s">
         <v>272</v>
@@ -4895,7 +4889,7 @@
         <v>84</v>
       </c>
       <c r="B160" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="C160" t="s">
         <v>17</v>
@@ -4913,7 +4907,7 @@
         <v>61</v>
       </c>
       <c r="K160" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="L160" s="1" t="s">
         <v>269</v>
@@ -4924,16 +4918,16 @@
         <v>84</v>
       </c>
       <c r="B161" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="C161" t="s">
-        <v>9</v>
+        <v>36</v>
       </c>
       <c r="K161" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="L161" t="s">
-        <v>136</v>
+        <v>272</v>
       </c>
     </row>
     <row r="162" spans="1:12" ht="16.5" customHeight="1">
@@ -4941,19 +4935,28 @@
         <v>84</v>
       </c>
       <c r="B162" t="s">
-        <v>183</v>
+        <v>327</v>
       </c>
       <c r="C162" t="s">
         <v>17</v>
       </c>
-      <c r="H162" t="s">
-        <v>180</v>
+      <c r="D162" t="s">
+        <v>335</v>
+      </c>
+      <c r="E162" t="s">
+        <v>271</v>
+      </c>
+      <c r="F162" t="s">
+        <v>12</v>
+      </c>
+      <c r="G162" t="s">
+        <v>61</v>
       </c>
       <c r="K162" t="s">
-        <v>183</v>
-      </c>
-      <c r="L162" t="s">
-        <v>133</v>
+        <v>330</v>
+      </c>
+      <c r="L162" s="1" t="s">
+        <v>269</v>
       </c>
     </row>
     <row r="163" spans="1:12" ht="16.5" customHeight="1">
@@ -4961,19 +4964,16 @@
         <v>84</v>
       </c>
       <c r="B163" t="s">
-        <v>184</v>
+        <v>328</v>
       </c>
       <c r="C163" t="s">
-        <v>17</v>
-      </c>
-      <c r="H163" t="s">
-        <v>179</v>
+        <v>9</v>
       </c>
       <c r="K163" t="s">
-        <v>184</v>
+        <v>328</v>
       </c>
       <c r="L163" t="s">
-        <v>133</v>
+        <v>136</v>
       </c>
     </row>
     <row r="164" spans="1:12" ht="16.5" customHeight="1">
@@ -4981,16 +4981,16 @@
         <v>84</v>
       </c>
       <c r="B164" t="s">
-        <v>200</v>
+        <v>183</v>
       </c>
       <c r="C164" t="s">
         <v>17</v>
       </c>
       <c r="H164" t="s">
-        <v>178</v>
+        <v>180</v>
       </c>
       <c r="K164" t="s">
-        <v>200</v>
+        <v>183</v>
       </c>
       <c r="L164" t="s">
         <v>133</v>
@@ -5001,19 +5001,19 @@
         <v>84</v>
       </c>
       <c r="B165" t="s">
-        <v>245</v>
+        <v>184</v>
       </c>
       <c r="C165" t="s">
         <v>17</v>
       </c>
       <c r="H165" t="s">
-        <v>246</v>
+        <v>179</v>
       </c>
       <c r="K165" t="s">
-        <v>245</v>
+        <v>184</v>
       </c>
       <c r="L165" t="s">
-        <v>243</v>
+        <v>133</v>
       </c>
     </row>
     <row r="166" spans="1:12" ht="16.5" customHeight="1">
@@ -5021,16 +5021,19 @@
         <v>84</v>
       </c>
       <c r="B166" t="s">
-        <v>187</v>
+        <v>200</v>
       </c>
       <c r="C166" t="s">
-        <v>36</v>
+        <v>17</v>
+      </c>
+      <c r="H166" t="s">
+        <v>178</v>
       </c>
       <c r="K166" t="s">
-        <v>187</v>
+        <v>200</v>
       </c>
       <c r="L166" t="s">
-        <v>272</v>
+        <v>133</v>
       </c>
     </row>
     <row r="167" spans="1:12" ht="16.5" customHeight="1">
@@ -5038,28 +5041,19 @@
         <v>84</v>
       </c>
       <c r="B167" t="s">
-        <v>187</v>
+        <v>245</v>
       </c>
       <c r="C167" t="s">
         <v>17</v>
       </c>
-      <c r="D167" t="s">
-        <v>335</v>
-      </c>
-      <c r="E167" t="s">
-        <v>271</v>
-      </c>
-      <c r="F167" t="s">
-        <v>12</v>
-      </c>
-      <c r="G167" t="s">
-        <v>61</v>
+      <c r="H167" t="s">
+        <v>246</v>
       </c>
       <c r="K167" t="s">
-        <v>259</v>
-      </c>
-      <c r="L167" s="1" t="s">
-        <v>269</v>
+        <v>245</v>
+      </c>
+      <c r="L167" t="s">
+        <v>243</v>
       </c>
     </row>
     <row r="168" spans="1:12" ht="16.5" customHeight="1">
@@ -5067,13 +5061,13 @@
         <v>84</v>
       </c>
       <c r="B168" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="C168" t="s">
         <v>36</v>
       </c>
       <c r="K168" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="L168" t="s">
         <v>272</v>
@@ -5084,7 +5078,7 @@
         <v>84</v>
       </c>
       <c r="B169" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="C169" t="s">
         <v>17</v>
@@ -5102,7 +5096,7 @@
         <v>61</v>
       </c>
       <c r="K169" t="s">
-        <v>258</v>
+        <v>259</v>
       </c>
       <c r="L169" s="1" t="s">
         <v>269</v>
@@ -5113,16 +5107,16 @@
         <v>84</v>
       </c>
       <c r="B170" t="s">
-        <v>177</v>
+        <v>188</v>
       </c>
       <c r="C170" t="s">
-        <v>9</v>
+        <v>36</v>
       </c>
       <c r="K170" t="s">
-        <v>177</v>
+        <v>188</v>
       </c>
       <c r="L170" t="s">
-        <v>136</v>
+        <v>272</v>
       </c>
     </row>
     <row r="171" spans="1:12" ht="16.5" customHeight="1">
@@ -5130,28 +5124,28 @@
         <v>84</v>
       </c>
       <c r="B171" t="s">
-        <v>207</v>
+        <v>188</v>
       </c>
       <c r="C171" t="s">
-        <v>9</v>
+        <v>17</v>
       </c>
       <c r="D171" t="s">
-        <v>351</v>
+        <v>335</v>
       </c>
       <c r="E171" t="s">
-        <v>208</v>
+        <v>271</v>
       </c>
       <c r="F171" t="s">
         <v>12</v>
       </c>
       <c r="G171" t="s">
-        <v>13</v>
+        <v>61</v>
       </c>
       <c r="K171" t="s">
-        <v>207</v>
-      </c>
-      <c r="L171" t="s">
-        <v>132</v>
+        <v>258</v>
+      </c>
+      <c r="L171" s="1" t="s">
+        <v>269</v>
       </c>
     </row>
     <row r="172" spans="1:12" ht="16.5" customHeight="1">
@@ -5159,19 +5153,16 @@
         <v>84</v>
       </c>
       <c r="B172" t="s">
-        <v>203</v>
+        <v>177</v>
       </c>
       <c r="C172" t="s">
-        <v>89</v>
-      </c>
-      <c r="H172" t="s">
-        <v>205</v>
+        <v>9</v>
       </c>
       <c r="K172" t="s">
-        <v>203</v>
+        <v>177</v>
       </c>
       <c r="L172" t="s">
-        <v>132</v>
+        <v>136</v>
       </c>
     </row>
     <row r="173" spans="1:12" ht="16.5" customHeight="1">
@@ -5179,16 +5170,25 @@
         <v>84</v>
       </c>
       <c r="B173" t="s">
-        <v>204</v>
+        <v>207</v>
       </c>
       <c r="C173" t="s">
-        <v>89</v>
-      </c>
-      <c r="H173" t="s">
-        <v>206</v>
+        <v>9</v>
+      </c>
+      <c r="D173" t="s">
+        <v>351</v>
+      </c>
+      <c r="E173" t="s">
+        <v>208</v>
+      </c>
+      <c r="F173" t="s">
+        <v>12</v>
+      </c>
+      <c r="G173" t="s">
+        <v>13</v>
       </c>
       <c r="K173" t="s">
-        <v>204</v>
+        <v>207</v>
       </c>
       <c r="L173" t="s">
         <v>132</v>
@@ -5196,28 +5196,19 @@
     </row>
     <row r="174" spans="1:12" ht="16.5" customHeight="1">
       <c r="A174" t="s">
-        <v>198</v>
+        <v>84</v>
       </c>
       <c r="B174" t="s">
-        <v>96</v>
+        <v>203</v>
       </c>
       <c r="C174" t="s">
-        <v>9</v>
-      </c>
-      <c r="D174" t="s">
-        <v>352</v>
-      </c>
-      <c r="E174" t="s">
-        <v>97</v>
-      </c>
-      <c r="F174" t="s">
-        <v>98</v>
-      </c>
-      <c r="G174" t="s">
-        <v>13</v>
+        <v>89</v>
+      </c>
+      <c r="H174" t="s">
+        <v>205</v>
       </c>
       <c r="K174" t="s">
-        <v>96</v>
+        <v>203</v>
       </c>
       <c r="L174" t="s">
         <v>132</v>
@@ -5228,25 +5219,16 @@
         <v>84</v>
       </c>
       <c r="B175" t="s">
-        <v>96</v>
+        <v>204</v>
       </c>
       <c r="C175" t="s">
-        <v>9</v>
-      </c>
-      <c r="D175" t="s">
-        <v>352</v>
-      </c>
-      <c r="F175" t="s">
-        <v>98</v>
+        <v>89</v>
       </c>
       <c r="H175" t="s">
-        <v>295</v>
-      </c>
-      <c r="I175" t="s">
-        <v>296</v>
+        <v>206</v>
       </c>
       <c r="K175" t="s">
-        <v>96</v>
+        <v>204</v>
       </c>
       <c r="L175" t="s">
         <v>132</v>
@@ -5257,25 +5239,25 @@
         <v>198</v>
       </c>
       <c r="B176" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="C176" t="s">
         <v>9</v>
       </c>
       <c r="D176" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="E176" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="F176" t="s">
-        <v>12</v>
+        <v>98</v>
       </c>
       <c r="G176" t="s">
         <v>13</v>
       </c>
       <c r="K176" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="L176" t="s">
         <v>132</v>
@@ -5286,25 +5268,25 @@
         <v>84</v>
       </c>
       <c r="B177" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="C177" t="s">
         <v>9</v>
       </c>
       <c r="D177" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="F177" t="s">
-        <v>12</v>
+        <v>98</v>
       </c>
       <c r="H177" t="s">
-        <v>297</v>
+        <v>295</v>
       </c>
       <c r="I177" t="s">
-        <v>298</v>
+        <v>296</v>
       </c>
       <c r="K177" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="L177" t="s">
         <v>132</v>
@@ -5312,19 +5294,31 @@
     </row>
     <row r="178" spans="1:12" ht="16.5" customHeight="1">
       <c r="A178" t="s">
-        <v>84</v>
+        <v>198</v>
       </c>
       <c r="B178" t="s">
-        <v>197</v>
+        <v>99</v>
       </c>
       <c r="C178" t="s">
         <v>9</v>
       </c>
+      <c r="D178" t="s">
+        <v>353</v>
+      </c>
+      <c r="E178" t="s">
+        <v>100</v>
+      </c>
+      <c r="F178" t="s">
+        <v>12</v>
+      </c>
+      <c r="G178" t="s">
+        <v>13</v>
+      </c>
       <c r="K178" t="s">
-        <v>197</v>
+        <v>99</v>
       </c>
       <c r="L178" t="s">
-        <v>136</v>
+        <v>132</v>
       </c>
     </row>
     <row r="179" spans="1:12" ht="16.5" customHeight="1">
@@ -5332,16 +5326,25 @@
         <v>84</v>
       </c>
       <c r="B179" t="s">
-        <v>195</v>
+        <v>99</v>
       </c>
       <c r="C179" t="s">
         <v>9</v>
       </c>
-      <c r="J179" t="s">
-        <v>42</v>
+      <c r="D179" t="s">
+        <v>353</v>
+      </c>
+      <c r="F179" t="s">
+        <v>12</v>
+      </c>
+      <c r="H179" t="s">
+        <v>297</v>
+      </c>
+      <c r="I179" t="s">
+        <v>298</v>
       </c>
       <c r="K179" t="s">
-        <v>195</v>
+        <v>99</v>
       </c>
       <c r="L179" t="s">
         <v>132</v>
@@ -5352,16 +5355,16 @@
         <v>84</v>
       </c>
       <c r="B180" t="s">
-        <v>140</v>
+        <v>197</v>
       </c>
       <c r="C180" t="s">
-        <v>56</v>
+        <v>9</v>
       </c>
       <c r="K180" t="s">
-        <v>140</v>
+        <v>197</v>
       </c>
       <c r="L180" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
     </row>
     <row r="181" spans="1:12" ht="16.5" customHeight="1">
@@ -5369,28 +5372,19 @@
         <v>84</v>
       </c>
       <c r="B181" t="s">
-        <v>140</v>
+        <v>195</v>
       </c>
       <c r="C181" t="s">
-        <v>17</v>
-      </c>
-      <c r="D181" t="s">
-        <v>335</v>
-      </c>
-      <c r="E181" t="s">
-        <v>271</v>
-      </c>
-      <c r="F181" t="s">
-        <v>12</v>
-      </c>
-      <c r="G181" t="s">
-        <v>61</v>
+        <v>9</v>
+      </c>
+      <c r="J181" t="s">
+        <v>42</v>
       </c>
       <c r="K181" t="s">
-        <v>257</v>
-      </c>
-      <c r="L181" s="1" t="s">
-        <v>270</v>
+        <v>195</v>
+      </c>
+      <c r="L181" t="s">
+        <v>132</v>
       </c>
     </row>
     <row r="182" spans="1:12" ht="16.5" customHeight="1">
@@ -5398,19 +5392,16 @@
         <v>84</v>
       </c>
       <c r="B182" t="s">
-        <v>144</v>
+        <v>140</v>
       </c>
       <c r="C182" t="s">
-        <v>17</v>
-      </c>
-      <c r="H182" t="s">
-        <v>143</v>
+        <v>56</v>
       </c>
       <c r="K182" t="s">
-        <v>144</v>
+        <v>140</v>
       </c>
       <c r="L182" t="s">
-        <v>133</v>
+        <v>138</v>
       </c>
     </row>
     <row r="183" spans="1:12" ht="16.5" customHeight="1">
@@ -5418,16 +5409,28 @@
         <v>84</v>
       </c>
       <c r="B183" t="s">
-        <v>101</v>
+        <v>140</v>
       </c>
       <c r="C183" t="s">
-        <v>19</v>
+        <v>17</v>
+      </c>
+      <c r="D183" t="s">
+        <v>335</v>
+      </c>
+      <c r="E183" t="s">
+        <v>271</v>
+      </c>
+      <c r="F183" t="s">
+        <v>12</v>
+      </c>
+      <c r="G183" t="s">
+        <v>61</v>
       </c>
       <c r="K183" t="s">
-        <v>101</v>
-      </c>
-      <c r="L183" t="s">
-        <v>132</v>
+        <v>257</v>
+      </c>
+      <c r="L183" s="1" t="s">
+        <v>270</v>
       </c>
     </row>
     <row r="184" spans="1:12" ht="16.5" customHeight="1">
@@ -5435,16 +5438,19 @@
         <v>84</v>
       </c>
       <c r="B184" t="s">
-        <v>102</v>
+        <v>144</v>
       </c>
       <c r="C184" t="s">
-        <v>9</v>
+        <v>17</v>
+      </c>
+      <c r="H184" t="s">
+        <v>143</v>
       </c>
       <c r="K184" t="s">
-        <v>102</v>
+        <v>144</v>
       </c>
       <c r="L184" t="s">
-        <v>138</v>
+        <v>133</v>
       </c>
     </row>
     <row r="185" spans="1:12" ht="16.5" customHeight="1">
@@ -5452,16 +5458,16 @@
         <v>84</v>
       </c>
       <c r="B185" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="C185" t="s">
-        <v>104</v>
+        <v>19</v>
       </c>
       <c r="K185" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="L185" t="s">
-        <v>138</v>
+        <v>132</v>
       </c>
     </row>
     <row r="186" spans="1:12" ht="16.5" customHeight="1">
@@ -5469,13 +5475,13 @@
         <v>84</v>
       </c>
       <c r="B186" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="C186" t="s">
-        <v>36</v>
+        <v>9</v>
       </c>
       <c r="K186" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="L186" t="s">
         <v>138</v>
@@ -5486,28 +5492,16 @@
         <v>84</v>
       </c>
       <c r="B187" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="C187" t="s">
-        <v>17</v>
-      </c>
-      <c r="D187" t="s">
-        <v>335</v>
-      </c>
-      <c r="E187" t="s">
-        <v>271</v>
-      </c>
-      <c r="F187" t="s">
-        <v>12</v>
-      </c>
-      <c r="G187" t="s">
-        <v>61</v>
+        <v>104</v>
       </c>
       <c r="K187" t="s">
-        <v>256</v>
-      </c>
-      <c r="L187" s="1" t="s">
-        <v>269</v>
+        <v>103</v>
+      </c>
+      <c r="L187" t="s">
+        <v>138</v>
       </c>
     </row>
     <row r="188" spans="1:12" ht="16.5" customHeight="1">
@@ -5515,13 +5509,13 @@
         <v>84</v>
       </c>
       <c r="B188" t="s">
-        <v>211</v>
+        <v>105</v>
       </c>
       <c r="C188" t="s">
-        <v>56</v>
+        <v>36</v>
       </c>
       <c r="K188" t="s">
-        <v>211</v>
+        <v>105</v>
       </c>
       <c r="L188" t="s">
         <v>138</v>
@@ -5532,7 +5526,7 @@
         <v>84</v>
       </c>
       <c r="B189" t="s">
-        <v>211</v>
+        <v>105</v>
       </c>
       <c r="C189" t="s">
         <v>17</v>
@@ -5550,10 +5544,10 @@
         <v>61</v>
       </c>
       <c r="K189" t="s">
-        <v>255</v>
+        <v>256</v>
       </c>
       <c r="L189" s="1" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
     </row>
     <row r="190" spans="1:12" ht="16.5" customHeight="1">
@@ -5561,13 +5555,13 @@
         <v>84</v>
       </c>
       <c r="B190" t="s">
-        <v>313</v>
+        <v>211</v>
       </c>
       <c r="C190" t="s">
-        <v>310</v>
+        <v>56</v>
       </c>
       <c r="K190" t="s">
-        <v>313</v>
+        <v>211</v>
       </c>
       <c r="L190" t="s">
         <v>138</v>
@@ -5578,45 +5572,45 @@
         <v>84</v>
       </c>
       <c r="B191" t="s">
-        <v>313</v>
+        <v>211</v>
       </c>
       <c r="C191" t="s">
-        <v>9</v>
+        <v>17</v>
+      </c>
+      <c r="D191" t="s">
+        <v>335</v>
+      </c>
+      <c r="E191" t="s">
+        <v>271</v>
+      </c>
+      <c r="F191" t="s">
+        <v>12</v>
+      </c>
+      <c r="G191" t="s">
+        <v>61</v>
       </c>
       <c r="K191" t="s">
-        <v>314</v>
+        <v>255</v>
       </c>
       <c r="L191" s="1" t="s">
-        <v>315</v>
+        <v>270</v>
       </c>
     </row>
     <row r="192" spans="1:12" ht="16.5" customHeight="1">
       <c r="A192" t="s">
-        <v>198</v>
+        <v>84</v>
       </c>
       <c r="B192" t="s">
-        <v>106</v>
+        <v>313</v>
       </c>
       <c r="C192" t="s">
-        <v>9</v>
-      </c>
-      <c r="D192" t="s">
-        <v>354</v>
-      </c>
-      <c r="E192" t="s">
-        <v>107</v>
-      </c>
-      <c r="F192" t="s">
-        <v>98</v>
-      </c>
-      <c r="G192" t="s">
-        <v>13</v>
+        <v>310</v>
       </c>
       <c r="K192" t="s">
-        <v>106</v>
+        <v>313</v>
       </c>
       <c r="L192" t="s">
-        <v>132</v>
+        <v>138</v>
       </c>
     </row>
     <row r="193" spans="1:12" ht="16.5" customHeight="1">
@@ -5624,48 +5618,45 @@
         <v>84</v>
       </c>
       <c r="B193" t="s">
-        <v>106</v>
+        <v>313</v>
       </c>
       <c r="C193" t="s">
         <v>9</v>
       </c>
-      <c r="D193" t="s">
-        <v>354</v>
-      </c>
-      <c r="F193" t="s">
-        <v>98</v>
-      </c>
-      <c r="H193" t="s">
-        <v>299</v>
-      </c>
-      <c r="I193" t="s">
-        <v>300</v>
-      </c>
       <c r="K193" t="s">
-        <v>106</v>
-      </c>
-      <c r="L193" t="s">
-        <v>132</v>
+        <v>314</v>
+      </c>
+      <c r="L193" s="1" t="s">
+        <v>315</v>
       </c>
     </row>
     <row r="194" spans="1:12" ht="16.5" customHeight="1">
       <c r="A194" t="s">
-        <v>84</v>
+        <v>198</v>
       </c>
       <c r="B194" t="s">
-        <v>153</v>
+        <v>106</v>
       </c>
       <c r="C194" t="s">
-        <v>17</v>
-      </c>
-      <c r="H194" t="s">
-        <v>154</v>
+        <v>9</v>
+      </c>
+      <c r="D194" t="s">
+        <v>354</v>
+      </c>
+      <c r="E194" t="s">
+        <v>107</v>
+      </c>
+      <c r="F194" t="s">
+        <v>98</v>
+      </c>
+      <c r="G194" t="s">
+        <v>13</v>
       </c>
       <c r="K194" t="s">
-        <v>153</v>
+        <v>106</v>
       </c>
       <c r="L194" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
     </row>
     <row r="195" spans="1:12" ht="16.5" customHeight="1">
@@ -5673,45 +5664,48 @@
         <v>84</v>
       </c>
       <c r="B195" t="s">
-        <v>147</v>
+        <v>106</v>
       </c>
       <c r="C195" t="s">
         <v>9</v>
       </c>
+      <c r="D195" t="s">
+        <v>354</v>
+      </c>
+      <c r="F195" t="s">
+        <v>98</v>
+      </c>
+      <c r="H195" t="s">
+        <v>299</v>
+      </c>
+      <c r="I195" t="s">
+        <v>300</v>
+      </c>
       <c r="K195" t="s">
-        <v>147</v>
+        <v>106</v>
       </c>
       <c r="L195" t="s">
-        <v>136</v>
+        <v>132</v>
       </c>
     </row>
     <row r="196" spans="1:12" ht="16.5" customHeight="1">
       <c r="A196" t="s">
-        <v>198</v>
+        <v>84</v>
       </c>
       <c r="B196" t="s">
-        <v>108</v>
+        <v>153</v>
       </c>
       <c r="C196" t="s">
-        <v>9</v>
-      </c>
-      <c r="D196" t="s">
-        <v>355</v>
-      </c>
-      <c r="E196" t="s">
-        <v>109</v>
-      </c>
-      <c r="F196" t="s">
-        <v>98</v>
-      </c>
-      <c r="G196" t="s">
-        <v>13</v>
+        <v>17</v>
+      </c>
+      <c r="H196" t="s">
+        <v>154</v>
       </c>
       <c r="K196" t="s">
-        <v>108</v>
+        <v>153</v>
       </c>
       <c r="L196" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
     </row>
     <row r="197" spans="1:12" ht="16.5" customHeight="1">
@@ -5719,28 +5713,16 @@
         <v>84</v>
       </c>
       <c r="B197" t="s">
-        <v>108</v>
+        <v>147</v>
       </c>
       <c r="C197" t="s">
         <v>9</v>
       </c>
-      <c r="D197" t="s">
-        <v>355</v>
-      </c>
-      <c r="F197" t="s">
-        <v>98</v>
-      </c>
-      <c r="H197" t="s">
-        <v>301</v>
-      </c>
-      <c r="I197" t="s">
-        <v>302</v>
-      </c>
       <c r="K197" t="s">
-        <v>108</v>
+        <v>147</v>
       </c>
       <c r="L197" t="s">
-        <v>132</v>
+        <v>136</v>
       </c>
     </row>
     <row r="198" spans="1:12" ht="16.5" customHeight="1">
@@ -5748,25 +5730,25 @@
         <v>198</v>
       </c>
       <c r="B198" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="C198" t="s">
         <v>9</v>
       </c>
       <c r="D198" t="s">
-        <v>353</v>
+        <v>355</v>
       </c>
       <c r="E198" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="F198" t="s">
-        <v>12</v>
+        <v>98</v>
       </c>
       <c r="G198" t="s">
         <v>13</v>
       </c>
       <c r="K198" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="L198" t="s">
         <v>132</v>
@@ -5777,25 +5759,25 @@
         <v>84</v>
       </c>
       <c r="B199" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="C199" t="s">
         <v>9</v>
       </c>
       <c r="D199" t="s">
-        <v>353</v>
+        <v>355</v>
       </c>
       <c r="F199" t="s">
-        <v>12</v>
+        <v>98</v>
       </c>
       <c r="H199" t="s">
-        <v>303</v>
+        <v>301</v>
       </c>
       <c r="I199" t="s">
-        <v>298</v>
+        <v>302</v>
       </c>
       <c r="K199" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="L199" t="s">
         <v>132</v>
@@ -5803,36 +5785,57 @@
     </row>
     <row r="200" spans="1:12" ht="16.5" customHeight="1">
       <c r="A200" t="s">
-        <v>84</v>
+        <v>198</v>
       </c>
       <c r="B200" t="s">
-        <v>196</v>
+        <v>110</v>
       </c>
       <c r="C200" t="s">
         <v>9</v>
       </c>
+      <c r="D200" t="s">
+        <v>353</v>
+      </c>
+      <c r="E200" t="s">
+        <v>111</v>
+      </c>
+      <c r="F200" t="s">
+        <v>12</v>
+      </c>
+      <c r="G200" t="s">
+        <v>13</v>
+      </c>
       <c r="K200" t="s">
-        <v>196</v>
+        <v>110</v>
       </c>
       <c r="L200" t="s">
-        <v>136</v>
+        <v>132</v>
       </c>
     </row>
     <row r="201" spans="1:12" ht="16.5" customHeight="1">
       <c r="A201" t="s">
-        <v>198</v>
+        <v>84</v>
       </c>
       <c r="B201" t="s">
-        <v>122</v>
+        <v>110</v>
       </c>
       <c r="C201" t="s">
         <v>9</v>
       </c>
-      <c r="J201" t="s">
-        <v>42</v>
+      <c r="D201" t="s">
+        <v>353</v>
+      </c>
+      <c r="F201" t="s">
+        <v>12</v>
+      </c>
+      <c r="H201" t="s">
+        <v>303</v>
+      </c>
+      <c r="I201" t="s">
+        <v>298</v>
       </c>
       <c r="K201" t="s">
-        <v>122</v>
+        <v>110</v>
       </c>
       <c r="L201" t="s">
         <v>132</v>
@@ -5843,45 +5846,36 @@
         <v>84</v>
       </c>
       <c r="B202" t="s">
-        <v>141</v>
+        <v>196</v>
       </c>
       <c r="C202" t="s">
-        <v>56</v>
+        <v>9</v>
       </c>
       <c r="K202" t="s">
-        <v>141</v>
+        <v>196</v>
       </c>
       <c r="L202" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
     </row>
     <row r="203" spans="1:12" ht="16.5" customHeight="1">
       <c r="A203" t="s">
-        <v>84</v>
+        <v>198</v>
       </c>
       <c r="B203" t="s">
-        <v>141</v>
+        <v>122</v>
       </c>
       <c r="C203" t="s">
-        <v>17</v>
-      </c>
-      <c r="D203" t="s">
-        <v>335</v>
-      </c>
-      <c r="E203" t="s">
-        <v>271</v>
-      </c>
-      <c r="F203" t="s">
-        <v>12</v>
-      </c>
-      <c r="G203" t="s">
-        <v>61</v>
+        <v>9</v>
+      </c>
+      <c r="J203" t="s">
+        <v>42</v>
       </c>
       <c r="K203" t="s">
-        <v>254</v>
-      </c>
-      <c r="L203" s="1" t="s">
-        <v>270</v>
+        <v>122</v>
+      </c>
+      <c r="L203" t="s">
+        <v>132</v>
       </c>
     </row>
     <row r="204" spans="1:12" ht="16.5" customHeight="1">
@@ -5889,19 +5883,16 @@
         <v>84</v>
       </c>
       <c r="B204" t="s">
-        <v>145</v>
+        <v>141</v>
       </c>
       <c r="C204" t="s">
-        <v>17</v>
-      </c>
-      <c r="H204" t="s">
-        <v>143</v>
+        <v>56</v>
       </c>
       <c r="K204" t="s">
-        <v>145</v>
+        <v>141</v>
       </c>
       <c r="L204" t="s">
-        <v>133</v>
+        <v>138</v>
       </c>
     </row>
     <row r="205" spans="1:12" ht="16.5" customHeight="1">
@@ -5909,16 +5900,28 @@
         <v>84</v>
       </c>
       <c r="B205" t="s">
-        <v>112</v>
+        <v>141</v>
       </c>
       <c r="C205" t="s">
-        <v>19</v>
+        <v>17</v>
+      </c>
+      <c r="D205" t="s">
+        <v>335</v>
+      </c>
+      <c r="E205" t="s">
+        <v>271</v>
+      </c>
+      <c r="F205" t="s">
+        <v>12</v>
+      </c>
+      <c r="G205" t="s">
+        <v>61</v>
       </c>
       <c r="K205" t="s">
-        <v>112</v>
-      </c>
-      <c r="L205" t="s">
-        <v>132</v>
+        <v>254</v>
+      </c>
+      <c r="L205" s="1" t="s">
+        <v>270</v>
       </c>
     </row>
     <row r="206" spans="1:12" ht="16.5" customHeight="1">
@@ -5926,16 +5929,19 @@
         <v>84</v>
       </c>
       <c r="B206" t="s">
-        <v>113</v>
+        <v>145</v>
       </c>
       <c r="C206" t="s">
-        <v>9</v>
+        <v>17</v>
+      </c>
+      <c r="H206" t="s">
+        <v>143</v>
       </c>
       <c r="K206" t="s">
-        <v>113</v>
+        <v>145</v>
       </c>
       <c r="L206" t="s">
-        <v>138</v>
+        <v>133</v>
       </c>
     </row>
     <row r="207" spans="1:12" ht="16.5" customHeight="1">
@@ -5943,16 +5949,16 @@
         <v>84</v>
       </c>
       <c r="B207" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="C207" t="s">
-        <v>104</v>
+        <v>19</v>
       </c>
       <c r="K207" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="L207" t="s">
-        <v>138</v>
+        <v>132</v>
       </c>
     </row>
     <row r="208" spans="1:12" ht="16.5" customHeight="1">
@@ -5960,13 +5966,13 @@
         <v>84</v>
       </c>
       <c r="B208" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="C208" t="s">
-        <v>36</v>
+        <v>9</v>
       </c>
       <c r="K208" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="L208" t="s">
         <v>138</v>
@@ -5977,28 +5983,16 @@
         <v>84</v>
       </c>
       <c r="B209" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="C209" t="s">
-        <v>17</v>
-      </c>
-      <c r="D209" t="s">
-        <v>335</v>
-      </c>
-      <c r="E209" t="s">
-        <v>271</v>
-      </c>
-      <c r="F209" t="s">
-        <v>12</v>
-      </c>
-      <c r="G209" t="s">
-        <v>61</v>
+        <v>104</v>
       </c>
       <c r="K209" t="s">
-        <v>253</v>
-      </c>
-      <c r="L209" s="1" t="s">
-        <v>269</v>
+        <v>114</v>
+      </c>
+      <c r="L209" t="s">
+        <v>138</v>
       </c>
     </row>
     <row r="210" spans="1:12" ht="16.5" customHeight="1">
@@ -6006,13 +6000,13 @@
         <v>84</v>
       </c>
       <c r="B210" t="s">
-        <v>210</v>
+        <v>115</v>
       </c>
       <c r="C210" t="s">
-        <v>56</v>
+        <v>36</v>
       </c>
       <c r="K210" t="s">
-        <v>210</v>
+        <v>115</v>
       </c>
       <c r="L210" t="s">
         <v>138</v>
@@ -6023,7 +6017,7 @@
         <v>84</v>
       </c>
       <c r="B211" t="s">
-        <v>210</v>
+        <v>115</v>
       </c>
       <c r="C211" t="s">
         <v>17</v>
@@ -6041,10 +6035,10 @@
         <v>61</v>
       </c>
       <c r="K211" t="s">
-        <v>252</v>
+        <v>253</v>
       </c>
       <c r="L211" s="1" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
     </row>
     <row r="212" spans="1:12" ht="16.5" customHeight="1">
@@ -6052,13 +6046,13 @@
         <v>84</v>
       </c>
       <c r="B212" t="s">
-        <v>316</v>
+        <v>210</v>
       </c>
       <c r="C212" t="s">
-        <v>310</v>
+        <v>56</v>
       </c>
       <c r="K212" t="s">
-        <v>316</v>
+        <v>210</v>
       </c>
       <c r="L212" t="s">
         <v>138</v>
@@ -6069,45 +6063,45 @@
         <v>84</v>
       </c>
       <c r="B213" t="s">
-        <v>316</v>
+        <v>210</v>
       </c>
       <c r="C213" t="s">
-        <v>9</v>
+        <v>17</v>
+      </c>
+      <c r="D213" t="s">
+        <v>335</v>
+      </c>
+      <c r="E213" t="s">
+        <v>271</v>
+      </c>
+      <c r="F213" t="s">
+        <v>12</v>
+      </c>
+      <c r="G213" t="s">
+        <v>61</v>
       </c>
       <c r="K213" t="s">
-        <v>317</v>
+        <v>252</v>
       </c>
       <c r="L213" s="1" t="s">
-        <v>315</v>
+        <v>270</v>
       </c>
     </row>
     <row r="214" spans="1:12" ht="16.5" customHeight="1">
       <c r="A214" t="s">
-        <v>198</v>
+        <v>84</v>
       </c>
       <c r="B214" t="s">
-        <v>116</v>
+        <v>316</v>
       </c>
       <c r="C214" t="s">
-        <v>9</v>
-      </c>
-      <c r="D214" t="s">
-        <v>354</v>
-      </c>
-      <c r="E214" t="s">
-        <v>117</v>
-      </c>
-      <c r="F214" t="s">
-        <v>98</v>
-      </c>
-      <c r="G214" t="s">
-        <v>13</v>
+        <v>310</v>
       </c>
       <c r="K214" t="s">
-        <v>116</v>
+        <v>316</v>
       </c>
       <c r="L214" t="s">
-        <v>132</v>
+        <v>138</v>
       </c>
     </row>
     <row r="215" spans="1:12" ht="16.5" customHeight="1">
@@ -6115,48 +6109,45 @@
         <v>84</v>
       </c>
       <c r="B215" t="s">
-        <v>116</v>
+        <v>316</v>
       </c>
       <c r="C215" t="s">
         <v>9</v>
       </c>
-      <c r="D215" t="s">
-        <v>354</v>
-      </c>
-      <c r="F215" t="s">
-        <v>98</v>
-      </c>
-      <c r="H215" t="s">
-        <v>304</v>
-      </c>
-      <c r="I215" t="s">
-        <v>300</v>
-      </c>
       <c r="K215" t="s">
-        <v>116</v>
-      </c>
-      <c r="L215" t="s">
-        <v>132</v>
+        <v>317</v>
+      </c>
+      <c r="L215" s="1" t="s">
+        <v>315</v>
       </c>
     </row>
     <row r="216" spans="1:12" ht="16.5" customHeight="1">
       <c r="A216" t="s">
-        <v>84</v>
+        <v>198</v>
       </c>
       <c r="B216" t="s">
-        <v>155</v>
+        <v>116</v>
       </c>
       <c r="C216" t="s">
-        <v>17</v>
-      </c>
-      <c r="H216" t="s">
-        <v>154</v>
+        <v>9</v>
+      </c>
+      <c r="D216" t="s">
+        <v>354</v>
+      </c>
+      <c r="E216" t="s">
+        <v>117</v>
+      </c>
+      <c r="F216" t="s">
+        <v>98</v>
+      </c>
+      <c r="G216" t="s">
+        <v>13</v>
       </c>
       <c r="K216" t="s">
-        <v>155</v>
+        <v>116</v>
       </c>
       <c r="L216" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
     </row>
     <row r="217" spans="1:12" ht="16.5" customHeight="1">
@@ -6164,16 +6155,28 @@
         <v>84</v>
       </c>
       <c r="B217" t="s">
-        <v>146</v>
+        <v>116</v>
       </c>
       <c r="C217" t="s">
         <v>9</v>
       </c>
+      <c r="D217" t="s">
+        <v>354</v>
+      </c>
+      <c r="F217" t="s">
+        <v>98</v>
+      </c>
+      <c r="H217" t="s">
+        <v>304</v>
+      </c>
+      <c r="I217" t="s">
+        <v>300</v>
+      </c>
       <c r="K217" t="s">
-        <v>146</v>
+        <v>116</v>
       </c>
       <c r="L217" t="s">
-        <v>136</v>
+        <v>132</v>
       </c>
     </row>
     <row r="218" spans="1:12" ht="16.5" customHeight="1">
@@ -6181,16 +6184,19 @@
         <v>84</v>
       </c>
       <c r="B218" t="s">
-        <v>118</v>
+        <v>155</v>
       </c>
       <c r="C218" t="s">
-        <v>89</v>
+        <v>17</v>
+      </c>
+      <c r="H218" t="s">
+        <v>154</v>
       </c>
       <c r="K218" t="s">
-        <v>118</v>
+        <v>155</v>
       </c>
       <c r="L218" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
     </row>
     <row r="219" spans="1:12" ht="16.5" customHeight="1">
@@ -6198,28 +6204,16 @@
         <v>84</v>
       </c>
       <c r="B219" t="s">
-        <v>119</v>
+        <v>146</v>
       </c>
       <c r="C219" t="s">
         <v>9</v>
       </c>
-      <c r="D219" t="s">
-        <v>360</v>
-      </c>
-      <c r="E219" t="s">
-        <v>120</v>
-      </c>
-      <c r="F219" t="s">
-        <v>12</v>
-      </c>
-      <c r="G219" t="s">
-        <v>13</v>
-      </c>
       <c r="K219" t="s">
-        <v>119</v>
+        <v>146</v>
       </c>
       <c r="L219" t="s">
-        <v>132</v>
+        <v>136</v>
       </c>
     </row>
     <row r="220" spans="1:12" ht="16.5" customHeight="1">
@@ -6227,42 +6221,42 @@
         <v>84</v>
       </c>
       <c r="B220" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="C220" t="s">
-        <v>9</v>
+        <v>89</v>
       </c>
       <c r="K220" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="L220" t="s">
-        <v>136</v>
+        <v>132</v>
       </c>
     </row>
     <row r="221" spans="1:12" ht="16.5" customHeight="1">
       <c r="A221" t="s">
-        <v>198</v>
+        <v>84</v>
       </c>
       <c r="B221" t="s">
-        <v>361</v>
+        <v>119</v>
       </c>
       <c r="C221" t="s">
         <v>9</v>
       </c>
       <c r="D221" t="s">
-        <v>362</v>
+        <v>360</v>
       </c>
       <c r="E221" t="s">
-        <v>363</v>
+        <v>120</v>
       </c>
       <c r="F221" t="s">
-        <v>98</v>
+        <v>12</v>
       </c>
       <c r="G221" t="s">
         <v>13</v>
       </c>
       <c r="K221" t="s">
-        <v>361</v>
+        <v>119</v>
       </c>
       <c r="L221" t="s">
         <v>132</v>
@@ -6273,28 +6267,16 @@
         <v>84</v>
       </c>
       <c r="B222" t="s">
-        <v>361</v>
+        <v>121</v>
       </c>
       <c r="C222" t="s">
         <v>9</v>
       </c>
-      <c r="D222" t="s">
-        <v>362</v>
-      </c>
-      <c r="F222" t="s">
-        <v>98</v>
-      </c>
-      <c r="H222" t="s">
-        <v>364</v>
-      </c>
-      <c r="I222" t="s">
-        <v>365</v>
-      </c>
       <c r="K222" t="s">
-        <v>361</v>
+        <v>121</v>
       </c>
       <c r="L222" t="s">
-        <v>132</v>
+        <v>136</v>
       </c>
     </row>
     <row r="223" spans="1:12" ht="16.5" customHeight="1">
@@ -6302,25 +6284,25 @@
         <v>198</v>
       </c>
       <c r="B223" t="s">
-        <v>366</v>
+        <v>361</v>
       </c>
       <c r="C223" t="s">
         <v>9</v>
       </c>
       <c r="D223" t="s">
-        <v>353</v>
+        <v>362</v>
       </c>
       <c r="E223" t="s">
-        <v>367</v>
+        <v>363</v>
       </c>
       <c r="F223" t="s">
-        <v>12</v>
+        <v>98</v>
       </c>
       <c r="G223" t="s">
         <v>13</v>
       </c>
       <c r="K223" t="s">
-        <v>366</v>
+        <v>361</v>
       </c>
       <c r="L223" t="s">
         <v>132</v>
@@ -6331,25 +6313,25 @@
         <v>84</v>
       </c>
       <c r="B224" t="s">
-        <v>366</v>
+        <v>361</v>
       </c>
       <c r="C224" t="s">
         <v>9</v>
       </c>
       <c r="D224" t="s">
-        <v>353</v>
+        <v>362</v>
       </c>
       <c r="F224" t="s">
-        <v>12</v>
+        <v>98</v>
       </c>
       <c r="H224" t="s">
-        <v>368</v>
+        <v>364</v>
       </c>
       <c r="I224" t="s">
-        <v>298</v>
+        <v>365</v>
       </c>
       <c r="K224" t="s">
-        <v>366</v>
+        <v>361</v>
       </c>
       <c r="L224" t="s">
         <v>132</v>
@@ -6357,36 +6339,57 @@
     </row>
     <row r="225" spans="1:12" ht="16.5" customHeight="1">
       <c r="A225" t="s">
-        <v>84</v>
+        <v>198</v>
       </c>
       <c r="B225" t="s">
-        <v>369</v>
+        <v>366</v>
       </c>
       <c r="C225" t="s">
         <v>9</v>
       </c>
+      <c r="D225" t="s">
+        <v>353</v>
+      </c>
+      <c r="E225" t="s">
+        <v>367</v>
+      </c>
+      <c r="F225" t="s">
+        <v>12</v>
+      </c>
+      <c r="G225" t="s">
+        <v>13</v>
+      </c>
       <c r="K225" t="s">
-        <v>369</v>
+        <v>366</v>
       </c>
       <c r="L225" t="s">
-        <v>136</v>
+        <v>132</v>
       </c>
     </row>
     <row r="226" spans="1:12" ht="16.5" customHeight="1">
       <c r="A226" t="s">
-        <v>198</v>
+        <v>84</v>
       </c>
       <c r="B226" t="s">
-        <v>122</v>
+        <v>366</v>
       </c>
       <c r="C226" t="s">
         <v>9</v>
       </c>
-      <c r="J226" t="s">
-        <v>42</v>
+      <c r="D226" t="s">
+        <v>353</v>
+      </c>
+      <c r="F226" t="s">
+        <v>12</v>
+      </c>
+      <c r="H226" t="s">
+        <v>368</v>
+      </c>
+      <c r="I226" t="s">
+        <v>298</v>
       </c>
       <c r="K226" t="s">
-        <v>122</v>
+        <v>366</v>
       </c>
       <c r="L226" t="s">
         <v>132</v>
@@ -6397,45 +6400,36 @@
         <v>84</v>
       </c>
       <c r="B227" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
       <c r="C227" t="s">
-        <v>56</v>
+        <v>9</v>
       </c>
       <c r="K227" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
       <c r="L227" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
     </row>
     <row r="228" spans="1:12" ht="16.5" customHeight="1">
       <c r="A228" t="s">
-        <v>84</v>
+        <v>198</v>
       </c>
       <c r="B228" t="s">
-        <v>370</v>
+        <v>122</v>
       </c>
       <c r="C228" t="s">
-        <v>17</v>
-      </c>
-      <c r="D228" t="s">
-        <v>335</v>
-      </c>
-      <c r="E228" t="s">
-        <v>271</v>
-      </c>
-      <c r="F228" t="s">
-        <v>12</v>
-      </c>
-      <c r="G228" t="s">
-        <v>61</v>
+        <v>9</v>
+      </c>
+      <c r="J228" t="s">
+        <v>42</v>
       </c>
       <c r="K228" t="s">
-        <v>371</v>
-      </c>
-      <c r="L228" s="1" t="s">
-        <v>270</v>
+        <v>122</v>
+      </c>
+      <c r="L228" t="s">
+        <v>132</v>
       </c>
     </row>
     <row r="229" spans="1:12" ht="16.5" customHeight="1">
@@ -6443,19 +6437,16 @@
         <v>84</v>
       </c>
       <c r="B229" t="s">
-        <v>372</v>
+        <v>370</v>
       </c>
       <c r="C229" t="s">
-        <v>17</v>
-      </c>
-      <c r="H229" t="s">
-        <v>143</v>
+        <v>56</v>
       </c>
       <c r="K229" t="s">
-        <v>372</v>
+        <v>370</v>
       </c>
       <c r="L229" t="s">
-        <v>133</v>
+        <v>138</v>
       </c>
     </row>
     <row r="230" spans="1:12" ht="16.5" customHeight="1">
@@ -6463,16 +6454,28 @@
         <v>84</v>
       </c>
       <c r="B230" t="s">
-        <v>373</v>
+        <v>370</v>
       </c>
       <c r="C230" t="s">
-        <v>19</v>
+        <v>17</v>
+      </c>
+      <c r="D230" t="s">
+        <v>335</v>
+      </c>
+      <c r="E230" t="s">
+        <v>271</v>
+      </c>
+      <c r="F230" t="s">
+        <v>12</v>
+      </c>
+      <c r="G230" t="s">
+        <v>61</v>
       </c>
       <c r="K230" t="s">
-        <v>373</v>
-      </c>
-      <c r="L230" t="s">
-        <v>132</v>
+        <v>371</v>
+      </c>
+      <c r="L230" s="1" t="s">
+        <v>270</v>
       </c>
     </row>
     <row r="231" spans="1:12" ht="16.5" customHeight="1">
@@ -6480,16 +6483,19 @@
         <v>84</v>
       </c>
       <c r="B231" t="s">
-        <v>374</v>
+        <v>372</v>
       </c>
       <c r="C231" t="s">
-        <v>9</v>
+        <v>17</v>
+      </c>
+      <c r="H231" t="s">
+        <v>143</v>
       </c>
       <c r="K231" t="s">
-        <v>374</v>
+        <v>372</v>
       </c>
       <c r="L231" t="s">
-        <v>138</v>
+        <v>133</v>
       </c>
     </row>
     <row r="232" spans="1:12" ht="16.5" customHeight="1">
@@ -6497,16 +6503,16 @@
         <v>84</v>
       </c>
       <c r="B232" t="s">
-        <v>375</v>
+        <v>373</v>
       </c>
       <c r="C232" t="s">
-        <v>104</v>
+        <v>19</v>
       </c>
       <c r="K232" t="s">
-        <v>375</v>
+        <v>373</v>
       </c>
       <c r="L232" t="s">
-        <v>138</v>
+        <v>132</v>
       </c>
     </row>
     <row r="233" spans="1:12" ht="16.5" customHeight="1">
@@ -6514,13 +6520,13 @@
         <v>84</v>
       </c>
       <c r="B233" t="s">
-        <v>376</v>
+        <v>374</v>
       </c>
       <c r="C233" t="s">
-        <v>36</v>
+        <v>9</v>
       </c>
       <c r="K233" t="s">
-        <v>376</v>
+        <v>374</v>
       </c>
       <c r="L233" t="s">
         <v>138</v>
@@ -6531,28 +6537,16 @@
         <v>84</v>
       </c>
       <c r="B234" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="C234" t="s">
-        <v>17</v>
-      </c>
-      <c r="D234" t="s">
-        <v>335</v>
-      </c>
-      <c r="E234" t="s">
-        <v>271</v>
-      </c>
-      <c r="F234" t="s">
-        <v>12</v>
-      </c>
-      <c r="G234" t="s">
-        <v>61</v>
+        <v>104</v>
       </c>
       <c r="K234" t="s">
-        <v>377</v>
-      </c>
-      <c r="L234" s="1" t="s">
-        <v>269</v>
+        <v>375</v>
+      </c>
+      <c r="L234" t="s">
+        <v>138</v>
       </c>
     </row>
     <row r="235" spans="1:12" ht="16.5" customHeight="1">
@@ -6560,13 +6554,13 @@
         <v>84</v>
       </c>
       <c r="B235" t="s">
-        <v>378</v>
+        <v>376</v>
       </c>
       <c r="C235" t="s">
-        <v>56</v>
+        <v>36</v>
       </c>
       <c r="K235" t="s">
-        <v>378</v>
+        <v>376</v>
       </c>
       <c r="L235" t="s">
         <v>138</v>
@@ -6577,7 +6571,7 @@
         <v>84</v>
       </c>
       <c r="B236" t="s">
-        <v>378</v>
+        <v>376</v>
       </c>
       <c r="C236" t="s">
         <v>17</v>
@@ -6595,10 +6589,10 @@
         <v>61</v>
       </c>
       <c r="K236" t="s">
-        <v>379</v>
+        <v>377</v>
       </c>
       <c r="L236" s="1" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
     </row>
     <row r="237" spans="1:12" ht="16.5" customHeight="1">
@@ -6606,13 +6600,13 @@
         <v>84</v>
       </c>
       <c r="B237" t="s">
-        <v>380</v>
+        <v>378</v>
       </c>
       <c r="C237" t="s">
-        <v>310</v>
+        <v>56</v>
       </c>
       <c r="K237" t="s">
-        <v>380</v>
+        <v>378</v>
       </c>
       <c r="L237" t="s">
         <v>138</v>
@@ -6623,45 +6617,45 @@
         <v>84</v>
       </c>
       <c r="B238" t="s">
-        <v>380</v>
+        <v>378</v>
       </c>
       <c r="C238" t="s">
-        <v>9</v>
+        <v>17</v>
+      </c>
+      <c r="D238" t="s">
+        <v>335</v>
+      </c>
+      <c r="E238" t="s">
+        <v>271</v>
+      </c>
+      <c r="F238" t="s">
+        <v>12</v>
+      </c>
+      <c r="G238" t="s">
+        <v>61</v>
       </c>
       <c r="K238" t="s">
-        <v>381</v>
+        <v>379</v>
       </c>
       <c r="L238" s="1" t="s">
-        <v>315</v>
+        <v>270</v>
       </c>
     </row>
     <row r="239" spans="1:12" ht="16.5" customHeight="1">
       <c r="A239" t="s">
-        <v>198</v>
+        <v>84</v>
       </c>
       <c r="B239" t="s">
-        <v>382</v>
+        <v>380</v>
       </c>
       <c r="C239" t="s">
-        <v>9</v>
-      </c>
-      <c r="D239" t="s">
-        <v>354</v>
-      </c>
-      <c r="E239" t="s">
-        <v>385</v>
-      </c>
-      <c r="F239" t="s">
-        <v>98</v>
-      </c>
-      <c r="G239" t="s">
-        <v>13</v>
+        <v>310</v>
       </c>
       <c r="K239" t="s">
-        <v>382</v>
+        <v>380</v>
       </c>
       <c r="L239" t="s">
-        <v>132</v>
+        <v>138</v>
       </c>
     </row>
     <row r="240" spans="1:12" ht="16.5" customHeight="1">
@@ -6669,48 +6663,45 @@
         <v>84</v>
       </c>
       <c r="B240" t="s">
-        <v>382</v>
+        <v>380</v>
       </c>
       <c r="C240" t="s">
         <v>9</v>
       </c>
-      <c r="D240" t="s">
-        <v>354</v>
-      </c>
-      <c r="F240" t="s">
-        <v>98</v>
-      </c>
-      <c r="H240" t="s">
-        <v>386</v>
-      </c>
-      <c r="I240" t="s">
-        <v>300</v>
-      </c>
       <c r="K240" t="s">
-        <v>382</v>
-      </c>
-      <c r="L240" t="s">
-        <v>132</v>
+        <v>381</v>
+      </c>
+      <c r="L240" s="1" t="s">
+        <v>315</v>
       </c>
     </row>
     <row r="241" spans="1:12" ht="16.5" customHeight="1">
       <c r="A241" t="s">
-        <v>84</v>
+        <v>198</v>
       </c>
       <c r="B241" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
       <c r="C241" t="s">
-        <v>17</v>
-      </c>
-      <c r="H241" t="s">
-        <v>154</v>
+        <v>9</v>
+      </c>
+      <c r="D241" t="s">
+        <v>354</v>
+      </c>
+      <c r="E241" t="s">
+        <v>385</v>
+      </c>
+      <c r="F241" t="s">
+        <v>98</v>
+      </c>
+      <c r="G241" t="s">
+        <v>13</v>
       </c>
       <c r="K241" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
       <c r="L241" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
     </row>
     <row r="242" spans="1:12" ht="16.5" customHeight="1">
@@ -6718,16 +6709,28 @@
         <v>84</v>
       </c>
       <c r="B242" t="s">
-        <v>384</v>
+        <v>382</v>
       </c>
       <c r="C242" t="s">
         <v>9</v>
       </c>
+      <c r="D242" t="s">
+        <v>354</v>
+      </c>
+      <c r="F242" t="s">
+        <v>98</v>
+      </c>
+      <c r="H242" t="s">
+        <v>386</v>
+      </c>
+      <c r="I242" t="s">
+        <v>300</v>
+      </c>
       <c r="K242" t="s">
-        <v>384</v>
+        <v>382</v>
       </c>
       <c r="L242" t="s">
-        <v>136</v>
+        <v>132</v>
       </c>
     </row>
     <row r="243" spans="1:12" ht="16.5" customHeight="1">
@@ -6735,16 +6738,19 @@
         <v>84</v>
       </c>
       <c r="B243" t="s">
-        <v>164</v>
+        <v>383</v>
       </c>
       <c r="C243" t="s">
-        <v>89</v>
+        <v>17</v>
+      </c>
+      <c r="H243" t="s">
+        <v>154</v>
       </c>
       <c r="K243" t="s">
-        <v>164</v>
+        <v>383</v>
       </c>
       <c r="L243" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
     </row>
     <row r="244" spans="1:12" ht="16.5" customHeight="1">
@@ -6752,28 +6758,16 @@
         <v>84</v>
       </c>
       <c r="B244" t="s">
-        <v>165</v>
+        <v>384</v>
       </c>
       <c r="C244" t="s">
         <v>9</v>
       </c>
-      <c r="D244" t="s">
-        <v>341</v>
-      </c>
-      <c r="E244" t="s">
-        <v>167</v>
-      </c>
-      <c r="F244" t="s">
-        <v>12</v>
-      </c>
-      <c r="G244" t="s">
-        <v>13</v>
-      </c>
       <c r="K244" t="s">
-        <v>165</v>
+        <v>384</v>
       </c>
       <c r="L244" t="s">
-        <v>132</v>
+        <v>136</v>
       </c>
     </row>
     <row r="245" spans="1:12" ht="16.5" customHeight="1">
@@ -6781,16 +6775,16 @@
         <v>84</v>
       </c>
       <c r="B245" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="C245" t="s">
-        <v>9</v>
+        <v>89</v>
       </c>
       <c r="K245" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="L245" t="s">
-        <v>136</v>
+        <v>132</v>
       </c>
     </row>
     <row r="246" spans="1:12" ht="16.5" customHeight="1">
@@ -6798,13 +6792,25 @@
         <v>84</v>
       </c>
       <c r="B246" t="s">
-        <v>168</v>
+        <v>165</v>
       </c>
       <c r="C246" t="s">
-        <v>19</v>
+        <v>9</v>
+      </c>
+      <c r="D246" t="s">
+        <v>341</v>
+      </c>
+      <c r="E246" t="s">
+        <v>167</v>
+      </c>
+      <c r="F246" t="s">
+        <v>12</v>
+      </c>
+      <c r="G246" t="s">
+        <v>13</v>
       </c>
       <c r="K246" t="s">
-        <v>168</v>
+        <v>165</v>
       </c>
       <c r="L246" t="s">
         <v>132</v>
@@ -6815,19 +6821,16 @@
         <v>84</v>
       </c>
       <c r="B247" t="s">
-        <v>122</v>
+        <v>166</v>
       </c>
       <c r="C247" t="s">
         <v>9</v>
       </c>
-      <c r="J247" t="s">
-        <v>42</v>
-      </c>
       <c r="K247" t="s">
-        <v>122</v>
+        <v>166</v>
       </c>
       <c r="L247" t="s">
-        <v>132</v>
+        <v>136</v>
       </c>
     </row>
     <row r="248" spans="1:12" ht="16.5" customHeight="1">
@@ -6835,25 +6838,13 @@
         <v>84</v>
       </c>
       <c r="B248" t="s">
-        <v>123</v>
+        <v>168</v>
       </c>
       <c r="C248" t="s">
-        <v>9</v>
-      </c>
-      <c r="D248" t="s">
-        <v>335</v>
-      </c>
-      <c r="E248" t="s">
-        <v>124</v>
-      </c>
-      <c r="F248" t="s">
-        <v>12</v>
-      </c>
-      <c r="G248" t="s">
-        <v>13</v>
+        <v>19</v>
       </c>
       <c r="K248" t="s">
-        <v>123</v>
+        <v>168</v>
       </c>
       <c r="L248" t="s">
         <v>132</v>
@@ -6864,16 +6855,19 @@
         <v>84</v>
       </c>
       <c r="B249" t="s">
-        <v>228</v>
+        <v>122</v>
       </c>
       <c r="C249" t="s">
-        <v>56</v>
+        <v>9</v>
+      </c>
+      <c r="J249" t="s">
+        <v>42</v>
       </c>
       <c r="K249" t="s">
-        <v>228</v>
+        <v>122</v>
       </c>
       <c r="L249" t="s">
-        <v>138</v>
+        <v>132</v>
       </c>
     </row>
     <row r="250" spans="1:12" ht="16.5" customHeight="1">
@@ -6881,28 +6875,28 @@
         <v>84</v>
       </c>
       <c r="B250" t="s">
-        <v>228</v>
+        <v>123</v>
       </c>
       <c r="C250" t="s">
-        <v>17</v>
+        <v>9</v>
       </c>
       <c r="D250" t="s">
         <v>335</v>
       </c>
       <c r="E250" t="s">
-        <v>271</v>
+        <v>124</v>
       </c>
       <c r="F250" t="s">
         <v>12</v>
       </c>
       <c r="G250" t="s">
-        <v>61</v>
+        <v>13</v>
       </c>
       <c r="K250" t="s">
-        <v>251</v>
-      </c>
-      <c r="L250" s="1" t="s">
-        <v>270</v>
+        <v>123</v>
+      </c>
+      <c r="L250" t="s">
+        <v>132</v>
       </c>
     </row>
     <row r="251" spans="1:12" ht="16.5" customHeight="1">
@@ -6910,16 +6904,16 @@
         <v>84</v>
       </c>
       <c r="B251" t="s">
-        <v>161</v>
+        <v>228</v>
       </c>
       <c r="C251" t="s">
-        <v>9</v>
+        <v>56</v>
       </c>
       <c r="K251" t="s">
-        <v>161</v>
+        <v>228</v>
       </c>
       <c r="L251" t="s">
-        <v>136</v>
+        <v>138</v>
       </c>
     </row>
     <row r="252" spans="1:12" ht="16.5" customHeight="1">
@@ -6927,62 +6921,62 @@
         <v>84</v>
       </c>
       <c r="B252" t="s">
-        <v>209</v>
+        <v>228</v>
       </c>
       <c r="C252" t="s">
-        <v>89</v>
+        <v>17</v>
+      </c>
+      <c r="D252" t="s">
+        <v>335</v>
+      </c>
+      <c r="E252" t="s">
+        <v>271</v>
+      </c>
+      <c r="F252" t="s">
+        <v>12</v>
+      </c>
+      <c r="G252" t="s">
+        <v>61</v>
       </c>
       <c r="K252" t="s">
-        <v>209</v>
-      </c>
-      <c r="L252" t="s">
-        <v>132</v>
+        <v>251</v>
+      </c>
+      <c r="L252" s="1" t="s">
+        <v>270</v>
       </c>
     </row>
     <row r="253" spans="1:12" ht="16.5" customHeight="1">
       <c r="A253" t="s">
-        <v>125</v>
+        <v>84</v>
       </c>
       <c r="B253" t="s">
-        <v>126</v>
+        <v>161</v>
       </c>
       <c r="C253" t="s">
         <v>9</v>
       </c>
       <c r="K253" t="s">
-        <v>126</v>
+        <v>161</v>
       </c>
       <c r="L253" t="s">
-        <v>131</v>
+        <v>136</v>
       </c>
     </row>
     <row r="254" spans="1:12" ht="16.5" customHeight="1">
       <c r="A254" t="s">
-        <v>125</v>
+        <v>84</v>
       </c>
       <c r="B254" t="s">
-        <v>127</v>
+        <v>209</v>
       </c>
       <c r="C254" t="s">
-        <v>9</v>
-      </c>
-      <c r="D254" t="s">
-        <v>332</v>
-      </c>
-      <c r="E254" t="s">
-        <v>11</v>
-      </c>
-      <c r="F254" t="s">
-        <v>12</v>
-      </c>
-      <c r="G254" t="s">
-        <v>13</v>
+        <v>89</v>
       </c>
       <c r="K254" t="s">
-        <v>127</v>
+        <v>209</v>
       </c>
       <c r="L254" t="s">
-        <v>163</v>
+        <v>132</v>
       </c>
     </row>
     <row r="255" spans="1:12" ht="16.5" customHeight="1">
@@ -6990,16 +6984,16 @@
         <v>125</v>
       </c>
       <c r="B255" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="C255" t="s">
-        <v>17</v>
+        <v>9</v>
       </c>
       <c r="K255" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="L255" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
     </row>
     <row r="256" spans="1:12" ht="16.5" customHeight="1">
@@ -7007,16 +7001,28 @@
         <v>125</v>
       </c>
       <c r="B256" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="C256" t="s">
-        <v>19</v>
+        <v>9</v>
+      </c>
+      <c r="D256" t="s">
+        <v>332</v>
+      </c>
+      <c r="E256" t="s">
+        <v>11</v>
+      </c>
+      <c r="F256" t="s">
+        <v>12</v>
+      </c>
+      <c r="G256" t="s">
+        <v>13</v>
       </c>
       <c r="K256" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="L256" t="s">
-        <v>132</v>
+        <v>163</v>
       </c>
     </row>
     <row r="257" spans="1:12" ht="16.5" customHeight="1">
@@ -7024,16 +7030,16 @@
         <v>125</v>
       </c>
       <c r="B257" t="s">
-        <v>294</v>
+        <v>128</v>
       </c>
       <c r="C257" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="K257" t="s">
-        <v>294</v>
+        <v>128</v>
       </c>
       <c r="L257" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
     </row>
     <row r="258" spans="1:12" ht="16.5" customHeight="1">
@@ -7041,25 +7047,13 @@
         <v>125</v>
       </c>
       <c r="B258" t="s">
-        <v>216</v>
+        <v>129</v>
       </c>
       <c r="C258" t="s">
-        <v>17</v>
-      </c>
-      <c r="D258" t="s">
-        <v>356</v>
-      </c>
-      <c r="E258" t="s">
-        <v>219</v>
-      </c>
-      <c r="F258" t="s">
-        <v>215</v>
-      </c>
-      <c r="G258" t="s">
-        <v>221</v>
+        <v>19</v>
       </c>
       <c r="K258" t="s">
-        <v>216</v>
+        <v>129</v>
       </c>
       <c r="L258" t="s">
         <v>132</v>
@@ -7070,13 +7064,13 @@
         <v>125</v>
       </c>
       <c r="B259" t="s">
-        <v>217</v>
+        <v>294</v>
       </c>
       <c r="C259" t="s">
         <v>19</v>
       </c>
       <c r="K259" t="s">
-        <v>217</v>
+        <v>294</v>
       </c>
       <c r="L259" t="s">
         <v>132</v>
@@ -7087,16 +7081,28 @@
         <v>125</v>
       </c>
       <c r="B260" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="C260" t="s">
-        <v>56</v>
+        <v>17</v>
+      </c>
+      <c r="D260" t="s">
+        <v>356</v>
+      </c>
+      <c r="E260" t="s">
+        <v>219</v>
+      </c>
+      <c r="F260" t="s">
+        <v>215</v>
+      </c>
+      <c r="G260" t="s">
+        <v>221</v>
       </c>
       <c r="K260" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="L260" t="s">
-        <v>138</v>
+        <v>132</v>
       </c>
     </row>
     <row r="261" spans="1:12" ht="16.5" customHeight="1">
@@ -7104,28 +7110,16 @@
         <v>125</v>
       </c>
       <c r="B261" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="C261" t="s">
-        <v>17</v>
-      </c>
-      <c r="D261" t="s">
-        <v>335</v>
-      </c>
-      <c r="E261" t="s">
-        <v>271</v>
-      </c>
-      <c r="F261" t="s">
-        <v>12</v>
-      </c>
-      <c r="G261" t="s">
-        <v>61</v>
+        <v>19</v>
       </c>
       <c r="K261" t="s">
-        <v>250</v>
-      </c>
-      <c r="L261" s="1" t="s">
-        <v>270</v>
+        <v>217</v>
+      </c>
+      <c r="L261" t="s">
+        <v>132</v>
       </c>
     </row>
     <row r="262" spans="1:12" ht="16.5" customHeight="1">
@@ -7133,19 +7127,16 @@
         <v>125</v>
       </c>
       <c r="B262" t="s">
-        <v>229</v>
+        <v>218</v>
       </c>
       <c r="C262" t="s">
-        <v>9</v>
-      </c>
-      <c r="J262" t="s">
-        <v>22</v>
+        <v>56</v>
       </c>
       <c r="K262" t="s">
-        <v>229</v>
+        <v>218</v>
       </c>
       <c r="L262" t="s">
-        <v>132</v>
+        <v>138</v>
       </c>
     </row>
     <row r="263" spans="1:12" ht="16.5" customHeight="1">
@@ -7153,27 +7144,76 @@
         <v>125</v>
       </c>
       <c r="B263" t="s">
-        <v>239</v>
+        <v>218</v>
       </c>
       <c r="C263" t="s">
         <v>17</v>
       </c>
       <c r="D263" t="s">
-        <v>357</v>
+        <v>335</v>
       </c>
       <c r="E263" t="s">
-        <v>240</v>
+        <v>271</v>
       </c>
       <c r="F263" t="s">
         <v>12</v>
       </c>
       <c r="G263" t="s">
+        <v>61</v>
+      </c>
+      <c r="K263" t="s">
+        <v>250</v>
+      </c>
+      <c r="L263" s="1" t="s">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="264" spans="1:12" ht="16.5" customHeight="1">
+      <c r="A264" t="s">
+        <v>125</v>
+      </c>
+      <c r="B264" t="s">
+        <v>229</v>
+      </c>
+      <c r="C264" t="s">
+        <v>9</v>
+      </c>
+      <c r="J264" t="s">
+        <v>22</v>
+      </c>
+      <c r="K264" t="s">
+        <v>229</v>
+      </c>
+      <c r="L264" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="265" spans="1:12" ht="16.5" customHeight="1">
+      <c r="A265" t="s">
+        <v>125</v>
+      </c>
+      <c r="B265" t="s">
+        <v>239</v>
+      </c>
+      <c r="C265" t="s">
+        <v>17</v>
+      </c>
+      <c r="D265" t="s">
+        <v>357</v>
+      </c>
+      <c r="E265" t="s">
+        <v>240</v>
+      </c>
+      <c r="F265" t="s">
+        <v>12</v>
+      </c>
+      <c r="G265" t="s">
         <v>241</v>
       </c>
-      <c r="K263" t="s">
+      <c r="K265" t="s">
         <v>239</v>
       </c>
-      <c r="L263" t="s">
+      <c r="L265" t="s">
         <v>132</v>
       </c>
     </row>

</xml_diff>

<commit_message>
add input field 'external id' search criterion
</commit_message>
<xml_diff>
--- a/criterion_property_definitions.xlsx
+++ b/criterion_property_definitions.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1702" uniqueCount="404">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1717" uniqueCount="407">
   <si>
     <t>property</t>
   </si>
@@ -1229,6 +1229,15 @@
   </si>
   <si>
     <t>proband.animalParticulars.alias</t>
+  </si>
+  <si>
+    <t>inputField.titleL10nKey</t>
+  </si>
+  <si>
+    <t>inputField.externalId</t>
+  </si>
+  <si>
+    <t>inputField.localized</t>
   </si>
 </sst>
 </file>
@@ -1561,10 +1570,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:L265"/>
+  <dimension ref="A1:L268"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A97" workbookViewId="0">
-      <selection activeCell="B135" sqref="B135"/>
+    <sheetView tabSelected="1" topLeftCell="A94" workbookViewId="0">
+      <selection activeCell="B114" sqref="B114"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="15.7109375" defaultRowHeight="16.5" customHeight="1"/>
@@ -3909,36 +3918,36 @@
     </row>
     <row r="111" spans="1:12" ht="16.5" customHeight="1">
       <c r="A111" t="s">
-        <v>318</v>
+        <v>78</v>
       </c>
       <c r="B111" t="s">
-        <v>307</v>
+        <v>404</v>
       </c>
       <c r="C111" t="s">
-        <v>9</v>
+        <v>17</v>
       </c>
       <c r="K111" t="s">
-        <v>308</v>
+        <v>404</v>
       </c>
       <c r="L111" t="s">
-        <v>309</v>
+        <v>133</v>
       </c>
     </row>
     <row r="112" spans="1:12" ht="16.5" customHeight="1">
       <c r="A112" t="s">
-        <v>318</v>
+        <v>78</v>
       </c>
       <c r="B112" t="s">
-        <v>307</v>
+        <v>405</v>
       </c>
       <c r="C112" t="s">
-        <v>310</v>
+        <v>17</v>
       </c>
       <c r="K112" t="s">
-        <v>311</v>
+        <v>405</v>
       </c>
       <c r="L112" t="s">
-        <v>312</v>
+        <v>133</v>
       </c>
     </row>
     <row r="113" spans="1:12" ht="16.5" customHeight="1">
@@ -3946,16 +3955,13 @@
         <v>78</v>
       </c>
       <c r="B113" t="s">
-        <v>81</v>
+        <v>406</v>
       </c>
       <c r="C113" t="s">
-        <v>9</v>
-      </c>
-      <c r="J113" t="s">
-        <v>42</v>
+        <v>19</v>
       </c>
       <c r="K113" t="s">
-        <v>81</v>
+        <v>406</v>
       </c>
       <c r="L113" t="s">
         <v>132</v>
@@ -3963,42 +3969,36 @@
     </row>
     <row r="114" spans="1:12" ht="16.5" customHeight="1">
       <c r="A114" t="s">
-        <v>78</v>
+        <v>318</v>
       </c>
       <c r="B114" t="s">
-        <v>82</v>
+        <v>307</v>
       </c>
       <c r="C114" t="s">
         <v>9</v>
       </c>
-      <c r="J114" t="s">
-        <v>42</v>
-      </c>
       <c r="K114" t="s">
-        <v>82</v>
+        <v>308</v>
       </c>
       <c r="L114" t="s">
-        <v>132</v>
+        <v>309</v>
       </c>
     </row>
     <row r="115" spans="1:12" ht="16.5" customHeight="1">
       <c r="A115" t="s">
-        <v>78</v>
+        <v>318</v>
       </c>
       <c r="B115" t="s">
-        <v>305</v>
+        <v>307</v>
       </c>
       <c r="C115" t="s">
-        <v>9</v>
-      </c>
-      <c r="J115" t="s">
-        <v>42</v>
+        <v>310</v>
       </c>
       <c r="K115" t="s">
-        <v>305</v>
+        <v>311</v>
       </c>
       <c r="L115" t="s">
-        <v>132</v>
+        <v>312</v>
       </c>
     </row>
     <row r="116" spans="1:12" ht="16.5" customHeight="1">
@@ -4006,16 +4006,19 @@
         <v>78</v>
       </c>
       <c r="B116" t="s">
-        <v>306</v>
+        <v>81</v>
       </c>
       <c r="C116" t="s">
         <v>9</v>
       </c>
+      <c r="J116" t="s">
+        <v>42</v>
+      </c>
       <c r="K116" t="s">
-        <v>306</v>
+        <v>81</v>
       </c>
       <c r="L116" t="s">
-        <v>136</v>
+        <v>132</v>
       </c>
     </row>
     <row r="117" spans="1:12" ht="16.5" customHeight="1">
@@ -4023,16 +4026,19 @@
         <v>78</v>
       </c>
       <c r="B117" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C117" t="s">
-        <v>17</v>
+        <v>9</v>
+      </c>
+      <c r="J117" t="s">
+        <v>42</v>
       </c>
       <c r="K117" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="L117" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
     </row>
     <row r="118" spans="1:12" ht="16.5" customHeight="1">
@@ -4040,19 +4046,19 @@
         <v>78</v>
       </c>
       <c r="B118" t="s">
-        <v>213</v>
+        <v>305</v>
       </c>
       <c r="C118" t="s">
-        <v>17</v>
-      </c>
-      <c r="H118" t="s">
-        <v>154</v>
+        <v>9</v>
+      </c>
+      <c r="J118" t="s">
+        <v>42</v>
       </c>
       <c r="K118" t="s">
-        <v>213</v>
+        <v>305</v>
       </c>
       <c r="L118" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
     </row>
     <row r="119" spans="1:12" ht="16.5" customHeight="1">
@@ -4060,28 +4066,16 @@
         <v>78</v>
       </c>
       <c r="B119" t="s">
-        <v>222</v>
+        <v>306</v>
       </c>
       <c r="C119" t="s">
-        <v>17</v>
-      </c>
-      <c r="D119" t="s">
-        <v>358</v>
-      </c>
-      <c r="E119" t="s">
-        <v>214</v>
-      </c>
-      <c r="F119" t="s">
-        <v>12</v>
-      </c>
-      <c r="G119" t="s">
-        <v>220</v>
+        <v>9</v>
       </c>
       <c r="K119" t="s">
-        <v>222</v>
+        <v>306</v>
       </c>
       <c r="L119" t="s">
-        <v>132</v>
+        <v>136</v>
       </c>
     </row>
     <row r="120" spans="1:12" ht="16.5" customHeight="1">
@@ -4089,13 +4083,13 @@
         <v>78</v>
       </c>
       <c r="B120" t="s">
-        <v>401</v>
+        <v>83</v>
       </c>
       <c r="C120" t="s">
         <v>17</v>
       </c>
       <c r="K120" t="s">
-        <v>401</v>
+        <v>83</v>
       </c>
       <c r="L120" t="s">
         <v>133</v>
@@ -4106,88 +4100,79 @@
         <v>78</v>
       </c>
       <c r="B121" t="s">
-        <v>292</v>
+        <v>213</v>
       </c>
       <c r="C121" t="s">
-        <v>19</v>
+        <v>17</v>
+      </c>
+      <c r="H121" t="s">
+        <v>154</v>
       </c>
       <c r="K121" t="s">
-        <v>292</v>
+        <v>213</v>
       </c>
       <c r="L121" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
     </row>
     <row r="122" spans="1:12" ht="16.5" customHeight="1">
       <c r="A122" t="s">
-        <v>84</v>
+        <v>78</v>
       </c>
       <c r="B122" t="s">
-        <v>85</v>
+        <v>222</v>
       </c>
       <c r="C122" t="s">
-        <v>9</v>
+        <v>17</v>
+      </c>
+      <c r="D122" t="s">
+        <v>358</v>
+      </c>
+      <c r="E122" t="s">
+        <v>214</v>
+      </c>
+      <c r="F122" t="s">
+        <v>12</v>
+      </c>
+      <c r="G122" t="s">
+        <v>220</v>
       </c>
       <c r="K122" t="s">
-        <v>85</v>
+        <v>222</v>
       </c>
       <c r="L122" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
     </row>
     <row r="123" spans="1:12" ht="16.5" customHeight="1">
       <c r="A123" t="s">
-        <v>84</v>
+        <v>78</v>
       </c>
       <c r="B123" t="s">
-        <v>86</v>
+        <v>401</v>
       </c>
       <c r="C123" t="s">
-        <v>9</v>
-      </c>
-      <c r="D123" t="s">
-        <v>332</v>
-      </c>
-      <c r="E123" t="s">
-        <v>11</v>
-      </c>
-      <c r="F123" t="s">
-        <v>12</v>
-      </c>
-      <c r="G123" t="s">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="K123" t="s">
-        <v>86</v>
+        <v>401</v>
       </c>
       <c r="L123" t="s">
-        <v>163</v>
+        <v>133</v>
       </c>
     </row>
     <row r="124" spans="1:12" ht="16.5" customHeight="1">
       <c r="A124" t="s">
-        <v>84</v>
+        <v>78</v>
       </c>
       <c r="B124" t="s">
-        <v>87</v>
+        <v>292</v>
       </c>
       <c r="C124" t="s">
-        <v>9</v>
-      </c>
-      <c r="D124" t="s">
-        <v>349</v>
-      </c>
-      <c r="E124" t="s">
-        <v>88</v>
-      </c>
-      <c r="F124" t="s">
-        <v>12</v>
-      </c>
-      <c r="G124" t="s">
-        <v>13</v>
+        <v>19</v>
       </c>
       <c r="K124" t="s">
-        <v>87</v>
+        <v>292</v>
       </c>
       <c r="L124" t="s">
         <v>132</v>
@@ -4198,16 +4183,16 @@
         <v>84</v>
       </c>
       <c r="B125" t="s">
-        <v>389</v>
+        <v>85</v>
       </c>
       <c r="C125" t="s">
-        <v>89</v>
+        <v>9</v>
       </c>
       <c r="K125" t="s">
-        <v>389</v>
+        <v>85</v>
       </c>
       <c r="L125" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="126" spans="1:12" ht="16.5" customHeight="1">
@@ -4215,16 +4200,28 @@
         <v>84</v>
       </c>
       <c r="B126" t="s">
-        <v>390</v>
+        <v>86</v>
       </c>
       <c r="C126" t="s">
-        <v>89</v>
+        <v>9</v>
+      </c>
+      <c r="D126" t="s">
+        <v>332</v>
+      </c>
+      <c r="E126" t="s">
+        <v>11</v>
+      </c>
+      <c r="F126" t="s">
+        <v>12</v>
+      </c>
+      <c r="G126" t="s">
+        <v>13</v>
       </c>
       <c r="K126" t="s">
-        <v>390</v>
+        <v>86</v>
       </c>
       <c r="L126" t="s">
-        <v>132</v>
+        <v>163</v>
       </c>
     </row>
     <row r="127" spans="1:12" ht="16.5" customHeight="1">
@@ -4232,16 +4229,28 @@
         <v>84</v>
       </c>
       <c r="B127" t="s">
-        <v>391</v>
+        <v>87</v>
       </c>
       <c r="C127" t="s">
-        <v>17</v>
+        <v>9</v>
+      </c>
+      <c r="D127" t="s">
+        <v>349</v>
+      </c>
+      <c r="E127" t="s">
+        <v>88</v>
+      </c>
+      <c r="F127" t="s">
+        <v>12</v>
+      </c>
+      <c r="G127" t="s">
+        <v>13</v>
       </c>
       <c r="K127" t="s">
-        <v>391</v>
+        <v>87</v>
       </c>
       <c r="L127" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
     </row>
     <row r="128" spans="1:12" ht="16.5" customHeight="1">
@@ -4249,13 +4258,13 @@
         <v>84</v>
       </c>
       <c r="B128" t="s">
-        <v>392</v>
+        <v>389</v>
       </c>
       <c r="C128" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="K128" t="s">
-        <v>392</v>
+        <v>389</v>
       </c>
       <c r="L128" t="s">
         <v>132</v>
@@ -4266,16 +4275,16 @@
         <v>84</v>
       </c>
       <c r="B129" t="s">
-        <v>393</v>
+        <v>390</v>
       </c>
       <c r="C129" t="s">
-        <v>9</v>
+        <v>89</v>
       </c>
       <c r="K129" t="s">
-        <v>393</v>
+        <v>390</v>
       </c>
       <c r="L129" t="s">
-        <v>138</v>
+        <v>132</v>
       </c>
     </row>
     <row r="130" spans="1:12" ht="16.5" customHeight="1">
@@ -4283,28 +4292,16 @@
         <v>84</v>
       </c>
       <c r="B130" t="s">
-        <v>394</v>
+        <v>391</v>
       </c>
       <c r="C130" t="s">
         <v>17</v>
       </c>
-      <c r="D130" t="s">
-        <v>350</v>
-      </c>
-      <c r="E130" t="s">
-        <v>91</v>
-      </c>
-      <c r="F130" t="s">
-        <v>12</v>
-      </c>
-      <c r="G130" t="s">
-        <v>92</v>
-      </c>
       <c r="K130" t="s">
-        <v>394</v>
+        <v>391</v>
       </c>
       <c r="L130" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
     </row>
     <row r="131" spans="1:12" ht="16.5" customHeight="1">
@@ -4312,16 +4309,16 @@
         <v>84</v>
       </c>
       <c r="B131" t="s">
-        <v>402</v>
+        <v>392</v>
       </c>
       <c r="C131" t="s">
-        <v>17</v>
+        <v>90</v>
       </c>
       <c r="K131" t="s">
-        <v>402</v>
+        <v>392</v>
       </c>
       <c r="L131" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
     </row>
     <row r="132" spans="1:12" ht="16.5" customHeight="1">
@@ -4329,16 +4326,16 @@
         <v>84</v>
       </c>
       <c r="B132" t="s">
-        <v>397</v>
+        <v>393</v>
       </c>
       <c r="C132" t="s">
-        <v>17</v>
+        <v>9</v>
       </c>
       <c r="K132" t="s">
-        <v>397</v>
+        <v>393</v>
       </c>
       <c r="L132" t="s">
-        <v>133</v>
+        <v>138</v>
       </c>
     </row>
     <row r="133" spans="1:12" ht="16.5" customHeight="1">
@@ -4346,16 +4343,28 @@
         <v>84</v>
       </c>
       <c r="B133" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="C133" t="s">
-        <v>36</v>
+        <v>17</v>
+      </c>
+      <c r="D133" t="s">
+        <v>350</v>
+      </c>
+      <c r="E133" t="s">
+        <v>91</v>
+      </c>
+      <c r="F133" t="s">
+        <v>12</v>
+      </c>
+      <c r="G133" t="s">
+        <v>92</v>
       </c>
       <c r="K133" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="L133" t="s">
-        <v>138</v>
+        <v>132</v>
       </c>
     </row>
     <row r="134" spans="1:12" ht="16.5" customHeight="1">
@@ -4363,28 +4372,16 @@
         <v>84</v>
       </c>
       <c r="B134" t="s">
-        <v>396</v>
+        <v>402</v>
       </c>
       <c r="C134" t="s">
         <v>17</v>
       </c>
-      <c r="D134" t="s">
-        <v>350</v>
-      </c>
-      <c r="E134" t="s">
-        <v>91</v>
-      </c>
-      <c r="F134" t="s">
-        <v>12</v>
-      </c>
-      <c r="G134" t="s">
-        <v>92</v>
-      </c>
       <c r="K134" t="s">
-        <v>396</v>
+        <v>402</v>
       </c>
       <c r="L134" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
     </row>
     <row r="135" spans="1:12" ht="16.5" customHeight="1">
@@ -4392,13 +4389,13 @@
         <v>84</v>
       </c>
       <c r="B135" t="s">
-        <v>403</v>
+        <v>397</v>
       </c>
       <c r="C135" t="s">
         <v>17</v>
       </c>
       <c r="K135" t="s">
-        <v>403</v>
+        <v>397</v>
       </c>
       <c r="L135" t="s">
         <v>133</v>
@@ -4406,19 +4403,19 @@
     </row>
     <row r="136" spans="1:12" ht="16.5" customHeight="1">
       <c r="A136" t="s">
-        <v>198</v>
+        <v>84</v>
       </c>
       <c r="B136" t="s">
-        <v>93</v>
+        <v>395</v>
       </c>
       <c r="C136" t="s">
-        <v>19</v>
+        <v>36</v>
       </c>
       <c r="K136" t="s">
-        <v>93</v>
+        <v>395</v>
       </c>
       <c r="L136" t="s">
-        <v>132</v>
+        <v>138</v>
       </c>
     </row>
     <row r="137" spans="1:12" ht="16.5" customHeight="1">
@@ -4426,13 +4423,25 @@
         <v>84</v>
       </c>
       <c r="B137" t="s">
-        <v>398</v>
+        <v>396</v>
       </c>
       <c r="C137" t="s">
-        <v>19</v>
+        <v>17</v>
+      </c>
+      <c r="D137" t="s">
+        <v>350</v>
+      </c>
+      <c r="E137" t="s">
+        <v>91</v>
+      </c>
+      <c r="F137" t="s">
+        <v>12</v>
+      </c>
+      <c r="G137" t="s">
+        <v>92</v>
       </c>
       <c r="K137" t="s">
-        <v>398</v>
+        <v>396</v>
       </c>
       <c r="L137" t="s">
         <v>132</v>
@@ -4443,36 +4452,33 @@
         <v>84</v>
       </c>
       <c r="B138" t="s">
-        <v>399</v>
+        <v>403</v>
       </c>
       <c r="C138" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="K138" t="s">
-        <v>399</v>
+        <v>403</v>
       </c>
       <c r="L138" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
     </row>
     <row r="139" spans="1:12" ht="16.5" customHeight="1">
       <c r="A139" t="s">
-        <v>84</v>
+        <v>198</v>
       </c>
       <c r="B139" t="s">
-        <v>400</v>
+        <v>93</v>
       </c>
       <c r="C139" t="s">
-        <v>9</v>
-      </c>
-      <c r="J139" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="K139" t="s">
-        <v>400</v>
+        <v>93</v>
       </c>
       <c r="L139" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
     </row>
     <row r="140" spans="1:12" ht="16.5" customHeight="1">
@@ -4480,13 +4486,13 @@
         <v>84</v>
       </c>
       <c r="B140" t="s">
-        <v>293</v>
+        <v>398</v>
       </c>
       <c r="C140" t="s">
         <v>19</v>
       </c>
       <c r="K140" t="s">
-        <v>293</v>
+        <v>398</v>
       </c>
       <c r="L140" t="s">
         <v>132</v>
@@ -4497,13 +4503,13 @@
         <v>84</v>
       </c>
       <c r="B141" t="s">
-        <v>287</v>
+        <v>399</v>
       </c>
       <c r="C141" t="s">
         <v>19</v>
       </c>
       <c r="K141" t="s">
-        <v>287</v>
+        <v>399</v>
       </c>
       <c r="L141" t="s">
         <v>132</v>
@@ -4511,19 +4517,22 @@
     </row>
     <row r="142" spans="1:12" ht="16.5" customHeight="1">
       <c r="A142" t="s">
-        <v>198</v>
+        <v>84</v>
       </c>
       <c r="B142" t="s">
-        <v>94</v>
+        <v>400</v>
       </c>
       <c r="C142" t="s">
-        <v>19</v>
+        <v>9</v>
+      </c>
+      <c r="J142" t="s">
+        <v>22</v>
       </c>
       <c r="K142" t="s">
-        <v>94</v>
+        <v>400</v>
       </c>
       <c r="L142" t="s">
-        <v>132</v>
+        <v>135</v>
       </c>
     </row>
     <row r="143" spans="1:12" ht="16.5" customHeight="1">
@@ -4531,25 +4540,13 @@
         <v>84</v>
       </c>
       <c r="B143" t="s">
-        <v>151</v>
+        <v>293</v>
       </c>
       <c r="C143" t="s">
-        <v>9</v>
-      </c>
-      <c r="D143" t="s">
-        <v>359</v>
-      </c>
-      <c r="E143" t="s">
-        <v>152</v>
-      </c>
-      <c r="F143" t="s">
-        <v>12</v>
-      </c>
-      <c r="G143" t="s">
-        <v>13</v>
+        <v>19</v>
       </c>
       <c r="K143" t="s">
-        <v>151</v>
+        <v>293</v>
       </c>
       <c r="L143" t="s">
         <v>132</v>
@@ -4560,13 +4557,13 @@
         <v>84</v>
       </c>
       <c r="B144" t="s">
-        <v>150</v>
+        <v>287</v>
       </c>
       <c r="C144" t="s">
         <v>19</v>
       </c>
       <c r="K144" t="s">
-        <v>150</v>
+        <v>287</v>
       </c>
       <c r="L144" t="s">
         <v>132</v>
@@ -4574,19 +4571,19 @@
     </row>
     <row r="145" spans="1:12" ht="16.5" customHeight="1">
       <c r="A145" t="s">
-        <v>84</v>
+        <v>198</v>
       </c>
       <c r="B145" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C145" t="s">
-        <v>36</v>
+        <v>19</v>
       </c>
       <c r="K145" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="L145" t="s">
-        <v>138</v>
+        <v>132</v>
       </c>
     </row>
     <row r="146" spans="1:12" ht="16.5" customHeight="1">
@@ -4594,28 +4591,28 @@
         <v>84</v>
       </c>
       <c r="B146" t="s">
-        <v>95</v>
+        <v>151</v>
       </c>
       <c r="C146" t="s">
-        <v>17</v>
+        <v>9</v>
       </c>
       <c r="D146" t="s">
-        <v>335</v>
+        <v>359</v>
       </c>
       <c r="E146" t="s">
-        <v>271</v>
+        <v>152</v>
       </c>
       <c r="F146" t="s">
         <v>12</v>
       </c>
       <c r="G146" t="s">
-        <v>61</v>
+        <v>13</v>
       </c>
       <c r="K146" t="s">
-        <v>262</v>
-      </c>
-      <c r="L146" s="1" t="s">
-        <v>269</v>
+        <v>151</v>
+      </c>
+      <c r="L146" t="s">
+        <v>132</v>
       </c>
     </row>
     <row r="147" spans="1:12" ht="16.5" customHeight="1">
@@ -4623,19 +4620,16 @@
         <v>84</v>
       </c>
       <c r="B147" t="s">
-        <v>181</v>
+        <v>150</v>
       </c>
       <c r="C147" t="s">
-        <v>17</v>
-      </c>
-      <c r="H147" t="s">
-        <v>175</v>
+        <v>19</v>
       </c>
       <c r="K147" t="s">
-        <v>181</v>
+        <v>150</v>
       </c>
       <c r="L147" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
     </row>
     <row r="148" spans="1:12" ht="16.5" customHeight="1">
@@ -4643,19 +4637,16 @@
         <v>84</v>
       </c>
       <c r="B148" t="s">
-        <v>182</v>
+        <v>95</v>
       </c>
       <c r="C148" t="s">
-        <v>17</v>
-      </c>
-      <c r="H148" t="s">
-        <v>176</v>
+        <v>36</v>
       </c>
       <c r="K148" t="s">
-        <v>182</v>
+        <v>95</v>
       </c>
       <c r="L148" t="s">
-        <v>133</v>
+        <v>138</v>
       </c>
     </row>
     <row r="149" spans="1:12" ht="16.5" customHeight="1">
@@ -4663,19 +4654,28 @@
         <v>84</v>
       </c>
       <c r="B149" t="s">
-        <v>199</v>
+        <v>95</v>
       </c>
       <c r="C149" t="s">
         <v>17</v>
       </c>
-      <c r="H149" t="s">
-        <v>174</v>
+      <c r="D149" t="s">
+        <v>335</v>
+      </c>
+      <c r="E149" t="s">
+        <v>271</v>
+      </c>
+      <c r="F149" t="s">
+        <v>12</v>
+      </c>
+      <c r="G149" t="s">
+        <v>61</v>
       </c>
       <c r="K149" t="s">
-        <v>199</v>
-      </c>
-      <c r="L149" t="s">
-        <v>133</v>
+        <v>262</v>
+      </c>
+      <c r="L149" s="1" t="s">
+        <v>269</v>
       </c>
     </row>
     <row r="150" spans="1:12" ht="16.5" customHeight="1">
@@ -4683,19 +4683,19 @@
         <v>84</v>
       </c>
       <c r="B150" t="s">
-        <v>242</v>
+        <v>181</v>
       </c>
       <c r="C150" t="s">
         <v>17</v>
       </c>
       <c r="H150" t="s">
-        <v>244</v>
+        <v>175</v>
       </c>
       <c r="K150" t="s">
-        <v>242</v>
+        <v>181</v>
       </c>
       <c r="L150" t="s">
-        <v>243</v>
+        <v>133</v>
       </c>
     </row>
     <row r="151" spans="1:12" ht="16.5" customHeight="1">
@@ -4703,16 +4703,19 @@
         <v>84</v>
       </c>
       <c r="B151" t="s">
-        <v>185</v>
+        <v>182</v>
       </c>
       <c r="C151" t="s">
-        <v>36</v>
+        <v>17</v>
+      </c>
+      <c r="H151" t="s">
+        <v>176</v>
       </c>
       <c r="K151" t="s">
-        <v>185</v>
+        <v>182</v>
       </c>
       <c r="L151" t="s">
-        <v>272</v>
+        <v>133</v>
       </c>
     </row>
     <row r="152" spans="1:12" ht="16.5" customHeight="1">
@@ -4720,28 +4723,19 @@
         <v>84</v>
       </c>
       <c r="B152" t="s">
-        <v>185</v>
+        <v>199</v>
       </c>
       <c r="C152" t="s">
         <v>17</v>
       </c>
-      <c r="D152" t="s">
-        <v>335</v>
-      </c>
-      <c r="E152" t="s">
-        <v>271</v>
-      </c>
-      <c r="F152" t="s">
-        <v>12</v>
-      </c>
-      <c r="G152" t="s">
-        <v>61</v>
+      <c r="H152" t="s">
+        <v>174</v>
       </c>
       <c r="K152" t="s">
-        <v>261</v>
-      </c>
-      <c r="L152" s="1" t="s">
-        <v>269</v>
+        <v>199</v>
+      </c>
+      <c r="L152" t="s">
+        <v>133</v>
       </c>
     </row>
     <row r="153" spans="1:12" ht="16.5" customHeight="1">
@@ -4749,16 +4743,19 @@
         <v>84</v>
       </c>
       <c r="B153" t="s">
-        <v>186</v>
+        <v>242</v>
       </c>
       <c r="C153" t="s">
-        <v>36</v>
+        <v>17</v>
+      </c>
+      <c r="H153" t="s">
+        <v>244</v>
       </c>
       <c r="K153" t="s">
-        <v>186</v>
+        <v>242</v>
       </c>
       <c r="L153" t="s">
-        <v>272</v>
+        <v>243</v>
       </c>
     </row>
     <row r="154" spans="1:12" ht="16.5" customHeight="1">
@@ -4766,28 +4763,16 @@
         <v>84</v>
       </c>
       <c r="B154" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="C154" t="s">
-        <v>17</v>
-      </c>
-      <c r="D154" t="s">
-        <v>335</v>
-      </c>
-      <c r="E154" t="s">
-        <v>271</v>
-      </c>
-      <c r="F154" t="s">
-        <v>12</v>
-      </c>
-      <c r="G154" t="s">
-        <v>61</v>
+        <v>36</v>
       </c>
       <c r="K154" t="s">
-        <v>260</v>
-      </c>
-      <c r="L154" s="1" t="s">
-        <v>269</v>
+        <v>185</v>
+      </c>
+      <c r="L154" t="s">
+        <v>272</v>
       </c>
     </row>
     <row r="155" spans="1:12" ht="16.5" customHeight="1">
@@ -4795,16 +4780,28 @@
         <v>84</v>
       </c>
       <c r="B155" t="s">
-        <v>173</v>
+        <v>185</v>
       </c>
       <c r="C155" t="s">
-        <v>9</v>
+        <v>17</v>
+      </c>
+      <c r="D155" t="s">
+        <v>335</v>
+      </c>
+      <c r="E155" t="s">
+        <v>271</v>
+      </c>
+      <c r="F155" t="s">
+        <v>12</v>
+      </c>
+      <c r="G155" t="s">
+        <v>61</v>
       </c>
       <c r="K155" t="s">
-        <v>173</v>
-      </c>
-      <c r="L155" t="s">
-        <v>136</v>
+        <v>261</v>
+      </c>
+      <c r="L155" s="1" t="s">
+        <v>269</v>
       </c>
     </row>
     <row r="156" spans="1:12" ht="16.5" customHeight="1">
@@ -4812,19 +4809,16 @@
         <v>84</v>
       </c>
       <c r="B156" t="s">
-        <v>320</v>
+        <v>186</v>
       </c>
       <c r="C156" t="s">
-        <v>17</v>
-      </c>
-      <c r="H156" t="s">
-        <v>322</v>
+        <v>36</v>
       </c>
       <c r="K156" t="s">
-        <v>320</v>
+        <v>186</v>
       </c>
       <c r="L156" t="s">
-        <v>243</v>
+        <v>272</v>
       </c>
     </row>
     <row r="157" spans="1:12" ht="16.5" customHeight="1">
@@ -4832,19 +4826,28 @@
         <v>84</v>
       </c>
       <c r="B157" t="s">
-        <v>321</v>
+        <v>186</v>
       </c>
       <c r="C157" t="s">
         <v>17</v>
       </c>
-      <c r="H157" t="s">
-        <v>323</v>
+      <c r="D157" t="s">
+        <v>335</v>
+      </c>
+      <c r="E157" t="s">
+        <v>271</v>
+      </c>
+      <c r="F157" t="s">
+        <v>12</v>
+      </c>
+      <c r="G157" t="s">
+        <v>61</v>
       </c>
       <c r="K157" t="s">
-        <v>321</v>
-      </c>
-      <c r="L157" t="s">
-        <v>243</v>
+        <v>260</v>
+      </c>
+      <c r="L157" s="1" t="s">
+        <v>269</v>
       </c>
     </row>
     <row r="158" spans="1:12" ht="16.5" customHeight="1">
@@ -4852,19 +4855,16 @@
         <v>84</v>
       </c>
       <c r="B158" t="s">
-        <v>324</v>
+        <v>173</v>
       </c>
       <c r="C158" t="s">
-        <v>17</v>
-      </c>
-      <c r="H158" t="s">
-        <v>325</v>
+        <v>9</v>
       </c>
       <c r="K158" t="s">
-        <v>324</v>
+        <v>173</v>
       </c>
       <c r="L158" t="s">
-        <v>243</v>
+        <v>136</v>
       </c>
     </row>
     <row r="159" spans="1:12" ht="16.5" customHeight="1">
@@ -4872,16 +4872,19 @@
         <v>84</v>
       </c>
       <c r="B159" t="s">
-        <v>326</v>
+        <v>320</v>
       </c>
       <c r="C159" t="s">
-        <v>36</v>
+        <v>17</v>
+      </c>
+      <c r="H159" t="s">
+        <v>322</v>
       </c>
       <c r="K159" t="s">
-        <v>326</v>
+        <v>320</v>
       </c>
       <c r="L159" t="s">
-        <v>272</v>
+        <v>243</v>
       </c>
     </row>
     <row r="160" spans="1:12" ht="16.5" customHeight="1">
@@ -4889,28 +4892,19 @@
         <v>84</v>
       </c>
       <c r="B160" t="s">
-        <v>326</v>
+        <v>321</v>
       </c>
       <c r="C160" t="s">
         <v>17</v>
       </c>
-      <c r="D160" t="s">
-        <v>335</v>
-      </c>
-      <c r="E160" t="s">
-        <v>271</v>
-      </c>
-      <c r="F160" t="s">
-        <v>12</v>
-      </c>
-      <c r="G160" t="s">
-        <v>61</v>
+      <c r="H160" t="s">
+        <v>323</v>
       </c>
       <c r="K160" t="s">
-        <v>329</v>
-      </c>
-      <c r="L160" s="1" t="s">
-        <v>269</v>
+        <v>321</v>
+      </c>
+      <c r="L160" t="s">
+        <v>243</v>
       </c>
     </row>
     <row r="161" spans="1:12" ht="16.5" customHeight="1">
@@ -4918,16 +4912,19 @@
         <v>84</v>
       </c>
       <c r="B161" t="s">
-        <v>327</v>
+        <v>324</v>
       </c>
       <c r="C161" t="s">
-        <v>36</v>
+        <v>17</v>
+      </c>
+      <c r="H161" t="s">
+        <v>325</v>
       </c>
       <c r="K161" t="s">
-        <v>327</v>
+        <v>324</v>
       </c>
       <c r="L161" t="s">
-        <v>272</v>
+        <v>243</v>
       </c>
     </row>
     <row r="162" spans="1:12" ht="16.5" customHeight="1">
@@ -4935,28 +4932,16 @@
         <v>84</v>
       </c>
       <c r="B162" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="C162" t="s">
-        <v>17</v>
-      </c>
-      <c r="D162" t="s">
-        <v>335</v>
-      </c>
-      <c r="E162" t="s">
-        <v>271</v>
-      </c>
-      <c r="F162" t="s">
-        <v>12</v>
-      </c>
-      <c r="G162" t="s">
-        <v>61</v>
+        <v>36</v>
       </c>
       <c r="K162" t="s">
-        <v>330</v>
-      </c>
-      <c r="L162" s="1" t="s">
-        <v>269</v>
+        <v>326</v>
+      </c>
+      <c r="L162" t="s">
+        <v>272</v>
       </c>
     </row>
     <row r="163" spans="1:12" ht="16.5" customHeight="1">
@@ -4964,16 +4949,28 @@
         <v>84</v>
       </c>
       <c r="B163" t="s">
-        <v>328</v>
+        <v>326</v>
       </c>
       <c r="C163" t="s">
-        <v>9</v>
+        <v>17</v>
+      </c>
+      <c r="D163" t="s">
+        <v>335</v>
+      </c>
+      <c r="E163" t="s">
+        <v>271</v>
+      </c>
+      <c r="F163" t="s">
+        <v>12</v>
+      </c>
+      <c r="G163" t="s">
+        <v>61</v>
       </c>
       <c r="K163" t="s">
-        <v>328</v>
-      </c>
-      <c r="L163" t="s">
-        <v>136</v>
+        <v>329</v>
+      </c>
+      <c r="L163" s="1" t="s">
+        <v>269</v>
       </c>
     </row>
     <row r="164" spans="1:12" ht="16.5" customHeight="1">
@@ -4981,19 +4978,16 @@
         <v>84</v>
       </c>
       <c r="B164" t="s">
-        <v>183</v>
+        <v>327</v>
       </c>
       <c r="C164" t="s">
-        <v>17</v>
-      </c>
-      <c r="H164" t="s">
-        <v>180</v>
+        <v>36</v>
       </c>
       <c r="K164" t="s">
-        <v>183</v>
+        <v>327</v>
       </c>
       <c r="L164" t="s">
-        <v>133</v>
+        <v>272</v>
       </c>
     </row>
     <row r="165" spans="1:12" ht="16.5" customHeight="1">
@@ -5001,19 +4995,28 @@
         <v>84</v>
       </c>
       <c r="B165" t="s">
-        <v>184</v>
+        <v>327</v>
       </c>
       <c r="C165" t="s">
         <v>17</v>
       </c>
-      <c r="H165" t="s">
-        <v>179</v>
+      <c r="D165" t="s">
+        <v>335</v>
+      </c>
+      <c r="E165" t="s">
+        <v>271</v>
+      </c>
+      <c r="F165" t="s">
+        <v>12</v>
+      </c>
+      <c r="G165" t="s">
+        <v>61</v>
       </c>
       <c r="K165" t="s">
-        <v>184</v>
-      </c>
-      <c r="L165" t="s">
-        <v>133</v>
+        <v>330</v>
+      </c>
+      <c r="L165" s="1" t="s">
+        <v>269</v>
       </c>
     </row>
     <row r="166" spans="1:12" ht="16.5" customHeight="1">
@@ -5021,19 +5024,16 @@
         <v>84</v>
       </c>
       <c r="B166" t="s">
-        <v>200</v>
+        <v>328</v>
       </c>
       <c r="C166" t="s">
-        <v>17</v>
-      </c>
-      <c r="H166" t="s">
-        <v>178</v>
+        <v>9</v>
       </c>
       <c r="K166" t="s">
-        <v>200</v>
+        <v>328</v>
       </c>
       <c r="L166" t="s">
-        <v>133</v>
+        <v>136</v>
       </c>
     </row>
     <row r="167" spans="1:12" ht="16.5" customHeight="1">
@@ -5041,19 +5041,19 @@
         <v>84</v>
       </c>
       <c r="B167" t="s">
-        <v>245</v>
+        <v>183</v>
       </c>
       <c r="C167" t="s">
         <v>17</v>
       </c>
       <c r="H167" t="s">
-        <v>246</v>
+        <v>180</v>
       </c>
       <c r="K167" t="s">
-        <v>245</v>
+        <v>183</v>
       </c>
       <c r="L167" t="s">
-        <v>243</v>
+        <v>133</v>
       </c>
     </row>
     <row r="168" spans="1:12" ht="16.5" customHeight="1">
@@ -5061,16 +5061,19 @@
         <v>84</v>
       </c>
       <c r="B168" t="s">
-        <v>187</v>
+        <v>184</v>
       </c>
       <c r="C168" t="s">
-        <v>36</v>
+        <v>17</v>
+      </c>
+      <c r="H168" t="s">
+        <v>179</v>
       </c>
       <c r="K168" t="s">
-        <v>187</v>
+        <v>184</v>
       </c>
       <c r="L168" t="s">
-        <v>272</v>
+        <v>133</v>
       </c>
     </row>
     <row r="169" spans="1:12" ht="16.5" customHeight="1">
@@ -5078,28 +5081,19 @@
         <v>84</v>
       </c>
       <c r="B169" t="s">
-        <v>187</v>
+        <v>200</v>
       </c>
       <c r="C169" t="s">
         <v>17</v>
       </c>
-      <c r="D169" t="s">
-        <v>335</v>
-      </c>
-      <c r="E169" t="s">
-        <v>271</v>
-      </c>
-      <c r="F169" t="s">
-        <v>12</v>
-      </c>
-      <c r="G169" t="s">
-        <v>61</v>
+      <c r="H169" t="s">
+        <v>178</v>
       </c>
       <c r="K169" t="s">
-        <v>259</v>
-      </c>
-      <c r="L169" s="1" t="s">
-        <v>269</v>
+        <v>200</v>
+      </c>
+      <c r="L169" t="s">
+        <v>133</v>
       </c>
     </row>
     <row r="170" spans="1:12" ht="16.5" customHeight="1">
@@ -5107,16 +5101,19 @@
         <v>84</v>
       </c>
       <c r="B170" t="s">
-        <v>188</v>
+        <v>245</v>
       </c>
       <c r="C170" t="s">
-        <v>36</v>
+        <v>17</v>
+      </c>
+      <c r="H170" t="s">
+        <v>246</v>
       </c>
       <c r="K170" t="s">
-        <v>188</v>
+        <v>245</v>
       </c>
       <c r="L170" t="s">
-        <v>272</v>
+        <v>243</v>
       </c>
     </row>
     <row r="171" spans="1:12" ht="16.5" customHeight="1">
@@ -5124,28 +5121,16 @@
         <v>84</v>
       </c>
       <c r="B171" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="C171" t="s">
-        <v>17</v>
-      </c>
-      <c r="D171" t="s">
-        <v>335</v>
-      </c>
-      <c r="E171" t="s">
-        <v>271</v>
-      </c>
-      <c r="F171" t="s">
-        <v>12</v>
-      </c>
-      <c r="G171" t="s">
-        <v>61</v>
+        <v>36</v>
       </c>
       <c r="K171" t="s">
-        <v>258</v>
-      </c>
-      <c r="L171" s="1" t="s">
-        <v>269</v>
+        <v>187</v>
+      </c>
+      <c r="L171" t="s">
+        <v>272</v>
       </c>
     </row>
     <row r="172" spans="1:12" ht="16.5" customHeight="1">
@@ -5153,16 +5138,28 @@
         <v>84</v>
       </c>
       <c r="B172" t="s">
-        <v>177</v>
+        <v>187</v>
       </c>
       <c r="C172" t="s">
-        <v>9</v>
+        <v>17</v>
+      </c>
+      <c r="D172" t="s">
+        <v>335</v>
+      </c>
+      <c r="E172" t="s">
+        <v>271</v>
+      </c>
+      <c r="F172" t="s">
+        <v>12</v>
+      </c>
+      <c r="G172" t="s">
+        <v>61</v>
       </c>
       <c r="K172" t="s">
-        <v>177</v>
-      </c>
-      <c r="L172" t="s">
-        <v>136</v>
+        <v>259</v>
+      </c>
+      <c r="L172" s="1" t="s">
+        <v>269</v>
       </c>
     </row>
     <row r="173" spans="1:12" ht="16.5" customHeight="1">
@@ -5170,28 +5167,16 @@
         <v>84</v>
       </c>
       <c r="B173" t="s">
-        <v>207</v>
+        <v>188</v>
       </c>
       <c r="C173" t="s">
-        <v>9</v>
-      </c>
-      <c r="D173" t="s">
-        <v>351</v>
-      </c>
-      <c r="E173" t="s">
-        <v>208</v>
-      </c>
-      <c r="F173" t="s">
-        <v>12</v>
-      </c>
-      <c r="G173" t="s">
-        <v>13</v>
+        <v>36</v>
       </c>
       <c r="K173" t="s">
-        <v>207</v>
+        <v>188</v>
       </c>
       <c r="L173" t="s">
-        <v>132</v>
+        <v>272</v>
       </c>
     </row>
     <row r="174" spans="1:12" ht="16.5" customHeight="1">
@@ -5199,19 +5184,28 @@
         <v>84</v>
       </c>
       <c r="B174" t="s">
-        <v>203</v>
+        <v>188</v>
       </c>
       <c r="C174" t="s">
-        <v>89</v>
-      </c>
-      <c r="H174" t="s">
-        <v>205</v>
+        <v>17</v>
+      </c>
+      <c r="D174" t="s">
+        <v>335</v>
+      </c>
+      <c r="E174" t="s">
+        <v>271</v>
+      </c>
+      <c r="F174" t="s">
+        <v>12</v>
+      </c>
+      <c r="G174" t="s">
+        <v>61</v>
       </c>
       <c r="K174" t="s">
-        <v>203</v>
-      </c>
-      <c r="L174" t="s">
-        <v>132</v>
+        <v>258</v>
+      </c>
+      <c r="L174" s="1" t="s">
+        <v>269</v>
       </c>
     </row>
     <row r="175" spans="1:12" ht="16.5" customHeight="1">
@@ -5219,45 +5213,42 @@
         <v>84</v>
       </c>
       <c r="B175" t="s">
-        <v>204</v>
+        <v>177</v>
       </c>
       <c r="C175" t="s">
-        <v>89</v>
-      </c>
-      <c r="H175" t="s">
-        <v>206</v>
+        <v>9</v>
       </c>
       <c r="K175" t="s">
-        <v>204</v>
+        <v>177</v>
       </c>
       <c r="L175" t="s">
-        <v>132</v>
+        <v>136</v>
       </c>
     </row>
     <row r="176" spans="1:12" ht="16.5" customHeight="1">
       <c r="A176" t="s">
-        <v>198</v>
+        <v>84</v>
       </c>
       <c r="B176" t="s">
-        <v>96</v>
+        <v>207</v>
       </c>
       <c r="C176" t="s">
         <v>9</v>
       </c>
       <c r="D176" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="E176" t="s">
-        <v>97</v>
+        <v>208</v>
       </c>
       <c r="F176" t="s">
-        <v>98</v>
+        <v>12</v>
       </c>
       <c r="G176" t="s">
         <v>13</v>
       </c>
       <c r="K176" t="s">
-        <v>96</v>
+        <v>207</v>
       </c>
       <c r="L176" t="s">
         <v>132</v>
@@ -5268,25 +5259,16 @@
         <v>84</v>
       </c>
       <c r="B177" t="s">
-        <v>96</v>
+        <v>203</v>
       </c>
       <c r="C177" t="s">
-        <v>9</v>
-      </c>
-      <c r="D177" t="s">
-        <v>352</v>
-      </c>
-      <c r="F177" t="s">
-        <v>98</v>
+        <v>89</v>
       </c>
       <c r="H177" t="s">
-        <v>295</v>
-      </c>
-      <c r="I177" t="s">
-        <v>296</v>
+        <v>205</v>
       </c>
       <c r="K177" t="s">
-        <v>96</v>
+        <v>203</v>
       </c>
       <c r="L177" t="s">
         <v>132</v>
@@ -5294,28 +5276,19 @@
     </row>
     <row r="178" spans="1:12" ht="16.5" customHeight="1">
       <c r="A178" t="s">
-        <v>198</v>
+        <v>84</v>
       </c>
       <c r="B178" t="s">
-        <v>99</v>
+        <v>204</v>
       </c>
       <c r="C178" t="s">
-        <v>9</v>
-      </c>
-      <c r="D178" t="s">
-        <v>353</v>
-      </c>
-      <c r="E178" t="s">
-        <v>100</v>
-      </c>
-      <c r="F178" t="s">
-        <v>12</v>
-      </c>
-      <c r="G178" t="s">
-        <v>13</v>
+        <v>89</v>
+      </c>
+      <c r="H178" t="s">
+        <v>206</v>
       </c>
       <c r="K178" t="s">
-        <v>99</v>
+        <v>204</v>
       </c>
       <c r="L178" t="s">
         <v>132</v>
@@ -5323,28 +5296,28 @@
     </row>
     <row r="179" spans="1:12" ht="16.5" customHeight="1">
       <c r="A179" t="s">
-        <v>84</v>
+        <v>198</v>
       </c>
       <c r="B179" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="C179" t="s">
         <v>9</v>
       </c>
       <c r="D179" t="s">
-        <v>353</v>
+        <v>352</v>
+      </c>
+      <c r="E179" t="s">
+        <v>97</v>
       </c>
       <c r="F179" t="s">
-        <v>12</v>
-      </c>
-      <c r="H179" t="s">
-        <v>297</v>
-      </c>
-      <c r="I179" t="s">
-        <v>298</v>
+        <v>98</v>
+      </c>
+      <c r="G179" t="s">
+        <v>13</v>
       </c>
       <c r="K179" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="L179" t="s">
         <v>132</v>
@@ -5355,33 +5328,54 @@
         <v>84</v>
       </c>
       <c r="B180" t="s">
-        <v>197</v>
+        <v>96</v>
       </c>
       <c r="C180" t="s">
         <v>9</v>
       </c>
+      <c r="D180" t="s">
+        <v>352</v>
+      </c>
+      <c r="F180" t="s">
+        <v>98</v>
+      </c>
+      <c r="H180" t="s">
+        <v>295</v>
+      </c>
+      <c r="I180" t="s">
+        <v>296</v>
+      </c>
       <c r="K180" t="s">
-        <v>197</v>
+        <v>96</v>
       </c>
       <c r="L180" t="s">
-        <v>136</v>
+        <v>132</v>
       </c>
     </row>
     <row r="181" spans="1:12" ht="16.5" customHeight="1">
       <c r="A181" t="s">
-        <v>84</v>
+        <v>198</v>
       </c>
       <c r="B181" t="s">
-        <v>195</v>
+        <v>99</v>
       </c>
       <c r="C181" t="s">
         <v>9</v>
       </c>
-      <c r="J181" t="s">
-        <v>42</v>
+      <c r="D181" t="s">
+        <v>353</v>
+      </c>
+      <c r="E181" t="s">
+        <v>100</v>
+      </c>
+      <c r="F181" t="s">
+        <v>12</v>
+      </c>
+      <c r="G181" t="s">
+        <v>13</v>
       </c>
       <c r="K181" t="s">
-        <v>195</v>
+        <v>99</v>
       </c>
       <c r="L181" t="s">
         <v>132</v>
@@ -5392,16 +5386,28 @@
         <v>84</v>
       </c>
       <c r="B182" t="s">
-        <v>140</v>
+        <v>99</v>
       </c>
       <c r="C182" t="s">
-        <v>56</v>
+        <v>9</v>
+      </c>
+      <c r="D182" t="s">
+        <v>353</v>
+      </c>
+      <c r="F182" t="s">
+        <v>12</v>
+      </c>
+      <c r="H182" t="s">
+        <v>297</v>
+      </c>
+      <c r="I182" t="s">
+        <v>298</v>
       </c>
       <c r="K182" t="s">
-        <v>140</v>
+        <v>99</v>
       </c>
       <c r="L182" t="s">
-        <v>138</v>
+        <v>132</v>
       </c>
     </row>
     <row r="183" spans="1:12" ht="16.5" customHeight="1">
@@ -5409,28 +5415,16 @@
         <v>84</v>
       </c>
       <c r="B183" t="s">
-        <v>140</v>
+        <v>197</v>
       </c>
       <c r="C183" t="s">
-        <v>17</v>
-      </c>
-      <c r="D183" t="s">
-        <v>335</v>
-      </c>
-      <c r="E183" t="s">
-        <v>271</v>
-      </c>
-      <c r="F183" t="s">
-        <v>12</v>
-      </c>
-      <c r="G183" t="s">
-        <v>61</v>
+        <v>9</v>
       </c>
       <c r="K183" t="s">
-        <v>257</v>
-      </c>
-      <c r="L183" s="1" t="s">
-        <v>270</v>
+        <v>197</v>
+      </c>
+      <c r="L183" t="s">
+        <v>136</v>
       </c>
     </row>
     <row r="184" spans="1:12" ht="16.5" customHeight="1">
@@ -5438,19 +5432,19 @@
         <v>84</v>
       </c>
       <c r="B184" t="s">
-        <v>144</v>
+        <v>195</v>
       </c>
       <c r="C184" t="s">
-        <v>17</v>
-      </c>
-      <c r="H184" t="s">
-        <v>143</v>
+        <v>9</v>
+      </c>
+      <c r="J184" t="s">
+        <v>42</v>
       </c>
       <c r="K184" t="s">
-        <v>144</v>
+        <v>195</v>
       </c>
       <c r="L184" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
     </row>
     <row r="185" spans="1:12" ht="16.5" customHeight="1">
@@ -5458,16 +5452,16 @@
         <v>84</v>
       </c>
       <c r="B185" t="s">
-        <v>101</v>
+        <v>140</v>
       </c>
       <c r="C185" t="s">
-        <v>19</v>
+        <v>56</v>
       </c>
       <c r="K185" t="s">
-        <v>101</v>
+        <v>140</v>
       </c>
       <c r="L185" t="s">
-        <v>132</v>
+        <v>138</v>
       </c>
     </row>
     <row r="186" spans="1:12" ht="16.5" customHeight="1">
@@ -5475,16 +5469,28 @@
         <v>84</v>
       </c>
       <c r="B186" t="s">
-        <v>102</v>
+        <v>140</v>
       </c>
       <c r="C186" t="s">
-        <v>9</v>
+        <v>17</v>
+      </c>
+      <c r="D186" t="s">
+        <v>335</v>
+      </c>
+      <c r="E186" t="s">
+        <v>271</v>
+      </c>
+      <c r="F186" t="s">
+        <v>12</v>
+      </c>
+      <c r="G186" t="s">
+        <v>61</v>
       </c>
       <c r="K186" t="s">
-        <v>102</v>
-      </c>
-      <c r="L186" t="s">
-        <v>138</v>
+        <v>257</v>
+      </c>
+      <c r="L186" s="1" t="s">
+        <v>270</v>
       </c>
     </row>
     <row r="187" spans="1:12" ht="16.5" customHeight="1">
@@ -5492,16 +5498,19 @@
         <v>84</v>
       </c>
       <c r="B187" t="s">
-        <v>103</v>
+        <v>144</v>
       </c>
       <c r="C187" t="s">
-        <v>104</v>
+        <v>17</v>
+      </c>
+      <c r="H187" t="s">
+        <v>143</v>
       </c>
       <c r="K187" t="s">
-        <v>103</v>
+        <v>144</v>
       </c>
       <c r="L187" t="s">
-        <v>138</v>
+        <v>133</v>
       </c>
     </row>
     <row r="188" spans="1:12" ht="16.5" customHeight="1">
@@ -5509,16 +5518,16 @@
         <v>84</v>
       </c>
       <c r="B188" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
       <c r="C188" t="s">
-        <v>36</v>
+        <v>19</v>
       </c>
       <c r="K188" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
       <c r="L188" t="s">
-        <v>138</v>
+        <v>132</v>
       </c>
     </row>
     <row r="189" spans="1:12" ht="16.5" customHeight="1">
@@ -5526,28 +5535,16 @@
         <v>84</v>
       </c>
       <c r="B189" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="C189" t="s">
-        <v>17</v>
-      </c>
-      <c r="D189" t="s">
-        <v>335</v>
-      </c>
-      <c r="E189" t="s">
-        <v>271</v>
-      </c>
-      <c r="F189" t="s">
-        <v>12</v>
-      </c>
-      <c r="G189" t="s">
-        <v>61</v>
+        <v>9</v>
       </c>
       <c r="K189" t="s">
-        <v>256</v>
-      </c>
-      <c r="L189" s="1" t="s">
-        <v>269</v>
+        <v>102</v>
+      </c>
+      <c r="L189" t="s">
+        <v>138</v>
       </c>
     </row>
     <row r="190" spans="1:12" ht="16.5" customHeight="1">
@@ -5555,13 +5552,13 @@
         <v>84</v>
       </c>
       <c r="B190" t="s">
-        <v>211</v>
+        <v>103</v>
       </c>
       <c r="C190" t="s">
-        <v>56</v>
+        <v>104</v>
       </c>
       <c r="K190" t="s">
-        <v>211</v>
+        <v>103</v>
       </c>
       <c r="L190" t="s">
         <v>138</v>
@@ -5572,28 +5569,16 @@
         <v>84</v>
       </c>
       <c r="B191" t="s">
-        <v>211</v>
+        <v>105</v>
       </c>
       <c r="C191" t="s">
-        <v>17</v>
-      </c>
-      <c r="D191" t="s">
-        <v>335</v>
-      </c>
-      <c r="E191" t="s">
-        <v>271</v>
-      </c>
-      <c r="F191" t="s">
-        <v>12</v>
-      </c>
-      <c r="G191" t="s">
-        <v>61</v>
+        <v>36</v>
       </c>
       <c r="K191" t="s">
-        <v>255</v>
-      </c>
-      <c r="L191" s="1" t="s">
-        <v>270</v>
+        <v>105</v>
+      </c>
+      <c r="L191" t="s">
+        <v>138</v>
       </c>
     </row>
     <row r="192" spans="1:12" ht="16.5" customHeight="1">
@@ -5601,16 +5586,28 @@
         <v>84</v>
       </c>
       <c r="B192" t="s">
-        <v>313</v>
+        <v>105</v>
       </c>
       <c r="C192" t="s">
-        <v>310</v>
+        <v>17</v>
+      </c>
+      <c r="D192" t="s">
+        <v>335</v>
+      </c>
+      <c r="E192" t="s">
+        <v>271</v>
+      </c>
+      <c r="F192" t="s">
+        <v>12</v>
+      </c>
+      <c r="G192" t="s">
+        <v>61</v>
       </c>
       <c r="K192" t="s">
-        <v>313</v>
-      </c>
-      <c r="L192" t="s">
-        <v>138</v>
+        <v>256</v>
+      </c>
+      <c r="L192" s="1" t="s">
+        <v>269</v>
       </c>
     </row>
     <row r="193" spans="1:12" ht="16.5" customHeight="1">
@@ -5618,45 +5615,45 @@
         <v>84</v>
       </c>
       <c r="B193" t="s">
-        <v>313</v>
+        <v>211</v>
       </c>
       <c r="C193" t="s">
-        <v>9</v>
+        <v>56</v>
       </c>
       <c r="K193" t="s">
-        <v>314</v>
-      </c>
-      <c r="L193" s="1" t="s">
-        <v>315</v>
+        <v>211</v>
+      </c>
+      <c r="L193" t="s">
+        <v>138</v>
       </c>
     </row>
     <row r="194" spans="1:12" ht="16.5" customHeight="1">
       <c r="A194" t="s">
-        <v>198</v>
+        <v>84</v>
       </c>
       <c r="B194" t="s">
-        <v>106</v>
+        <v>211</v>
       </c>
       <c r="C194" t="s">
-        <v>9</v>
+        <v>17</v>
       </c>
       <c r="D194" t="s">
-        <v>354</v>
+        <v>335</v>
       </c>
       <c r="E194" t="s">
-        <v>107</v>
+        <v>271</v>
       </c>
       <c r="F194" t="s">
-        <v>98</v>
+        <v>12</v>
       </c>
       <c r="G194" t="s">
-        <v>13</v>
+        <v>61</v>
       </c>
       <c r="K194" t="s">
-        <v>106</v>
-      </c>
-      <c r="L194" t="s">
-        <v>132</v>
+        <v>255</v>
+      </c>
+      <c r="L194" s="1" t="s">
+        <v>270</v>
       </c>
     </row>
     <row r="195" spans="1:12" ht="16.5" customHeight="1">
@@ -5664,28 +5661,16 @@
         <v>84</v>
       </c>
       <c r="B195" t="s">
-        <v>106</v>
+        <v>313</v>
       </c>
       <c r="C195" t="s">
-        <v>9</v>
-      </c>
-      <c r="D195" t="s">
-        <v>354</v>
-      </c>
-      <c r="F195" t="s">
-        <v>98</v>
-      </c>
-      <c r="H195" t="s">
-        <v>299</v>
-      </c>
-      <c r="I195" t="s">
-        <v>300</v>
+        <v>310</v>
       </c>
       <c r="K195" t="s">
-        <v>106</v>
+        <v>313</v>
       </c>
       <c r="L195" t="s">
-        <v>132</v>
+        <v>138</v>
       </c>
     </row>
     <row r="196" spans="1:12" ht="16.5" customHeight="1">
@@ -5693,62 +5678,71 @@
         <v>84</v>
       </c>
       <c r="B196" t="s">
-        <v>153</v>
+        <v>313</v>
       </c>
       <c r="C196" t="s">
-        <v>17</v>
-      </c>
-      <c r="H196" t="s">
-        <v>154</v>
+        <v>9</v>
       </c>
       <c r="K196" t="s">
-        <v>153</v>
-      </c>
-      <c r="L196" t="s">
-        <v>133</v>
+        <v>314</v>
+      </c>
+      <c r="L196" s="1" t="s">
+        <v>315</v>
       </c>
     </row>
     <row r="197" spans="1:12" ht="16.5" customHeight="1">
       <c r="A197" t="s">
-        <v>84</v>
+        <v>198</v>
       </c>
       <c r="B197" t="s">
-        <v>147</v>
+        <v>106</v>
       </c>
       <c r="C197" t="s">
         <v>9</v>
       </c>
+      <c r="D197" t="s">
+        <v>354</v>
+      </c>
+      <c r="E197" t="s">
+        <v>107</v>
+      </c>
+      <c r="F197" t="s">
+        <v>98</v>
+      </c>
+      <c r="G197" t="s">
+        <v>13</v>
+      </c>
       <c r="K197" t="s">
-        <v>147</v>
+        <v>106</v>
       </c>
       <c r="L197" t="s">
-        <v>136</v>
+        <v>132</v>
       </c>
     </row>
     <row r="198" spans="1:12" ht="16.5" customHeight="1">
       <c r="A198" t="s">
-        <v>198</v>
+        <v>84</v>
       </c>
       <c r="B198" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="C198" t="s">
         <v>9</v>
       </c>
       <c r="D198" t="s">
-        <v>355</v>
-      </c>
-      <c r="E198" t="s">
-        <v>109</v>
+        <v>354</v>
       </c>
       <c r="F198" t="s">
         <v>98</v>
       </c>
-      <c r="G198" t="s">
-        <v>13</v>
+      <c r="H198" t="s">
+        <v>299</v>
+      </c>
+      <c r="I198" t="s">
+        <v>300</v>
       </c>
       <c r="K198" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="L198" t="s">
         <v>132</v>
@@ -5759,83 +5753,62 @@
         <v>84</v>
       </c>
       <c r="B199" t="s">
-        <v>108</v>
+        <v>153</v>
       </c>
       <c r="C199" t="s">
-        <v>9</v>
-      </c>
-      <c r="D199" t="s">
-        <v>355</v>
-      </c>
-      <c r="F199" t="s">
-        <v>98</v>
+        <v>17</v>
       </c>
       <c r="H199" t="s">
-        <v>301</v>
-      </c>
-      <c r="I199" t="s">
-        <v>302</v>
+        <v>154</v>
       </c>
       <c r="K199" t="s">
-        <v>108</v>
+        <v>153</v>
       </c>
       <c r="L199" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
     </row>
     <row r="200" spans="1:12" ht="16.5" customHeight="1">
       <c r="A200" t="s">
-        <v>198</v>
+        <v>84</v>
       </c>
       <c r="B200" t="s">
-        <v>110</v>
+        <v>147</v>
       </c>
       <c r="C200" t="s">
         <v>9</v>
       </c>
-      <c r="D200" t="s">
-        <v>353</v>
-      </c>
-      <c r="E200" t="s">
-        <v>111</v>
-      </c>
-      <c r="F200" t="s">
-        <v>12</v>
-      </c>
-      <c r="G200" t="s">
-        <v>13</v>
-      </c>
       <c r="K200" t="s">
-        <v>110</v>
+        <v>147</v>
       </c>
       <c r="L200" t="s">
-        <v>132</v>
+        <v>136</v>
       </c>
     </row>
     <row r="201" spans="1:12" ht="16.5" customHeight="1">
       <c r="A201" t="s">
-        <v>84</v>
+        <v>198</v>
       </c>
       <c r="B201" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="C201" t="s">
         <v>9</v>
       </c>
       <c r="D201" t="s">
-        <v>353</v>
+        <v>355</v>
+      </c>
+      <c r="E201" t="s">
+        <v>109</v>
       </c>
       <c r="F201" t="s">
-        <v>12</v>
-      </c>
-      <c r="H201" t="s">
-        <v>303</v>
-      </c>
-      <c r="I201" t="s">
-        <v>298</v>
+        <v>98</v>
+      </c>
+      <c r="G201" t="s">
+        <v>13</v>
       </c>
       <c r="K201" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="L201" t="s">
         <v>132</v>
@@ -5846,16 +5819,28 @@
         <v>84</v>
       </c>
       <c r="B202" t="s">
-        <v>196</v>
+        <v>108</v>
       </c>
       <c r="C202" t="s">
         <v>9</v>
       </c>
+      <c r="D202" t="s">
+        <v>355</v>
+      </c>
+      <c r="F202" t="s">
+        <v>98</v>
+      </c>
+      <c r="H202" t="s">
+        <v>301</v>
+      </c>
+      <c r="I202" t="s">
+        <v>302</v>
+      </c>
       <c r="K202" t="s">
-        <v>196</v>
+        <v>108</v>
       </c>
       <c r="L202" t="s">
-        <v>136</v>
+        <v>132</v>
       </c>
     </row>
     <row r="203" spans="1:12" ht="16.5" customHeight="1">
@@ -5863,16 +5848,25 @@
         <v>198</v>
       </c>
       <c r="B203" t="s">
-        <v>122</v>
+        <v>110</v>
       </c>
       <c r="C203" t="s">
         <v>9</v>
       </c>
-      <c r="J203" t="s">
-        <v>42</v>
+      <c r="D203" t="s">
+        <v>353</v>
+      </c>
+      <c r="E203" t="s">
+        <v>111</v>
+      </c>
+      <c r="F203" t="s">
+        <v>12</v>
+      </c>
+      <c r="G203" t="s">
+        <v>13</v>
       </c>
       <c r="K203" t="s">
-        <v>122</v>
+        <v>110</v>
       </c>
       <c r="L203" t="s">
         <v>132</v>
@@ -5883,16 +5877,28 @@
         <v>84</v>
       </c>
       <c r="B204" t="s">
-        <v>141</v>
+        <v>110</v>
       </c>
       <c r="C204" t="s">
-        <v>56</v>
+        <v>9</v>
+      </c>
+      <c r="D204" t="s">
+        <v>353</v>
+      </c>
+      <c r="F204" t="s">
+        <v>12</v>
+      </c>
+      <c r="H204" t="s">
+        <v>303</v>
+      </c>
+      <c r="I204" t="s">
+        <v>298</v>
       </c>
       <c r="K204" t="s">
-        <v>141</v>
+        <v>110</v>
       </c>
       <c r="L204" t="s">
-        <v>138</v>
+        <v>132</v>
       </c>
     </row>
     <row r="205" spans="1:12" ht="16.5" customHeight="1">
@@ -5900,48 +5906,36 @@
         <v>84</v>
       </c>
       <c r="B205" t="s">
-        <v>141</v>
+        <v>196</v>
       </c>
       <c r="C205" t="s">
-        <v>17</v>
-      </c>
-      <c r="D205" t="s">
-        <v>335</v>
-      </c>
-      <c r="E205" t="s">
-        <v>271</v>
-      </c>
-      <c r="F205" t="s">
-        <v>12</v>
-      </c>
-      <c r="G205" t="s">
-        <v>61</v>
+        <v>9</v>
       </c>
       <c r="K205" t="s">
-        <v>254</v>
-      </c>
-      <c r="L205" s="1" t="s">
-        <v>270</v>
+        <v>196</v>
+      </c>
+      <c r="L205" t="s">
+        <v>136</v>
       </c>
     </row>
     <row r="206" spans="1:12" ht="16.5" customHeight="1">
       <c r="A206" t="s">
-        <v>84</v>
+        <v>198</v>
       </c>
       <c r="B206" t="s">
-        <v>145</v>
+        <v>122</v>
       </c>
       <c r="C206" t="s">
-        <v>17</v>
-      </c>
-      <c r="H206" t="s">
-        <v>143</v>
+        <v>9</v>
+      </c>
+      <c r="J206" t="s">
+        <v>42</v>
       </c>
       <c r="K206" t="s">
-        <v>145</v>
+        <v>122</v>
       </c>
       <c r="L206" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
     </row>
     <row r="207" spans="1:12" ht="16.5" customHeight="1">
@@ -5949,16 +5943,16 @@
         <v>84</v>
       </c>
       <c r="B207" t="s">
-        <v>112</v>
+        <v>141</v>
       </c>
       <c r="C207" t="s">
-        <v>19</v>
+        <v>56</v>
       </c>
       <c r="K207" t="s">
-        <v>112</v>
+        <v>141</v>
       </c>
       <c r="L207" t="s">
-        <v>132</v>
+        <v>138</v>
       </c>
     </row>
     <row r="208" spans="1:12" ht="16.5" customHeight="1">
@@ -5966,16 +5960,28 @@
         <v>84</v>
       </c>
       <c r="B208" t="s">
-        <v>113</v>
+        <v>141</v>
       </c>
       <c r="C208" t="s">
-        <v>9</v>
+        <v>17</v>
+      </c>
+      <c r="D208" t="s">
+        <v>335</v>
+      </c>
+      <c r="E208" t="s">
+        <v>271</v>
+      </c>
+      <c r="F208" t="s">
+        <v>12</v>
+      </c>
+      <c r="G208" t="s">
+        <v>61</v>
       </c>
       <c r="K208" t="s">
-        <v>113</v>
-      </c>
-      <c r="L208" t="s">
-        <v>138</v>
+        <v>254</v>
+      </c>
+      <c r="L208" s="1" t="s">
+        <v>270</v>
       </c>
     </row>
     <row r="209" spans="1:12" ht="16.5" customHeight="1">
@@ -5983,16 +5989,19 @@
         <v>84</v>
       </c>
       <c r="B209" t="s">
-        <v>114</v>
+        <v>145</v>
       </c>
       <c r="C209" t="s">
-        <v>104</v>
+        <v>17</v>
+      </c>
+      <c r="H209" t="s">
+        <v>143</v>
       </c>
       <c r="K209" t="s">
-        <v>114</v>
+        <v>145</v>
       </c>
       <c r="L209" t="s">
-        <v>138</v>
+        <v>133</v>
       </c>
     </row>
     <row r="210" spans="1:12" ht="16.5" customHeight="1">
@@ -6000,16 +6009,16 @@
         <v>84</v>
       </c>
       <c r="B210" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="C210" t="s">
-        <v>36</v>
+        <v>19</v>
       </c>
       <c r="K210" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="L210" t="s">
-        <v>138</v>
+        <v>132</v>
       </c>
     </row>
     <row r="211" spans="1:12" ht="16.5" customHeight="1">
@@ -6017,28 +6026,16 @@
         <v>84</v>
       </c>
       <c r="B211" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="C211" t="s">
-        <v>17</v>
-      </c>
-      <c r="D211" t="s">
-        <v>335</v>
-      </c>
-      <c r="E211" t="s">
-        <v>271</v>
-      </c>
-      <c r="F211" t="s">
-        <v>12</v>
-      </c>
-      <c r="G211" t="s">
-        <v>61</v>
+        <v>9</v>
       </c>
       <c r="K211" t="s">
-        <v>253</v>
-      </c>
-      <c r="L211" s="1" t="s">
-        <v>269</v>
+        <v>113</v>
+      </c>
+      <c r="L211" t="s">
+        <v>138</v>
       </c>
     </row>
     <row r="212" spans="1:12" ht="16.5" customHeight="1">
@@ -6046,13 +6043,13 @@
         <v>84</v>
       </c>
       <c r="B212" t="s">
-        <v>210</v>
+        <v>114</v>
       </c>
       <c r="C212" t="s">
-        <v>56</v>
+        <v>104</v>
       </c>
       <c r="K212" t="s">
-        <v>210</v>
+        <v>114</v>
       </c>
       <c r="L212" t="s">
         <v>138</v>
@@ -6063,28 +6060,16 @@
         <v>84</v>
       </c>
       <c r="B213" t="s">
-        <v>210</v>
+        <v>115</v>
       </c>
       <c r="C213" t="s">
-        <v>17</v>
-      </c>
-      <c r="D213" t="s">
-        <v>335</v>
-      </c>
-      <c r="E213" t="s">
-        <v>271</v>
-      </c>
-      <c r="F213" t="s">
-        <v>12</v>
-      </c>
-      <c r="G213" t="s">
-        <v>61</v>
+        <v>36</v>
       </c>
       <c r="K213" t="s">
-        <v>252</v>
-      </c>
-      <c r="L213" s="1" t="s">
-        <v>270</v>
+        <v>115</v>
+      </c>
+      <c r="L213" t="s">
+        <v>138</v>
       </c>
     </row>
     <row r="214" spans="1:12" ht="16.5" customHeight="1">
@@ -6092,16 +6077,28 @@
         <v>84</v>
       </c>
       <c r="B214" t="s">
-        <v>316</v>
+        <v>115</v>
       </c>
       <c r="C214" t="s">
-        <v>310</v>
+        <v>17</v>
+      </c>
+      <c r="D214" t="s">
+        <v>335</v>
+      </c>
+      <c r="E214" t="s">
+        <v>271</v>
+      </c>
+      <c r="F214" t="s">
+        <v>12</v>
+      </c>
+      <c r="G214" t="s">
+        <v>61</v>
       </c>
       <c r="K214" t="s">
-        <v>316</v>
-      </c>
-      <c r="L214" t="s">
-        <v>138</v>
+        <v>253</v>
+      </c>
+      <c r="L214" s="1" t="s">
+        <v>269</v>
       </c>
     </row>
     <row r="215" spans="1:12" ht="16.5" customHeight="1">
@@ -6109,45 +6106,45 @@
         <v>84</v>
       </c>
       <c r="B215" t="s">
-        <v>316</v>
+        <v>210</v>
       </c>
       <c r="C215" t="s">
-        <v>9</v>
+        <v>56</v>
       </c>
       <c r="K215" t="s">
-        <v>317</v>
-      </c>
-      <c r="L215" s="1" t="s">
-        <v>315</v>
+        <v>210</v>
+      </c>
+      <c r="L215" t="s">
+        <v>138</v>
       </c>
     </row>
     <row r="216" spans="1:12" ht="16.5" customHeight="1">
       <c r="A216" t="s">
-        <v>198</v>
+        <v>84</v>
       </c>
       <c r="B216" t="s">
-        <v>116</v>
+        <v>210</v>
       </c>
       <c r="C216" t="s">
-        <v>9</v>
+        <v>17</v>
       </c>
       <c r="D216" t="s">
-        <v>354</v>
+        <v>335</v>
       </c>
       <c r="E216" t="s">
-        <v>117</v>
+        <v>271</v>
       </c>
       <c r="F216" t="s">
-        <v>98</v>
+        <v>12</v>
       </c>
       <c r="G216" t="s">
-        <v>13</v>
+        <v>61</v>
       </c>
       <c r="K216" t="s">
-        <v>116</v>
-      </c>
-      <c r="L216" t="s">
-        <v>132</v>
+        <v>252</v>
+      </c>
+      <c r="L216" s="1" t="s">
+        <v>270</v>
       </c>
     </row>
     <row r="217" spans="1:12" ht="16.5" customHeight="1">
@@ -6155,28 +6152,16 @@
         <v>84</v>
       </c>
       <c r="B217" t="s">
-        <v>116</v>
+        <v>316</v>
       </c>
       <c r="C217" t="s">
-        <v>9</v>
-      </c>
-      <c r="D217" t="s">
-        <v>354</v>
-      </c>
-      <c r="F217" t="s">
-        <v>98</v>
-      </c>
-      <c r="H217" t="s">
-        <v>304</v>
-      </c>
-      <c r="I217" t="s">
-        <v>300</v>
+        <v>310</v>
       </c>
       <c r="K217" t="s">
-        <v>116</v>
+        <v>316</v>
       </c>
       <c r="L217" t="s">
-        <v>132</v>
+        <v>138</v>
       </c>
     </row>
     <row r="218" spans="1:12" ht="16.5" customHeight="1">
@@ -6184,36 +6169,45 @@
         <v>84</v>
       </c>
       <c r="B218" t="s">
-        <v>155</v>
+        <v>316</v>
       </c>
       <c r="C218" t="s">
-        <v>17</v>
-      </c>
-      <c r="H218" t="s">
-        <v>154</v>
+        <v>9</v>
       </c>
       <c r="K218" t="s">
-        <v>155</v>
-      </c>
-      <c r="L218" t="s">
-        <v>133</v>
+        <v>317</v>
+      </c>
+      <c r="L218" s="1" t="s">
+        <v>315</v>
       </c>
     </row>
     <row r="219" spans="1:12" ht="16.5" customHeight="1">
       <c r="A219" t="s">
-        <v>84</v>
+        <v>198</v>
       </c>
       <c r="B219" t="s">
-        <v>146</v>
+        <v>116</v>
       </c>
       <c r="C219" t="s">
         <v>9</v>
       </c>
+      <c r="D219" t="s">
+        <v>354</v>
+      </c>
+      <c r="E219" t="s">
+        <v>117</v>
+      </c>
+      <c r="F219" t="s">
+        <v>98</v>
+      </c>
+      <c r="G219" t="s">
+        <v>13</v>
+      </c>
       <c r="K219" t="s">
-        <v>146</v>
+        <v>116</v>
       </c>
       <c r="L219" t="s">
-        <v>136</v>
+        <v>132</v>
       </c>
     </row>
     <row r="220" spans="1:12" ht="16.5" customHeight="1">
@@ -6221,13 +6215,25 @@
         <v>84</v>
       </c>
       <c r="B220" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="C220" t="s">
-        <v>89</v>
+        <v>9</v>
+      </c>
+      <c r="D220" t="s">
+        <v>354</v>
+      </c>
+      <c r="F220" t="s">
+        <v>98</v>
+      </c>
+      <c r="H220" t="s">
+        <v>304</v>
+      </c>
+      <c r="I220" t="s">
+        <v>300</v>
       </c>
       <c r="K220" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="L220" t="s">
         <v>132</v>
@@ -6238,28 +6244,19 @@
         <v>84</v>
       </c>
       <c r="B221" t="s">
-        <v>119</v>
+        <v>155</v>
       </c>
       <c r="C221" t="s">
-        <v>9</v>
-      </c>
-      <c r="D221" t="s">
-        <v>360</v>
-      </c>
-      <c r="E221" t="s">
-        <v>120</v>
-      </c>
-      <c r="F221" t="s">
-        <v>12</v>
-      </c>
-      <c r="G221" t="s">
-        <v>13</v>
+        <v>17</v>
+      </c>
+      <c r="H221" t="s">
+        <v>154</v>
       </c>
       <c r="K221" t="s">
-        <v>119</v>
+        <v>155</v>
       </c>
       <c r="L221" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
     </row>
     <row r="222" spans="1:12" ht="16.5" customHeight="1">
@@ -6267,13 +6264,13 @@
         <v>84</v>
       </c>
       <c r="B222" t="s">
-        <v>121</v>
+        <v>146</v>
       </c>
       <c r="C222" t="s">
         <v>9</v>
       </c>
       <c r="K222" t="s">
-        <v>121</v>
+        <v>146</v>
       </c>
       <c r="L222" t="s">
         <v>136</v>
@@ -6281,28 +6278,16 @@
     </row>
     <row r="223" spans="1:12" ht="16.5" customHeight="1">
       <c r="A223" t="s">
-        <v>198</v>
+        <v>84</v>
       </c>
       <c r="B223" t="s">
-        <v>361</v>
+        <v>118</v>
       </c>
       <c r="C223" t="s">
-        <v>9</v>
-      </c>
-      <c r="D223" t="s">
-        <v>362</v>
-      </c>
-      <c r="E223" t="s">
-        <v>363</v>
-      </c>
-      <c r="F223" t="s">
-        <v>98</v>
-      </c>
-      <c r="G223" t="s">
-        <v>13</v>
+        <v>89</v>
       </c>
       <c r="K223" t="s">
-        <v>361</v>
+        <v>118</v>
       </c>
       <c r="L223" t="s">
         <v>132</v>
@@ -6313,25 +6298,25 @@
         <v>84</v>
       </c>
       <c r="B224" t="s">
-        <v>361</v>
+        <v>119</v>
       </c>
       <c r="C224" t="s">
         <v>9</v>
       </c>
       <c r="D224" t="s">
-        <v>362</v>
+        <v>360</v>
+      </c>
+      <c r="E224" t="s">
+        <v>120</v>
       </c>
       <c r="F224" t="s">
-        <v>98</v>
-      </c>
-      <c r="H224" t="s">
-        <v>364</v>
-      </c>
-      <c r="I224" t="s">
-        <v>365</v>
+        <v>12</v>
+      </c>
+      <c r="G224" t="s">
+        <v>13</v>
       </c>
       <c r="K224" t="s">
-        <v>361</v>
+        <v>119</v>
       </c>
       <c r="L224" t="s">
         <v>132</v>
@@ -6339,57 +6324,45 @@
     </row>
     <row r="225" spans="1:12" ht="16.5" customHeight="1">
       <c r="A225" t="s">
-        <v>198</v>
+        <v>84</v>
       </c>
       <c r="B225" t="s">
-        <v>366</v>
+        <v>121</v>
       </c>
       <c r="C225" t="s">
         <v>9</v>
       </c>
-      <c r="D225" t="s">
-        <v>353</v>
-      </c>
-      <c r="E225" t="s">
-        <v>367</v>
-      </c>
-      <c r="F225" t="s">
-        <v>12</v>
-      </c>
-      <c r="G225" t="s">
-        <v>13</v>
-      </c>
       <c r="K225" t="s">
-        <v>366</v>
+        <v>121</v>
       </c>
       <c r="L225" t="s">
-        <v>132</v>
+        <v>136</v>
       </c>
     </row>
     <row r="226" spans="1:12" ht="16.5" customHeight="1">
       <c r="A226" t="s">
-        <v>84</v>
+        <v>198</v>
       </c>
       <c r="B226" t="s">
-        <v>366</v>
+        <v>361</v>
       </c>
       <c r="C226" t="s">
         <v>9</v>
       </c>
       <c r="D226" t="s">
-        <v>353</v>
+        <v>362</v>
+      </c>
+      <c r="E226" t="s">
+        <v>363</v>
       </c>
       <c r="F226" t="s">
-        <v>12</v>
-      </c>
-      <c r="H226" t="s">
-        <v>368</v>
-      </c>
-      <c r="I226" t="s">
-        <v>298</v>
+        <v>98</v>
+      </c>
+      <c r="G226" t="s">
+        <v>13</v>
       </c>
       <c r="K226" t="s">
-        <v>366</v>
+        <v>361</v>
       </c>
       <c r="L226" t="s">
         <v>132</v>
@@ -6400,16 +6373,28 @@
         <v>84</v>
       </c>
       <c r="B227" t="s">
-        <v>369</v>
+        <v>361</v>
       </c>
       <c r="C227" t="s">
         <v>9</v>
       </c>
+      <c r="D227" t="s">
+        <v>362</v>
+      </c>
+      <c r="F227" t="s">
+        <v>98</v>
+      </c>
+      <c r="H227" t="s">
+        <v>364</v>
+      </c>
+      <c r="I227" t="s">
+        <v>365</v>
+      </c>
       <c r="K227" t="s">
-        <v>369</v>
+        <v>361</v>
       </c>
       <c r="L227" t="s">
-        <v>136</v>
+        <v>132</v>
       </c>
     </row>
     <row r="228" spans="1:12" ht="16.5" customHeight="1">
@@ -6417,16 +6402,25 @@
         <v>198</v>
       </c>
       <c r="B228" t="s">
-        <v>122</v>
+        <v>366</v>
       </c>
       <c r="C228" t="s">
         <v>9</v>
       </c>
-      <c r="J228" t="s">
-        <v>42</v>
+      <c r="D228" t="s">
+        <v>353</v>
+      </c>
+      <c r="E228" t="s">
+        <v>367</v>
+      </c>
+      <c r="F228" t="s">
+        <v>12</v>
+      </c>
+      <c r="G228" t="s">
+        <v>13</v>
       </c>
       <c r="K228" t="s">
-        <v>122</v>
+        <v>366</v>
       </c>
       <c r="L228" t="s">
         <v>132</v>
@@ -6437,16 +6431,28 @@
         <v>84</v>
       </c>
       <c r="B229" t="s">
-        <v>370</v>
+        <v>366</v>
       </c>
       <c r="C229" t="s">
-        <v>56</v>
+        <v>9</v>
+      </c>
+      <c r="D229" t="s">
+        <v>353</v>
+      </c>
+      <c r="F229" t="s">
+        <v>12</v>
+      </c>
+      <c r="H229" t="s">
+        <v>368</v>
+      </c>
+      <c r="I229" t="s">
+        <v>298</v>
       </c>
       <c r="K229" t="s">
-        <v>370</v>
+        <v>366</v>
       </c>
       <c r="L229" t="s">
-        <v>138</v>
+        <v>132</v>
       </c>
     </row>
     <row r="230" spans="1:12" ht="16.5" customHeight="1">
@@ -6454,48 +6460,36 @@
         <v>84</v>
       </c>
       <c r="B230" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
       <c r="C230" t="s">
-        <v>17</v>
-      </c>
-      <c r="D230" t="s">
-        <v>335</v>
-      </c>
-      <c r="E230" t="s">
-        <v>271</v>
-      </c>
-      <c r="F230" t="s">
-        <v>12</v>
-      </c>
-      <c r="G230" t="s">
-        <v>61</v>
+        <v>9</v>
       </c>
       <c r="K230" t="s">
-        <v>371</v>
-      </c>
-      <c r="L230" s="1" t="s">
-        <v>270</v>
+        <v>369</v>
+      </c>
+      <c r="L230" t="s">
+        <v>136</v>
       </c>
     </row>
     <row r="231" spans="1:12" ht="16.5" customHeight="1">
       <c r="A231" t="s">
-        <v>84</v>
+        <v>198</v>
       </c>
       <c r="B231" t="s">
-        <v>372</v>
+        <v>122</v>
       </c>
       <c r="C231" t="s">
-        <v>17</v>
-      </c>
-      <c r="H231" t="s">
-        <v>143</v>
+        <v>9</v>
+      </c>
+      <c r="J231" t="s">
+        <v>42</v>
       </c>
       <c r="K231" t="s">
-        <v>372</v>
+        <v>122</v>
       </c>
       <c r="L231" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
     </row>
     <row r="232" spans="1:12" ht="16.5" customHeight="1">
@@ -6503,16 +6497,16 @@
         <v>84</v>
       </c>
       <c r="B232" t="s">
-        <v>373</v>
+        <v>370</v>
       </c>
       <c r="C232" t="s">
-        <v>19</v>
+        <v>56</v>
       </c>
       <c r="K232" t="s">
-        <v>373</v>
+        <v>370</v>
       </c>
       <c r="L232" t="s">
-        <v>132</v>
+        <v>138</v>
       </c>
     </row>
     <row r="233" spans="1:12" ht="16.5" customHeight="1">
@@ -6520,16 +6514,28 @@
         <v>84</v>
       </c>
       <c r="B233" t="s">
-        <v>374</v>
+        <v>370</v>
       </c>
       <c r="C233" t="s">
-        <v>9</v>
+        <v>17</v>
+      </c>
+      <c r="D233" t="s">
+        <v>335</v>
+      </c>
+      <c r="E233" t="s">
+        <v>271</v>
+      </c>
+      <c r="F233" t="s">
+        <v>12</v>
+      </c>
+      <c r="G233" t="s">
+        <v>61</v>
       </c>
       <c r="K233" t="s">
-        <v>374</v>
-      </c>
-      <c r="L233" t="s">
-        <v>138</v>
+        <v>371</v>
+      </c>
+      <c r="L233" s="1" t="s">
+        <v>270</v>
       </c>
     </row>
     <row r="234" spans="1:12" ht="16.5" customHeight="1">
@@ -6537,16 +6543,19 @@
         <v>84</v>
       </c>
       <c r="B234" t="s">
-        <v>375</v>
+        <v>372</v>
       </c>
       <c r="C234" t="s">
-        <v>104</v>
+        <v>17</v>
+      </c>
+      <c r="H234" t="s">
+        <v>143</v>
       </c>
       <c r="K234" t="s">
-        <v>375</v>
+        <v>372</v>
       </c>
       <c r="L234" t="s">
-        <v>138</v>
+        <v>133</v>
       </c>
     </row>
     <row r="235" spans="1:12" ht="16.5" customHeight="1">
@@ -6554,16 +6563,16 @@
         <v>84</v>
       </c>
       <c r="B235" t="s">
-        <v>376</v>
+        <v>373</v>
       </c>
       <c r="C235" t="s">
-        <v>36</v>
+        <v>19</v>
       </c>
       <c r="K235" t="s">
-        <v>376</v>
+        <v>373</v>
       </c>
       <c r="L235" t="s">
-        <v>138</v>
+        <v>132</v>
       </c>
     </row>
     <row r="236" spans="1:12" ht="16.5" customHeight="1">
@@ -6571,28 +6580,16 @@
         <v>84</v>
       </c>
       <c r="B236" t="s">
-        <v>376</v>
+        <v>374</v>
       </c>
       <c r="C236" t="s">
-        <v>17</v>
-      </c>
-      <c r="D236" t="s">
-        <v>335</v>
-      </c>
-      <c r="E236" t="s">
-        <v>271</v>
-      </c>
-      <c r="F236" t="s">
-        <v>12</v>
-      </c>
-      <c r="G236" t="s">
-        <v>61</v>
+        <v>9</v>
       </c>
       <c r="K236" t="s">
-        <v>377</v>
-      </c>
-      <c r="L236" s="1" t="s">
-        <v>269</v>
+        <v>374</v>
+      </c>
+      <c r="L236" t="s">
+        <v>138</v>
       </c>
     </row>
     <row r="237" spans="1:12" ht="16.5" customHeight="1">
@@ -6600,13 +6597,13 @@
         <v>84</v>
       </c>
       <c r="B237" t="s">
-        <v>378</v>
+        <v>375</v>
       </c>
       <c r="C237" t="s">
-        <v>56</v>
+        <v>104</v>
       </c>
       <c r="K237" t="s">
-        <v>378</v>
+        <v>375</v>
       </c>
       <c r="L237" t="s">
         <v>138</v>
@@ -6617,28 +6614,16 @@
         <v>84</v>
       </c>
       <c r="B238" t="s">
-        <v>378</v>
+        <v>376</v>
       </c>
       <c r="C238" t="s">
-        <v>17</v>
-      </c>
-      <c r="D238" t="s">
-        <v>335</v>
-      </c>
-      <c r="E238" t="s">
-        <v>271</v>
-      </c>
-      <c r="F238" t="s">
-        <v>12</v>
-      </c>
-      <c r="G238" t="s">
-        <v>61</v>
+        <v>36</v>
       </c>
       <c r="K238" t="s">
-        <v>379</v>
-      </c>
-      <c r="L238" s="1" t="s">
-        <v>270</v>
+        <v>376</v>
+      </c>
+      <c r="L238" t="s">
+        <v>138</v>
       </c>
     </row>
     <row r="239" spans="1:12" ht="16.5" customHeight="1">
@@ -6646,16 +6631,28 @@
         <v>84</v>
       </c>
       <c r="B239" t="s">
-        <v>380</v>
+        <v>376</v>
       </c>
       <c r="C239" t="s">
-        <v>310</v>
+        <v>17</v>
+      </c>
+      <c r="D239" t="s">
+        <v>335</v>
+      </c>
+      <c r="E239" t="s">
+        <v>271</v>
+      </c>
+      <c r="F239" t="s">
+        <v>12</v>
+      </c>
+      <c r="G239" t="s">
+        <v>61</v>
       </c>
       <c r="K239" t="s">
-        <v>380</v>
-      </c>
-      <c r="L239" t="s">
-        <v>138</v>
+        <v>377</v>
+      </c>
+      <c r="L239" s="1" t="s">
+        <v>269</v>
       </c>
     </row>
     <row r="240" spans="1:12" ht="16.5" customHeight="1">
@@ -6663,45 +6660,45 @@
         <v>84</v>
       </c>
       <c r="B240" t="s">
-        <v>380</v>
+        <v>378</v>
       </c>
       <c r="C240" t="s">
-        <v>9</v>
+        <v>56</v>
       </c>
       <c r="K240" t="s">
-        <v>381</v>
-      </c>
-      <c r="L240" s="1" t="s">
-        <v>315</v>
+        <v>378</v>
+      </c>
+      <c r="L240" t="s">
+        <v>138</v>
       </c>
     </row>
     <row r="241" spans="1:12" ht="16.5" customHeight="1">
       <c r="A241" t="s">
-        <v>198</v>
+        <v>84</v>
       </c>
       <c r="B241" t="s">
-        <v>382</v>
+        <v>378</v>
       </c>
       <c r="C241" t="s">
-        <v>9</v>
+        <v>17</v>
       </c>
       <c r="D241" t="s">
-        <v>354</v>
+        <v>335</v>
       </c>
       <c r="E241" t="s">
-        <v>385</v>
+        <v>271</v>
       </c>
       <c r="F241" t="s">
-        <v>98</v>
+        <v>12</v>
       </c>
       <c r="G241" t="s">
-        <v>13</v>
+        <v>61</v>
       </c>
       <c r="K241" t="s">
-        <v>382</v>
-      </c>
-      <c r="L241" t="s">
-        <v>132</v>
+        <v>379</v>
+      </c>
+      <c r="L241" s="1" t="s">
+        <v>270</v>
       </c>
     </row>
     <row r="242" spans="1:12" ht="16.5" customHeight="1">
@@ -6709,28 +6706,16 @@
         <v>84</v>
       </c>
       <c r="B242" t="s">
-        <v>382</v>
+        <v>380</v>
       </c>
       <c r="C242" t="s">
-        <v>9</v>
-      </c>
-      <c r="D242" t="s">
-        <v>354</v>
-      </c>
-      <c r="F242" t="s">
-        <v>98</v>
-      </c>
-      <c r="H242" t="s">
-        <v>386</v>
-      </c>
-      <c r="I242" t="s">
-        <v>300</v>
+        <v>310</v>
       </c>
       <c r="K242" t="s">
-        <v>382</v>
+        <v>380</v>
       </c>
       <c r="L242" t="s">
-        <v>132</v>
+        <v>138</v>
       </c>
     </row>
     <row r="243" spans="1:12" ht="16.5" customHeight="1">
@@ -6738,36 +6723,45 @@
         <v>84</v>
       </c>
       <c r="B243" t="s">
-        <v>383</v>
+        <v>380</v>
       </c>
       <c r="C243" t="s">
-        <v>17</v>
-      </c>
-      <c r="H243" t="s">
-        <v>154</v>
+        <v>9</v>
       </c>
       <c r="K243" t="s">
-        <v>383</v>
-      </c>
-      <c r="L243" t="s">
-        <v>133</v>
+        <v>381</v>
+      </c>
+      <c r="L243" s="1" t="s">
+        <v>315</v>
       </c>
     </row>
     <row r="244" spans="1:12" ht="16.5" customHeight="1">
       <c r="A244" t="s">
-        <v>84</v>
+        <v>198</v>
       </c>
       <c r="B244" t="s">
-        <v>384</v>
+        <v>382</v>
       </c>
       <c r="C244" t="s">
         <v>9</v>
       </c>
+      <c r="D244" t="s">
+        <v>354</v>
+      </c>
+      <c r="E244" t="s">
+        <v>385</v>
+      </c>
+      <c r="F244" t="s">
+        <v>98</v>
+      </c>
+      <c r="G244" t="s">
+        <v>13</v>
+      </c>
       <c r="K244" t="s">
-        <v>384</v>
+        <v>382</v>
       </c>
       <c r="L244" t="s">
-        <v>136</v>
+        <v>132</v>
       </c>
     </row>
     <row r="245" spans="1:12" ht="16.5" customHeight="1">
@@ -6775,13 +6769,25 @@
         <v>84</v>
       </c>
       <c r="B245" t="s">
-        <v>164</v>
+        <v>382</v>
       </c>
       <c r="C245" t="s">
-        <v>89</v>
+        <v>9</v>
+      </c>
+      <c r="D245" t="s">
+        <v>354</v>
+      </c>
+      <c r="F245" t="s">
+        <v>98</v>
+      </c>
+      <c r="H245" t="s">
+        <v>386</v>
+      </c>
+      <c r="I245" t="s">
+        <v>300</v>
       </c>
       <c r="K245" t="s">
-        <v>164</v>
+        <v>382</v>
       </c>
       <c r="L245" t="s">
         <v>132</v>
@@ -6792,28 +6798,19 @@
         <v>84</v>
       </c>
       <c r="B246" t="s">
-        <v>165</v>
+        <v>383</v>
       </c>
       <c r="C246" t="s">
-        <v>9</v>
-      </c>
-      <c r="D246" t="s">
-        <v>341</v>
-      </c>
-      <c r="E246" t="s">
-        <v>167</v>
-      </c>
-      <c r="F246" t="s">
-        <v>12</v>
-      </c>
-      <c r="G246" t="s">
-        <v>13</v>
+        <v>17</v>
+      </c>
+      <c r="H246" t="s">
+        <v>154</v>
       </c>
       <c r="K246" t="s">
-        <v>165</v>
+        <v>383</v>
       </c>
       <c r="L246" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
     </row>
     <row r="247" spans="1:12" ht="16.5" customHeight="1">
@@ -6821,13 +6818,13 @@
         <v>84</v>
       </c>
       <c r="B247" t="s">
-        <v>166</v>
+        <v>384</v>
       </c>
       <c r="C247" t="s">
         <v>9</v>
       </c>
       <c r="K247" t="s">
-        <v>166</v>
+        <v>384</v>
       </c>
       <c r="L247" t="s">
         <v>136</v>
@@ -6838,13 +6835,13 @@
         <v>84</v>
       </c>
       <c r="B248" t="s">
-        <v>168</v>
+        <v>164</v>
       </c>
       <c r="C248" t="s">
-        <v>19</v>
+        <v>89</v>
       </c>
       <c r="K248" t="s">
-        <v>168</v>
+        <v>164</v>
       </c>
       <c r="L248" t="s">
         <v>132</v>
@@ -6855,16 +6852,25 @@
         <v>84</v>
       </c>
       <c r="B249" t="s">
-        <v>122</v>
+        <v>165</v>
       </c>
       <c r="C249" t="s">
         <v>9</v>
       </c>
-      <c r="J249" t="s">
-        <v>42</v>
+      <c r="D249" t="s">
+        <v>341</v>
+      </c>
+      <c r="E249" t="s">
+        <v>167</v>
+      </c>
+      <c r="F249" t="s">
+        <v>12</v>
+      </c>
+      <c r="G249" t="s">
+        <v>13</v>
       </c>
       <c r="K249" t="s">
-        <v>122</v>
+        <v>165</v>
       </c>
       <c r="L249" t="s">
         <v>132</v>
@@ -6875,28 +6881,16 @@
         <v>84</v>
       </c>
       <c r="B250" t="s">
-        <v>123</v>
+        <v>166</v>
       </c>
       <c r="C250" t="s">
         <v>9</v>
       </c>
-      <c r="D250" t="s">
-        <v>335</v>
-      </c>
-      <c r="E250" t="s">
-        <v>124</v>
-      </c>
-      <c r="F250" t="s">
-        <v>12</v>
-      </c>
-      <c r="G250" t="s">
-        <v>13</v>
-      </c>
       <c r="K250" t="s">
-        <v>123</v>
+        <v>166</v>
       </c>
       <c r="L250" t="s">
-        <v>132</v>
+        <v>136</v>
       </c>
     </row>
     <row r="251" spans="1:12" ht="16.5" customHeight="1">
@@ -6904,16 +6898,16 @@
         <v>84</v>
       </c>
       <c r="B251" t="s">
-        <v>228</v>
+        <v>168</v>
       </c>
       <c r="C251" t="s">
-        <v>56</v>
+        <v>19</v>
       </c>
       <c r="K251" t="s">
-        <v>228</v>
+        <v>168</v>
       </c>
       <c r="L251" t="s">
-        <v>138</v>
+        <v>132</v>
       </c>
     </row>
     <row r="252" spans="1:12" ht="16.5" customHeight="1">
@@ -6921,28 +6915,19 @@
         <v>84</v>
       </c>
       <c r="B252" t="s">
-        <v>228</v>
+        <v>122</v>
       </c>
       <c r="C252" t="s">
-        <v>17</v>
-      </c>
-      <c r="D252" t="s">
-        <v>335</v>
-      </c>
-      <c r="E252" t="s">
-        <v>271</v>
-      </c>
-      <c r="F252" t="s">
-        <v>12</v>
-      </c>
-      <c r="G252" t="s">
-        <v>61</v>
+        <v>9</v>
+      </c>
+      <c r="J252" t="s">
+        <v>42</v>
       </c>
       <c r="K252" t="s">
-        <v>251</v>
-      </c>
-      <c r="L252" s="1" t="s">
-        <v>270</v>
+        <v>122</v>
+      </c>
+      <c r="L252" t="s">
+        <v>132</v>
       </c>
     </row>
     <row r="253" spans="1:12" ht="16.5" customHeight="1">
@@ -6950,16 +6935,28 @@
         <v>84</v>
       </c>
       <c r="B253" t="s">
-        <v>161</v>
+        <v>123</v>
       </c>
       <c r="C253" t="s">
         <v>9</v>
       </c>
+      <c r="D253" t="s">
+        <v>335</v>
+      </c>
+      <c r="E253" t="s">
+        <v>124</v>
+      </c>
+      <c r="F253" t="s">
+        <v>12</v>
+      </c>
+      <c r="G253" t="s">
+        <v>13</v>
+      </c>
       <c r="K253" t="s">
-        <v>161</v>
+        <v>123</v>
       </c>
       <c r="L253" t="s">
-        <v>136</v>
+        <v>132</v>
       </c>
     </row>
     <row r="254" spans="1:12" ht="16.5" customHeight="1">
@@ -6967,79 +6964,79 @@
         <v>84</v>
       </c>
       <c r="B254" t="s">
-        <v>209</v>
+        <v>228</v>
       </c>
       <c r="C254" t="s">
-        <v>89</v>
+        <v>56</v>
       </c>
       <c r="K254" t="s">
-        <v>209</v>
+        <v>228</v>
       </c>
       <c r="L254" t="s">
-        <v>132</v>
+        <v>138</v>
       </c>
     </row>
     <row r="255" spans="1:12" ht="16.5" customHeight="1">
       <c r="A255" t="s">
-        <v>125</v>
+        <v>84</v>
       </c>
       <c r="B255" t="s">
-        <v>126</v>
+        <v>228</v>
       </c>
       <c r="C255" t="s">
-        <v>9</v>
+        <v>17</v>
+      </c>
+      <c r="D255" t="s">
+        <v>335</v>
+      </c>
+      <c r="E255" t="s">
+        <v>271</v>
+      </c>
+      <c r="F255" t="s">
+        <v>12</v>
+      </c>
+      <c r="G255" t="s">
+        <v>61</v>
       </c>
       <c r="K255" t="s">
-        <v>126</v>
-      </c>
-      <c r="L255" t="s">
-        <v>131</v>
+        <v>251</v>
+      </c>
+      <c r="L255" s="1" t="s">
+        <v>270</v>
       </c>
     </row>
     <row r="256" spans="1:12" ht="16.5" customHeight="1">
       <c r="A256" t="s">
-        <v>125</v>
+        <v>84</v>
       </c>
       <c r="B256" t="s">
-        <v>127</v>
+        <v>161</v>
       </c>
       <c r="C256" t="s">
         <v>9</v>
       </c>
-      <c r="D256" t="s">
-        <v>332</v>
-      </c>
-      <c r="E256" t="s">
-        <v>11</v>
-      </c>
-      <c r="F256" t="s">
-        <v>12</v>
-      </c>
-      <c r="G256" t="s">
-        <v>13</v>
-      </c>
       <c r="K256" t="s">
-        <v>127</v>
+        <v>161</v>
       </c>
       <c r="L256" t="s">
-        <v>163</v>
+        <v>136</v>
       </c>
     </row>
     <row r="257" spans="1:12" ht="16.5" customHeight="1">
       <c r="A257" t="s">
-        <v>125</v>
+        <v>84</v>
       </c>
       <c r="B257" t="s">
-        <v>128</v>
+        <v>209</v>
       </c>
       <c r="C257" t="s">
-        <v>17</v>
+        <v>89</v>
       </c>
       <c r="K257" t="s">
-        <v>128</v>
+        <v>209</v>
       </c>
       <c r="L257" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
     </row>
     <row r="258" spans="1:12" ht="16.5" customHeight="1">
@@ -7047,16 +7044,16 @@
         <v>125</v>
       </c>
       <c r="B258" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="C258" t="s">
-        <v>19</v>
+        <v>9</v>
       </c>
       <c r="K258" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="L258" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="259" spans="1:12" ht="16.5" customHeight="1">
@@ -7064,16 +7061,28 @@
         <v>125</v>
       </c>
       <c r="B259" t="s">
-        <v>294</v>
+        <v>127</v>
       </c>
       <c r="C259" t="s">
-        <v>19</v>
+        <v>9</v>
+      </c>
+      <c r="D259" t="s">
+        <v>332</v>
+      </c>
+      <c r="E259" t="s">
+        <v>11</v>
+      </c>
+      <c r="F259" t="s">
+        <v>12</v>
+      </c>
+      <c r="G259" t="s">
+        <v>13</v>
       </c>
       <c r="K259" t="s">
-        <v>294</v>
+        <v>127</v>
       </c>
       <c r="L259" t="s">
-        <v>132</v>
+        <v>163</v>
       </c>
     </row>
     <row r="260" spans="1:12" ht="16.5" customHeight="1">
@@ -7081,28 +7090,16 @@
         <v>125</v>
       </c>
       <c r="B260" t="s">
-        <v>216</v>
+        <v>128</v>
       </c>
       <c r="C260" t="s">
         <v>17</v>
       </c>
-      <c r="D260" t="s">
-        <v>356</v>
-      </c>
-      <c r="E260" t="s">
-        <v>219</v>
-      </c>
-      <c r="F260" t="s">
-        <v>215</v>
-      </c>
-      <c r="G260" t="s">
-        <v>221</v>
-      </c>
       <c r="K260" t="s">
-        <v>216</v>
+        <v>128</v>
       </c>
       <c r="L260" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
     </row>
     <row r="261" spans="1:12" ht="16.5" customHeight="1">
@@ -7110,13 +7107,13 @@
         <v>125</v>
       </c>
       <c r="B261" t="s">
-        <v>217</v>
+        <v>129</v>
       </c>
       <c r="C261" t="s">
         <v>19</v>
       </c>
       <c r="K261" t="s">
-        <v>217</v>
+        <v>129</v>
       </c>
       <c r="L261" t="s">
         <v>132</v>
@@ -7127,16 +7124,16 @@
         <v>125</v>
       </c>
       <c r="B262" t="s">
-        <v>218</v>
+        <v>294</v>
       </c>
       <c r="C262" t="s">
-        <v>56</v>
+        <v>19</v>
       </c>
       <c r="K262" t="s">
-        <v>218</v>
+        <v>294</v>
       </c>
       <c r="L262" t="s">
-        <v>138</v>
+        <v>132</v>
       </c>
     </row>
     <row r="263" spans="1:12" ht="16.5" customHeight="1">
@@ -7144,28 +7141,28 @@
         <v>125</v>
       </c>
       <c r="B263" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="C263" t="s">
         <v>17</v>
       </c>
       <c r="D263" t="s">
-        <v>335</v>
+        <v>356</v>
       </c>
       <c r="E263" t="s">
-        <v>271</v>
+        <v>219</v>
       </c>
       <c r="F263" t="s">
-        <v>12</v>
+        <v>215</v>
       </c>
       <c r="G263" t="s">
-        <v>61</v>
+        <v>221</v>
       </c>
       <c r="K263" t="s">
-        <v>250</v>
-      </c>
-      <c r="L263" s="1" t="s">
-        <v>270</v>
+        <v>216</v>
+      </c>
+      <c r="L263" t="s">
+        <v>132</v>
       </c>
     </row>
     <row r="264" spans="1:12" ht="16.5" customHeight="1">
@@ -7173,16 +7170,13 @@
         <v>125</v>
       </c>
       <c r="B264" t="s">
-        <v>229</v>
+        <v>217</v>
       </c>
       <c r="C264" t="s">
-        <v>9</v>
-      </c>
-      <c r="J264" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="K264" t="s">
-        <v>229</v>
+        <v>217</v>
       </c>
       <c r="L264" t="s">
         <v>132</v>
@@ -7193,27 +7187,93 @@
         <v>125</v>
       </c>
       <c r="B265" t="s">
+        <v>218</v>
+      </c>
+      <c r="C265" t="s">
+        <v>56</v>
+      </c>
+      <c r="K265" t="s">
+        <v>218</v>
+      </c>
+      <c r="L265" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="266" spans="1:12" ht="16.5" customHeight="1">
+      <c r="A266" t="s">
+        <v>125</v>
+      </c>
+      <c r="B266" t="s">
+        <v>218</v>
+      </c>
+      <c r="C266" t="s">
+        <v>17</v>
+      </c>
+      <c r="D266" t="s">
+        <v>335</v>
+      </c>
+      <c r="E266" t="s">
+        <v>271</v>
+      </c>
+      <c r="F266" t="s">
+        <v>12</v>
+      </c>
+      <c r="G266" t="s">
+        <v>61</v>
+      </c>
+      <c r="K266" t="s">
+        <v>250</v>
+      </c>
+      <c r="L266" s="1" t="s">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="267" spans="1:12" ht="16.5" customHeight="1">
+      <c r="A267" t="s">
+        <v>125</v>
+      </c>
+      <c r="B267" t="s">
+        <v>229</v>
+      </c>
+      <c r="C267" t="s">
+        <v>9</v>
+      </c>
+      <c r="J267" t="s">
+        <v>22</v>
+      </c>
+      <c r="K267" t="s">
+        <v>229</v>
+      </c>
+      <c r="L267" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="268" spans="1:12" ht="16.5" customHeight="1">
+      <c r="A268" t="s">
+        <v>125</v>
+      </c>
+      <c r="B268" t="s">
         <v>239</v>
       </c>
-      <c r="C265" t="s">
+      <c r="C268" t="s">
         <v>17</v>
       </c>
-      <c r="D265" t="s">
+      <c r="D268" t="s">
         <v>357</v>
       </c>
-      <c r="E265" t="s">
+      <c r="E268" t="s">
         <v>240</v>
       </c>
-      <c r="F265" t="s">
+      <c r="F268" t="s">
         <v>12</v>
       </c>
-      <c r="G265" t="s">
+      <c r="G268" t="s">
         <v>241</v>
       </c>
-      <c r="K265" t="s">
+      <c r="K268" t="s">
         <v>239</v>
       </c>
-      <c r="L265" t="s">
+      <c r="L268" t="s">
         <v>132</v>
       </c>
     </row>

</xml_diff>

<commit_message>
journal system message code search criterion
</commit_message>
<xml_diff>
--- a/criterion_property_definitions.xlsx
+++ b/criterion_property_definitions.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1717" uniqueCount="407">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1742" uniqueCount="412">
   <si>
     <t>property</t>
   </si>
@@ -1238,6 +1238,21 @@
   </si>
   <si>
     <t>inputField.localized</t>
+  </si>
+  <si>
+    <t>proband.journalEntries</t>
+  </si>
+  <si>
+    <t>proband.journalEntries.systemMessageCode</t>
+  </si>
+  <si>
+    <t>completeSystemMessageCode</t>
+  </si>
+  <si>
+    <t>proband.journalEntries.modifiedTimestamp</t>
+  </si>
+  <si>
+    <t>proband.journalEntries.modifiedTimestampByPeriod</t>
   </si>
 </sst>
 </file>
@@ -1570,10 +1585,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:L268"/>
+  <dimension ref="A1:L272"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A94" workbookViewId="0">
-      <selection activeCell="B114" sqref="B114"/>
+    <sheetView tabSelected="1" topLeftCell="A234" workbookViewId="0">
+      <selection activeCell="A261" sqref="A261"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="15.7109375" defaultRowHeight="16.5" customHeight="1"/>
@@ -7041,82 +7056,85 @@
     </row>
     <row r="258" spans="1:12" ht="16.5" customHeight="1">
       <c r="A258" t="s">
-        <v>125</v>
+        <v>84</v>
       </c>
       <c r="B258" t="s">
-        <v>126</v>
+        <v>407</v>
       </c>
       <c r="C258" t="s">
         <v>9</v>
       </c>
       <c r="K258" t="s">
-        <v>126</v>
+        <v>407</v>
       </c>
       <c r="L258" t="s">
-        <v>131</v>
+        <v>136</v>
       </c>
     </row>
     <row r="259" spans="1:12" ht="16.5" customHeight="1">
       <c r="A259" t="s">
-        <v>125</v>
+        <v>84</v>
       </c>
       <c r="B259" t="s">
-        <v>127</v>
+        <v>408</v>
       </c>
       <c r="C259" t="s">
-        <v>9</v>
-      </c>
-      <c r="D259" t="s">
-        <v>332</v>
-      </c>
-      <c r="E259" t="s">
-        <v>11</v>
-      </c>
-      <c r="F259" t="s">
-        <v>12</v>
-      </c>
-      <c r="G259" t="s">
-        <v>13</v>
+        <v>17</v>
+      </c>
+      <c r="H259" t="s">
+        <v>409</v>
       </c>
       <c r="K259" t="s">
-        <v>127</v>
+        <v>408</v>
       </c>
       <c r="L259" t="s">
-        <v>163</v>
+        <v>133</v>
       </c>
     </row>
     <row r="260" spans="1:12" ht="16.5" customHeight="1">
       <c r="A260" t="s">
-        <v>125</v>
+        <v>84</v>
       </c>
       <c r="B260" t="s">
-        <v>128</v>
+        <v>410</v>
       </c>
       <c r="C260" t="s">
-        <v>17</v>
+        <v>56</v>
       </c>
       <c r="K260" t="s">
-        <v>128</v>
+        <v>410</v>
       </c>
       <c r="L260" t="s">
-        <v>133</v>
+        <v>138</v>
       </c>
     </row>
     <row r="261" spans="1:12" ht="16.5" customHeight="1">
       <c r="A261" t="s">
-        <v>125</v>
+        <v>84</v>
       </c>
       <c r="B261" t="s">
-        <v>129</v>
+        <v>410</v>
       </c>
       <c r="C261" t="s">
-        <v>19</v>
+        <v>17</v>
+      </c>
+      <c r="D261" t="s">
+        <v>335</v>
+      </c>
+      <c r="E261" t="s">
+        <v>271</v>
+      </c>
+      <c r="F261" t="s">
+        <v>12</v>
+      </c>
+      <c r="G261" t="s">
+        <v>61</v>
       </c>
       <c r="K261" t="s">
-        <v>129</v>
-      </c>
-      <c r="L261" t="s">
-        <v>132</v>
+        <v>411</v>
+      </c>
+      <c r="L261" s="1" t="s">
+        <v>270</v>
       </c>
     </row>
     <row r="262" spans="1:12" ht="16.5" customHeight="1">
@@ -7124,16 +7142,16 @@
         <v>125</v>
       </c>
       <c r="B262" t="s">
-        <v>294</v>
+        <v>126</v>
       </c>
       <c r="C262" t="s">
-        <v>19</v>
+        <v>9</v>
       </c>
       <c r="K262" t="s">
-        <v>294</v>
+        <v>126</v>
       </c>
       <c r="L262" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="263" spans="1:12" ht="16.5" customHeight="1">
@@ -7141,28 +7159,28 @@
         <v>125</v>
       </c>
       <c r="B263" t="s">
-        <v>216</v>
+        <v>127</v>
       </c>
       <c r="C263" t="s">
-        <v>17</v>
+        <v>9</v>
       </c>
       <c r="D263" t="s">
-        <v>356</v>
+        <v>332</v>
       </c>
       <c r="E263" t="s">
-        <v>219</v>
+        <v>11</v>
       </c>
       <c r="F263" t="s">
-        <v>215</v>
+        <v>12</v>
       </c>
       <c r="G263" t="s">
-        <v>221</v>
+        <v>13</v>
       </c>
       <c r="K263" t="s">
-        <v>216</v>
+        <v>127</v>
       </c>
       <c r="L263" t="s">
-        <v>132</v>
+        <v>163</v>
       </c>
     </row>
     <row r="264" spans="1:12" ht="16.5" customHeight="1">
@@ -7170,16 +7188,16 @@
         <v>125</v>
       </c>
       <c r="B264" t="s">
-        <v>217</v>
+        <v>128</v>
       </c>
       <c r="C264" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="K264" t="s">
-        <v>217</v>
+        <v>128</v>
       </c>
       <c r="L264" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
     </row>
     <row r="265" spans="1:12" ht="16.5" customHeight="1">
@@ -7187,16 +7205,16 @@
         <v>125</v>
       </c>
       <c r="B265" t="s">
-        <v>218</v>
+        <v>129</v>
       </c>
       <c r="C265" t="s">
-        <v>56</v>
+        <v>19</v>
       </c>
       <c r="K265" t="s">
-        <v>218</v>
+        <v>129</v>
       </c>
       <c r="L265" t="s">
-        <v>138</v>
+        <v>132</v>
       </c>
     </row>
     <row r="266" spans="1:12" ht="16.5" customHeight="1">
@@ -7204,28 +7222,16 @@
         <v>125</v>
       </c>
       <c r="B266" t="s">
-        <v>218</v>
+        <v>294</v>
       </c>
       <c r="C266" t="s">
-        <v>17</v>
-      </c>
-      <c r="D266" t="s">
-        <v>335</v>
-      </c>
-      <c r="E266" t="s">
-        <v>271</v>
-      </c>
-      <c r="F266" t="s">
-        <v>12</v>
-      </c>
-      <c r="G266" t="s">
-        <v>61</v>
+        <v>19</v>
       </c>
       <c r="K266" t="s">
-        <v>250</v>
-      </c>
-      <c r="L266" s="1" t="s">
-        <v>270</v>
+        <v>294</v>
+      </c>
+      <c r="L266" t="s">
+        <v>132</v>
       </c>
     </row>
     <row r="267" spans="1:12" ht="16.5" customHeight="1">
@@ -7233,16 +7239,25 @@
         <v>125</v>
       </c>
       <c r="B267" t="s">
-        <v>229</v>
+        <v>216</v>
       </c>
       <c r="C267" t="s">
-        <v>9</v>
-      </c>
-      <c r="J267" t="s">
-        <v>22</v>
+        <v>17</v>
+      </c>
+      <c r="D267" t="s">
+        <v>356</v>
+      </c>
+      <c r="E267" t="s">
+        <v>219</v>
+      </c>
+      <c r="F267" t="s">
+        <v>215</v>
+      </c>
+      <c r="G267" t="s">
+        <v>221</v>
       </c>
       <c r="K267" t="s">
-        <v>229</v>
+        <v>216</v>
       </c>
       <c r="L267" t="s">
         <v>132</v>
@@ -7253,27 +7268,110 @@
         <v>125</v>
       </c>
       <c r="B268" t="s">
+        <v>217</v>
+      </c>
+      <c r="C268" t="s">
+        <v>19</v>
+      </c>
+      <c r="K268" t="s">
+        <v>217</v>
+      </c>
+      <c r="L268" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="269" spans="1:12" ht="16.5" customHeight="1">
+      <c r="A269" t="s">
+        <v>125</v>
+      </c>
+      <c r="B269" t="s">
+        <v>218</v>
+      </c>
+      <c r="C269" t="s">
+        <v>56</v>
+      </c>
+      <c r="K269" t="s">
+        <v>218</v>
+      </c>
+      <c r="L269" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="270" spans="1:12" ht="16.5" customHeight="1">
+      <c r="A270" t="s">
+        <v>125</v>
+      </c>
+      <c r="B270" t="s">
+        <v>218</v>
+      </c>
+      <c r="C270" t="s">
+        <v>17</v>
+      </c>
+      <c r="D270" t="s">
+        <v>335</v>
+      </c>
+      <c r="E270" t="s">
+        <v>271</v>
+      </c>
+      <c r="F270" t="s">
+        <v>12</v>
+      </c>
+      <c r="G270" t="s">
+        <v>61</v>
+      </c>
+      <c r="K270" t="s">
+        <v>250</v>
+      </c>
+      <c r="L270" s="1" t="s">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="271" spans="1:12" ht="16.5" customHeight="1">
+      <c r="A271" t="s">
+        <v>125</v>
+      </c>
+      <c r="B271" t="s">
+        <v>229</v>
+      </c>
+      <c r="C271" t="s">
+        <v>9</v>
+      </c>
+      <c r="J271" t="s">
+        <v>22</v>
+      </c>
+      <c r="K271" t="s">
+        <v>229</v>
+      </c>
+      <c r="L271" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="272" spans="1:12" ht="16.5" customHeight="1">
+      <c r="A272" t="s">
+        <v>125</v>
+      </c>
+      <c r="B272" t="s">
         <v>239</v>
       </c>
-      <c r="C268" t="s">
+      <c r="C272" t="s">
         <v>17</v>
       </c>
-      <c r="D268" t="s">
+      <c r="D272" t="s">
         <v>357</v>
       </c>
-      <c r="E268" t="s">
+      <c r="E272" t="s">
         <v>240</v>
       </c>
-      <c r="F268" t="s">
+      <c r="F272" t="s">
         <v>12</v>
       </c>
-      <c r="G268" t="s">
+      <c r="G272" t="s">
         <v>241</v>
       </c>
-      <c r="K268" t="s">
+      <c r="K272" t="s">
         <v>239</v>
       </c>
-      <c r="L268" t="s">
+      <c r="L272" t="s">
         <v>132</v>
       </c>
     </row>

</xml_diff>

<commit_message>
mass mail module permissions and query editor criteria
+ fix trial timeline event permission
</commit_message>
<xml_diff>
--- a/criterion_property_definitions.xlsx
+++ b/criterion_property_definitions.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1742" uniqueCount="412">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1855" uniqueCount="435">
   <si>
     <t>property</t>
   </si>
@@ -1253,6 +1253,75 @@
   </si>
   <si>
     <t>proband.journalEntries.modifiedTimestampByPeriod</t>
+  </si>
+  <si>
+    <t>MASS_MAIL_DB</t>
+  </si>
+  <si>
+    <t>massMail.id</t>
+  </si>
+  <si>
+    <t>massMail.name</t>
+  </si>
+  <si>
+    <t>massMail.start</t>
+  </si>
+  <si>
+    <t>massMail.start.startByPeriod</t>
+  </si>
+  <si>
+    <t>massMail.status.id</t>
+  </si>
+  <si>
+    <t>massMail.type.id</t>
+  </si>
+  <si>
+    <t>massMail.trial.id</t>
+  </si>
+  <si>
+    <t>massMail.probandListStatus.id</t>
+  </si>
+  <si>
+    <t>massMail.fromAddress</t>
+  </si>
+  <si>
+    <t>massMail.fromName</t>
+  </si>
+  <si>
+    <t>massMail.locale</t>
+  </si>
+  <si>
+    <t>massMail.textTemplate</t>
+  </si>
+  <si>
+    <t>massMail.probandTo</t>
+  </si>
+  <si>
+    <t>massMail.physicianTo</t>
+  </si>
+  <si>
+    <t>massMail.useBeacon</t>
+  </si>
+  <si>
+    <t>massMail.recipients</t>
+  </si>
+  <si>
+    <t>massMail.recipients.proband.id</t>
+  </si>
+  <si>
+    <t>massMail.department.id</t>
+  </si>
+  <si>
+    <t>getLocales</t>
+  </si>
+  <si>
+    <t>getLanguage</t>
+  </si>
+  <si>
+    <t>getAllMassMailStatusTypes</t>
+  </si>
+  <si>
+    <t>getAllMassMailTypes</t>
   </si>
 </sst>
 </file>
@@ -1585,10 +1654,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:L272"/>
+  <dimension ref="A1:L290"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A234" workbookViewId="0">
-      <selection activeCell="A261" sqref="A261"/>
+    <sheetView tabSelected="1" topLeftCell="A253" workbookViewId="0">
+      <selection activeCell="E280" sqref="E280"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="15.7109375" defaultRowHeight="16.5" customHeight="1"/>
@@ -6955,9 +7024,6 @@
       <c r="C253" t="s">
         <v>9</v>
       </c>
-      <c r="D253" t="s">
-        <v>335</v>
-      </c>
       <c r="E253" t="s">
         <v>124</v>
       </c>
@@ -7372,6 +7438,384 @@
         <v>239</v>
       </c>
       <c r="L272" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="273" spans="1:12" ht="16.5" customHeight="1">
+      <c r="A273" t="s">
+        <v>412</v>
+      </c>
+      <c r="B273" t="s">
+        <v>413</v>
+      </c>
+      <c r="C273" t="s">
+        <v>9</v>
+      </c>
+      <c r="K273" t="s">
+        <v>413</v>
+      </c>
+      <c r="L273" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="274" spans="1:12" ht="16.5" customHeight="1">
+      <c r="A274" t="s">
+        <v>412</v>
+      </c>
+      <c r="B274" t="s">
+        <v>430</v>
+      </c>
+      <c r="C274" t="s">
+        <v>9</v>
+      </c>
+      <c r="D274" t="s">
+        <v>332</v>
+      </c>
+      <c r="E274" t="s">
+        <v>11</v>
+      </c>
+      <c r="F274" t="s">
+        <v>12</v>
+      </c>
+      <c r="G274" t="s">
+        <v>13</v>
+      </c>
+      <c r="K274" t="s">
+        <v>430</v>
+      </c>
+      <c r="L274" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="275" spans="1:12" ht="16.5" customHeight="1">
+      <c r="A275" t="s">
+        <v>412</v>
+      </c>
+      <c r="B275" t="s">
+        <v>414</v>
+      </c>
+      <c r="C275" t="s">
+        <v>17</v>
+      </c>
+      <c r="K275" t="s">
+        <v>414</v>
+      </c>
+      <c r="L275" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="276" spans="1:12" ht="16.5" customHeight="1">
+      <c r="A276" t="s">
+        <v>412</v>
+      </c>
+      <c r="B276" t="s">
+        <v>415</v>
+      </c>
+      <c r="C276" t="s">
+        <v>56</v>
+      </c>
+      <c r="K276" t="s">
+        <v>415</v>
+      </c>
+      <c r="L276" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="277" spans="1:12" ht="16.5" customHeight="1">
+      <c r="A277" t="s">
+        <v>412</v>
+      </c>
+      <c r="B277" t="s">
+        <v>415</v>
+      </c>
+      <c r="C277" t="s">
+        <v>17</v>
+      </c>
+      <c r="D277" t="s">
+        <v>335</v>
+      </c>
+      <c r="E277" t="s">
+        <v>271</v>
+      </c>
+      <c r="F277" t="s">
+        <v>12</v>
+      </c>
+      <c r="G277" t="s">
+        <v>61</v>
+      </c>
+      <c r="K277" t="s">
+        <v>416</v>
+      </c>
+      <c r="L277" s="1" t="s">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="278" spans="1:12" ht="16.5" customHeight="1">
+      <c r="A278" t="s">
+        <v>412</v>
+      </c>
+      <c r="B278" t="s">
+        <v>417</v>
+      </c>
+      <c r="C278" t="s">
+        <v>9</v>
+      </c>
+      <c r="D278" t="s">
+        <v>343</v>
+      </c>
+      <c r="E278" t="s">
+        <v>433</v>
+      </c>
+      <c r="F278" t="s">
+        <v>12</v>
+      </c>
+      <c r="G278" t="s">
+        <v>13</v>
+      </c>
+      <c r="K278" t="s">
+        <v>417</v>
+      </c>
+      <c r="L278" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="279" spans="1:12" ht="16.5" customHeight="1">
+      <c r="A279" t="s">
+        <v>412</v>
+      </c>
+      <c r="B279" t="s">
+        <v>418</v>
+      </c>
+      <c r="C279" t="s">
+        <v>9</v>
+      </c>
+      <c r="D279" t="s">
+        <v>344</v>
+      </c>
+      <c r="E279" t="s">
+        <v>434</v>
+      </c>
+      <c r="F279" t="s">
+        <v>12</v>
+      </c>
+      <c r="G279" t="s">
+        <v>13</v>
+      </c>
+      <c r="K279" t="s">
+        <v>418</v>
+      </c>
+      <c r="L279" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="280" spans="1:12" ht="16.5" customHeight="1">
+      <c r="A280" t="s">
+        <v>412</v>
+      </c>
+      <c r="B280" t="s">
+        <v>419</v>
+      </c>
+      <c r="C280" t="s">
+        <v>9</v>
+      </c>
+      <c r="J280" t="s">
+        <v>42</v>
+      </c>
+      <c r="K280" t="s">
+        <v>419</v>
+      </c>
+      <c r="L280" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="281" spans="1:12" ht="16.5" customHeight="1">
+      <c r="A281" t="s">
+        <v>412</v>
+      </c>
+      <c r="B281" t="s">
+        <v>420</v>
+      </c>
+      <c r="C281" t="s">
+        <v>9</v>
+      </c>
+      <c r="E281" t="s">
+        <v>124</v>
+      </c>
+      <c r="F281" t="s">
+        <v>12</v>
+      </c>
+      <c r="G281" t="s">
+        <v>13</v>
+      </c>
+      <c r="K281" t="s">
+        <v>420</v>
+      </c>
+      <c r="L281" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="282" spans="1:12" ht="16.5" customHeight="1">
+      <c r="A282" t="s">
+        <v>412</v>
+      </c>
+      <c r="B282" t="s">
+        <v>421</v>
+      </c>
+      <c r="C282" t="s">
+        <v>17</v>
+      </c>
+      <c r="K282" t="s">
+        <v>421</v>
+      </c>
+      <c r="L282" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="283" spans="1:12" ht="16.5" customHeight="1">
+      <c r="A283" t="s">
+        <v>412</v>
+      </c>
+      <c r="B283" t="s">
+        <v>422</v>
+      </c>
+      <c r="C283" t="s">
+        <v>17</v>
+      </c>
+      <c r="K283" t="s">
+        <v>422</v>
+      </c>
+      <c r="L283" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="284" spans="1:12" ht="16.5" customHeight="1">
+      <c r="A284" t="s">
+        <v>412</v>
+      </c>
+      <c r="B284" t="s">
+        <v>423</v>
+      </c>
+      <c r="C284" t="s">
+        <v>17</v>
+      </c>
+      <c r="E284" t="s">
+        <v>431</v>
+      </c>
+      <c r="F284" t="s">
+        <v>12</v>
+      </c>
+      <c r="G284" t="s">
+        <v>432</v>
+      </c>
+      <c r="K284" t="s">
+        <v>423</v>
+      </c>
+      <c r="L284" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="285" spans="1:12" ht="16.5" customHeight="1">
+      <c r="A285" t="s">
+        <v>412</v>
+      </c>
+      <c r="B285" t="s">
+        <v>424</v>
+      </c>
+      <c r="C285" t="s">
+        <v>17</v>
+      </c>
+      <c r="K285" t="s">
+        <v>424</v>
+      </c>
+      <c r="L285" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="286" spans="1:12" ht="16.5" customHeight="1">
+      <c r="A286" t="s">
+        <v>412</v>
+      </c>
+      <c r="B286" t="s">
+        <v>425</v>
+      </c>
+      <c r="C286" t="s">
+        <v>19</v>
+      </c>
+      <c r="K286" t="s">
+        <v>425</v>
+      </c>
+      <c r="L286" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="287" spans="1:12" ht="16.5" customHeight="1">
+      <c r="A287" t="s">
+        <v>412</v>
+      </c>
+      <c r="B287" t="s">
+        <v>426</v>
+      </c>
+      <c r="C287" t="s">
+        <v>19</v>
+      </c>
+      <c r="K287" t="s">
+        <v>426</v>
+      </c>
+      <c r="L287" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="288" spans="1:12" ht="16.5" customHeight="1">
+      <c r="A288" t="s">
+        <v>412</v>
+      </c>
+      <c r="B288" t="s">
+        <v>427</v>
+      </c>
+      <c r="C288" t="s">
+        <v>19</v>
+      </c>
+      <c r="K288" t="s">
+        <v>427</v>
+      </c>
+      <c r="L288" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="289" spans="1:12" ht="16.5" customHeight="1">
+      <c r="A289" t="s">
+        <v>412</v>
+      </c>
+      <c r="B289" t="s">
+        <v>428</v>
+      </c>
+      <c r="C289" t="s">
+        <v>9</v>
+      </c>
+      <c r="K289" t="s">
+        <v>428</v>
+      </c>
+      <c r="L289" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="290" spans="1:12" ht="16.5" customHeight="1">
+      <c r="A290" t="s">
+        <v>412</v>
+      </c>
+      <c r="B290" t="s">
+        <v>429</v>
+      </c>
+      <c r="C290" t="s">
+        <v>9</v>
+      </c>
+      <c r="J290" t="s">
+        <v>84</v>
+      </c>
+      <c r="K290" t="s">
+        <v>429</v>
+      </c>
+      <c r="L290" t="s">
         <v>132</v>
       </c>
     </row>

</xml_diff>

<commit_message>
new criterions: subject mass mail, number of addresses
+ add office tmpfiles to gitignore
</commit_message>
<xml_diff>
--- a/criterion_property_definitions.xlsx
+++ b/criterion_property_definitions.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1855" uniqueCount="435">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1866" uniqueCount="437">
   <si>
     <t>property</t>
   </si>
@@ -1322,6 +1322,12 @@
   </si>
   <si>
     <t>getAllMassMailTypes</t>
+  </si>
+  <si>
+    <t>proband.addresses</t>
+  </si>
+  <si>
+    <t>proband.massMailReceipts.massMail.id</t>
   </si>
 </sst>
 </file>
@@ -1654,10 +1660,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:L290"/>
+  <dimension ref="A1:L292"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A253" workbookViewId="0">
-      <selection activeCell="E280" sqref="E280"/>
+    <sheetView tabSelected="1" topLeftCell="A244" workbookViewId="0">
+      <selection activeCell="A253" sqref="A253"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="15.7109375" defaultRowHeight="16.5" customHeight="1"/>
@@ -5380,36 +5386,24 @@
     </row>
     <row r="179" spans="1:12" ht="16.5" customHeight="1">
       <c r="A179" t="s">
-        <v>198</v>
+        <v>84</v>
       </c>
       <c r="B179" t="s">
-        <v>96</v>
+        <v>435</v>
       </c>
       <c r="C179" t="s">
         <v>9</v>
       </c>
-      <c r="D179" t="s">
-        <v>352</v>
-      </c>
-      <c r="E179" t="s">
-        <v>97</v>
-      </c>
-      <c r="F179" t="s">
-        <v>98</v>
-      </c>
-      <c r="G179" t="s">
-        <v>13</v>
-      </c>
       <c r="K179" t="s">
-        <v>96</v>
+        <v>435</v>
       </c>
       <c r="L179" t="s">
-        <v>132</v>
+        <v>136</v>
       </c>
     </row>
     <row r="180" spans="1:12" ht="16.5" customHeight="1">
       <c r="A180" t="s">
-        <v>84</v>
+        <v>198</v>
       </c>
       <c r="B180" t="s">
         <v>96</v>
@@ -5420,14 +5414,14 @@
       <c r="D180" t="s">
         <v>352</v>
       </c>
+      <c r="E180" t="s">
+        <v>97</v>
+      </c>
       <c r="F180" t="s">
         <v>98</v>
       </c>
-      <c r="H180" t="s">
-        <v>295</v>
-      </c>
-      <c r="I180" t="s">
-        <v>296</v>
+      <c r="G180" t="s">
+        <v>13</v>
       </c>
       <c r="K180" t="s">
         <v>96</v>
@@ -5438,28 +5432,28 @@
     </row>
     <row r="181" spans="1:12" ht="16.5" customHeight="1">
       <c r="A181" t="s">
-        <v>198</v>
+        <v>84</v>
       </c>
       <c r="B181" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="C181" t="s">
         <v>9</v>
       </c>
       <c r="D181" t="s">
-        <v>353</v>
-      </c>
-      <c r="E181" t="s">
-        <v>100</v>
+        <v>352</v>
       </c>
       <c r="F181" t="s">
-        <v>12</v>
-      </c>
-      <c r="G181" t="s">
-        <v>13</v>
+        <v>98</v>
+      </c>
+      <c r="H181" t="s">
+        <v>295</v>
+      </c>
+      <c r="I181" t="s">
+        <v>296</v>
       </c>
       <c r="K181" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="L181" t="s">
         <v>132</v>
@@ -5467,7 +5461,7 @@
     </row>
     <row r="182" spans="1:12" ht="16.5" customHeight="1">
       <c r="A182" t="s">
-        <v>84</v>
+        <v>198</v>
       </c>
       <c r="B182" t="s">
         <v>99</v>
@@ -5478,14 +5472,14 @@
       <c r="D182" t="s">
         <v>353</v>
       </c>
+      <c r="E182" t="s">
+        <v>100</v>
+      </c>
       <c r="F182" t="s">
         <v>12</v>
       </c>
-      <c r="H182" t="s">
-        <v>297</v>
-      </c>
-      <c r="I182" t="s">
-        <v>298</v>
+      <c r="G182" t="s">
+        <v>13</v>
       </c>
       <c r="K182" t="s">
         <v>99</v>
@@ -5499,16 +5493,28 @@
         <v>84</v>
       </c>
       <c r="B183" t="s">
-        <v>197</v>
+        <v>99</v>
       </c>
       <c r="C183" t="s">
         <v>9</v>
       </c>
+      <c r="D183" t="s">
+        <v>353</v>
+      </c>
+      <c r="F183" t="s">
+        <v>12</v>
+      </c>
+      <c r="H183" t="s">
+        <v>297</v>
+      </c>
+      <c r="I183" t="s">
+        <v>298</v>
+      </c>
       <c r="K183" t="s">
-        <v>197</v>
+        <v>99</v>
       </c>
       <c r="L183" t="s">
-        <v>136</v>
+        <v>132</v>
       </c>
     </row>
     <row r="184" spans="1:12" ht="16.5" customHeight="1">
@@ -5516,19 +5522,16 @@
         <v>84</v>
       </c>
       <c r="B184" t="s">
-        <v>195</v>
+        <v>197</v>
       </c>
       <c r="C184" t="s">
         <v>9</v>
       </c>
-      <c r="J184" t="s">
-        <v>42</v>
-      </c>
       <c r="K184" t="s">
-        <v>195</v>
+        <v>197</v>
       </c>
       <c r="L184" t="s">
-        <v>132</v>
+        <v>136</v>
       </c>
     </row>
     <row r="185" spans="1:12" ht="16.5" customHeight="1">
@@ -5536,16 +5539,19 @@
         <v>84</v>
       </c>
       <c r="B185" t="s">
-        <v>140</v>
+        <v>195</v>
       </c>
       <c r="C185" t="s">
-        <v>56</v>
+        <v>9</v>
+      </c>
+      <c r="J185" t="s">
+        <v>42</v>
       </c>
       <c r="K185" t="s">
-        <v>140</v>
+        <v>195</v>
       </c>
       <c r="L185" t="s">
-        <v>138</v>
+        <v>132</v>
       </c>
     </row>
     <row r="186" spans="1:12" ht="16.5" customHeight="1">
@@ -5556,25 +5562,13 @@
         <v>140</v>
       </c>
       <c r="C186" t="s">
-        <v>17</v>
-      </c>
-      <c r="D186" t="s">
-        <v>335</v>
-      </c>
-      <c r="E186" t="s">
-        <v>271</v>
-      </c>
-      <c r="F186" t="s">
-        <v>12</v>
-      </c>
-      <c r="G186" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
       <c r="K186" t="s">
-        <v>257</v>
-      </c>
-      <c r="L186" s="1" t="s">
-        <v>270</v>
+        <v>140</v>
+      </c>
+      <c r="L186" t="s">
+        <v>138</v>
       </c>
     </row>
     <row r="187" spans="1:12" ht="16.5" customHeight="1">
@@ -5582,19 +5576,28 @@
         <v>84</v>
       </c>
       <c r="B187" t="s">
-        <v>144</v>
+        <v>140</v>
       </c>
       <c r="C187" t="s">
         <v>17</v>
       </c>
-      <c r="H187" t="s">
-        <v>143</v>
+      <c r="D187" t="s">
+        <v>335</v>
+      </c>
+      <c r="E187" t="s">
+        <v>271</v>
+      </c>
+      <c r="F187" t="s">
+        <v>12</v>
+      </c>
+      <c r="G187" t="s">
+        <v>61</v>
       </c>
       <c r="K187" t="s">
-        <v>144</v>
-      </c>
-      <c r="L187" t="s">
-        <v>133</v>
+        <v>257</v>
+      </c>
+      <c r="L187" s="1" t="s">
+        <v>270</v>
       </c>
     </row>
     <row r="188" spans="1:12" ht="16.5" customHeight="1">
@@ -5602,16 +5605,19 @@
         <v>84</v>
       </c>
       <c r="B188" t="s">
-        <v>101</v>
+        <v>144</v>
       </c>
       <c r="C188" t="s">
-        <v>19</v>
+        <v>17</v>
+      </c>
+      <c r="H188" t="s">
+        <v>143</v>
       </c>
       <c r="K188" t="s">
-        <v>101</v>
+        <v>144</v>
       </c>
       <c r="L188" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
     </row>
     <row r="189" spans="1:12" ht="16.5" customHeight="1">
@@ -5619,16 +5625,16 @@
         <v>84</v>
       </c>
       <c r="B189" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C189" t="s">
-        <v>9</v>
+        <v>19</v>
       </c>
       <c r="K189" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="L189" t="s">
-        <v>138</v>
+        <v>132</v>
       </c>
     </row>
     <row r="190" spans="1:12" ht="16.5" customHeight="1">
@@ -5636,13 +5642,13 @@
         <v>84</v>
       </c>
       <c r="B190" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="C190" t="s">
-        <v>104</v>
+        <v>9</v>
       </c>
       <c r="K190" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="L190" t="s">
         <v>138</v>
@@ -5653,13 +5659,13 @@
         <v>84</v>
       </c>
       <c r="B191" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="C191" t="s">
-        <v>36</v>
+        <v>104</v>
       </c>
       <c r="K191" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="L191" t="s">
         <v>138</v>
@@ -5673,25 +5679,13 @@
         <v>105</v>
       </c>
       <c r="C192" t="s">
-        <v>17</v>
-      </c>
-      <c r="D192" t="s">
-        <v>335</v>
-      </c>
-      <c r="E192" t="s">
-        <v>271</v>
-      </c>
-      <c r="F192" t="s">
-        <v>12</v>
-      </c>
-      <c r="G192" t="s">
-        <v>61</v>
+        <v>36</v>
       </c>
       <c r="K192" t="s">
-        <v>256</v>
-      </c>
-      <c r="L192" s="1" t="s">
-        <v>269</v>
+        <v>105</v>
+      </c>
+      <c r="L192" t="s">
+        <v>138</v>
       </c>
     </row>
     <row r="193" spans="1:12" ht="16.5" customHeight="1">
@@ -5699,16 +5693,28 @@
         <v>84</v>
       </c>
       <c r="B193" t="s">
-        <v>211</v>
+        <v>105</v>
       </c>
       <c r="C193" t="s">
-        <v>56</v>
+        <v>17</v>
+      </c>
+      <c r="D193" t="s">
+        <v>335</v>
+      </c>
+      <c r="E193" t="s">
+        <v>271</v>
+      </c>
+      <c r="F193" t="s">
+        <v>12</v>
+      </c>
+      <c r="G193" t="s">
+        <v>61</v>
       </c>
       <c r="K193" t="s">
-        <v>211</v>
-      </c>
-      <c r="L193" t="s">
-        <v>138</v>
+        <v>256</v>
+      </c>
+      <c r="L193" s="1" t="s">
+        <v>269</v>
       </c>
     </row>
     <row r="194" spans="1:12" ht="16.5" customHeight="1">
@@ -5719,25 +5725,13 @@
         <v>211</v>
       </c>
       <c r="C194" t="s">
-        <v>17</v>
-      </c>
-      <c r="D194" t="s">
-        <v>335</v>
-      </c>
-      <c r="E194" t="s">
-        <v>271</v>
-      </c>
-      <c r="F194" t="s">
-        <v>12</v>
-      </c>
-      <c r="G194" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
       <c r="K194" t="s">
-        <v>255</v>
-      </c>
-      <c r="L194" s="1" t="s">
-        <v>270</v>
+        <v>211</v>
+      </c>
+      <c r="L194" t="s">
+        <v>138</v>
       </c>
     </row>
     <row r="195" spans="1:12" ht="16.5" customHeight="1">
@@ -5745,16 +5739,28 @@
         <v>84</v>
       </c>
       <c r="B195" t="s">
-        <v>313</v>
+        <v>211</v>
       </c>
       <c r="C195" t="s">
-        <v>310</v>
+        <v>17</v>
+      </c>
+      <c r="D195" t="s">
+        <v>335</v>
+      </c>
+      <c r="E195" t="s">
+        <v>271</v>
+      </c>
+      <c r="F195" t="s">
+        <v>12</v>
+      </c>
+      <c r="G195" t="s">
+        <v>61</v>
       </c>
       <c r="K195" t="s">
-        <v>313</v>
-      </c>
-      <c r="L195" t="s">
-        <v>138</v>
+        <v>255</v>
+      </c>
+      <c r="L195" s="1" t="s">
+        <v>270</v>
       </c>
     </row>
     <row r="196" spans="1:12" ht="16.5" customHeight="1">
@@ -5765,47 +5771,35 @@
         <v>313</v>
       </c>
       <c r="C196" t="s">
-        <v>9</v>
+        <v>310</v>
       </c>
       <c r="K196" t="s">
-        <v>314</v>
-      </c>
-      <c r="L196" s="1" t="s">
-        <v>315</v>
+        <v>313</v>
+      </c>
+      <c r="L196" t="s">
+        <v>138</v>
       </c>
     </row>
     <row r="197" spans="1:12" ht="16.5" customHeight="1">
       <c r="A197" t="s">
-        <v>198</v>
+        <v>84</v>
       </c>
       <c r="B197" t="s">
-        <v>106</v>
+        <v>313</v>
       </c>
       <c r="C197" t="s">
         <v>9</v>
       </c>
-      <c r="D197" t="s">
-        <v>354</v>
-      </c>
-      <c r="E197" t="s">
-        <v>107</v>
-      </c>
-      <c r="F197" t="s">
-        <v>98</v>
-      </c>
-      <c r="G197" t="s">
-        <v>13</v>
-      </c>
       <c r="K197" t="s">
-        <v>106</v>
-      </c>
-      <c r="L197" t="s">
-        <v>132</v>
+        <v>314</v>
+      </c>
+      <c r="L197" s="1" t="s">
+        <v>315</v>
       </c>
     </row>
     <row r="198" spans="1:12" ht="16.5" customHeight="1">
       <c r="A198" t="s">
-        <v>84</v>
+        <v>198</v>
       </c>
       <c r="B198" t="s">
         <v>106</v>
@@ -5816,14 +5810,14 @@
       <c r="D198" t="s">
         <v>354</v>
       </c>
+      <c r="E198" t="s">
+        <v>107</v>
+      </c>
       <c r="F198" t="s">
         <v>98</v>
       </c>
-      <c r="H198" t="s">
-        <v>299</v>
-      </c>
-      <c r="I198" t="s">
-        <v>300</v>
+      <c r="G198" t="s">
+        <v>13</v>
       </c>
       <c r="K198" t="s">
         <v>106</v>
@@ -5837,19 +5831,28 @@
         <v>84</v>
       </c>
       <c r="B199" t="s">
-        <v>153</v>
+        <v>106</v>
       </c>
       <c r="C199" t="s">
-        <v>17</v>
+        <v>9</v>
+      </c>
+      <c r="D199" t="s">
+        <v>354</v>
+      </c>
+      <c r="F199" t="s">
+        <v>98</v>
       </c>
       <c r="H199" t="s">
-        <v>154</v>
+        <v>299</v>
+      </c>
+      <c r="I199" t="s">
+        <v>300</v>
       </c>
       <c r="K199" t="s">
-        <v>153</v>
+        <v>106</v>
       </c>
       <c r="L199" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
     </row>
     <row r="200" spans="1:12" ht="16.5" customHeight="1">
@@ -5857,50 +5860,41 @@
         <v>84</v>
       </c>
       <c r="B200" t="s">
-        <v>147</v>
+        <v>153</v>
       </c>
       <c r="C200" t="s">
-        <v>9</v>
+        <v>17</v>
+      </c>
+      <c r="H200" t="s">
+        <v>154</v>
       </c>
       <c r="K200" t="s">
-        <v>147</v>
+        <v>153</v>
       </c>
       <c r="L200" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
     </row>
     <row r="201" spans="1:12" ht="16.5" customHeight="1">
       <c r="A201" t="s">
-        <v>198</v>
+        <v>84</v>
       </c>
       <c r="B201" t="s">
-        <v>108</v>
+        <v>147</v>
       </c>
       <c r="C201" t="s">
         <v>9</v>
       </c>
-      <c r="D201" t="s">
-        <v>355</v>
-      </c>
-      <c r="E201" t="s">
-        <v>109</v>
-      </c>
-      <c r="F201" t="s">
-        <v>98</v>
-      </c>
-      <c r="G201" t="s">
-        <v>13</v>
-      </c>
       <c r="K201" t="s">
-        <v>108</v>
+        <v>147</v>
       </c>
       <c r="L201" t="s">
-        <v>132</v>
+        <v>136</v>
       </c>
     </row>
     <row r="202" spans="1:12" ht="16.5" customHeight="1">
       <c r="A202" t="s">
-        <v>84</v>
+        <v>198</v>
       </c>
       <c r="B202" t="s">
         <v>108</v>
@@ -5911,14 +5905,14 @@
       <c r="D202" t="s">
         <v>355</v>
       </c>
+      <c r="E202" t="s">
+        <v>109</v>
+      </c>
       <c r="F202" t="s">
         <v>98</v>
       </c>
-      <c r="H202" t="s">
-        <v>301</v>
-      </c>
-      <c r="I202" t="s">
-        <v>302</v>
+      <c r="G202" t="s">
+        <v>13</v>
       </c>
       <c r="K202" t="s">
         <v>108</v>
@@ -5929,28 +5923,28 @@
     </row>
     <row r="203" spans="1:12" ht="16.5" customHeight="1">
       <c r="A203" t="s">
-        <v>198</v>
+        <v>84</v>
       </c>
       <c r="B203" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="C203" t="s">
         <v>9</v>
       </c>
       <c r="D203" t="s">
-        <v>353</v>
-      </c>
-      <c r="E203" t="s">
-        <v>111</v>
+        <v>355</v>
       </c>
       <c r="F203" t="s">
-        <v>12</v>
-      </c>
-      <c r="G203" t="s">
-        <v>13</v>
+        <v>98</v>
+      </c>
+      <c r="H203" t="s">
+        <v>301</v>
+      </c>
+      <c r="I203" t="s">
+        <v>302</v>
       </c>
       <c r="K203" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="L203" t="s">
         <v>132</v>
@@ -5958,7 +5952,7 @@
     </row>
     <row r="204" spans="1:12" ht="16.5" customHeight="1">
       <c r="A204" t="s">
-        <v>84</v>
+        <v>198</v>
       </c>
       <c r="B204" t="s">
         <v>110</v>
@@ -5969,14 +5963,14 @@
       <c r="D204" t="s">
         <v>353</v>
       </c>
+      <c r="E204" t="s">
+        <v>111</v>
+      </c>
       <c r="F204" t="s">
         <v>12</v>
       </c>
-      <c r="H204" t="s">
-        <v>303</v>
-      </c>
-      <c r="I204" t="s">
-        <v>298</v>
+      <c r="G204" t="s">
+        <v>13</v>
       </c>
       <c r="K204" t="s">
         <v>110</v>
@@ -5990,53 +5984,65 @@
         <v>84</v>
       </c>
       <c r="B205" t="s">
-        <v>196</v>
+        <v>110</v>
       </c>
       <c r="C205" t="s">
         <v>9</v>
       </c>
+      <c r="D205" t="s">
+        <v>353</v>
+      </c>
+      <c r="F205" t="s">
+        <v>12</v>
+      </c>
+      <c r="H205" t="s">
+        <v>303</v>
+      </c>
+      <c r="I205" t="s">
+        <v>298</v>
+      </c>
       <c r="K205" t="s">
-        <v>196</v>
+        <v>110</v>
       </c>
       <c r="L205" t="s">
-        <v>136</v>
+        <v>132</v>
       </c>
     </row>
     <row r="206" spans="1:12" ht="16.5" customHeight="1">
       <c r="A206" t="s">
-        <v>198</v>
+        <v>84</v>
       </c>
       <c r="B206" t="s">
-        <v>122</v>
+        <v>196</v>
       </c>
       <c r="C206" t="s">
         <v>9</v>
       </c>
-      <c r="J206" t="s">
-        <v>42</v>
-      </c>
       <c r="K206" t="s">
-        <v>122</v>
+        <v>196</v>
       </c>
       <c r="L206" t="s">
-        <v>132</v>
+        <v>136</v>
       </c>
     </row>
     <row r="207" spans="1:12" ht="16.5" customHeight="1">
       <c r="A207" t="s">
-        <v>84</v>
+        <v>198</v>
       </c>
       <c r="B207" t="s">
-        <v>141</v>
+        <v>122</v>
       </c>
       <c r="C207" t="s">
-        <v>56</v>
+        <v>9</v>
+      </c>
+      <c r="J207" t="s">
+        <v>42</v>
       </c>
       <c r="K207" t="s">
-        <v>141</v>
+        <v>122</v>
       </c>
       <c r="L207" t="s">
-        <v>138</v>
+        <v>132</v>
       </c>
     </row>
     <row r="208" spans="1:12" ht="16.5" customHeight="1">
@@ -6047,25 +6053,13 @@
         <v>141</v>
       </c>
       <c r="C208" t="s">
-        <v>17</v>
-      </c>
-      <c r="D208" t="s">
-        <v>335</v>
-      </c>
-      <c r="E208" t="s">
-        <v>271</v>
-      </c>
-      <c r="F208" t="s">
-        <v>12</v>
-      </c>
-      <c r="G208" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
       <c r="K208" t="s">
-        <v>254</v>
-      </c>
-      <c r="L208" s="1" t="s">
-        <v>270</v>
+        <v>141</v>
+      </c>
+      <c r="L208" t="s">
+        <v>138</v>
       </c>
     </row>
     <row r="209" spans="1:12" ht="16.5" customHeight="1">
@@ -6073,19 +6067,28 @@
         <v>84</v>
       </c>
       <c r="B209" t="s">
-        <v>145</v>
+        <v>141</v>
       </c>
       <c r="C209" t="s">
         <v>17</v>
       </c>
-      <c r="H209" t="s">
-        <v>143</v>
+      <c r="D209" t="s">
+        <v>335</v>
+      </c>
+      <c r="E209" t="s">
+        <v>271</v>
+      </c>
+      <c r="F209" t="s">
+        <v>12</v>
+      </c>
+      <c r="G209" t="s">
+        <v>61</v>
       </c>
       <c r="K209" t="s">
-        <v>145</v>
-      </c>
-      <c r="L209" t="s">
-        <v>133</v>
+        <v>254</v>
+      </c>
+      <c r="L209" s="1" t="s">
+        <v>270</v>
       </c>
     </row>
     <row r="210" spans="1:12" ht="16.5" customHeight="1">
@@ -6093,16 +6096,19 @@
         <v>84</v>
       </c>
       <c r="B210" t="s">
-        <v>112</v>
+        <v>145</v>
       </c>
       <c r="C210" t="s">
-        <v>19</v>
+        <v>17</v>
+      </c>
+      <c r="H210" t="s">
+        <v>143</v>
       </c>
       <c r="K210" t="s">
-        <v>112</v>
+        <v>145</v>
       </c>
       <c r="L210" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
     </row>
     <row r="211" spans="1:12" ht="16.5" customHeight="1">
@@ -6110,16 +6116,16 @@
         <v>84</v>
       </c>
       <c r="B211" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="C211" t="s">
-        <v>9</v>
+        <v>19</v>
       </c>
       <c r="K211" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="L211" t="s">
-        <v>138</v>
+        <v>132</v>
       </c>
     </row>
     <row r="212" spans="1:12" ht="16.5" customHeight="1">
@@ -6127,13 +6133,13 @@
         <v>84</v>
       </c>
       <c r="B212" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="C212" t="s">
-        <v>104</v>
+        <v>9</v>
       </c>
       <c r="K212" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="L212" t="s">
         <v>138</v>
@@ -6144,13 +6150,13 @@
         <v>84</v>
       </c>
       <c r="B213" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="C213" t="s">
-        <v>36</v>
+        <v>104</v>
       </c>
       <c r="K213" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="L213" t="s">
         <v>138</v>
@@ -6164,25 +6170,13 @@
         <v>115</v>
       </c>
       <c r="C214" t="s">
-        <v>17</v>
-      </c>
-      <c r="D214" t="s">
-        <v>335</v>
-      </c>
-      <c r="E214" t="s">
-        <v>271</v>
-      </c>
-      <c r="F214" t="s">
-        <v>12</v>
-      </c>
-      <c r="G214" t="s">
-        <v>61</v>
+        <v>36</v>
       </c>
       <c r="K214" t="s">
-        <v>253</v>
-      </c>
-      <c r="L214" s="1" t="s">
-        <v>269</v>
+        <v>115</v>
+      </c>
+      <c r="L214" t="s">
+        <v>138</v>
       </c>
     </row>
     <row r="215" spans="1:12" ht="16.5" customHeight="1">
@@ -6190,16 +6184,28 @@
         <v>84</v>
       </c>
       <c r="B215" t="s">
-        <v>210</v>
+        <v>115</v>
       </c>
       <c r="C215" t="s">
-        <v>56</v>
+        <v>17</v>
+      </c>
+      <c r="D215" t="s">
+        <v>335</v>
+      </c>
+      <c r="E215" t="s">
+        <v>271</v>
+      </c>
+      <c r="F215" t="s">
+        <v>12</v>
+      </c>
+      <c r="G215" t="s">
+        <v>61</v>
       </c>
       <c r="K215" t="s">
-        <v>210</v>
-      </c>
-      <c r="L215" t="s">
-        <v>138</v>
+        <v>253</v>
+      </c>
+      <c r="L215" s="1" t="s">
+        <v>269</v>
       </c>
     </row>
     <row r="216" spans="1:12" ht="16.5" customHeight="1">
@@ -6210,25 +6216,13 @@
         <v>210</v>
       </c>
       <c r="C216" t="s">
-        <v>17</v>
-      </c>
-      <c r="D216" t="s">
-        <v>335</v>
-      </c>
-      <c r="E216" t="s">
-        <v>271</v>
-      </c>
-      <c r="F216" t="s">
-        <v>12</v>
-      </c>
-      <c r="G216" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
       <c r="K216" t="s">
-        <v>252</v>
-      </c>
-      <c r="L216" s="1" t="s">
-        <v>270</v>
+        <v>210</v>
+      </c>
+      <c r="L216" t="s">
+        <v>138</v>
       </c>
     </row>
     <row r="217" spans="1:12" ht="16.5" customHeight="1">
@@ -6236,16 +6230,28 @@
         <v>84</v>
       </c>
       <c r="B217" t="s">
-        <v>316</v>
+        <v>210</v>
       </c>
       <c r="C217" t="s">
-        <v>310</v>
+        <v>17</v>
+      </c>
+      <c r="D217" t="s">
+        <v>335</v>
+      </c>
+      <c r="E217" t="s">
+        <v>271</v>
+      </c>
+      <c r="F217" t="s">
+        <v>12</v>
+      </c>
+      <c r="G217" t="s">
+        <v>61</v>
       </c>
       <c r="K217" t="s">
-        <v>316</v>
-      </c>
-      <c r="L217" t="s">
-        <v>138</v>
+        <v>252</v>
+      </c>
+      <c r="L217" s="1" t="s">
+        <v>270</v>
       </c>
     </row>
     <row r="218" spans="1:12" ht="16.5" customHeight="1">
@@ -6256,47 +6262,35 @@
         <v>316</v>
       </c>
       <c r="C218" t="s">
-        <v>9</v>
+        <v>310</v>
       </c>
       <c r="K218" t="s">
-        <v>317</v>
-      </c>
-      <c r="L218" s="1" t="s">
-        <v>315</v>
+        <v>316</v>
+      </c>
+      <c r="L218" t="s">
+        <v>138</v>
       </c>
     </row>
     <row r="219" spans="1:12" ht="16.5" customHeight="1">
       <c r="A219" t="s">
-        <v>198</v>
+        <v>84</v>
       </c>
       <c r="B219" t="s">
-        <v>116</v>
+        <v>316</v>
       </c>
       <c r="C219" t="s">
         <v>9</v>
       </c>
-      <c r="D219" t="s">
-        <v>354</v>
-      </c>
-      <c r="E219" t="s">
-        <v>117</v>
-      </c>
-      <c r="F219" t="s">
-        <v>98</v>
-      </c>
-      <c r="G219" t="s">
-        <v>13</v>
-      </c>
       <c r="K219" t="s">
-        <v>116</v>
-      </c>
-      <c r="L219" t="s">
-        <v>132</v>
+        <v>317</v>
+      </c>
+      <c r="L219" s="1" t="s">
+        <v>315</v>
       </c>
     </row>
     <row r="220" spans="1:12" ht="16.5" customHeight="1">
       <c r="A220" t="s">
-        <v>84</v>
+        <v>198</v>
       </c>
       <c r="B220" t="s">
         <v>116</v>
@@ -6307,14 +6301,14 @@
       <c r="D220" t="s">
         <v>354</v>
       </c>
+      <c r="E220" t="s">
+        <v>117</v>
+      </c>
       <c r="F220" t="s">
         <v>98</v>
       </c>
-      <c r="H220" t="s">
-        <v>304</v>
-      </c>
-      <c r="I220" t="s">
-        <v>300</v>
+      <c r="G220" t="s">
+        <v>13</v>
       </c>
       <c r="K220" t="s">
         <v>116</v>
@@ -6328,19 +6322,28 @@
         <v>84</v>
       </c>
       <c r="B221" t="s">
-        <v>155</v>
+        <v>116</v>
       </c>
       <c r="C221" t="s">
-        <v>17</v>
+        <v>9</v>
+      </c>
+      <c r="D221" t="s">
+        <v>354</v>
+      </c>
+      <c r="F221" t="s">
+        <v>98</v>
       </c>
       <c r="H221" t="s">
-        <v>154</v>
+        <v>304</v>
+      </c>
+      <c r="I221" t="s">
+        <v>300</v>
       </c>
       <c r="K221" t="s">
-        <v>155</v>
+        <v>116</v>
       </c>
       <c r="L221" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
     </row>
     <row r="222" spans="1:12" ht="16.5" customHeight="1">
@@ -6348,16 +6351,19 @@
         <v>84</v>
       </c>
       <c r="B222" t="s">
-        <v>146</v>
+        <v>155</v>
       </c>
       <c r="C222" t="s">
-        <v>9</v>
+        <v>17</v>
+      </c>
+      <c r="H222" t="s">
+        <v>154</v>
       </c>
       <c r="K222" t="s">
-        <v>146</v>
+        <v>155</v>
       </c>
       <c r="L222" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
     </row>
     <row r="223" spans="1:12" ht="16.5" customHeight="1">
@@ -6365,16 +6371,16 @@
         <v>84</v>
       </c>
       <c r="B223" t="s">
-        <v>118</v>
+        <v>146</v>
       </c>
       <c r="C223" t="s">
-        <v>89</v>
+        <v>9</v>
       </c>
       <c r="K223" t="s">
-        <v>118</v>
+        <v>146</v>
       </c>
       <c r="L223" t="s">
-        <v>132</v>
+        <v>136</v>
       </c>
     </row>
     <row r="224" spans="1:12" ht="16.5" customHeight="1">
@@ -6382,25 +6388,13 @@
         <v>84</v>
       </c>
       <c r="B224" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="C224" t="s">
-        <v>9</v>
-      </c>
-      <c r="D224" t="s">
-        <v>360</v>
-      </c>
-      <c r="E224" t="s">
-        <v>120</v>
-      </c>
-      <c r="F224" t="s">
-        <v>12</v>
-      </c>
-      <c r="G224" t="s">
-        <v>13</v>
+        <v>89</v>
       </c>
       <c r="K224" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="L224" t="s">
         <v>132</v>
@@ -6411,50 +6405,50 @@
         <v>84</v>
       </c>
       <c r="B225" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="C225" t="s">
         <v>9</v>
       </c>
+      <c r="D225" t="s">
+        <v>360</v>
+      </c>
+      <c r="E225" t="s">
+        <v>120</v>
+      </c>
+      <c r="F225" t="s">
+        <v>12</v>
+      </c>
+      <c r="G225" t="s">
+        <v>13</v>
+      </c>
       <c r="K225" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="L225" t="s">
-        <v>136</v>
+        <v>132</v>
       </c>
     </row>
     <row r="226" spans="1:12" ht="16.5" customHeight="1">
       <c r="A226" t="s">
-        <v>198</v>
+        <v>84</v>
       </c>
       <c r="B226" t="s">
-        <v>361</v>
+        <v>121</v>
       </c>
       <c r="C226" t="s">
         <v>9</v>
       </c>
-      <c r="D226" t="s">
-        <v>362</v>
-      </c>
-      <c r="E226" t="s">
-        <v>363</v>
-      </c>
-      <c r="F226" t="s">
-        <v>98</v>
-      </c>
-      <c r="G226" t="s">
-        <v>13</v>
-      </c>
       <c r="K226" t="s">
-        <v>361</v>
+        <v>121</v>
       </c>
       <c r="L226" t="s">
-        <v>132</v>
+        <v>136</v>
       </c>
     </row>
     <row r="227" spans="1:12" ht="16.5" customHeight="1">
       <c r="A227" t="s">
-        <v>84</v>
+        <v>198</v>
       </c>
       <c r="B227" t="s">
         <v>361</v>
@@ -6465,14 +6459,14 @@
       <c r="D227" t="s">
         <v>362</v>
       </c>
+      <c r="E227" t="s">
+        <v>363</v>
+      </c>
       <c r="F227" t="s">
         <v>98</v>
       </c>
-      <c r="H227" t="s">
-        <v>364</v>
-      </c>
-      <c r="I227" t="s">
-        <v>365</v>
+      <c r="G227" t="s">
+        <v>13</v>
       </c>
       <c r="K227" t="s">
         <v>361</v>
@@ -6483,28 +6477,28 @@
     </row>
     <row r="228" spans="1:12" ht="16.5" customHeight="1">
       <c r="A228" t="s">
-        <v>198</v>
+        <v>84</v>
       </c>
       <c r="B228" t="s">
-        <v>366</v>
+        <v>361</v>
       </c>
       <c r="C228" t="s">
         <v>9</v>
       </c>
       <c r="D228" t="s">
-        <v>353</v>
-      </c>
-      <c r="E228" t="s">
-        <v>367</v>
+        <v>362</v>
       </c>
       <c r="F228" t="s">
-        <v>12</v>
-      </c>
-      <c r="G228" t="s">
-        <v>13</v>
+        <v>98</v>
+      </c>
+      <c r="H228" t="s">
+        <v>364</v>
+      </c>
+      <c r="I228" t="s">
+        <v>365</v>
       </c>
       <c r="K228" t="s">
-        <v>366</v>
+        <v>361</v>
       </c>
       <c r="L228" t="s">
         <v>132</v>
@@ -6512,7 +6506,7 @@
     </row>
     <row r="229" spans="1:12" ht="16.5" customHeight="1">
       <c r="A229" t="s">
-        <v>84</v>
+        <v>198</v>
       </c>
       <c r="B229" t="s">
         <v>366</v>
@@ -6523,14 +6517,14 @@
       <c r="D229" t="s">
         <v>353</v>
       </c>
+      <c r="E229" t="s">
+        <v>367</v>
+      </c>
       <c r="F229" t="s">
         <v>12</v>
       </c>
-      <c r="H229" t="s">
-        <v>368</v>
-      </c>
-      <c r="I229" t="s">
-        <v>298</v>
+      <c r="G229" t="s">
+        <v>13</v>
       </c>
       <c r="K229" t="s">
         <v>366</v>
@@ -6544,53 +6538,65 @@
         <v>84</v>
       </c>
       <c r="B230" t="s">
-        <v>369</v>
+        <v>366</v>
       </c>
       <c r="C230" t="s">
         <v>9</v>
       </c>
+      <c r="D230" t="s">
+        <v>353</v>
+      </c>
+      <c r="F230" t="s">
+        <v>12</v>
+      </c>
+      <c r="H230" t="s">
+        <v>368</v>
+      </c>
+      <c r="I230" t="s">
+        <v>298</v>
+      </c>
       <c r="K230" t="s">
-        <v>369</v>
+        <v>366</v>
       </c>
       <c r="L230" t="s">
-        <v>136</v>
+        <v>132</v>
       </c>
     </row>
     <row r="231" spans="1:12" ht="16.5" customHeight="1">
       <c r="A231" t="s">
-        <v>198</v>
+        <v>84</v>
       </c>
       <c r="B231" t="s">
-        <v>122</v>
+        <v>369</v>
       </c>
       <c r="C231" t="s">
         <v>9</v>
       </c>
-      <c r="J231" t="s">
-        <v>42</v>
-      </c>
       <c r="K231" t="s">
-        <v>122</v>
+        <v>369</v>
       </c>
       <c r="L231" t="s">
-        <v>132</v>
+        <v>136</v>
       </c>
     </row>
     <row r="232" spans="1:12" ht="16.5" customHeight="1">
       <c r="A232" t="s">
-        <v>84</v>
+        <v>198</v>
       </c>
       <c r="B232" t="s">
-        <v>370</v>
+        <v>122</v>
       </c>
       <c r="C232" t="s">
-        <v>56</v>
+        <v>9</v>
+      </c>
+      <c r="J232" t="s">
+        <v>42</v>
       </c>
       <c r="K232" t="s">
-        <v>370</v>
+        <v>122</v>
       </c>
       <c r="L232" t="s">
-        <v>138</v>
+        <v>132</v>
       </c>
     </row>
     <row r="233" spans="1:12" ht="16.5" customHeight="1">
@@ -6601,25 +6607,13 @@
         <v>370</v>
       </c>
       <c r="C233" t="s">
-        <v>17</v>
-      </c>
-      <c r="D233" t="s">
-        <v>335</v>
-      </c>
-      <c r="E233" t="s">
-        <v>271</v>
-      </c>
-      <c r="F233" t="s">
-        <v>12</v>
-      </c>
-      <c r="G233" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
       <c r="K233" t="s">
-        <v>371</v>
-      </c>
-      <c r="L233" s="1" t="s">
-        <v>270</v>
+        <v>370</v>
+      </c>
+      <c r="L233" t="s">
+        <v>138</v>
       </c>
     </row>
     <row r="234" spans="1:12" ht="16.5" customHeight="1">
@@ -6627,19 +6621,28 @@
         <v>84</v>
       </c>
       <c r="B234" t="s">
-        <v>372</v>
+        <v>370</v>
       </c>
       <c r="C234" t="s">
         <v>17</v>
       </c>
-      <c r="H234" t="s">
-        <v>143</v>
+      <c r="D234" t="s">
+        <v>335</v>
+      </c>
+      <c r="E234" t="s">
+        <v>271</v>
+      </c>
+      <c r="F234" t="s">
+        <v>12</v>
+      </c>
+      <c r="G234" t="s">
+        <v>61</v>
       </c>
       <c r="K234" t="s">
-        <v>372</v>
-      </c>
-      <c r="L234" t="s">
-        <v>133</v>
+        <v>371</v>
+      </c>
+      <c r="L234" s="1" t="s">
+        <v>270</v>
       </c>
     </row>
     <row r="235" spans="1:12" ht="16.5" customHeight="1">
@@ -6647,16 +6650,19 @@
         <v>84</v>
       </c>
       <c r="B235" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="C235" t="s">
-        <v>19</v>
+        <v>17</v>
+      </c>
+      <c r="H235" t="s">
+        <v>143</v>
       </c>
       <c r="K235" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="L235" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
     </row>
     <row r="236" spans="1:12" ht="16.5" customHeight="1">
@@ -6664,16 +6670,16 @@
         <v>84</v>
       </c>
       <c r="B236" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
       <c r="C236" t="s">
-        <v>9</v>
+        <v>19</v>
       </c>
       <c r="K236" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
       <c r="L236" t="s">
-        <v>138</v>
+        <v>132</v>
       </c>
     </row>
     <row r="237" spans="1:12" ht="16.5" customHeight="1">
@@ -6681,13 +6687,13 @@
         <v>84</v>
       </c>
       <c r="B237" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
       <c r="C237" t="s">
-        <v>104</v>
+        <v>9</v>
       </c>
       <c r="K237" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
       <c r="L237" t="s">
         <v>138</v>
@@ -6698,13 +6704,13 @@
         <v>84</v>
       </c>
       <c r="B238" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="C238" t="s">
-        <v>36</v>
+        <v>104</v>
       </c>
       <c r="K238" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="L238" t="s">
         <v>138</v>
@@ -6718,25 +6724,13 @@
         <v>376</v>
       </c>
       <c r="C239" t="s">
-        <v>17</v>
-      </c>
-      <c r="D239" t="s">
-        <v>335</v>
-      </c>
-      <c r="E239" t="s">
-        <v>271</v>
-      </c>
-      <c r="F239" t="s">
-        <v>12</v>
-      </c>
-      <c r="G239" t="s">
-        <v>61</v>
+        <v>36</v>
       </c>
       <c r="K239" t="s">
-        <v>377</v>
-      </c>
-      <c r="L239" s="1" t="s">
-        <v>269</v>
+        <v>376</v>
+      </c>
+      <c r="L239" t="s">
+        <v>138</v>
       </c>
     </row>
     <row r="240" spans="1:12" ht="16.5" customHeight="1">
@@ -6744,16 +6738,28 @@
         <v>84</v>
       </c>
       <c r="B240" t="s">
-        <v>378</v>
+        <v>376</v>
       </c>
       <c r="C240" t="s">
-        <v>56</v>
+        <v>17</v>
+      </c>
+      <c r="D240" t="s">
+        <v>335</v>
+      </c>
+      <c r="E240" t="s">
+        <v>271</v>
+      </c>
+      <c r="F240" t="s">
+        <v>12</v>
+      </c>
+      <c r="G240" t="s">
+        <v>61</v>
       </c>
       <c r="K240" t="s">
-        <v>378</v>
-      </c>
-      <c r="L240" t="s">
-        <v>138</v>
+        <v>377</v>
+      </c>
+      <c r="L240" s="1" t="s">
+        <v>269</v>
       </c>
     </row>
     <row r="241" spans="1:12" ht="16.5" customHeight="1">
@@ -6764,25 +6770,13 @@
         <v>378</v>
       </c>
       <c r="C241" t="s">
-        <v>17</v>
-      </c>
-      <c r="D241" t="s">
-        <v>335</v>
-      </c>
-      <c r="E241" t="s">
-        <v>271</v>
-      </c>
-      <c r="F241" t="s">
-        <v>12</v>
-      </c>
-      <c r="G241" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
       <c r="K241" t="s">
-        <v>379</v>
-      </c>
-      <c r="L241" s="1" t="s">
-        <v>270</v>
+        <v>378</v>
+      </c>
+      <c r="L241" t="s">
+        <v>138</v>
       </c>
     </row>
     <row r="242" spans="1:12" ht="16.5" customHeight="1">
@@ -6790,16 +6784,28 @@
         <v>84</v>
       </c>
       <c r="B242" t="s">
-        <v>380</v>
+        <v>378</v>
       </c>
       <c r="C242" t="s">
-        <v>310</v>
+        <v>17</v>
+      </c>
+      <c r="D242" t="s">
+        <v>335</v>
+      </c>
+      <c r="E242" t="s">
+        <v>271</v>
+      </c>
+      <c r="F242" t="s">
+        <v>12</v>
+      </c>
+      <c r="G242" t="s">
+        <v>61</v>
       </c>
       <c r="K242" t="s">
-        <v>380</v>
-      </c>
-      <c r="L242" t="s">
-        <v>138</v>
+        <v>379</v>
+      </c>
+      <c r="L242" s="1" t="s">
+        <v>270</v>
       </c>
     </row>
     <row r="243" spans="1:12" ht="16.5" customHeight="1">
@@ -6810,47 +6816,35 @@
         <v>380</v>
       </c>
       <c r="C243" t="s">
-        <v>9</v>
+        <v>310</v>
       </c>
       <c r="K243" t="s">
-        <v>381</v>
-      </c>
-      <c r="L243" s="1" t="s">
-        <v>315</v>
+        <v>380</v>
+      </c>
+      <c r="L243" t="s">
+        <v>138</v>
       </c>
     </row>
     <row r="244" spans="1:12" ht="16.5" customHeight="1">
       <c r="A244" t="s">
-        <v>198</v>
+        <v>84</v>
       </c>
       <c r="B244" t="s">
-        <v>382</v>
+        <v>380</v>
       </c>
       <c r="C244" t="s">
         <v>9</v>
       </c>
-      <c r="D244" t="s">
-        <v>354</v>
-      </c>
-      <c r="E244" t="s">
-        <v>385</v>
-      </c>
-      <c r="F244" t="s">
-        <v>98</v>
-      </c>
-      <c r="G244" t="s">
-        <v>13</v>
-      </c>
       <c r="K244" t="s">
-        <v>382</v>
-      </c>
-      <c r="L244" t="s">
-        <v>132</v>
+        <v>381</v>
+      </c>
+      <c r="L244" s="1" t="s">
+        <v>315</v>
       </c>
     </row>
     <row r="245" spans="1:12" ht="16.5" customHeight="1">
       <c r="A245" t="s">
-        <v>84</v>
+        <v>198</v>
       </c>
       <c r="B245" t="s">
         <v>382</v>
@@ -6861,14 +6855,14 @@
       <c r="D245" t="s">
         <v>354</v>
       </c>
+      <c r="E245" t="s">
+        <v>385</v>
+      </c>
       <c r="F245" t="s">
         <v>98</v>
       </c>
-      <c r="H245" t="s">
-        <v>386</v>
-      </c>
-      <c r="I245" t="s">
-        <v>300</v>
+      <c r="G245" t="s">
+        <v>13</v>
       </c>
       <c r="K245" t="s">
         <v>382</v>
@@ -6882,19 +6876,28 @@
         <v>84</v>
       </c>
       <c r="B246" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
       <c r="C246" t="s">
-        <v>17</v>
+        <v>9</v>
+      </c>
+      <c r="D246" t="s">
+        <v>354</v>
+      </c>
+      <c r="F246" t="s">
+        <v>98</v>
       </c>
       <c r="H246" t="s">
-        <v>154</v>
+        <v>386</v>
+      </c>
+      <c r="I246" t="s">
+        <v>300</v>
       </c>
       <c r="K246" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
       <c r="L246" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
     </row>
     <row r="247" spans="1:12" ht="16.5" customHeight="1">
@@ -6902,16 +6905,19 @@
         <v>84</v>
       </c>
       <c r="B247" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="C247" t="s">
-        <v>9</v>
+        <v>17</v>
+      </c>
+      <c r="H247" t="s">
+        <v>154</v>
       </c>
       <c r="K247" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="L247" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
     </row>
     <row r="248" spans="1:12" ht="16.5" customHeight="1">
@@ -6919,16 +6925,16 @@
         <v>84</v>
       </c>
       <c r="B248" t="s">
-        <v>164</v>
+        <v>384</v>
       </c>
       <c r="C248" t="s">
-        <v>89</v>
+        <v>9</v>
       </c>
       <c r="K248" t="s">
-        <v>164</v>
+        <v>384</v>
       </c>
       <c r="L248" t="s">
-        <v>132</v>
+        <v>136</v>
       </c>
     </row>
     <row r="249" spans="1:12" ht="16.5" customHeight="1">
@@ -6936,25 +6942,13 @@
         <v>84</v>
       </c>
       <c r="B249" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="C249" t="s">
-        <v>9</v>
-      </c>
-      <c r="D249" t="s">
-        <v>341</v>
-      </c>
-      <c r="E249" t="s">
-        <v>167</v>
-      </c>
-      <c r="F249" t="s">
-        <v>12</v>
-      </c>
-      <c r="G249" t="s">
-        <v>13</v>
+        <v>89</v>
       </c>
       <c r="K249" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="L249" t="s">
         <v>132</v>
@@ -6965,16 +6959,28 @@
         <v>84</v>
       </c>
       <c r="B250" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="C250" t="s">
         <v>9</v>
       </c>
+      <c r="D250" t="s">
+        <v>341</v>
+      </c>
+      <c r="E250" t="s">
+        <v>167</v>
+      </c>
+      <c r="F250" t="s">
+        <v>12</v>
+      </c>
+      <c r="G250" t="s">
+        <v>13</v>
+      </c>
       <c r="K250" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="L250" t="s">
-        <v>136</v>
+        <v>132</v>
       </c>
     </row>
     <row r="251" spans="1:12" ht="16.5" customHeight="1">
@@ -6982,16 +6988,16 @@
         <v>84</v>
       </c>
       <c r="B251" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="C251" t="s">
-        <v>19</v>
+        <v>9</v>
       </c>
       <c r="K251" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="L251" t="s">
-        <v>132</v>
+        <v>136</v>
       </c>
     </row>
     <row r="252" spans="1:12" ht="16.5" customHeight="1">
@@ -6999,16 +7005,13 @@
         <v>84</v>
       </c>
       <c r="B252" t="s">
-        <v>122</v>
+        <v>168</v>
       </c>
       <c r="C252" t="s">
-        <v>9</v>
-      </c>
-      <c r="J252" t="s">
-        <v>42</v>
+        <v>19</v>
       </c>
       <c r="K252" t="s">
-        <v>122</v>
+        <v>168</v>
       </c>
       <c r="L252" t="s">
         <v>132</v>
@@ -7019,22 +7022,16 @@
         <v>84</v>
       </c>
       <c r="B253" t="s">
-        <v>123</v>
+        <v>436</v>
       </c>
       <c r="C253" t="s">
         <v>9</v>
       </c>
-      <c r="E253" t="s">
-        <v>124</v>
-      </c>
-      <c r="F253" t="s">
-        <v>12</v>
-      </c>
-      <c r="G253" t="s">
-        <v>13</v>
+      <c r="J253" t="s">
+        <v>412</v>
       </c>
       <c r="K253" t="s">
-        <v>123</v>
+        <v>436</v>
       </c>
       <c r="L253" t="s">
         <v>132</v>
@@ -7045,16 +7042,19 @@
         <v>84</v>
       </c>
       <c r="B254" t="s">
-        <v>228</v>
+        <v>122</v>
       </c>
       <c r="C254" t="s">
-        <v>56</v>
+        <v>9</v>
+      </c>
+      <c r="J254" t="s">
+        <v>42</v>
       </c>
       <c r="K254" t="s">
-        <v>228</v>
+        <v>122</v>
       </c>
       <c r="L254" t="s">
-        <v>138</v>
+        <v>132</v>
       </c>
     </row>
     <row r="255" spans="1:12" ht="16.5" customHeight="1">
@@ -7062,28 +7062,25 @@
         <v>84</v>
       </c>
       <c r="B255" t="s">
-        <v>228</v>
+        <v>123</v>
       </c>
       <c r="C255" t="s">
-        <v>17</v>
-      </c>
-      <c r="D255" t="s">
-        <v>335</v>
+        <v>9</v>
       </c>
       <c r="E255" t="s">
-        <v>271</v>
+        <v>124</v>
       </c>
       <c r="F255" t="s">
         <v>12</v>
       </c>
       <c r="G255" t="s">
-        <v>61</v>
+        <v>13</v>
       </c>
       <c r="K255" t="s">
-        <v>251</v>
-      </c>
-      <c r="L255" s="1" t="s">
-        <v>270</v>
+        <v>123</v>
+      </c>
+      <c r="L255" t="s">
+        <v>132</v>
       </c>
     </row>
     <row r="256" spans="1:12" ht="16.5" customHeight="1">
@@ -7091,16 +7088,16 @@
         <v>84</v>
       </c>
       <c r="B256" t="s">
-        <v>161</v>
+        <v>228</v>
       </c>
       <c r="C256" t="s">
-        <v>9</v>
+        <v>56</v>
       </c>
       <c r="K256" t="s">
-        <v>161</v>
+        <v>228</v>
       </c>
       <c r="L256" t="s">
-        <v>136</v>
+        <v>138</v>
       </c>
     </row>
     <row r="257" spans="1:12" ht="16.5" customHeight="1">
@@ -7108,16 +7105,28 @@
         <v>84</v>
       </c>
       <c r="B257" t="s">
-        <v>209</v>
+        <v>228</v>
       </c>
       <c r="C257" t="s">
-        <v>89</v>
+        <v>17</v>
+      </c>
+      <c r="D257" t="s">
+        <v>335</v>
+      </c>
+      <c r="E257" t="s">
+        <v>271</v>
+      </c>
+      <c r="F257" t="s">
+        <v>12</v>
+      </c>
+      <c r="G257" t="s">
+        <v>61</v>
       </c>
       <c r="K257" t="s">
-        <v>209</v>
-      </c>
-      <c r="L257" t="s">
-        <v>132</v>
+        <v>251</v>
+      </c>
+      <c r="L257" s="1" t="s">
+        <v>270</v>
       </c>
     </row>
     <row r="258" spans="1:12" ht="16.5" customHeight="1">
@@ -7125,13 +7134,13 @@
         <v>84</v>
       </c>
       <c r="B258" t="s">
-        <v>407</v>
+        <v>161</v>
       </c>
       <c r="C258" t="s">
         <v>9</v>
       </c>
       <c r="K258" t="s">
-        <v>407</v>
+        <v>161</v>
       </c>
       <c r="L258" t="s">
         <v>136</v>
@@ -7142,19 +7151,16 @@
         <v>84</v>
       </c>
       <c r="B259" t="s">
-        <v>408</v>
+        <v>209</v>
       </c>
       <c r="C259" t="s">
-        <v>17</v>
-      </c>
-      <c r="H259" t="s">
-        <v>409</v>
+        <v>89</v>
       </c>
       <c r="K259" t="s">
-        <v>408</v>
+        <v>209</v>
       </c>
       <c r="L259" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
     </row>
     <row r="260" spans="1:12" ht="16.5" customHeight="1">
@@ -7162,16 +7168,16 @@
         <v>84</v>
       </c>
       <c r="B260" t="s">
-        <v>410</v>
+        <v>407</v>
       </c>
       <c r="C260" t="s">
-        <v>56</v>
+        <v>9</v>
       </c>
       <c r="K260" t="s">
-        <v>410</v>
+        <v>407</v>
       </c>
       <c r="L260" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
     </row>
     <row r="261" spans="1:12" ht="16.5" customHeight="1">
@@ -7179,74 +7185,65 @@
         <v>84</v>
       </c>
       <c r="B261" t="s">
-        <v>410</v>
+        <v>408</v>
       </c>
       <c r="C261" t="s">
         <v>17</v>
       </c>
-      <c r="D261" t="s">
-        <v>335</v>
-      </c>
-      <c r="E261" t="s">
-        <v>271</v>
-      </c>
-      <c r="F261" t="s">
-        <v>12</v>
-      </c>
-      <c r="G261" t="s">
-        <v>61</v>
+      <c r="H261" t="s">
+        <v>409</v>
       </c>
       <c r="K261" t="s">
-        <v>411</v>
-      </c>
-      <c r="L261" s="1" t="s">
-        <v>270</v>
+        <v>408</v>
+      </c>
+      <c r="L261" t="s">
+        <v>133</v>
       </c>
     </row>
     <row r="262" spans="1:12" ht="16.5" customHeight="1">
       <c r="A262" t="s">
-        <v>125</v>
+        <v>84</v>
       </c>
       <c r="B262" t="s">
-        <v>126</v>
+        <v>410</v>
       </c>
       <c r="C262" t="s">
-        <v>9</v>
+        <v>56</v>
       </c>
       <c r="K262" t="s">
-        <v>126</v>
+        <v>410</v>
       </c>
       <c r="L262" t="s">
-        <v>131</v>
+        <v>138</v>
       </c>
     </row>
     <row r="263" spans="1:12" ht="16.5" customHeight="1">
       <c r="A263" t="s">
-        <v>125</v>
+        <v>84</v>
       </c>
       <c r="B263" t="s">
-        <v>127</v>
+        <v>410</v>
       </c>
       <c r="C263" t="s">
-        <v>9</v>
+        <v>17</v>
       </c>
       <c r="D263" t="s">
-        <v>332</v>
+        <v>335</v>
       </c>
       <c r="E263" t="s">
-        <v>11</v>
+        <v>271</v>
       </c>
       <c r="F263" t="s">
         <v>12</v>
       </c>
       <c r="G263" t="s">
-        <v>13</v>
+        <v>61</v>
       </c>
       <c r="K263" t="s">
-        <v>127</v>
-      </c>
-      <c r="L263" t="s">
-        <v>163</v>
+        <v>411</v>
+      </c>
+      <c r="L263" s="1" t="s">
+        <v>270</v>
       </c>
     </row>
     <row r="264" spans="1:12" ht="16.5" customHeight="1">
@@ -7254,16 +7251,16 @@
         <v>125</v>
       </c>
       <c r="B264" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="C264" t="s">
-        <v>17</v>
+        <v>9</v>
       </c>
       <c r="K264" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="L264" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
     </row>
     <row r="265" spans="1:12" ht="16.5" customHeight="1">
@@ -7271,16 +7268,28 @@
         <v>125</v>
       </c>
       <c r="B265" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="C265" t="s">
-        <v>19</v>
+        <v>9</v>
+      </c>
+      <c r="D265" t="s">
+        <v>332</v>
+      </c>
+      <c r="E265" t="s">
+        <v>11</v>
+      </c>
+      <c r="F265" t="s">
+        <v>12</v>
+      </c>
+      <c r="G265" t="s">
+        <v>13</v>
       </c>
       <c r="K265" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="L265" t="s">
-        <v>132</v>
+        <v>163</v>
       </c>
     </row>
     <row r="266" spans="1:12" ht="16.5" customHeight="1">
@@ -7288,16 +7297,16 @@
         <v>125</v>
       </c>
       <c r="B266" t="s">
-        <v>294</v>
+        <v>128</v>
       </c>
       <c r="C266" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="K266" t="s">
-        <v>294</v>
+        <v>128</v>
       </c>
       <c r="L266" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
     </row>
     <row r="267" spans="1:12" ht="16.5" customHeight="1">
@@ -7305,25 +7314,13 @@
         <v>125</v>
       </c>
       <c r="B267" t="s">
-        <v>216</v>
+        <v>129</v>
       </c>
       <c r="C267" t="s">
-        <v>17</v>
-      </c>
-      <c r="D267" t="s">
-        <v>356</v>
-      </c>
-      <c r="E267" t="s">
-        <v>219</v>
-      </c>
-      <c r="F267" t="s">
-        <v>215</v>
-      </c>
-      <c r="G267" t="s">
-        <v>221</v>
+        <v>19</v>
       </c>
       <c r="K267" t="s">
-        <v>216</v>
+        <v>129</v>
       </c>
       <c r="L267" t="s">
         <v>132</v>
@@ -7334,13 +7331,13 @@
         <v>125</v>
       </c>
       <c r="B268" t="s">
-        <v>217</v>
+        <v>294</v>
       </c>
       <c r="C268" t="s">
         <v>19</v>
       </c>
       <c r="K268" t="s">
-        <v>217</v>
+        <v>294</v>
       </c>
       <c r="L268" t="s">
         <v>132</v>
@@ -7351,16 +7348,28 @@
         <v>125</v>
       </c>
       <c r="B269" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="C269" t="s">
-        <v>56</v>
+        <v>17</v>
+      </c>
+      <c r="D269" t="s">
+        <v>356</v>
+      </c>
+      <c r="E269" t="s">
+        <v>219</v>
+      </c>
+      <c r="F269" t="s">
+        <v>215</v>
+      </c>
+      <c r="G269" t="s">
+        <v>221</v>
       </c>
       <c r="K269" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="L269" t="s">
-        <v>138</v>
+        <v>132</v>
       </c>
     </row>
     <row r="270" spans="1:12" ht="16.5" customHeight="1">
@@ -7368,28 +7377,16 @@
         <v>125</v>
       </c>
       <c r="B270" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="C270" t="s">
-        <v>17</v>
-      </c>
-      <c r="D270" t="s">
-        <v>335</v>
-      </c>
-      <c r="E270" t="s">
-        <v>271</v>
-      </c>
-      <c r="F270" t="s">
-        <v>12</v>
-      </c>
-      <c r="G270" t="s">
-        <v>61</v>
+        <v>19</v>
       </c>
       <c r="K270" t="s">
-        <v>250</v>
-      </c>
-      <c r="L270" s="1" t="s">
-        <v>270</v>
+        <v>217</v>
+      </c>
+      <c r="L270" t="s">
+        <v>132</v>
       </c>
     </row>
     <row r="271" spans="1:12" ht="16.5" customHeight="1">
@@ -7397,19 +7394,16 @@
         <v>125</v>
       </c>
       <c r="B271" t="s">
-        <v>229</v>
+        <v>218</v>
       </c>
       <c r="C271" t="s">
-        <v>9</v>
-      </c>
-      <c r="J271" t="s">
-        <v>22</v>
+        <v>56</v>
       </c>
       <c r="K271" t="s">
-        <v>229</v>
+        <v>218</v>
       </c>
       <c r="L271" t="s">
-        <v>132</v>
+        <v>138</v>
       </c>
     </row>
     <row r="272" spans="1:12" ht="16.5" customHeight="1">
@@ -7417,74 +7411,77 @@
         <v>125</v>
       </c>
       <c r="B272" t="s">
-        <v>239</v>
+        <v>218</v>
       </c>
       <c r="C272" t="s">
         <v>17</v>
       </c>
       <c r="D272" t="s">
-        <v>357</v>
+        <v>335</v>
       </c>
       <c r="E272" t="s">
-        <v>240</v>
+        <v>271</v>
       </c>
       <c r="F272" t="s">
         <v>12</v>
       </c>
       <c r="G272" t="s">
-        <v>241</v>
+        <v>61</v>
       </c>
       <c r="K272" t="s">
-        <v>239</v>
-      </c>
-      <c r="L272" t="s">
-        <v>132</v>
+        <v>250</v>
+      </c>
+      <c r="L272" s="1" t="s">
+        <v>270</v>
       </c>
     </row>
     <row r="273" spans="1:12" ht="16.5" customHeight="1">
       <c r="A273" t="s">
-        <v>412</v>
+        <v>125</v>
       </c>
       <c r="B273" t="s">
-        <v>413</v>
+        <v>229</v>
       </c>
       <c r="C273" t="s">
         <v>9</v>
       </c>
+      <c r="J273" t="s">
+        <v>22</v>
+      </c>
       <c r="K273" t="s">
-        <v>413</v>
+        <v>229</v>
       </c>
       <c r="L273" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
     </row>
     <row r="274" spans="1:12" ht="16.5" customHeight="1">
       <c r="A274" t="s">
-        <v>412</v>
+        <v>125</v>
       </c>
       <c r="B274" t="s">
-        <v>430</v>
+        <v>239</v>
       </c>
       <c r="C274" t="s">
-        <v>9</v>
+        <v>17</v>
       </c>
       <c r="D274" t="s">
-        <v>332</v>
+        <v>357</v>
       </c>
       <c r="E274" t="s">
-        <v>11</v>
+        <v>240</v>
       </c>
       <c r="F274" t="s">
         <v>12</v>
       </c>
       <c r="G274" t="s">
-        <v>13</v>
+        <v>241</v>
       </c>
       <c r="K274" t="s">
-        <v>430</v>
+        <v>239</v>
       </c>
       <c r="L274" t="s">
-        <v>163</v>
+        <v>132</v>
       </c>
     </row>
     <row r="275" spans="1:12" ht="16.5" customHeight="1">
@@ -7492,16 +7489,16 @@
         <v>412</v>
       </c>
       <c r="B275" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
       <c r="C275" t="s">
-        <v>17</v>
+        <v>9</v>
       </c>
       <c r="K275" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
       <c r="L275" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
     </row>
     <row r="276" spans="1:12" ht="16.5" customHeight="1">
@@ -7509,16 +7506,28 @@
         <v>412</v>
       </c>
       <c r="B276" t="s">
-        <v>415</v>
+        <v>430</v>
       </c>
       <c r="C276" t="s">
-        <v>56</v>
+        <v>9</v>
+      </c>
+      <c r="D276" t="s">
+        <v>332</v>
+      </c>
+      <c r="E276" t="s">
+        <v>11</v>
+      </c>
+      <c r="F276" t="s">
+        <v>12</v>
+      </c>
+      <c r="G276" t="s">
+        <v>13</v>
       </c>
       <c r="K276" t="s">
-        <v>415</v>
+        <v>430</v>
       </c>
       <c r="L276" t="s">
-        <v>138</v>
+        <v>163</v>
       </c>
     </row>
     <row r="277" spans="1:12" ht="16.5" customHeight="1">
@@ -7526,28 +7535,16 @@
         <v>412</v>
       </c>
       <c r="B277" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
       <c r="C277" t="s">
         <v>17</v>
       </c>
-      <c r="D277" t="s">
-        <v>335</v>
-      </c>
-      <c r="E277" t="s">
-        <v>271</v>
-      </c>
-      <c r="F277" t="s">
-        <v>12</v>
-      </c>
-      <c r="G277" t="s">
-        <v>61</v>
-      </c>
       <c r="K277" t="s">
-        <v>416</v>
-      </c>
-      <c r="L277" s="1" t="s">
-        <v>270</v>
+        <v>414</v>
+      </c>
+      <c r="L277" t="s">
+        <v>133</v>
       </c>
     </row>
     <row r="278" spans="1:12" ht="16.5" customHeight="1">
@@ -7555,28 +7552,16 @@
         <v>412</v>
       </c>
       <c r="B278" t="s">
-        <v>417</v>
+        <v>415</v>
       </c>
       <c r="C278" t="s">
-        <v>9</v>
-      </c>
-      <c r="D278" t="s">
-        <v>343</v>
-      </c>
-      <c r="E278" t="s">
-        <v>433</v>
-      </c>
-      <c r="F278" t="s">
-        <v>12</v>
-      </c>
-      <c r="G278" t="s">
-        <v>13</v>
+        <v>56</v>
       </c>
       <c r="K278" t="s">
-        <v>417</v>
+        <v>415</v>
       </c>
       <c r="L278" t="s">
-        <v>132</v>
+        <v>138</v>
       </c>
     </row>
     <row r="279" spans="1:12" ht="16.5" customHeight="1">
@@ -7584,28 +7569,28 @@
         <v>412</v>
       </c>
       <c r="B279" t="s">
-        <v>418</v>
+        <v>415</v>
       </c>
       <c r="C279" t="s">
-        <v>9</v>
+        <v>17</v>
       </c>
       <c r="D279" t="s">
-        <v>344</v>
+        <v>335</v>
       </c>
       <c r="E279" t="s">
-        <v>434</v>
+        <v>271</v>
       </c>
       <c r="F279" t="s">
         <v>12</v>
       </c>
       <c r="G279" t="s">
-        <v>13</v>
+        <v>61</v>
       </c>
       <c r="K279" t="s">
-        <v>418</v>
-      </c>
-      <c r="L279" t="s">
-        <v>132</v>
+        <v>416</v>
+      </c>
+      <c r="L279" s="1" t="s">
+        <v>270</v>
       </c>
     </row>
     <row r="280" spans="1:12" ht="16.5" customHeight="1">
@@ -7613,16 +7598,25 @@
         <v>412</v>
       </c>
       <c r="B280" t="s">
-        <v>419</v>
+        <v>417</v>
       </c>
       <c r="C280" t="s">
         <v>9</v>
       </c>
-      <c r="J280" t="s">
-        <v>42</v>
+      <c r="D280" t="s">
+        <v>343</v>
+      </c>
+      <c r="E280" t="s">
+        <v>433</v>
+      </c>
+      <c r="F280" t="s">
+        <v>12</v>
+      </c>
+      <c r="G280" t="s">
+        <v>13</v>
       </c>
       <c r="K280" t="s">
-        <v>419</v>
+        <v>417</v>
       </c>
       <c r="L280" t="s">
         <v>132</v>
@@ -7633,13 +7627,16 @@
         <v>412</v>
       </c>
       <c r="B281" t="s">
-        <v>420</v>
+        <v>418</v>
       </c>
       <c r="C281" t="s">
         <v>9</v>
       </c>
+      <c r="D281" t="s">
+        <v>344</v>
+      </c>
       <c r="E281" t="s">
-        <v>124</v>
+        <v>434</v>
       </c>
       <c r="F281" t="s">
         <v>12</v>
@@ -7648,7 +7645,7 @@
         <v>13</v>
       </c>
       <c r="K281" t="s">
-        <v>420</v>
+        <v>418</v>
       </c>
       <c r="L281" t="s">
         <v>132</v>
@@ -7659,16 +7656,19 @@
         <v>412</v>
       </c>
       <c r="B282" t="s">
-        <v>421</v>
+        <v>419</v>
       </c>
       <c r="C282" t="s">
-        <v>17</v>
+        <v>9</v>
+      </c>
+      <c r="J282" t="s">
+        <v>42</v>
       </c>
       <c r="K282" t="s">
-        <v>421</v>
+        <v>419</v>
       </c>
       <c r="L282" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
     </row>
     <row r="283" spans="1:12" ht="16.5" customHeight="1">
@@ -7676,16 +7676,25 @@
         <v>412</v>
       </c>
       <c r="B283" t="s">
-        <v>422</v>
+        <v>420</v>
       </c>
       <c r="C283" t="s">
-        <v>17</v>
+        <v>9</v>
+      </c>
+      <c r="E283" t="s">
+        <v>124</v>
+      </c>
+      <c r="F283" t="s">
+        <v>12</v>
+      </c>
+      <c r="G283" t="s">
+        <v>13</v>
       </c>
       <c r="K283" t="s">
-        <v>422</v>
+        <v>420</v>
       </c>
       <c r="L283" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
     </row>
     <row r="284" spans="1:12" ht="16.5" customHeight="1">
@@ -7693,25 +7702,16 @@
         <v>412</v>
       </c>
       <c r="B284" t="s">
-        <v>423</v>
+        <v>421</v>
       </c>
       <c r="C284" t="s">
         <v>17</v>
       </c>
-      <c r="E284" t="s">
-        <v>431</v>
-      </c>
-      <c r="F284" t="s">
-        <v>12</v>
-      </c>
-      <c r="G284" t="s">
-        <v>432</v>
-      </c>
       <c r="K284" t="s">
-        <v>423</v>
+        <v>421</v>
       </c>
       <c r="L284" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
     </row>
     <row r="285" spans="1:12" ht="16.5" customHeight="1">
@@ -7719,13 +7719,13 @@
         <v>412</v>
       </c>
       <c r="B285" t="s">
-        <v>424</v>
+        <v>422</v>
       </c>
       <c r="C285" t="s">
         <v>17</v>
       </c>
       <c r="K285" t="s">
-        <v>424</v>
+        <v>422</v>
       </c>
       <c r="L285" t="s">
         <v>133</v>
@@ -7736,13 +7736,22 @@
         <v>412</v>
       </c>
       <c r="B286" t="s">
-        <v>425</v>
+        <v>423</v>
       </c>
       <c r="C286" t="s">
-        <v>19</v>
+        <v>17</v>
+      </c>
+      <c r="E286" t="s">
+        <v>431</v>
+      </c>
+      <c r="F286" t="s">
+        <v>12</v>
+      </c>
+      <c r="G286" t="s">
+        <v>432</v>
       </c>
       <c r="K286" t="s">
-        <v>425</v>
+        <v>423</v>
       </c>
       <c r="L286" t="s">
         <v>132</v>
@@ -7753,16 +7762,16 @@
         <v>412</v>
       </c>
       <c r="B287" t="s">
-        <v>426</v>
+        <v>424</v>
       </c>
       <c r="C287" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="K287" t="s">
-        <v>426</v>
+        <v>424</v>
       </c>
       <c r="L287" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
     </row>
     <row r="288" spans="1:12" ht="16.5" customHeight="1">
@@ -7770,13 +7779,13 @@
         <v>412</v>
       </c>
       <c r="B288" t="s">
-        <v>427</v>
+        <v>425</v>
       </c>
       <c r="C288" t="s">
         <v>19</v>
       </c>
       <c r="K288" t="s">
-        <v>427</v>
+        <v>425</v>
       </c>
       <c r="L288" t="s">
         <v>132</v>
@@ -7787,16 +7796,16 @@
         <v>412</v>
       </c>
       <c r="B289" t="s">
-        <v>428</v>
+        <v>426</v>
       </c>
       <c r="C289" t="s">
-        <v>9</v>
+        <v>19</v>
       </c>
       <c r="K289" t="s">
-        <v>428</v>
+        <v>426</v>
       </c>
       <c r="L289" t="s">
-        <v>136</v>
+        <v>132</v>
       </c>
     </row>
     <row r="290" spans="1:12" ht="16.5" customHeight="1">
@@ -7804,18 +7813,52 @@
         <v>412</v>
       </c>
       <c r="B290" t="s">
+        <v>427</v>
+      </c>
+      <c r="C290" t="s">
+        <v>19</v>
+      </c>
+      <c r="K290" t="s">
+        <v>427</v>
+      </c>
+      <c r="L290" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="291" spans="1:12" ht="16.5" customHeight="1">
+      <c r="A291" t="s">
+        <v>412</v>
+      </c>
+      <c r="B291" t="s">
+        <v>428</v>
+      </c>
+      <c r="C291" t="s">
+        <v>9</v>
+      </c>
+      <c r="K291" t="s">
+        <v>428</v>
+      </c>
+      <c r="L291" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="292" spans="1:12" ht="16.5" customHeight="1">
+      <c r="A292" t="s">
+        <v>412</v>
+      </c>
+      <c r="B292" t="s">
         <v>429</v>
       </c>
-      <c r="C290" t="s">
-        <v>9</v>
-      </c>
-      <c r="J290" t="s">
-        <v>84</v>
-      </c>
-      <c r="K290" t="s">
+      <c r="C292" t="s">
+        <v>9</v>
+      </c>
+      <c r="J292" t="s">
+        <v>84</v>
+      </c>
+      <c r="K292" t="s">
         <v>429</v>
       </c>
-      <c r="L290" t="s">
+      <c r="L292" t="s">
         <v>132</v>
       </c>
     </row>

</xml_diff>

<commit_message>
add user person/organisation category criterion
</commit_message>
<xml_diff>
--- a/criterion_property_definitions.xlsx
+++ b/criterion_property_definitions.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1871" uniqueCount="438">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1880" uniqueCount="439">
   <si>
     <t>property</t>
   </si>
@@ -1331,6 +1331,9 @@
   </si>
   <si>
     <t>user.decrypt</t>
+  </si>
+  <si>
+    <t>user.identity.category.id</t>
   </si>
 </sst>
 </file>
@@ -1663,10 +1666,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:L293"/>
+  <dimension ref="A1:L294"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A244" workbookViewId="0">
-      <selection activeCell="A268" sqref="A268"/>
+    <sheetView tabSelected="1" topLeftCell="A250" workbookViewId="0">
+      <selection activeCell="A275" sqref="A275"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="15.7109375" defaultRowHeight="16.5" customHeight="1"/>
@@ -7480,25 +7483,25 @@
         <v>125</v>
       </c>
       <c r="B275" t="s">
-        <v>239</v>
+        <v>438</v>
       </c>
       <c r="C275" t="s">
-        <v>17</v>
+        <v>9</v>
       </c>
       <c r="D275" t="s">
-        <v>357</v>
+        <v>337</v>
       </c>
       <c r="E275" t="s">
-        <v>240</v>
+        <v>31</v>
       </c>
       <c r="F275" t="s">
         <v>12</v>
       </c>
       <c r="G275" t="s">
-        <v>241</v>
+        <v>13</v>
       </c>
       <c r="K275" t="s">
-        <v>239</v>
+        <v>438</v>
       </c>
       <c r="L275" t="s">
         <v>132</v>
@@ -7506,19 +7509,31 @@
     </row>
     <row r="276" spans="1:12" ht="16.5" customHeight="1">
       <c r="A276" t="s">
-        <v>412</v>
+        <v>125</v>
       </c>
       <c r="B276" t="s">
-        <v>413</v>
+        <v>239</v>
       </c>
       <c r="C276" t="s">
-        <v>9</v>
+        <v>17</v>
+      </c>
+      <c r="D276" t="s">
+        <v>357</v>
+      </c>
+      <c r="E276" t="s">
+        <v>240</v>
+      </c>
+      <c r="F276" t="s">
+        <v>12</v>
+      </c>
+      <c r="G276" t="s">
+        <v>241</v>
       </c>
       <c r="K276" t="s">
-        <v>413</v>
+        <v>239</v>
       </c>
       <c r="L276" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
     </row>
     <row r="277" spans="1:12" ht="16.5" customHeight="1">
@@ -7526,28 +7541,16 @@
         <v>412</v>
       </c>
       <c r="B277" t="s">
-        <v>430</v>
+        <v>413</v>
       </c>
       <c r="C277" t="s">
         <v>9</v>
       </c>
-      <c r="D277" t="s">
-        <v>332</v>
-      </c>
-      <c r="E277" t="s">
-        <v>11</v>
-      </c>
-      <c r="F277" t="s">
-        <v>12</v>
-      </c>
-      <c r="G277" t="s">
-        <v>13</v>
-      </c>
       <c r="K277" t="s">
-        <v>430</v>
+        <v>413</v>
       </c>
       <c r="L277" t="s">
-        <v>163</v>
+        <v>131</v>
       </c>
     </row>
     <row r="278" spans="1:12" ht="16.5" customHeight="1">
@@ -7555,16 +7558,28 @@
         <v>412</v>
       </c>
       <c r="B278" t="s">
-        <v>414</v>
+        <v>430</v>
       </c>
       <c r="C278" t="s">
-        <v>17</v>
+        <v>9</v>
+      </c>
+      <c r="D278" t="s">
+        <v>332</v>
+      </c>
+      <c r="E278" t="s">
+        <v>11</v>
+      </c>
+      <c r="F278" t="s">
+        <v>12</v>
+      </c>
+      <c r="G278" t="s">
+        <v>13</v>
       </c>
       <c r="K278" t="s">
-        <v>414</v>
+        <v>430</v>
       </c>
       <c r="L278" t="s">
-        <v>133</v>
+        <v>163</v>
       </c>
     </row>
     <row r="279" spans="1:12" ht="16.5" customHeight="1">
@@ -7572,16 +7587,16 @@
         <v>412</v>
       </c>
       <c r="B279" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
       <c r="C279" t="s">
-        <v>56</v>
+        <v>17</v>
       </c>
       <c r="K279" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
       <c r="L279" t="s">
-        <v>138</v>
+        <v>133</v>
       </c>
     </row>
     <row r="280" spans="1:12" ht="16.5" customHeight="1">
@@ -7592,25 +7607,13 @@
         <v>415</v>
       </c>
       <c r="C280" t="s">
-        <v>17</v>
-      </c>
-      <c r="D280" t="s">
-        <v>335</v>
-      </c>
-      <c r="E280" t="s">
-        <v>271</v>
-      </c>
-      <c r="F280" t="s">
-        <v>12</v>
-      </c>
-      <c r="G280" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
       <c r="K280" t="s">
-        <v>416</v>
-      </c>
-      <c r="L280" s="1" t="s">
-        <v>270</v>
+        <v>415</v>
+      </c>
+      <c r="L280" t="s">
+        <v>138</v>
       </c>
     </row>
     <row r="281" spans="1:12" ht="16.5" customHeight="1">
@@ -7618,28 +7621,28 @@
         <v>412</v>
       </c>
       <c r="B281" t="s">
-        <v>417</v>
+        <v>415</v>
       </c>
       <c r="C281" t="s">
-        <v>9</v>
+        <v>17</v>
       </c>
       <c r="D281" t="s">
-        <v>343</v>
+        <v>335</v>
       </c>
       <c r="E281" t="s">
-        <v>433</v>
+        <v>271</v>
       </c>
       <c r="F281" t="s">
         <v>12</v>
       </c>
       <c r="G281" t="s">
-        <v>13</v>
+        <v>61</v>
       </c>
       <c r="K281" t="s">
-        <v>417</v>
-      </c>
-      <c r="L281" t="s">
-        <v>132</v>
+        <v>416</v>
+      </c>
+      <c r="L281" s="1" t="s">
+        <v>270</v>
       </c>
     </row>
     <row r="282" spans="1:12" ht="16.5" customHeight="1">
@@ -7647,16 +7650,16 @@
         <v>412</v>
       </c>
       <c r="B282" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
       <c r="C282" t="s">
         <v>9</v>
       </c>
       <c r="D282" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="E282" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="F282" t="s">
         <v>12</v>
@@ -7665,7 +7668,7 @@
         <v>13</v>
       </c>
       <c r="K282" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
       <c r="L282" t="s">
         <v>132</v>
@@ -7676,16 +7679,25 @@
         <v>412</v>
       </c>
       <c r="B283" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="C283" t="s">
         <v>9</v>
       </c>
-      <c r="J283" t="s">
-        <v>42</v>
+      <c r="D283" t="s">
+        <v>344</v>
+      </c>
+      <c r="E283" t="s">
+        <v>434</v>
+      </c>
+      <c r="F283" t="s">
+        <v>12</v>
+      </c>
+      <c r="G283" t="s">
+        <v>13</v>
       </c>
       <c r="K283" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="L283" t="s">
         <v>132</v>
@@ -7696,22 +7708,16 @@
         <v>412</v>
       </c>
       <c r="B284" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
       <c r="C284" t="s">
         <v>9</v>
       </c>
-      <c r="E284" t="s">
-        <v>124</v>
-      </c>
-      <c r="F284" t="s">
-        <v>12</v>
-      </c>
-      <c r="G284" t="s">
-        <v>13</v>
+      <c r="J284" t="s">
+        <v>42</v>
       </c>
       <c r="K284" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
       <c r="L284" t="s">
         <v>132</v>
@@ -7722,16 +7728,25 @@
         <v>412</v>
       </c>
       <c r="B285" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="C285" t="s">
-        <v>17</v>
+        <v>9</v>
+      </c>
+      <c r="E285" t="s">
+        <v>124</v>
+      </c>
+      <c r="F285" t="s">
+        <v>12</v>
+      </c>
+      <c r="G285" t="s">
+        <v>13</v>
       </c>
       <c r="K285" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="L285" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
     </row>
     <row r="286" spans="1:12" ht="16.5" customHeight="1">
@@ -7739,13 +7754,13 @@
         <v>412</v>
       </c>
       <c r="B286" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="C286" t="s">
         <v>17</v>
       </c>
       <c r="K286" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="L286" t="s">
         <v>133</v>
@@ -7756,25 +7771,16 @@
         <v>412</v>
       </c>
       <c r="B287" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
       <c r="C287" t="s">
         <v>17</v>
       </c>
-      <c r="E287" t="s">
-        <v>431</v>
-      </c>
-      <c r="F287" t="s">
-        <v>12</v>
-      </c>
-      <c r="G287" t="s">
-        <v>432</v>
-      </c>
       <c r="K287" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
       <c r="L287" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
     </row>
     <row r="288" spans="1:12" ht="16.5" customHeight="1">
@@ -7782,16 +7788,25 @@
         <v>412</v>
       </c>
       <c r="B288" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
       <c r="C288" t="s">
         <v>17</v>
       </c>
+      <c r="E288" t="s">
+        <v>431</v>
+      </c>
+      <c r="F288" t="s">
+        <v>12</v>
+      </c>
+      <c r="G288" t="s">
+        <v>432</v>
+      </c>
       <c r="K288" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
       <c r="L288" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
     </row>
     <row r="289" spans="1:12" ht="16.5" customHeight="1">
@@ -7799,16 +7814,16 @@
         <v>412</v>
       </c>
       <c r="B289" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
       <c r="C289" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="K289" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
       <c r="L289" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
     </row>
     <row r="290" spans="1:12" ht="16.5" customHeight="1">
@@ -7816,13 +7831,13 @@
         <v>412</v>
       </c>
       <c r="B290" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
       <c r="C290" t="s">
         <v>19</v>
       </c>
       <c r="K290" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
       <c r="L290" t="s">
         <v>132</v>
@@ -7833,13 +7848,13 @@
         <v>412</v>
       </c>
       <c r="B291" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
       <c r="C291" t="s">
         <v>19</v>
       </c>
       <c r="K291" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
       <c r="L291" t="s">
         <v>132</v>
@@ -7850,16 +7865,16 @@
         <v>412</v>
       </c>
       <c r="B292" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
       <c r="C292" t="s">
-        <v>9</v>
+        <v>19</v>
       </c>
       <c r="K292" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
       <c r="L292" t="s">
-        <v>136</v>
+        <v>132</v>
       </c>
     </row>
     <row r="293" spans="1:12" ht="16.5" customHeight="1">
@@ -7867,18 +7882,35 @@
         <v>412</v>
       </c>
       <c r="B293" t="s">
+        <v>428</v>
+      </c>
+      <c r="C293" t="s">
+        <v>9</v>
+      </c>
+      <c r="K293" t="s">
+        <v>428</v>
+      </c>
+      <c r="L293" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="294" spans="1:12" ht="16.5" customHeight="1">
+      <c r="A294" t="s">
+        <v>412</v>
+      </c>
+      <c r="B294" t="s">
         <v>429</v>
       </c>
-      <c r="C293" t="s">
-        <v>9</v>
-      </c>
-      <c r="J293" t="s">
-        <v>84</v>
-      </c>
-      <c r="K293" t="s">
+      <c r="C294" t="s">
+        <v>9</v>
+      </c>
+      <c r="J294" t="s">
+        <v>84</v>
+      </c>
+      <c r="K294" t="s">
         <v>429</v>
       </c>
-      <c r="L293" t="s">
+      <c r="L294" t="s">
         <v>132</v>
       </c>
     </row>

</xml_diff>

<commit_message>
fix dropdowns of selection value query criterions
</commit_message>
<xml_diff>
--- a/criterion_property_definitions.xlsx
+++ b/criterion_property_definitions.xlsx
@@ -481,9 +481,6 @@
     <t>proband.inquiryValues.value.selectionValues.value</t>
   </si>
   <si>
-    <t>completeInputFieldSelectionSetValue</t>
-  </si>
-  <si>
     <t>proband.trialParticipations.tagValues.value.selectionValues.value</t>
   </si>
   <si>
@@ -1346,6 +1343,9 @@
   </si>
   <si>
     <t>getMode.name</t>
+  </si>
+  <si>
+    <t>completeInputFieldSelectionSetValueValue</t>
   </si>
 </sst>
 </file>
@@ -1680,8 +1680,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:L295"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A79" workbookViewId="0">
-      <selection activeCell="A93" sqref="A93"/>
+    <sheetView tabSelected="1" topLeftCell="A185" workbookViewId="0">
+      <selection activeCell="H201" sqref="H201"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="15.7109375" defaultRowHeight="16.5" customHeight="1"/>
@@ -1709,7 +1709,7 @@
         <v>1</v>
       </c>
       <c r="D1" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="E1" t="s">
         <v>2</v>
@@ -1724,7 +1724,7 @@
         <v>142</v>
       </c>
       <c r="I1" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="J1" t="s">
         <v>5</v>
@@ -1764,7 +1764,7 @@
         <v>9</v>
       </c>
       <c r="D3" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="E3" t="s">
         <v>11</v>
@@ -1779,7 +1779,7 @@
         <v>10</v>
       </c>
       <c r="L3" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
     </row>
     <row r="4" spans="1:12" ht="16.5" customHeight="1">
@@ -1793,7 +1793,7 @@
         <v>9</v>
       </c>
       <c r="D4" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="E4" t="s">
         <v>15</v>
@@ -1850,13 +1850,13 @@
         <v>7</v>
       </c>
       <c r="B7" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="C7" t="s">
         <v>19</v>
       </c>
       <c r="K7" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="L7" t="s">
         <v>132</v>
@@ -1930,7 +1930,7 @@
         <v>9</v>
       </c>
       <c r="D11" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="E11" t="s">
         <v>25</v>
@@ -1990,7 +1990,7 @@
         <v>7</v>
       </c>
       <c r="B14" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="C14" t="s">
         <v>9</v>
@@ -1999,7 +1999,7 @@
         <v>84</v>
       </c>
       <c r="K14" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="L14" t="s">
         <v>132</v>
@@ -2010,7 +2010,7 @@
         <v>7</v>
       </c>
       <c r="B15" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="C15" t="s">
         <v>9</v>
@@ -2019,7 +2019,7 @@
         <v>42</v>
       </c>
       <c r="K15" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="L15" t="s">
         <v>132</v>
@@ -2030,7 +2030,7 @@
         <v>7</v>
       </c>
       <c r="B16" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="C16" t="s">
         <v>9</v>
@@ -2039,7 +2039,7 @@
         <v>44</v>
       </c>
       <c r="K16" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="L16" t="s">
         <v>132</v>
@@ -2050,13 +2050,13 @@
         <v>7</v>
       </c>
       <c r="B17" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="C17" t="s">
         <v>56</v>
       </c>
       <c r="K17" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="L17" t="s">
         <v>138</v>
@@ -2067,16 +2067,16 @@
         <v>7</v>
       </c>
       <c r="B18" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="C18" t="s">
         <v>17</v>
       </c>
       <c r="D18" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="E18" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="F18" t="s">
         <v>12</v>
@@ -2085,10 +2085,10 @@
         <v>61</v>
       </c>
       <c r="K18" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="L18" s="1" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
     </row>
     <row r="19" spans="1:12" ht="16.5" customHeight="1">
@@ -2096,16 +2096,16 @@
         <v>7</v>
       </c>
       <c r="B19" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="C19" t="s">
         <v>56</v>
       </c>
       <c r="K19" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="L19" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
     </row>
     <row r="20" spans="1:12" ht="16.5" customHeight="1">
@@ -2113,16 +2113,16 @@
         <v>7</v>
       </c>
       <c r="B20" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="C20" t="s">
         <v>17</v>
       </c>
       <c r="D20" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="E20" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="F20" t="s">
         <v>12</v>
@@ -2131,10 +2131,10 @@
         <v>61</v>
       </c>
       <c r="K20" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="L20" s="1" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
     </row>
     <row r="21" spans="1:12" ht="16.5" customHeight="1">
@@ -2142,16 +2142,16 @@
         <v>7</v>
       </c>
       <c r="B21" t="s">
+        <v>224</v>
+      </c>
+      <c r="C21" t="s">
+        <v>9</v>
+      </c>
+      <c r="D21" t="s">
+        <v>335</v>
+      </c>
+      <c r="E21" t="s">
         <v>225</v>
-      </c>
-      <c r="C21" t="s">
-        <v>9</v>
-      </c>
-      <c r="D21" t="s">
-        <v>336</v>
-      </c>
-      <c r="E21" t="s">
-        <v>226</v>
       </c>
       <c r="F21" t="s">
         <v>12</v>
@@ -2160,7 +2160,7 @@
         <v>13</v>
       </c>
       <c r="K21" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="L21" t="s">
         <v>132</v>
@@ -2171,13 +2171,13 @@
         <v>7</v>
       </c>
       <c r="B22" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="C22" t="s">
         <v>19</v>
       </c>
       <c r="K22" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="L22" t="s">
         <v>132</v>
@@ -2211,7 +2211,7 @@
         <v>9</v>
       </c>
       <c r="D24" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="E24" t="s">
         <v>11</v>
@@ -2226,7 +2226,7 @@
         <v>29</v>
       </c>
       <c r="L24" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
     </row>
     <row r="25" spans="1:12" ht="16.5" customHeight="1">
@@ -2240,7 +2240,7 @@
         <v>9</v>
       </c>
       <c r="D25" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="E25" t="s">
         <v>31</v>
@@ -2382,13 +2382,13 @@
         <v>22</v>
       </c>
       <c r="B33" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="C33" t="s">
         <v>19</v>
       </c>
       <c r="K33" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="L33" t="s">
         <v>132</v>
@@ -2459,13 +2459,13 @@
         <v>22</v>
       </c>
       <c r="B37" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="C37" t="s">
         <v>9</v>
       </c>
       <c r="D37" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="E37" t="s">
         <v>52</v>
@@ -2477,7 +2477,7 @@
         <v>13</v>
       </c>
       <c r="K37" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="L37" t="s">
         <v>132</v>
@@ -2488,7 +2488,7 @@
         <v>22</v>
       </c>
       <c r="B38" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="C38" t="s">
         <v>9</v>
@@ -2497,7 +2497,7 @@
         <v>42</v>
       </c>
       <c r="K38" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="L38" t="s">
         <v>132</v>
@@ -2508,13 +2508,13 @@
         <v>22</v>
       </c>
       <c r="B39" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="C39" t="s">
         <v>36</v>
       </c>
       <c r="K39" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="L39" t="s">
         <v>138</v>
@@ -2525,16 +2525,16 @@
         <v>22</v>
       </c>
       <c r="B40" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="C40" t="s">
         <v>17</v>
       </c>
       <c r="D40" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="E40" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="F40" t="s">
         <v>12</v>
@@ -2543,10 +2543,10 @@
         <v>61</v>
       </c>
       <c r="K40" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="L40" s="1" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
     </row>
     <row r="41" spans="1:12" ht="16.5" customHeight="1">
@@ -2554,13 +2554,13 @@
         <v>22</v>
       </c>
       <c r="B41" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="C41" t="s">
         <v>9</v>
       </c>
       <c r="K41" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="L41" t="s">
         <v>136</v>
@@ -2571,13 +2571,13 @@
         <v>22</v>
       </c>
       <c r="B42" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="C42" t="s">
         <v>9</v>
       </c>
       <c r="K42" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="L42" t="s">
         <v>136</v>
@@ -2588,16 +2588,16 @@
         <v>22</v>
       </c>
       <c r="B43" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="C43" t="s">
         <v>9</v>
       </c>
       <c r="D43" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="E43" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="F43" t="s">
         <v>12</v>
@@ -2606,7 +2606,7 @@
         <v>13</v>
       </c>
       <c r="K43" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="L43" t="s">
         <v>132</v>
@@ -2640,7 +2640,7 @@
         <v>9</v>
       </c>
       <c r="D45" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="E45" t="s">
         <v>47</v>
@@ -2680,13 +2680,13 @@
         <v>22</v>
       </c>
       <c r="B47" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="C47" t="s">
         <v>17</v>
       </c>
       <c r="K47" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="L47" t="s">
         <v>133</v>
@@ -2697,16 +2697,16 @@
         <v>22</v>
       </c>
       <c r="B48" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="C48" t="s">
         <v>9</v>
       </c>
       <c r="D48" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="E48" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="F48" t="s">
         <v>12</v>
@@ -2715,7 +2715,7 @@
         <v>13</v>
       </c>
       <c r="K48" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="L48" t="s">
         <v>132</v>
@@ -2726,13 +2726,13 @@
         <v>22</v>
       </c>
       <c r="B49" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="C49" t="s">
         <v>9</v>
       </c>
       <c r="K49" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="L49" t="s">
         <v>136</v>
@@ -2743,13 +2743,13 @@
         <v>22</v>
       </c>
       <c r="B50" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="C50" t="s">
         <v>19</v>
       </c>
       <c r="K50" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="L50" t="s">
         <v>132</v>
@@ -2760,13 +2760,13 @@
         <v>22</v>
       </c>
       <c r="B51" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="C51" t="s">
         <v>9</v>
       </c>
       <c r="K51" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="L51" t="s">
         <v>136</v>
@@ -2777,13 +2777,13 @@
         <v>22</v>
       </c>
       <c r="B52" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="C52" t="s">
         <v>56</v>
       </c>
       <c r="K52" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="L52" t="s">
         <v>138</v>
@@ -2794,16 +2794,16 @@
         <v>22</v>
       </c>
       <c r="B53" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="C53" t="s">
         <v>17</v>
       </c>
       <c r="D53" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="E53" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="F53" t="s">
         <v>12</v>
@@ -2812,10 +2812,10 @@
         <v>61</v>
       </c>
       <c r="K53" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="L53" s="1" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
     </row>
     <row r="54" spans="1:12" ht="16.5" customHeight="1">
@@ -2823,16 +2823,16 @@
         <v>22</v>
       </c>
       <c r="B54" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="C54" t="s">
         <v>56</v>
       </c>
       <c r="K54" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="L54" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
     </row>
     <row r="55" spans="1:12" ht="16.5" customHeight="1">
@@ -2840,16 +2840,16 @@
         <v>22</v>
       </c>
       <c r="B55" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="C55" t="s">
         <v>17</v>
       </c>
       <c r="D55" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="E55" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="F55" t="s">
         <v>12</v>
@@ -2858,10 +2858,10 @@
         <v>61</v>
       </c>
       <c r="K55" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="L55" s="1" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
     </row>
     <row r="56" spans="1:12" ht="16.5" customHeight="1">
@@ -2869,16 +2869,16 @@
         <v>22</v>
       </c>
       <c r="B56" t="s">
+        <v>235</v>
+      </c>
+      <c r="C56" t="s">
+        <v>9</v>
+      </c>
+      <c r="D56" t="s">
+        <v>341</v>
+      </c>
+      <c r="E56" t="s">
         <v>236</v>
-      </c>
-      <c r="C56" t="s">
-        <v>9</v>
-      </c>
-      <c r="D56" t="s">
-        <v>342</v>
-      </c>
-      <c r="E56" t="s">
-        <v>237</v>
       </c>
       <c r="F56" t="s">
         <v>12</v>
@@ -2887,7 +2887,7 @@
         <v>13</v>
       </c>
       <c r="K56" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="L56" t="s">
         <v>132</v>
@@ -2898,13 +2898,13 @@
         <v>22</v>
       </c>
       <c r="B57" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="C57" t="s">
         <v>19</v>
       </c>
       <c r="K57" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="L57" t="s">
         <v>132</v>
@@ -2915,7 +2915,7 @@
         <v>22</v>
       </c>
       <c r="B58" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="C58" t="s">
         <v>9</v>
@@ -2924,7 +2924,7 @@
         <v>42</v>
       </c>
       <c r="K58" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="L58" t="s">
         <v>132</v>
@@ -2935,13 +2935,13 @@
         <v>22</v>
       </c>
       <c r="B59" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="C59" t="s">
         <v>56</v>
       </c>
       <c r="K59" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="L59" t="s">
         <v>138</v>
@@ -2952,16 +2952,16 @@
         <v>22</v>
       </c>
       <c r="B60" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="C60" t="s">
         <v>17</v>
       </c>
       <c r="D60" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="E60" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="F60" t="s">
         <v>12</v>
@@ -2970,10 +2970,10 @@
         <v>61</v>
       </c>
       <c r="K60" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="L60" s="1" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
     </row>
     <row r="61" spans="1:12" ht="16.5" customHeight="1">
@@ -2981,13 +2981,13 @@
         <v>22</v>
       </c>
       <c r="B61" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="C61" t="s">
         <v>56</v>
       </c>
       <c r="K61" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="L61" t="s">
         <v>138</v>
@@ -2998,16 +2998,16 @@
         <v>22</v>
       </c>
       <c r="B62" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="C62" t="s">
         <v>17</v>
       </c>
       <c r="D62" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="E62" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="F62" t="s">
         <v>12</v>
@@ -3016,10 +3016,10 @@
         <v>61</v>
       </c>
       <c r="K62" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="L62" s="1" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
     </row>
     <row r="63" spans="1:12" ht="16.5" customHeight="1">
@@ -3050,7 +3050,7 @@
         <v>9</v>
       </c>
       <c r="D64" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="E64" t="s">
         <v>11</v>
@@ -3065,7 +3065,7 @@
         <v>50</v>
       </c>
       <c r="L64" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
     </row>
     <row r="65" spans="1:12" ht="16.5" customHeight="1">
@@ -3079,7 +3079,7 @@
         <v>9</v>
       </c>
       <c r="D65" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="E65" t="s">
         <v>52</v>
@@ -3102,7 +3102,7 @@
         <v>44</v>
       </c>
       <c r="B66" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="C66" t="s">
         <v>9</v>
@@ -3111,7 +3111,7 @@
         <v>42</v>
       </c>
       <c r="K66" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="L66" t="s">
         <v>132</v>
@@ -3162,10 +3162,10 @@
         <v>17</v>
       </c>
       <c r="D69" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="E69" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="F69" t="s">
         <v>12</v>
@@ -3174,10 +3174,10 @@
         <v>61</v>
       </c>
       <c r="K69" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="L69" s="1" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
     </row>
     <row r="70" spans="1:12" ht="16.5" customHeight="1">
@@ -3208,10 +3208,10 @@
         <v>17</v>
       </c>
       <c r="D71" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="E71" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="F71" t="s">
         <v>12</v>
@@ -3220,10 +3220,10 @@
         <v>61</v>
       </c>
       <c r="K71" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="L71" s="1" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
     </row>
     <row r="72" spans="1:12" ht="16.5" customHeight="1">
@@ -3271,7 +3271,7 @@
         <v>17</v>
       </c>
       <c r="D74" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="E74" t="s">
         <v>60</v>
@@ -3294,13 +3294,13 @@
         <v>44</v>
       </c>
       <c r="B75" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="C75" t="s">
         <v>19</v>
       </c>
       <c r="K75" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="L75" t="s">
         <v>132</v>
@@ -3331,13 +3331,13 @@
         <v>44</v>
       </c>
       <c r="B77" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="C77" t="s">
         <v>19</v>
       </c>
       <c r="K77" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="L77" t="s">
         <v>132</v>
@@ -3462,7 +3462,7 @@
         <v>9</v>
       </c>
       <c r="D84" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="E84" t="s">
         <v>11</v>
@@ -3477,7 +3477,7 @@
         <v>67</v>
       </c>
       <c r="L84" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
     </row>
     <row r="85" spans="1:12" ht="16.5" customHeight="1">
@@ -3508,7 +3508,7 @@
         <v>9</v>
       </c>
       <c r="D86" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="E86" t="s">
         <v>70</v>
@@ -3531,16 +3531,16 @@
         <v>42</v>
       </c>
       <c r="B87" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="C87" t="s">
         <v>9</v>
       </c>
       <c r="D87" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="E87" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="F87" t="s">
         <v>12</v>
@@ -3549,7 +3549,7 @@
         <v>13</v>
       </c>
       <c r="K87" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="L87" t="s">
         <v>132</v>
@@ -3560,16 +3560,16 @@
         <v>42</v>
       </c>
       <c r="B88" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="C88" t="s">
         <v>9</v>
       </c>
       <c r="D88" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="E88" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="F88" t="s">
         <v>12</v>
@@ -3578,7 +3578,7 @@
         <v>13</v>
       </c>
       <c r="K88" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="L88" t="s">
         <v>132</v>
@@ -3589,13 +3589,13 @@
         <v>42</v>
       </c>
       <c r="B89" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="C89" t="s">
         <v>19</v>
       </c>
       <c r="K89" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="L89" t="s">
         <v>132</v>
@@ -3606,16 +3606,16 @@
         <v>42</v>
       </c>
       <c r="B90" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="C90" t="s">
         <v>56</v>
       </c>
       <c r="K90" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="L90" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
     </row>
     <row r="91" spans="1:12" ht="16.5" customHeight="1">
@@ -3623,16 +3623,16 @@
         <v>42</v>
       </c>
       <c r="B91" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="C91" t="s">
         <v>17</v>
       </c>
       <c r="D91" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="E91" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="F91" t="s">
         <v>12</v>
@@ -3641,10 +3641,10 @@
         <v>61</v>
       </c>
       <c r="K91" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="L91" s="1" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
     </row>
     <row r="92" spans="1:12" ht="16.5" customHeight="1">
@@ -3652,16 +3652,16 @@
         <v>42</v>
       </c>
       <c r="B92" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="C92" t="s">
         <v>56</v>
       </c>
       <c r="K92" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="L92" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
     </row>
     <row r="93" spans="1:12" ht="16.5" customHeight="1">
@@ -3669,16 +3669,16 @@
         <v>42</v>
       </c>
       <c r="B93" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="C93" t="s">
         <v>17</v>
       </c>
       <c r="D93" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="E93" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="F93" t="s">
         <v>12</v>
@@ -3687,10 +3687,10 @@
         <v>61</v>
       </c>
       <c r="K93" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="L93" s="1" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
     </row>
     <row r="94" spans="1:12" ht="16.5" customHeight="1">
@@ -3698,25 +3698,25 @@
         <v>42</v>
       </c>
       <c r="B94" t="s">
+        <v>438</v>
+      </c>
+      <c r="C94" t="s">
+        <v>17</v>
+      </c>
+      <c r="D94" t="s">
         <v>439</v>
       </c>
-      <c r="C94" t="s">
-        <v>17</v>
-      </c>
-      <c r="D94" t="s">
+      <c r="E94" t="s">
         <v>440</v>
-      </c>
-      <c r="E94" t="s">
-        <v>441</v>
       </c>
       <c r="F94" t="s">
         <v>12</v>
       </c>
       <c r="G94" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="K94" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
       <c r="L94" t="s">
         <v>132</v>
@@ -3727,13 +3727,13 @@
         <v>42</v>
       </c>
       <c r="B95" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="C95" t="s">
         <v>19</v>
       </c>
       <c r="K95" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="L95" t="s">
         <v>132</v>
@@ -3744,13 +3744,13 @@
         <v>42</v>
       </c>
       <c r="B96" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
       <c r="C96" t="s">
         <v>19</v>
       </c>
       <c r="K96" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
       <c r="L96" t="s">
         <v>132</v>
@@ -3761,13 +3761,13 @@
         <v>42</v>
       </c>
       <c r="B97" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="C97" t="s">
         <v>19</v>
       </c>
       <c r="K97" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="L97" t="s">
         <v>132</v>
@@ -3778,13 +3778,13 @@
         <v>42</v>
       </c>
       <c r="B98" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="C98" t="s">
         <v>19</v>
       </c>
       <c r="K98" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="L98" t="s">
         <v>132</v>
@@ -3795,16 +3795,16 @@
         <v>42</v>
       </c>
       <c r="B99" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="C99" t="s">
         <v>9</v>
       </c>
       <c r="D99" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="E99" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="F99" t="s">
         <v>12</v>
@@ -3813,7 +3813,7 @@
         <v>13</v>
       </c>
       <c r="K99" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="L99" t="s">
         <v>132</v>
@@ -3844,16 +3844,16 @@
         <v>42</v>
       </c>
       <c r="B101" t="s">
+        <v>200</v>
+      </c>
+      <c r="C101" t="s">
+        <v>9</v>
+      </c>
+      <c r="D101" t="s">
+        <v>346</v>
+      </c>
+      <c r="E101" t="s">
         <v>201</v>
-      </c>
-      <c r="C101" t="s">
-        <v>9</v>
-      </c>
-      <c r="D101" t="s">
-        <v>347</v>
-      </c>
-      <c r="E101" t="s">
-        <v>202</v>
       </c>
       <c r="F101" t="s">
         <v>12</v>
@@ -3862,7 +3862,7 @@
         <v>13</v>
       </c>
       <c r="K101" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="L101" t="s">
         <v>132</v>
@@ -3890,7 +3890,7 @@
         <v>42</v>
       </c>
       <c r="B103" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="C103" t="s">
         <v>9</v>
@@ -3899,7 +3899,7 @@
         <v>84</v>
       </c>
       <c r="K103" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="L103" t="s">
         <v>132</v>
@@ -3950,7 +3950,7 @@
         <v>9</v>
       </c>
       <c r="D106" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="E106" t="s">
         <v>76</v>
@@ -3990,13 +3990,13 @@
         <v>42</v>
       </c>
       <c r="B108" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="C108" t="s">
         <v>9</v>
       </c>
       <c r="K108" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="L108" t="s">
         <v>136</v>
@@ -4007,13 +4007,13 @@
         <v>42</v>
       </c>
       <c r="B109" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="C109" t="s">
         <v>9</v>
       </c>
       <c r="K109" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="L109" t="s">
         <v>136</v>
@@ -4058,13 +4058,13 @@
         <v>78</v>
       </c>
       <c r="B112" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
       <c r="C112" t="s">
         <v>17</v>
       </c>
       <c r="K112" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
       <c r="L112" t="s">
         <v>133</v>
@@ -4075,13 +4075,13 @@
         <v>78</v>
       </c>
       <c r="B113" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
       <c r="C113" t="s">
         <v>17</v>
       </c>
       <c r="K113" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
       <c r="L113" t="s">
         <v>133</v>
@@ -4092,13 +4092,13 @@
         <v>78</v>
       </c>
       <c r="B114" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
       <c r="C114" t="s">
         <v>19</v>
       </c>
       <c r="K114" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
       <c r="L114" t="s">
         <v>132</v>
@@ -4106,36 +4106,36 @@
     </row>
     <row r="115" spans="1:12" ht="16.5" customHeight="1">
       <c r="A115" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="B115" t="s">
+        <v>306</v>
+      </c>
+      <c r="C115" t="s">
+        <v>9</v>
+      </c>
+      <c r="K115" t="s">
         <v>307</v>
       </c>
-      <c r="C115" t="s">
-        <v>9</v>
-      </c>
-      <c r="K115" t="s">
+      <c r="L115" t="s">
         <v>308</v>
-      </c>
-      <c r="L115" t="s">
-        <v>309</v>
       </c>
     </row>
     <row r="116" spans="1:12" ht="16.5" customHeight="1">
       <c r="A116" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="B116" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="C116" t="s">
+        <v>309</v>
+      </c>
+      <c r="K116" t="s">
         <v>310</v>
       </c>
-      <c r="K116" t="s">
+      <c r="L116" t="s">
         <v>311</v>
-      </c>
-      <c r="L116" t="s">
-        <v>312</v>
       </c>
     </row>
     <row r="117" spans="1:12" ht="16.5" customHeight="1">
@@ -4183,7 +4183,7 @@
         <v>78</v>
       </c>
       <c r="B119" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="C119" t="s">
         <v>9</v>
@@ -4192,7 +4192,7 @@
         <v>42</v>
       </c>
       <c r="K119" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="L119" t="s">
         <v>132</v>
@@ -4203,13 +4203,13 @@
         <v>78</v>
       </c>
       <c r="B120" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="C120" t="s">
         <v>9</v>
       </c>
       <c r="K120" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="L120" t="s">
         <v>136</v>
@@ -4237,16 +4237,16 @@
         <v>78</v>
       </c>
       <c r="B122" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="C122" t="s">
         <v>17</v>
       </c>
       <c r="H122" t="s">
-        <v>154</v>
+        <v>442</v>
       </c>
       <c r="K122" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="L122" t="s">
         <v>133</v>
@@ -4257,25 +4257,25 @@
         <v>78</v>
       </c>
       <c r="B123" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="C123" t="s">
         <v>17</v>
       </c>
       <c r="D123" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="E123" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="F123" t="s">
         <v>12</v>
       </c>
       <c r="G123" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="K123" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="L123" t="s">
         <v>132</v>
@@ -4286,13 +4286,13 @@
         <v>78</v>
       </c>
       <c r="B124" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="C124" t="s">
         <v>17</v>
       </c>
       <c r="K124" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="L124" t="s">
         <v>133</v>
@@ -4303,13 +4303,13 @@
         <v>78</v>
       </c>
       <c r="B125" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="C125" t="s">
         <v>19</v>
       </c>
       <c r="K125" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="L125" t="s">
         <v>132</v>
@@ -4343,7 +4343,7 @@
         <v>9</v>
       </c>
       <c r="D127" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="E127" t="s">
         <v>11</v>
@@ -4358,7 +4358,7 @@
         <v>86</v>
       </c>
       <c r="L127" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
     </row>
     <row r="128" spans="1:12" ht="16.5" customHeight="1">
@@ -4372,7 +4372,7 @@
         <v>9</v>
       </c>
       <c r="D128" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="E128" t="s">
         <v>88</v>
@@ -4395,13 +4395,13 @@
         <v>84</v>
       </c>
       <c r="B129" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
       <c r="C129" t="s">
         <v>89</v>
       </c>
       <c r="K129" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
       <c r="L129" t="s">
         <v>132</v>
@@ -4412,13 +4412,13 @@
         <v>84</v>
       </c>
       <c r="B130" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
       <c r="C130" t="s">
         <v>89</v>
       </c>
       <c r="K130" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
       <c r="L130" t="s">
         <v>132</v>
@@ -4429,13 +4429,13 @@
         <v>84</v>
       </c>
       <c r="B131" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="C131" t="s">
         <v>17</v>
       </c>
       <c r="K131" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="L131" t="s">
         <v>133</v>
@@ -4446,13 +4446,13 @@
         <v>84</v>
       </c>
       <c r="B132" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="C132" t="s">
         <v>90</v>
       </c>
       <c r="K132" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="L132" t="s">
         <v>132</v>
@@ -4463,13 +4463,13 @@
         <v>84</v>
       </c>
       <c r="B133" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="C133" t="s">
         <v>9</v>
       </c>
       <c r="K133" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="L133" t="s">
         <v>138</v>
@@ -4480,13 +4480,13 @@
         <v>84</v>
       </c>
       <c r="B134" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
       <c r="C134" t="s">
         <v>17</v>
       </c>
       <c r="D134" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="E134" t="s">
         <v>91</v>
@@ -4498,7 +4498,7 @@
         <v>92</v>
       </c>
       <c r="K134" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
       <c r="L134" t="s">
         <v>132</v>
@@ -4509,13 +4509,13 @@
         <v>84</v>
       </c>
       <c r="B135" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
       <c r="C135" t="s">
         <v>17</v>
       </c>
       <c r="K135" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
       <c r="L135" t="s">
         <v>133</v>
@@ -4526,13 +4526,13 @@
         <v>84</v>
       </c>
       <c r="B136" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
       <c r="C136" t="s">
         <v>17</v>
       </c>
       <c r="K136" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
       <c r="L136" t="s">
         <v>133</v>
@@ -4543,13 +4543,13 @@
         <v>84</v>
       </c>
       <c r="B137" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="C137" t="s">
         <v>36</v>
       </c>
       <c r="K137" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="L137" t="s">
         <v>138</v>
@@ -4560,13 +4560,13 @@
         <v>84</v>
       </c>
       <c r="B138" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="C138" t="s">
         <v>17</v>
       </c>
       <c r="D138" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="E138" t="s">
         <v>91</v>
@@ -4578,7 +4578,7 @@
         <v>92</v>
       </c>
       <c r="K138" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="L138" t="s">
         <v>132</v>
@@ -4589,13 +4589,13 @@
         <v>84</v>
       </c>
       <c r="B139" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
       <c r="C139" t="s">
         <v>17</v>
       </c>
       <c r="K139" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
       <c r="L139" t="s">
         <v>133</v>
@@ -4603,7 +4603,7 @@
     </row>
     <row r="140" spans="1:12" ht="16.5" customHeight="1">
       <c r="A140" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="B140" t="s">
         <v>93</v>
@@ -4623,13 +4623,13 @@
         <v>84</v>
       </c>
       <c r="B141" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
       <c r="C141" t="s">
         <v>19</v>
       </c>
       <c r="K141" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
       <c r="L141" t="s">
         <v>132</v>
@@ -4640,13 +4640,13 @@
         <v>84</v>
       </c>
       <c r="B142" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
       <c r="C142" t="s">
         <v>19</v>
       </c>
       <c r="K142" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
       <c r="L142" t="s">
         <v>132</v>
@@ -4657,7 +4657,7 @@
         <v>84</v>
       </c>
       <c r="B143" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="C143" t="s">
         <v>9</v>
@@ -4666,7 +4666,7 @@
         <v>22</v>
       </c>
       <c r="K143" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="L143" t="s">
         <v>135</v>
@@ -4677,13 +4677,13 @@
         <v>84</v>
       </c>
       <c r="B144" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="C144" t="s">
         <v>19</v>
       </c>
       <c r="K144" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="L144" t="s">
         <v>132</v>
@@ -4694,13 +4694,13 @@
         <v>84</v>
       </c>
       <c r="B145" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="C145" t="s">
         <v>19</v>
       </c>
       <c r="K145" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="L145" t="s">
         <v>132</v>
@@ -4708,7 +4708,7 @@
     </row>
     <row r="146" spans="1:12" ht="16.5" customHeight="1">
       <c r="A146" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="B146" t="s">
         <v>94</v>
@@ -4734,7 +4734,7 @@
         <v>9</v>
       </c>
       <c r="D147" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="E147" t="s">
         <v>152</v>
@@ -4797,10 +4797,10 @@
         <v>17</v>
       </c>
       <c r="D150" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="E150" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="F150" t="s">
         <v>12</v>
@@ -4809,10 +4809,10 @@
         <v>61</v>
       </c>
       <c r="K150" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="L150" s="1" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
     </row>
     <row r="151" spans="1:12" ht="16.5" customHeight="1">
@@ -4820,16 +4820,16 @@
         <v>84</v>
       </c>
       <c r="B151" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="C151" t="s">
         <v>17</v>
       </c>
       <c r="H151" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="K151" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="L151" t="s">
         <v>133</v>
@@ -4840,16 +4840,16 @@
         <v>84</v>
       </c>
       <c r="B152" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="C152" t="s">
         <v>17</v>
       </c>
       <c r="H152" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="K152" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="L152" t="s">
         <v>133</v>
@@ -4860,16 +4860,16 @@
         <v>84</v>
       </c>
       <c r="B153" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="C153" t="s">
         <v>17</v>
       </c>
       <c r="H153" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="K153" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="L153" t="s">
         <v>133</v>
@@ -4880,19 +4880,19 @@
         <v>84</v>
       </c>
       <c r="B154" t="s">
+        <v>241</v>
+      </c>
+      <c r="C154" t="s">
+        <v>17</v>
+      </c>
+      <c r="H154" t="s">
+        <v>243</v>
+      </c>
+      <c r="K154" t="s">
+        <v>241</v>
+      </c>
+      <c r="L154" t="s">
         <v>242</v>
-      </c>
-      <c r="C154" t="s">
-        <v>17</v>
-      </c>
-      <c r="H154" t="s">
-        <v>244</v>
-      </c>
-      <c r="K154" t="s">
-        <v>242</v>
-      </c>
-      <c r="L154" t="s">
-        <v>243</v>
       </c>
     </row>
     <row r="155" spans="1:12" ht="16.5" customHeight="1">
@@ -4900,16 +4900,16 @@
         <v>84</v>
       </c>
       <c r="B155" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="C155" t="s">
         <v>36</v>
       </c>
       <c r="K155" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="L155" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
     </row>
     <row r="156" spans="1:12" ht="16.5" customHeight="1">
@@ -4917,16 +4917,16 @@
         <v>84</v>
       </c>
       <c r="B156" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="C156" t="s">
         <v>17</v>
       </c>
       <c r="D156" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="E156" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="F156" t="s">
         <v>12</v>
@@ -4935,10 +4935,10 @@
         <v>61</v>
       </c>
       <c r="K156" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="L156" s="1" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
     </row>
     <row r="157" spans="1:12" ht="16.5" customHeight="1">
@@ -4946,16 +4946,16 @@
         <v>84</v>
       </c>
       <c r="B157" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="C157" t="s">
         <v>36</v>
       </c>
       <c r="K157" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="L157" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
     </row>
     <row r="158" spans="1:12" ht="16.5" customHeight="1">
@@ -4963,16 +4963,16 @@
         <v>84</v>
       </c>
       <c r="B158" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="C158" t="s">
         <v>17</v>
       </c>
       <c r="D158" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="E158" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="F158" t="s">
         <v>12</v>
@@ -4981,10 +4981,10 @@
         <v>61</v>
       </c>
       <c r="K158" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="L158" s="1" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
     </row>
     <row r="159" spans="1:12" ht="16.5" customHeight="1">
@@ -4992,13 +4992,13 @@
         <v>84</v>
       </c>
       <c r="B159" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="C159" t="s">
         <v>9</v>
       </c>
       <c r="K159" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="L159" t="s">
         <v>136</v>
@@ -5009,19 +5009,19 @@
         <v>84</v>
       </c>
       <c r="B160" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="C160" t="s">
         <v>17</v>
       </c>
       <c r="H160" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="K160" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="L160" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
     </row>
     <row r="161" spans="1:12" ht="16.5" customHeight="1">
@@ -5029,19 +5029,19 @@
         <v>84</v>
       </c>
       <c r="B161" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="C161" t="s">
         <v>17</v>
       </c>
       <c r="H161" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="K161" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="L161" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
     </row>
     <row r="162" spans="1:12" ht="16.5" customHeight="1">
@@ -5049,19 +5049,19 @@
         <v>84</v>
       </c>
       <c r="B162" t="s">
+        <v>323</v>
+      </c>
+      <c r="C162" t="s">
+        <v>17</v>
+      </c>
+      <c r="H162" t="s">
         <v>324</v>
       </c>
-      <c r="C162" t="s">
-        <v>17</v>
-      </c>
-      <c r="H162" t="s">
-        <v>325</v>
-      </c>
       <c r="K162" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="L162" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
     </row>
     <row r="163" spans="1:12" ht="16.5" customHeight="1">
@@ -5069,16 +5069,16 @@
         <v>84</v>
       </c>
       <c r="B163" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="C163" t="s">
         <v>36</v>
       </c>
       <c r="K163" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="L163" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
     </row>
     <row r="164" spans="1:12" ht="16.5" customHeight="1">
@@ -5086,16 +5086,16 @@
         <v>84</v>
       </c>
       <c r="B164" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="C164" t="s">
         <v>17</v>
       </c>
       <c r="D164" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="E164" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="F164" t="s">
         <v>12</v>
@@ -5104,10 +5104,10 @@
         <v>61</v>
       </c>
       <c r="K164" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="L164" s="1" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
     </row>
     <row r="165" spans="1:12" ht="16.5" customHeight="1">
@@ -5115,16 +5115,16 @@
         <v>84</v>
       </c>
       <c r="B165" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="C165" t="s">
         <v>36</v>
       </c>
       <c r="K165" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="L165" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
     </row>
     <row r="166" spans="1:12" ht="16.5" customHeight="1">
@@ -5132,16 +5132,16 @@
         <v>84</v>
       </c>
       <c r="B166" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="C166" t="s">
         <v>17</v>
       </c>
       <c r="D166" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="E166" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="F166" t="s">
         <v>12</v>
@@ -5150,10 +5150,10 @@
         <v>61</v>
       </c>
       <c r="K166" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="L166" s="1" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
     </row>
     <row r="167" spans="1:12" ht="16.5" customHeight="1">
@@ -5161,13 +5161,13 @@
         <v>84</v>
       </c>
       <c r="B167" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="C167" t="s">
         <v>9</v>
       </c>
       <c r="K167" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="L167" t="s">
         <v>136</v>
@@ -5178,16 +5178,16 @@
         <v>84</v>
       </c>
       <c r="B168" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="C168" t="s">
         <v>17</v>
       </c>
       <c r="H168" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="K168" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="L168" t="s">
         <v>133</v>
@@ -5198,16 +5198,16 @@
         <v>84</v>
       </c>
       <c r="B169" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="C169" t="s">
         <v>17</v>
       </c>
       <c r="H169" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="K169" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="L169" t="s">
         <v>133</v>
@@ -5218,16 +5218,16 @@
         <v>84</v>
       </c>
       <c r="B170" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="C170" t="s">
         <v>17</v>
       </c>
       <c r="H170" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="K170" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="L170" t="s">
         <v>133</v>
@@ -5238,19 +5238,19 @@
         <v>84</v>
       </c>
       <c r="B171" t="s">
+        <v>244</v>
+      </c>
+      <c r="C171" t="s">
+        <v>17</v>
+      </c>
+      <c r="H171" t="s">
         <v>245</v>
       </c>
-      <c r="C171" t="s">
-        <v>17</v>
-      </c>
-      <c r="H171" t="s">
-        <v>246</v>
-      </c>
       <c r="K171" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="L171" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
     </row>
     <row r="172" spans="1:12" ht="16.5" customHeight="1">
@@ -5258,16 +5258,16 @@
         <v>84</v>
       </c>
       <c r="B172" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="C172" t="s">
         <v>36</v>
       </c>
       <c r="K172" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="L172" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
     </row>
     <row r="173" spans="1:12" ht="16.5" customHeight="1">
@@ -5275,16 +5275,16 @@
         <v>84</v>
       </c>
       <c r="B173" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="C173" t="s">
         <v>17</v>
       </c>
       <c r="D173" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="E173" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="F173" t="s">
         <v>12</v>
@@ -5293,10 +5293,10 @@
         <v>61</v>
       </c>
       <c r="K173" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="L173" s="1" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
     </row>
     <row r="174" spans="1:12" ht="16.5" customHeight="1">
@@ -5304,16 +5304,16 @@
         <v>84</v>
       </c>
       <c r="B174" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="C174" t="s">
         <v>36</v>
       </c>
       <c r="K174" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="L174" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
     </row>
     <row r="175" spans="1:12" ht="16.5" customHeight="1">
@@ -5321,16 +5321,16 @@
         <v>84</v>
       </c>
       <c r="B175" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="C175" t="s">
         <v>17</v>
       </c>
       <c r="D175" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="E175" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="F175" t="s">
         <v>12</v>
@@ -5339,10 +5339,10 @@
         <v>61</v>
       </c>
       <c r="K175" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="L175" s="1" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
     </row>
     <row r="176" spans="1:12" ht="16.5" customHeight="1">
@@ -5350,13 +5350,13 @@
         <v>84</v>
       </c>
       <c r="B176" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="C176" t="s">
         <v>9</v>
       </c>
       <c r="K176" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="L176" t="s">
         <v>136</v>
@@ -5367,16 +5367,16 @@
         <v>84</v>
       </c>
       <c r="B177" t="s">
+        <v>206</v>
+      </c>
+      <c r="C177" t="s">
+        <v>9</v>
+      </c>
+      <c r="D177" t="s">
+        <v>350</v>
+      </c>
+      <c r="E177" t="s">
         <v>207</v>
-      </c>
-      <c r="C177" t="s">
-        <v>9</v>
-      </c>
-      <c r="D177" t="s">
-        <v>351</v>
-      </c>
-      <c r="E177" t="s">
-        <v>208</v>
       </c>
       <c r="F177" t="s">
         <v>12</v>
@@ -5385,7 +5385,7 @@
         <v>13</v>
       </c>
       <c r="K177" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="L177" t="s">
         <v>132</v>
@@ -5396,16 +5396,16 @@
         <v>84</v>
       </c>
       <c r="B178" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="C178" t="s">
         <v>89</v>
       </c>
       <c r="H178" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="K178" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="L178" t="s">
         <v>132</v>
@@ -5416,16 +5416,16 @@
         <v>84</v>
       </c>
       <c r="B179" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="C179" t="s">
         <v>89</v>
       </c>
       <c r="H179" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="K179" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="L179" t="s">
         <v>132</v>
@@ -5436,13 +5436,13 @@
         <v>84</v>
       </c>
       <c r="B180" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="C180" t="s">
         <v>9</v>
       </c>
       <c r="K180" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="L180" t="s">
         <v>136</v>
@@ -5450,7 +5450,7 @@
     </row>
     <row r="181" spans="1:12" ht="16.5" customHeight="1">
       <c r="A181" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="B181" t="s">
         <v>96</v>
@@ -5459,7 +5459,7 @@
         <v>9</v>
       </c>
       <c r="D181" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="E181" t="s">
         <v>97</v>
@@ -5488,16 +5488,16 @@
         <v>9</v>
       </c>
       <c r="D182" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="F182" t="s">
         <v>98</v>
       </c>
       <c r="H182" t="s">
+        <v>294</v>
+      </c>
+      <c r="I182" t="s">
         <v>295</v>
-      </c>
-      <c r="I182" t="s">
-        <v>296</v>
       </c>
       <c r="K182" t="s">
         <v>96</v>
@@ -5508,7 +5508,7 @@
     </row>
     <row r="183" spans="1:12" ht="16.5" customHeight="1">
       <c r="A183" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="B183" t="s">
         <v>99</v>
@@ -5517,7 +5517,7 @@
         <v>9</v>
       </c>
       <c r="D183" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="E183" t="s">
         <v>100</v>
@@ -5546,16 +5546,16 @@
         <v>9</v>
       </c>
       <c r="D184" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="F184" t="s">
         <v>12</v>
       </c>
       <c r="H184" t="s">
+        <v>296</v>
+      </c>
+      <c r="I184" t="s">
         <v>297</v>
-      </c>
-      <c r="I184" t="s">
-        <v>298</v>
       </c>
       <c r="K184" t="s">
         <v>99</v>
@@ -5569,13 +5569,13 @@
         <v>84</v>
       </c>
       <c r="B185" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="C185" t="s">
         <v>9</v>
       </c>
       <c r="K185" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="L185" t="s">
         <v>136</v>
@@ -5586,7 +5586,7 @@
         <v>84</v>
       </c>
       <c r="B186" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="C186" t="s">
         <v>9</v>
@@ -5595,7 +5595,7 @@
         <v>42</v>
       </c>
       <c r="K186" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="L186" t="s">
         <v>132</v>
@@ -5629,10 +5629,10 @@
         <v>17</v>
       </c>
       <c r="D188" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="E188" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="F188" t="s">
         <v>12</v>
@@ -5641,10 +5641,10 @@
         <v>61</v>
       </c>
       <c r="K188" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="L188" s="1" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
     </row>
     <row r="189" spans="1:12" ht="16.5" customHeight="1">
@@ -5746,10 +5746,10 @@
         <v>17</v>
       </c>
       <c r="D194" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="E194" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="F194" t="s">
         <v>12</v>
@@ -5758,10 +5758,10 @@
         <v>61</v>
       </c>
       <c r="K194" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="L194" s="1" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
     </row>
     <row r="195" spans="1:12" ht="16.5" customHeight="1">
@@ -5769,13 +5769,13 @@
         <v>84</v>
       </c>
       <c r="B195" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="C195" t="s">
         <v>56</v>
       </c>
       <c r="K195" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="L195" t="s">
         <v>138</v>
@@ -5786,16 +5786,16 @@
         <v>84</v>
       </c>
       <c r="B196" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="C196" t="s">
         <v>17</v>
       </c>
       <c r="D196" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="E196" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="F196" t="s">
         <v>12</v>
@@ -5804,10 +5804,10 @@
         <v>61</v>
       </c>
       <c r="K196" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="L196" s="1" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
     </row>
     <row r="197" spans="1:12" ht="16.5" customHeight="1">
@@ -5815,13 +5815,13 @@
         <v>84</v>
       </c>
       <c r="B197" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="C197" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="K197" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="L197" t="s">
         <v>138</v>
@@ -5832,21 +5832,21 @@
         <v>84</v>
       </c>
       <c r="B198" t="s">
+        <v>312</v>
+      </c>
+      <c r="C198" t="s">
+        <v>9</v>
+      </c>
+      <c r="K198" t="s">
         <v>313</v>
       </c>
-      <c r="C198" t="s">
-        <v>9</v>
-      </c>
-      <c r="K198" t="s">
+      <c r="L198" s="1" t="s">
         <v>314</v>
-      </c>
-      <c r="L198" s="1" t="s">
-        <v>315</v>
       </c>
     </row>
     <row r="199" spans="1:12" ht="16.5" customHeight="1">
       <c r="A199" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="B199" t="s">
         <v>106</v>
@@ -5855,7 +5855,7 @@
         <v>9</v>
       </c>
       <c r="D199" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="E199" t="s">
         <v>107</v>
@@ -5884,16 +5884,16 @@
         <v>9</v>
       </c>
       <c r="D200" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="F200" t="s">
         <v>98</v>
       </c>
       <c r="H200" t="s">
+        <v>298</v>
+      </c>
+      <c r="I200" t="s">
         <v>299</v>
-      </c>
-      <c r="I200" t="s">
-        <v>300</v>
       </c>
       <c r="K200" t="s">
         <v>106</v>
@@ -5913,7 +5913,7 @@
         <v>17</v>
       </c>
       <c r="H201" t="s">
-        <v>154</v>
+        <v>442</v>
       </c>
       <c r="K201" t="s">
         <v>153</v>
@@ -5941,7 +5941,7 @@
     </row>
     <row r="203" spans="1:12" ht="16.5" customHeight="1">
       <c r="A203" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="B203" t="s">
         <v>108</v>
@@ -5950,7 +5950,7 @@
         <v>9</v>
       </c>
       <c r="D203" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="E203" t="s">
         <v>109</v>
@@ -5979,16 +5979,16 @@
         <v>9</v>
       </c>
       <c r="D204" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="F204" t="s">
         <v>98</v>
       </c>
       <c r="H204" t="s">
+        <v>300</v>
+      </c>
+      <c r="I204" t="s">
         <v>301</v>
-      </c>
-      <c r="I204" t="s">
-        <v>302</v>
       </c>
       <c r="K204" t="s">
         <v>108</v>
@@ -5999,7 +5999,7 @@
     </row>
     <row r="205" spans="1:12" ht="16.5" customHeight="1">
       <c r="A205" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="B205" t="s">
         <v>110</v>
@@ -6008,7 +6008,7 @@
         <v>9</v>
       </c>
       <c r="D205" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="E205" t="s">
         <v>111</v>
@@ -6037,16 +6037,16 @@
         <v>9</v>
       </c>
       <c r="D206" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="F206" t="s">
         <v>12</v>
       </c>
       <c r="H206" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="I206" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="K206" t="s">
         <v>110</v>
@@ -6060,13 +6060,13 @@
         <v>84</v>
       </c>
       <c r="B207" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="C207" t="s">
         <v>9</v>
       </c>
       <c r="K207" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="L207" t="s">
         <v>136</v>
@@ -6074,7 +6074,7 @@
     </row>
     <row r="208" spans="1:12" ht="16.5" customHeight="1">
       <c r="A208" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="B208" t="s">
         <v>122</v>
@@ -6120,10 +6120,10 @@
         <v>17</v>
       </c>
       <c r="D210" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="E210" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="F210" t="s">
         <v>12</v>
@@ -6132,10 +6132,10 @@
         <v>61</v>
       </c>
       <c r="K210" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="L210" s="1" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
     </row>
     <row r="211" spans="1:12" ht="16.5" customHeight="1">
@@ -6237,10 +6237,10 @@
         <v>17</v>
       </c>
       <c r="D216" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="E216" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="F216" t="s">
         <v>12</v>
@@ -6249,10 +6249,10 @@
         <v>61</v>
       </c>
       <c r="K216" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="L216" s="1" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
     </row>
     <row r="217" spans="1:12" ht="16.5" customHeight="1">
@@ -6260,13 +6260,13 @@
         <v>84</v>
       </c>
       <c r="B217" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="C217" t="s">
         <v>56</v>
       </c>
       <c r="K217" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="L217" t="s">
         <v>138</v>
@@ -6277,16 +6277,16 @@
         <v>84</v>
       </c>
       <c r="B218" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="C218" t="s">
         <v>17</v>
       </c>
       <c r="D218" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="E218" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="F218" t="s">
         <v>12</v>
@@ -6295,10 +6295,10 @@
         <v>61</v>
       </c>
       <c r="K218" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="L218" s="1" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
     </row>
     <row r="219" spans="1:12" ht="16.5" customHeight="1">
@@ -6306,13 +6306,13 @@
         <v>84</v>
       </c>
       <c r="B219" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="C219" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="K219" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="L219" t="s">
         <v>138</v>
@@ -6323,21 +6323,21 @@
         <v>84</v>
       </c>
       <c r="B220" t="s">
+        <v>315</v>
+      </c>
+      <c r="C220" t="s">
+        <v>9</v>
+      </c>
+      <c r="K220" t="s">
         <v>316</v>
       </c>
-      <c r="C220" t="s">
-        <v>9</v>
-      </c>
-      <c r="K220" t="s">
-        <v>317</v>
-      </c>
       <c r="L220" s="1" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
     </row>
     <row r="221" spans="1:12" ht="16.5" customHeight="1">
       <c r="A221" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="B221" t="s">
         <v>116</v>
@@ -6346,7 +6346,7 @@
         <v>9</v>
       </c>
       <c r="D221" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="E221" t="s">
         <v>117</v>
@@ -6375,16 +6375,16 @@
         <v>9</v>
       </c>
       <c r="D222" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="F222" t="s">
         <v>98</v>
       </c>
       <c r="H222" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="I222" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="K222" t="s">
         <v>116</v>
@@ -6398,16 +6398,16 @@
         <v>84</v>
       </c>
       <c r="B223" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="C223" t="s">
         <v>17</v>
       </c>
       <c r="H223" t="s">
+        <v>442</v>
+      </c>
+      <c r="K223" t="s">
         <v>154</v>
-      </c>
-      <c r="K223" t="s">
-        <v>155</v>
       </c>
       <c r="L223" t="s">
         <v>133</v>
@@ -6458,7 +6458,7 @@
         <v>9</v>
       </c>
       <c r="D226" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="E226" t="s">
         <v>120</v>
@@ -6495,19 +6495,19 @@
     </row>
     <row r="228" spans="1:12" ht="16.5" customHeight="1">
       <c r="A228" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="B228" t="s">
+        <v>360</v>
+      </c>
+      <c r="C228" t="s">
+        <v>9</v>
+      </c>
+      <c r="D228" t="s">
         <v>361</v>
       </c>
-      <c r="C228" t="s">
-        <v>9</v>
-      </c>
-      <c r="D228" t="s">
+      <c r="E228" t="s">
         <v>362</v>
-      </c>
-      <c r="E228" t="s">
-        <v>363</v>
       </c>
       <c r="F228" t="s">
         <v>98</v>
@@ -6516,7 +6516,7 @@
         <v>13</v>
       </c>
       <c r="K228" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
       <c r="L228" t="s">
         <v>132</v>
@@ -6527,25 +6527,25 @@
         <v>84</v>
       </c>
       <c r="B229" t="s">
+        <v>360</v>
+      </c>
+      <c r="C229" t="s">
+        <v>9</v>
+      </c>
+      <c r="D229" t="s">
         <v>361</v>
-      </c>
-      <c r="C229" t="s">
-        <v>9</v>
-      </c>
-      <c r="D229" t="s">
-        <v>362</v>
       </c>
       <c r="F229" t="s">
         <v>98</v>
       </c>
       <c r="H229" t="s">
+        <v>363</v>
+      </c>
+      <c r="I229" t="s">
         <v>364</v>
       </c>
-      <c r="I229" t="s">
-        <v>365</v>
-      </c>
       <c r="K229" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
       <c r="L229" t="s">
         <v>132</v>
@@ -6553,19 +6553,19 @@
     </row>
     <row r="230" spans="1:12" ht="16.5" customHeight="1">
       <c r="A230" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="B230" t="s">
+        <v>365</v>
+      </c>
+      <c r="C230" t="s">
+        <v>9</v>
+      </c>
+      <c r="D230" t="s">
+        <v>352</v>
+      </c>
+      <c r="E230" t="s">
         <v>366</v>
-      </c>
-      <c r="C230" t="s">
-        <v>9</v>
-      </c>
-      <c r="D230" t="s">
-        <v>353</v>
-      </c>
-      <c r="E230" t="s">
-        <v>367</v>
       </c>
       <c r="F230" t="s">
         <v>12</v>
@@ -6574,7 +6574,7 @@
         <v>13</v>
       </c>
       <c r="K230" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="L230" t="s">
         <v>132</v>
@@ -6585,25 +6585,25 @@
         <v>84</v>
       </c>
       <c r="B231" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="C231" t="s">
         <v>9</v>
       </c>
       <c r="D231" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="F231" t="s">
         <v>12</v>
       </c>
       <c r="H231" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
       <c r="I231" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="K231" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="L231" t="s">
         <v>132</v>
@@ -6614,13 +6614,13 @@
         <v>84</v>
       </c>
       <c r="B232" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="C232" t="s">
         <v>9</v>
       </c>
       <c r="K232" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="L232" t="s">
         <v>136</v>
@@ -6628,7 +6628,7 @@
     </row>
     <row r="233" spans="1:12" ht="16.5" customHeight="1">
       <c r="A233" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="B233" t="s">
         <v>122</v>
@@ -6651,13 +6651,13 @@
         <v>84</v>
       </c>
       <c r="B234" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
       <c r="C234" t="s">
         <v>56</v>
       </c>
       <c r="K234" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
       <c r="L234" t="s">
         <v>138</v>
@@ -6668,16 +6668,16 @@
         <v>84</v>
       </c>
       <c r="B235" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
       <c r="C235" t="s">
         <v>17</v>
       </c>
       <c r="D235" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="E235" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="F235" t="s">
         <v>12</v>
@@ -6686,10 +6686,10 @@
         <v>61</v>
       </c>
       <c r="K235" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
       <c r="L235" s="1" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
     </row>
     <row r="236" spans="1:12" ht="16.5" customHeight="1">
@@ -6697,7 +6697,7 @@
         <v>84</v>
       </c>
       <c r="B236" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="C236" t="s">
         <v>17</v>
@@ -6706,7 +6706,7 @@
         <v>143</v>
       </c>
       <c r="K236" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="L236" t="s">
         <v>133</v>
@@ -6717,13 +6717,13 @@
         <v>84</v>
       </c>
       <c r="B237" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="C237" t="s">
         <v>19</v>
       </c>
       <c r="K237" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="L237" t="s">
         <v>132</v>
@@ -6734,13 +6734,13 @@
         <v>84</v>
       </c>
       <c r="B238" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
       <c r="C238" t="s">
         <v>9</v>
       </c>
       <c r="K238" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
       <c r="L238" t="s">
         <v>138</v>
@@ -6751,13 +6751,13 @@
         <v>84</v>
       </c>
       <c r="B239" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
       <c r="C239" t="s">
         <v>104</v>
       </c>
       <c r="K239" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
       <c r="L239" t="s">
         <v>138</v>
@@ -6768,13 +6768,13 @@
         <v>84</v>
       </c>
       <c r="B240" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="C240" t="s">
         <v>36</v>
       </c>
       <c r="K240" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="L240" t="s">
         <v>138</v>
@@ -6785,16 +6785,16 @@
         <v>84</v>
       </c>
       <c r="B241" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="C241" t="s">
         <v>17</v>
       </c>
       <c r="D241" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="E241" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="F241" t="s">
         <v>12</v>
@@ -6803,10 +6803,10 @@
         <v>61</v>
       </c>
       <c r="K241" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="L241" s="1" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
     </row>
     <row r="242" spans="1:12" ht="16.5" customHeight="1">
@@ -6814,13 +6814,13 @@
         <v>84</v>
       </c>
       <c r="B242" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="C242" t="s">
         <v>56</v>
       </c>
       <c r="K242" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="L242" t="s">
         <v>138</v>
@@ -6831,16 +6831,16 @@
         <v>84</v>
       </c>
       <c r="B243" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="C243" t="s">
         <v>17</v>
       </c>
       <c r="D243" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="E243" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="F243" t="s">
         <v>12</v>
@@ -6849,10 +6849,10 @@
         <v>61</v>
       </c>
       <c r="K243" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="L243" s="1" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
     </row>
     <row r="244" spans="1:12" ht="16.5" customHeight="1">
@@ -6860,13 +6860,13 @@
         <v>84</v>
       </c>
       <c r="B244" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
       <c r="C244" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="K244" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
       <c r="L244" t="s">
         <v>138</v>
@@ -6877,33 +6877,33 @@
         <v>84</v>
       </c>
       <c r="B245" t="s">
+        <v>379</v>
+      </c>
+      <c r="C245" t="s">
+        <v>9</v>
+      </c>
+      <c r="K245" t="s">
         <v>380</v>
       </c>
-      <c r="C245" t="s">
-        <v>9</v>
-      </c>
-      <c r="K245" t="s">
-        <v>381</v>
-      </c>
       <c r="L245" s="1" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
     </row>
     <row r="246" spans="1:12" ht="16.5" customHeight="1">
       <c r="A246" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="B246" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
       <c r="C246" t="s">
         <v>9</v>
       </c>
       <c r="D246" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="E246" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
       <c r="F246" t="s">
         <v>98</v>
@@ -6912,7 +6912,7 @@
         <v>13</v>
       </c>
       <c r="K246" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
       <c r="L246" t="s">
         <v>132</v>
@@ -6923,25 +6923,25 @@
         <v>84</v>
       </c>
       <c r="B247" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
       <c r="C247" t="s">
         <v>9</v>
       </c>
       <c r="D247" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="F247" t="s">
         <v>98</v>
       </c>
       <c r="H247" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
       <c r="I247" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="K247" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
       <c r="L247" t="s">
         <v>132</v>
@@ -6952,16 +6952,16 @@
         <v>84</v>
       </c>
       <c r="B248" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
       <c r="C248" t="s">
         <v>17</v>
       </c>
       <c r="H248" t="s">
-        <v>154</v>
+        <v>442</v>
       </c>
       <c r="K248" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
       <c r="L248" t="s">
         <v>133</v>
@@ -6972,13 +6972,13 @@
         <v>84</v>
       </c>
       <c r="B249" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="C249" t="s">
         <v>9</v>
       </c>
       <c r="K249" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="L249" t="s">
         <v>136</v>
@@ -6989,13 +6989,13 @@
         <v>84</v>
       </c>
       <c r="B250" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="C250" t="s">
         <v>89</v>
       </c>
       <c r="K250" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="L250" t="s">
         <v>132</v>
@@ -7006,16 +7006,16 @@
         <v>84</v>
       </c>
       <c r="B251" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="C251" t="s">
         <v>9</v>
       </c>
       <c r="D251" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="E251" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="F251" t="s">
         <v>12</v>
@@ -7024,7 +7024,7 @@
         <v>13</v>
       </c>
       <c r="K251" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="L251" t="s">
         <v>132</v>
@@ -7035,13 +7035,13 @@
         <v>84</v>
       </c>
       <c r="B252" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="C252" t="s">
         <v>9</v>
       </c>
       <c r="K252" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="L252" t="s">
         <v>136</v>
@@ -7052,13 +7052,13 @@
         <v>84</v>
       </c>
       <c r="B253" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="C253" t="s">
         <v>19</v>
       </c>
       <c r="K253" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="L253" t="s">
         <v>132</v>
@@ -7069,16 +7069,16 @@
         <v>84</v>
       </c>
       <c r="B254" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="C254" t="s">
         <v>9</v>
       </c>
       <c r="J254" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="K254" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="L254" t="s">
         <v>132</v>
@@ -7135,13 +7135,13 @@
         <v>84</v>
       </c>
       <c r="B257" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="C257" t="s">
         <v>56</v>
       </c>
       <c r="K257" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="L257" t="s">
         <v>138</v>
@@ -7152,16 +7152,16 @@
         <v>84</v>
       </c>
       <c r="B258" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="C258" t="s">
         <v>17</v>
       </c>
       <c r="D258" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="E258" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="F258" t="s">
         <v>12</v>
@@ -7170,10 +7170,10 @@
         <v>61</v>
       </c>
       <c r="K258" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="L258" s="1" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
     </row>
     <row r="259" spans="1:12" ht="16.5" customHeight="1">
@@ -7181,13 +7181,13 @@
         <v>84</v>
       </c>
       <c r="B259" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="C259" t="s">
         <v>9</v>
       </c>
       <c r="K259" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="L259" t="s">
         <v>136</v>
@@ -7198,13 +7198,13 @@
         <v>84</v>
       </c>
       <c r="B260" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="C260" t="s">
         <v>89</v>
       </c>
       <c r="K260" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="L260" t="s">
         <v>132</v>
@@ -7215,13 +7215,13 @@
         <v>84</v>
       </c>
       <c r="B261" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
       <c r="C261" t="s">
         <v>9</v>
       </c>
       <c r="K261" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
       <c r="L261" t="s">
         <v>136</v>
@@ -7232,16 +7232,16 @@
         <v>84</v>
       </c>
       <c r="B262" t="s">
+        <v>407</v>
+      </c>
+      <c r="C262" t="s">
+        <v>17</v>
+      </c>
+      <c r="H262" t="s">
         <v>408</v>
       </c>
-      <c r="C262" t="s">
-        <v>17</v>
-      </c>
-      <c r="H262" t="s">
-        <v>409</v>
-      </c>
       <c r="K262" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
       <c r="L262" t="s">
         <v>133</v>
@@ -7252,13 +7252,13 @@
         <v>84</v>
       </c>
       <c r="B263" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
       <c r="C263" t="s">
         <v>56</v>
       </c>
       <c r="K263" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
       <c r="L263" t="s">
         <v>138</v>
@@ -7269,16 +7269,16 @@
         <v>84</v>
       </c>
       <c r="B264" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
       <c r="C264" t="s">
         <v>17</v>
       </c>
       <c r="D264" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="E264" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="F264" t="s">
         <v>12</v>
@@ -7287,10 +7287,10 @@
         <v>61</v>
       </c>
       <c r="K264" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
       <c r="L264" s="1" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
     </row>
     <row r="265" spans="1:12" ht="16.5" customHeight="1">
@@ -7321,7 +7321,7 @@
         <v>9</v>
       </c>
       <c r="D266" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="E266" t="s">
         <v>11</v>
@@ -7336,7 +7336,7 @@
         <v>127</v>
       </c>
       <c r="L266" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
     </row>
     <row r="267" spans="1:12" ht="16.5" customHeight="1">
@@ -7378,13 +7378,13 @@
         <v>125</v>
       </c>
       <c r="B269" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
       <c r="C269" t="s">
         <v>19</v>
       </c>
       <c r="K269" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
       <c r="L269" t="s">
         <v>132</v>
@@ -7395,13 +7395,13 @@
         <v>125</v>
       </c>
       <c r="B270" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="C270" t="s">
         <v>19</v>
       </c>
       <c r="K270" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="L270" t="s">
         <v>132</v>
@@ -7412,25 +7412,25 @@
         <v>125</v>
       </c>
       <c r="B271" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="C271" t="s">
         <v>17</v>
       </c>
       <c r="D271" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="E271" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="F271" t="s">
+        <v>214</v>
+      </c>
+      <c r="G271" t="s">
+        <v>220</v>
+      </c>
+      <c r="K271" t="s">
         <v>215</v>
-      </c>
-      <c r="G271" t="s">
-        <v>221</v>
-      </c>
-      <c r="K271" t="s">
-        <v>216</v>
       </c>
       <c r="L271" t="s">
         <v>132</v>
@@ -7441,13 +7441,13 @@
         <v>125</v>
       </c>
       <c r="B272" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="C272" t="s">
         <v>19</v>
       </c>
       <c r="K272" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="L272" t="s">
         <v>132</v>
@@ -7458,13 +7458,13 @@
         <v>125</v>
       </c>
       <c r="B273" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="C273" t="s">
         <v>56</v>
       </c>
       <c r="K273" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="L273" t="s">
         <v>138</v>
@@ -7475,16 +7475,16 @@
         <v>125</v>
       </c>
       <c r="B274" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="C274" t="s">
         <v>17</v>
       </c>
       <c r="D274" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="E274" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="F274" t="s">
         <v>12</v>
@@ -7493,10 +7493,10 @@
         <v>61</v>
       </c>
       <c r="K274" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="L274" s="1" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
     </row>
     <row r="275" spans="1:12" ht="16.5" customHeight="1">
@@ -7504,7 +7504,7 @@
         <v>125</v>
       </c>
       <c r="B275" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="C275" t="s">
         <v>9</v>
@@ -7513,7 +7513,7 @@
         <v>22</v>
       </c>
       <c r="K275" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="L275" t="s">
         <v>132</v>
@@ -7524,13 +7524,13 @@
         <v>125</v>
       </c>
       <c r="B276" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
       <c r="C276" t="s">
         <v>9</v>
       </c>
       <c r="D276" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="E276" t="s">
         <v>31</v>
@@ -7542,7 +7542,7 @@
         <v>13</v>
       </c>
       <c r="K276" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
       <c r="L276" t="s">
         <v>132</v>
@@ -7553,25 +7553,25 @@
         <v>125</v>
       </c>
       <c r="B277" t="s">
+        <v>238</v>
+      </c>
+      <c r="C277" t="s">
+        <v>17</v>
+      </c>
+      <c r="D277" t="s">
+        <v>356</v>
+      </c>
+      <c r="E277" t="s">
         <v>239</v>
-      </c>
-      <c r="C277" t="s">
-        <v>17</v>
-      </c>
-      <c r="D277" t="s">
-        <v>357</v>
-      </c>
-      <c r="E277" t="s">
-        <v>240</v>
       </c>
       <c r="F277" t="s">
         <v>12</v>
       </c>
       <c r="G277" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="K277" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="L277" t="s">
         <v>132</v>
@@ -7579,16 +7579,16 @@
     </row>
     <row r="278" spans="1:12" ht="16.5" customHeight="1">
       <c r="A278" t="s">
+        <v>411</v>
+      </c>
+      <c r="B278" t="s">
         <v>412</v>
       </c>
-      <c r="B278" t="s">
-        <v>413</v>
-      </c>
       <c r="C278" t="s">
         <v>9</v>
       </c>
       <c r="K278" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="L278" t="s">
         <v>131</v>
@@ -7596,16 +7596,16 @@
     </row>
     <row r="279" spans="1:12" ht="16.5" customHeight="1">
       <c r="A279" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="B279" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
       <c r="C279" t="s">
         <v>9</v>
       </c>
       <c r="D279" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="E279" t="s">
         <v>11</v>
@@ -7617,24 +7617,24 @@
         <v>13</v>
       </c>
       <c r="K279" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
       <c r="L279" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
     </row>
     <row r="280" spans="1:12" ht="16.5" customHeight="1">
       <c r="A280" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="B280" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
       <c r="C280" t="s">
         <v>17</v>
       </c>
       <c r="K280" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
       <c r="L280" t="s">
         <v>133</v>
@@ -7642,16 +7642,16 @@
     </row>
     <row r="281" spans="1:12" ht="16.5" customHeight="1">
       <c r="A281" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="B281" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
       <c r="C281" t="s">
         <v>56</v>
       </c>
       <c r="K281" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
       <c r="L281" t="s">
         <v>138</v>
@@ -7659,19 +7659,19 @@
     </row>
     <row r="282" spans="1:12" ht="16.5" customHeight="1">
       <c r="A282" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="B282" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
       <c r="C282" t="s">
         <v>17</v>
       </c>
       <c r="D282" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="E282" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="F282" t="s">
         <v>12</v>
@@ -7680,27 +7680,27 @@
         <v>61</v>
       </c>
       <c r="K282" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
       <c r="L282" s="1" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
     </row>
     <row r="283" spans="1:12" ht="16.5" customHeight="1">
       <c r="A283" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="B283" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
       <c r="C283" t="s">
         <v>9</v>
       </c>
       <c r="D283" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="E283" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="F283" t="s">
         <v>12</v>
@@ -7709,7 +7709,7 @@
         <v>13</v>
       </c>
       <c r="K283" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
       <c r="L283" t="s">
         <v>132</v>
@@ -7717,19 +7717,19 @@
     </row>
     <row r="284" spans="1:12" ht="16.5" customHeight="1">
       <c r="A284" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="B284" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
       <c r="C284" t="s">
         <v>9</v>
       </c>
       <c r="D284" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="E284" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="F284" t="s">
         <v>12</v>
@@ -7738,7 +7738,7 @@
         <v>13</v>
       </c>
       <c r="K284" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
       <c r="L284" t="s">
         <v>132</v>
@@ -7746,10 +7746,10 @@
     </row>
     <row r="285" spans="1:12" ht="16.5" customHeight="1">
       <c r="A285" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="B285" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="C285" t="s">
         <v>9</v>
@@ -7758,7 +7758,7 @@
         <v>42</v>
       </c>
       <c r="K285" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="L285" t="s">
         <v>132</v>
@@ -7766,10 +7766,10 @@
     </row>
     <row r="286" spans="1:12" ht="16.5" customHeight="1">
       <c r="A286" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="B286" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
       <c r="C286" t="s">
         <v>9</v>
@@ -7784,7 +7784,7 @@
         <v>13</v>
       </c>
       <c r="K286" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
       <c r="L286" t="s">
         <v>132</v>
@@ -7792,16 +7792,16 @@
     </row>
     <row r="287" spans="1:12" ht="16.5" customHeight="1">
       <c r="A287" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="B287" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="C287" t="s">
         <v>17</v>
       </c>
       <c r="K287" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="L287" t="s">
         <v>133</v>
@@ -7809,16 +7809,16 @@
     </row>
     <row r="288" spans="1:12" ht="16.5" customHeight="1">
       <c r="A288" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="B288" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="C288" t="s">
         <v>17</v>
       </c>
       <c r="K288" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="L288" t="s">
         <v>133</v>
@@ -7826,25 +7826,25 @@
     </row>
     <row r="289" spans="1:12" ht="16.5" customHeight="1">
       <c r="A289" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="B289" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
       <c r="C289" t="s">
         <v>17</v>
       </c>
       <c r="E289" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="F289" t="s">
         <v>12</v>
       </c>
       <c r="G289" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
       <c r="K289" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
       <c r="L289" t="s">
         <v>132</v>
@@ -7852,16 +7852,16 @@
     </row>
     <row r="290" spans="1:12" ht="16.5" customHeight="1">
       <c r="A290" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="B290" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
       <c r="C290" t="s">
         <v>17</v>
       </c>
       <c r="K290" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
       <c r="L290" t="s">
         <v>133</v>
@@ -7869,16 +7869,16 @@
     </row>
     <row r="291" spans="1:12" ht="16.5" customHeight="1">
       <c r="A291" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="B291" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
       <c r="C291" t="s">
         <v>19</v>
       </c>
       <c r="K291" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
       <c r="L291" t="s">
         <v>132</v>
@@ -7886,16 +7886,16 @@
     </row>
     <row r="292" spans="1:12" ht="16.5" customHeight="1">
       <c r="A292" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="B292" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
       <c r="C292" t="s">
         <v>19</v>
       </c>
       <c r="K292" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
       <c r="L292" t="s">
         <v>132</v>
@@ -7903,16 +7903,16 @@
     </row>
     <row r="293" spans="1:12" ht="16.5" customHeight="1">
       <c r="A293" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="B293" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
       <c r="C293" t="s">
         <v>19</v>
       </c>
       <c r="K293" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
       <c r="L293" t="s">
         <v>132</v>
@@ -7920,16 +7920,16 @@
     </row>
     <row r="294" spans="1:12" ht="16.5" customHeight="1">
       <c r="A294" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="B294" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
       <c r="C294" t="s">
         <v>9</v>
       </c>
       <c r="K294" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
       <c r="L294" t="s">
         <v>136</v>
@@ -7937,10 +7937,10 @@
     </row>
     <row r="295" spans="1:12" ht="16.5" customHeight="1">
       <c r="A295" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="B295" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
       <c r="C295" t="s">
         <v>9</v>
@@ -7949,7 +7949,7 @@
         <v>84</v>
       </c>
       <c r="K295" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
       <c r="L295" t="s">
         <v>132</v>

</xml_diff>

<commit_message>
add user.decrpytUntrusted query criterion
</commit_message>
<xml_diff>
--- a/criterion_property_definitions.xlsx
+++ b/criterion_property_definitions.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1889" uniqueCount="443">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1894" uniqueCount="444">
   <si>
     <t>property</t>
   </si>
@@ -1346,6 +1346,9 @@
   </si>
   <si>
     <t>completeInputFieldSelectionSetValueValue</t>
+  </si>
+  <si>
+    <t>user.decryptUntrusted</t>
   </si>
 </sst>
 </file>
@@ -1678,10 +1681,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:L295"/>
+  <dimension ref="A1:L296"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A185" workbookViewId="0">
-      <selection activeCell="H201" sqref="H201"/>
+    <sheetView tabSelected="1" topLeftCell="A248" workbookViewId="0">
+      <selection activeCell="A270" sqref="A270"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="15.7109375" defaultRowHeight="16.5" customHeight="1"/>
@@ -7395,13 +7398,13 @@
         <v>125</v>
       </c>
       <c r="B270" t="s">
-        <v>293</v>
+        <v>443</v>
       </c>
       <c r="C270" t="s">
         <v>19</v>
       </c>
       <c r="K270" t="s">
-        <v>293</v>
+        <v>443</v>
       </c>
       <c r="L270" t="s">
         <v>132</v>
@@ -7412,25 +7415,13 @@
         <v>125</v>
       </c>
       <c r="B271" t="s">
-        <v>215</v>
+        <v>293</v>
       </c>
       <c r="C271" t="s">
-        <v>17</v>
-      </c>
-      <c r="D271" t="s">
-        <v>355</v>
-      </c>
-      <c r="E271" t="s">
-        <v>218</v>
-      </c>
-      <c r="F271" t="s">
-        <v>214</v>
-      </c>
-      <c r="G271" t="s">
-        <v>220</v>
+        <v>19</v>
       </c>
       <c r="K271" t="s">
-        <v>215</v>
+        <v>293</v>
       </c>
       <c r="L271" t="s">
         <v>132</v>
@@ -7441,13 +7432,25 @@
         <v>125</v>
       </c>
       <c r="B272" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="C272" t="s">
-        <v>19</v>
+        <v>17</v>
+      </c>
+      <c r="D272" t="s">
+        <v>355</v>
+      </c>
+      <c r="E272" t="s">
+        <v>218</v>
+      </c>
+      <c r="F272" t="s">
+        <v>214</v>
+      </c>
+      <c r="G272" t="s">
+        <v>220</v>
       </c>
       <c r="K272" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="L272" t="s">
         <v>132</v>
@@ -7458,16 +7461,16 @@
         <v>125</v>
       </c>
       <c r="B273" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="C273" t="s">
-        <v>56</v>
+        <v>19</v>
       </c>
       <c r="K273" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="L273" t="s">
-        <v>138</v>
+        <v>132</v>
       </c>
     </row>
     <row r="274" spans="1:12" ht="16.5" customHeight="1">
@@ -7478,25 +7481,13 @@
         <v>217</v>
       </c>
       <c r="C274" t="s">
-        <v>17</v>
-      </c>
-      <c r="D274" t="s">
-        <v>334</v>
-      </c>
-      <c r="E274" t="s">
-        <v>270</v>
-      </c>
-      <c r="F274" t="s">
-        <v>12</v>
-      </c>
-      <c r="G274" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
       <c r="K274" t="s">
-        <v>249</v>
-      </c>
-      <c r="L274" s="1" t="s">
-        <v>269</v>
+        <v>217</v>
+      </c>
+      <c r="L274" t="s">
+        <v>138</v>
       </c>
     </row>
     <row r="275" spans="1:12" ht="16.5" customHeight="1">
@@ -7504,19 +7495,28 @@
         <v>125</v>
       </c>
       <c r="B275" t="s">
-        <v>228</v>
+        <v>217</v>
       </c>
       <c r="C275" t="s">
-        <v>9</v>
-      </c>
-      <c r="J275" t="s">
-        <v>22</v>
+        <v>17</v>
+      </c>
+      <c r="D275" t="s">
+        <v>334</v>
+      </c>
+      <c r="E275" t="s">
+        <v>270</v>
+      </c>
+      <c r="F275" t="s">
+        <v>12</v>
+      </c>
+      <c r="G275" t="s">
+        <v>61</v>
       </c>
       <c r="K275" t="s">
-        <v>228</v>
-      </c>
-      <c r="L275" t="s">
-        <v>132</v>
+        <v>249</v>
+      </c>
+      <c r="L275" s="1" t="s">
+        <v>269</v>
       </c>
     </row>
     <row r="276" spans="1:12" ht="16.5" customHeight="1">
@@ -7524,25 +7524,16 @@
         <v>125</v>
       </c>
       <c r="B276" t="s">
-        <v>437</v>
+        <v>228</v>
       </c>
       <c r="C276" t="s">
         <v>9</v>
       </c>
-      <c r="D276" t="s">
-        <v>336</v>
-      </c>
-      <c r="E276" t="s">
-        <v>31</v>
-      </c>
-      <c r="F276" t="s">
-        <v>12</v>
-      </c>
-      <c r="G276" t="s">
-        <v>13</v>
+      <c r="J276" t="s">
+        <v>22</v>
       </c>
       <c r="K276" t="s">
-        <v>437</v>
+        <v>228</v>
       </c>
       <c r="L276" t="s">
         <v>132</v>
@@ -7553,25 +7544,25 @@
         <v>125</v>
       </c>
       <c r="B277" t="s">
-        <v>238</v>
+        <v>437</v>
       </c>
       <c r="C277" t="s">
-        <v>17</v>
+        <v>9</v>
       </c>
       <c r="D277" t="s">
-        <v>356</v>
+        <v>336</v>
       </c>
       <c r="E277" t="s">
-        <v>239</v>
+        <v>31</v>
       </c>
       <c r="F277" t="s">
         <v>12</v>
       </c>
       <c r="G277" t="s">
-        <v>240</v>
+        <v>13</v>
       </c>
       <c r="K277" t="s">
-        <v>238</v>
+        <v>437</v>
       </c>
       <c r="L277" t="s">
         <v>132</v>
@@ -7579,19 +7570,31 @@
     </row>
     <row r="278" spans="1:12" ht="16.5" customHeight="1">
       <c r="A278" t="s">
-        <v>411</v>
+        <v>125</v>
       </c>
       <c r="B278" t="s">
-        <v>412</v>
+        <v>238</v>
       </c>
       <c r="C278" t="s">
-        <v>9</v>
+        <v>17</v>
+      </c>
+      <c r="D278" t="s">
+        <v>356</v>
+      </c>
+      <c r="E278" t="s">
+        <v>239</v>
+      </c>
+      <c r="F278" t="s">
+        <v>12</v>
+      </c>
+      <c r="G278" t="s">
+        <v>240</v>
       </c>
       <c r="K278" t="s">
-        <v>412</v>
+        <v>238</v>
       </c>
       <c r="L278" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
     </row>
     <row r="279" spans="1:12" ht="16.5" customHeight="1">
@@ -7599,28 +7602,16 @@
         <v>411</v>
       </c>
       <c r="B279" t="s">
-        <v>429</v>
+        <v>412</v>
       </c>
       <c r="C279" t="s">
         <v>9</v>
       </c>
-      <c r="D279" t="s">
-        <v>331</v>
-      </c>
-      <c r="E279" t="s">
-        <v>11</v>
-      </c>
-      <c r="F279" t="s">
-        <v>12</v>
-      </c>
-      <c r="G279" t="s">
-        <v>13</v>
-      </c>
       <c r="K279" t="s">
-        <v>429</v>
+        <v>412</v>
       </c>
       <c r="L279" t="s">
-        <v>162</v>
+        <v>131</v>
       </c>
     </row>
     <row r="280" spans="1:12" ht="16.5" customHeight="1">
@@ -7628,16 +7619,28 @@
         <v>411</v>
       </c>
       <c r="B280" t="s">
-        <v>413</v>
+        <v>429</v>
       </c>
       <c r="C280" t="s">
-        <v>17</v>
+        <v>9</v>
+      </c>
+      <c r="D280" t="s">
+        <v>331</v>
+      </c>
+      <c r="E280" t="s">
+        <v>11</v>
+      </c>
+      <c r="F280" t="s">
+        <v>12</v>
+      </c>
+      <c r="G280" t="s">
+        <v>13</v>
       </c>
       <c r="K280" t="s">
-        <v>413</v>
+        <v>429</v>
       </c>
       <c r="L280" t="s">
-        <v>133</v>
+        <v>162</v>
       </c>
     </row>
     <row r="281" spans="1:12" ht="16.5" customHeight="1">
@@ -7645,16 +7648,16 @@
         <v>411</v>
       </c>
       <c r="B281" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
       <c r="C281" t="s">
-        <v>56</v>
+        <v>17</v>
       </c>
       <c r="K281" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
       <c r="L281" t="s">
-        <v>138</v>
+        <v>133</v>
       </c>
     </row>
     <row r="282" spans="1:12" ht="16.5" customHeight="1">
@@ -7665,25 +7668,13 @@
         <v>414</v>
       </c>
       <c r="C282" t="s">
-        <v>17</v>
-      </c>
-      <c r="D282" t="s">
-        <v>334</v>
-      </c>
-      <c r="E282" t="s">
-        <v>270</v>
-      </c>
-      <c r="F282" t="s">
-        <v>12</v>
-      </c>
-      <c r="G282" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
       <c r="K282" t="s">
-        <v>415</v>
-      </c>
-      <c r="L282" s="1" t="s">
-        <v>269</v>
+        <v>414</v>
+      </c>
+      <c r="L282" t="s">
+        <v>138</v>
       </c>
     </row>
     <row r="283" spans="1:12" ht="16.5" customHeight="1">
@@ -7691,28 +7682,28 @@
         <v>411</v>
       </c>
       <c r="B283" t="s">
-        <v>416</v>
+        <v>414</v>
       </c>
       <c r="C283" t="s">
-        <v>9</v>
+        <v>17</v>
       </c>
       <c r="D283" t="s">
-        <v>342</v>
+        <v>334</v>
       </c>
       <c r="E283" t="s">
-        <v>432</v>
+        <v>270</v>
       </c>
       <c r="F283" t="s">
         <v>12</v>
       </c>
       <c r="G283" t="s">
-        <v>13</v>
+        <v>61</v>
       </c>
       <c r="K283" t="s">
-        <v>416</v>
-      </c>
-      <c r="L283" t="s">
-        <v>132</v>
+        <v>415</v>
+      </c>
+      <c r="L283" s="1" t="s">
+        <v>269</v>
       </c>
     </row>
     <row r="284" spans="1:12" ht="16.5" customHeight="1">
@@ -7720,16 +7711,16 @@
         <v>411</v>
       </c>
       <c r="B284" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
       <c r="C284" t="s">
         <v>9</v>
       </c>
       <c r="D284" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="E284" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="F284" t="s">
         <v>12</v>
@@ -7738,7 +7729,7 @@
         <v>13</v>
       </c>
       <c r="K284" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
       <c r="L284" t="s">
         <v>132</v>
@@ -7749,16 +7740,25 @@
         <v>411</v>
       </c>
       <c r="B285" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
       <c r="C285" t="s">
         <v>9</v>
       </c>
-      <c r="J285" t="s">
-        <v>42</v>
+      <c r="D285" t="s">
+        <v>343</v>
+      </c>
+      <c r="E285" t="s">
+        <v>433</v>
+      </c>
+      <c r="F285" t="s">
+        <v>12</v>
+      </c>
+      <c r="G285" t="s">
+        <v>13</v>
       </c>
       <c r="K285" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
       <c r="L285" t="s">
         <v>132</v>
@@ -7769,22 +7769,16 @@
         <v>411</v>
       </c>
       <c r="B286" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="C286" t="s">
         <v>9</v>
       </c>
-      <c r="E286" t="s">
-        <v>124</v>
-      </c>
-      <c r="F286" t="s">
-        <v>12</v>
-      </c>
-      <c r="G286" t="s">
-        <v>13</v>
+      <c r="J286" t="s">
+        <v>42</v>
       </c>
       <c r="K286" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="L286" t="s">
         <v>132</v>
@@ -7795,16 +7789,25 @@
         <v>411</v>
       </c>
       <c r="B287" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
       <c r="C287" t="s">
-        <v>17</v>
+        <v>9</v>
+      </c>
+      <c r="E287" t="s">
+        <v>124</v>
+      </c>
+      <c r="F287" t="s">
+        <v>12</v>
+      </c>
+      <c r="G287" t="s">
+        <v>13</v>
       </c>
       <c r="K287" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
       <c r="L287" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
     </row>
     <row r="288" spans="1:12" ht="16.5" customHeight="1">
@@ -7812,13 +7815,13 @@
         <v>411</v>
       </c>
       <c r="B288" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="C288" t="s">
         <v>17</v>
       </c>
       <c r="K288" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="L288" t="s">
         <v>133</v>
@@ -7829,25 +7832,16 @@
         <v>411</v>
       </c>
       <c r="B289" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="C289" t="s">
         <v>17</v>
       </c>
-      <c r="E289" t="s">
-        <v>430</v>
-      </c>
-      <c r="F289" t="s">
-        <v>12</v>
-      </c>
-      <c r="G289" t="s">
-        <v>431</v>
-      </c>
       <c r="K289" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="L289" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
     </row>
     <row r="290" spans="1:12" ht="16.5" customHeight="1">
@@ -7855,16 +7849,25 @@
         <v>411</v>
       </c>
       <c r="B290" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
       <c r="C290" t="s">
         <v>17</v>
       </c>
+      <c r="E290" t="s">
+        <v>430</v>
+      </c>
+      <c r="F290" t="s">
+        <v>12</v>
+      </c>
+      <c r="G290" t="s">
+        <v>431</v>
+      </c>
       <c r="K290" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
       <c r="L290" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
     </row>
     <row r="291" spans="1:12" ht="16.5" customHeight="1">
@@ -7872,16 +7875,16 @@
         <v>411</v>
       </c>
       <c r="B291" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
       <c r="C291" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="K291" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
       <c r="L291" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
     </row>
     <row r="292" spans="1:12" ht="16.5" customHeight="1">
@@ -7889,13 +7892,13 @@
         <v>411</v>
       </c>
       <c r="B292" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
       <c r="C292" t="s">
         <v>19</v>
       </c>
       <c r="K292" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
       <c r="L292" t="s">
         <v>132</v>
@@ -7906,13 +7909,13 @@
         <v>411</v>
       </c>
       <c r="B293" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
       <c r="C293" t="s">
         <v>19</v>
       </c>
       <c r="K293" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
       <c r="L293" t="s">
         <v>132</v>
@@ -7923,16 +7926,16 @@
         <v>411</v>
       </c>
       <c r="B294" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
       <c r="C294" t="s">
-        <v>9</v>
+        <v>19</v>
       </c>
       <c r="K294" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
       <c r="L294" t="s">
-        <v>136</v>
+        <v>132</v>
       </c>
     </row>
     <row r="295" spans="1:12" ht="16.5" customHeight="1">
@@ -7940,18 +7943,35 @@
         <v>411</v>
       </c>
       <c r="B295" t="s">
+        <v>427</v>
+      </c>
+      <c r="C295" t="s">
+        <v>9</v>
+      </c>
+      <c r="K295" t="s">
+        <v>427</v>
+      </c>
+      <c r="L295" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="296" spans="1:12" ht="16.5" customHeight="1">
+      <c r="A296" t="s">
+        <v>411</v>
+      </c>
+      <c r="B296" t="s">
         <v>428</v>
       </c>
-      <c r="C295" t="s">
-        <v>9</v>
-      </c>
-      <c r="J295" t="s">
-        <v>84</v>
-      </c>
-      <c r="K295" t="s">
+      <c r="C296" t="s">
+        <v>9</v>
+      </c>
+      <c r="J296" t="s">
+        <v>84</v>
+      </c>
+      <c r="K296" t="s">
         <v>428</v>
       </c>
-      <c r="L295" t="s">
+      <c r="L296" t="s">
         <v>132</v>
       </c>
     </row>

</xml_diff>

<commit_message>
add search criterions for parent of a user
</commit_message>
<xml_diff>
--- a/criterion_property_definitions.xlsx
+++ b/criterion_property_definitions.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1763" uniqueCount="441">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1769" uniqueCount="442">
   <si>
     <t>property</t>
   </si>
@@ -1340,6 +1340,9 @@
   </si>
   <si>
     <t>getFilterVariablePeriods</t>
+  </si>
+  <si>
+    <t>user.parent.id</t>
   </si>
 </sst>
 </file>
@@ -1672,10 +1675,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:M296"/>
+  <dimension ref="A1:M297"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C244" workbookViewId="0">
-      <selection activeCell="J244" sqref="J244"/>
+    <sheetView tabSelected="1" topLeftCell="A261" workbookViewId="0">
+      <selection activeCell="A269" sqref="A269"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="15.7109375" defaultRowHeight="16.5" customHeight="1"/>
@@ -7033,16 +7036,19 @@
         <v>114</v>
       </c>
       <c r="B269" t="s">
-        <v>406</v>
+        <v>441</v>
       </c>
       <c r="C269" t="s">
-        <v>17</v>
+        <v>9</v>
+      </c>
+      <c r="K269" t="s">
+        <v>114</v>
       </c>
       <c r="L269" t="s">
-        <v>406</v>
+        <v>441</v>
       </c>
       <c r="M269" t="s">
-        <v>121</v>
+        <v>123</v>
       </c>
     </row>
     <row r="270" spans="1:13" ht="16.5" customHeight="1">
@@ -7050,13 +7056,13 @@
         <v>114</v>
       </c>
       <c r="B270" t="s">
-        <v>411</v>
+        <v>406</v>
       </c>
       <c r="C270" t="s">
         <v>17</v>
       </c>
       <c r="L270" t="s">
-        <v>411</v>
+        <v>406</v>
       </c>
       <c r="M270" t="s">
         <v>121</v>
@@ -7067,13 +7073,13 @@
         <v>114</v>
       </c>
       <c r="B271" t="s">
-        <v>268</v>
+        <v>411</v>
       </c>
       <c r="C271" t="s">
         <v>17</v>
       </c>
       <c r="L271" t="s">
-        <v>268</v>
+        <v>411</v>
       </c>
       <c r="M271" t="s">
         <v>121</v>
@@ -7084,25 +7090,13 @@
         <v>114</v>
       </c>
       <c r="B272" t="s">
-        <v>196</v>
+        <v>268</v>
       </c>
       <c r="C272" t="s">
-        <v>15</v>
-      </c>
-      <c r="D272" t="s">
-        <v>329</v>
-      </c>
-      <c r="E272" t="s">
-        <v>199</v>
-      </c>
-      <c r="F272" t="s">
-        <v>195</v>
-      </c>
-      <c r="G272" t="s">
-        <v>200</v>
+        <v>17</v>
       </c>
       <c r="L272" t="s">
-        <v>196</v>
+        <v>268</v>
       </c>
       <c r="M272" t="s">
         <v>121</v>
@@ -7113,13 +7107,25 @@
         <v>114</v>
       </c>
       <c r="B273" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="C273" t="s">
-        <v>17</v>
+        <v>15</v>
+      </c>
+      <c r="D273" t="s">
+        <v>329</v>
+      </c>
+      <c r="E273" t="s">
+        <v>199</v>
+      </c>
+      <c r="F273" t="s">
+        <v>195</v>
+      </c>
+      <c r="G273" t="s">
+        <v>200</v>
       </c>
       <c r="L273" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="M273" t="s">
         <v>121</v>
@@ -7130,16 +7136,16 @@
         <v>114</v>
       </c>
       <c r="B274" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="C274" t="s">
-        <v>52</v>
+        <v>17</v>
       </c>
       <c r="L274" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="M274" t="s">
-        <v>127</v>
+        <v>121</v>
       </c>
     </row>
     <row r="275" spans="1:13" ht="16.5" customHeight="1">
@@ -7150,19 +7156,13 @@
         <v>198</v>
       </c>
       <c r="C275" t="s">
-        <v>15</v>
-      </c>
-      <c r="D275" t="s">
-        <v>308</v>
-      </c>
-      <c r="J275" t="s">
-        <v>439</v>
+        <v>52</v>
       </c>
       <c r="L275" t="s">
-        <v>225</v>
-      </c>
-      <c r="M275" s="1" t="s">
-        <v>245</v>
+        <v>198</v>
+      </c>
+      <c r="M275" t="s">
+        <v>127</v>
       </c>
     </row>
     <row r="276" spans="1:13" ht="16.5" customHeight="1">
@@ -7170,19 +7170,22 @@
         <v>114</v>
       </c>
       <c r="B276" t="s">
-        <v>207</v>
+        <v>198</v>
       </c>
       <c r="C276" t="s">
-        <v>9</v>
-      </c>
-      <c r="K276" t="s">
-        <v>20</v>
+        <v>15</v>
+      </c>
+      <c r="D276" t="s">
+        <v>308</v>
+      </c>
+      <c r="J276" t="s">
+        <v>439</v>
       </c>
       <c r="L276" t="s">
-        <v>207</v>
-      </c>
-      <c r="M276" t="s">
-        <v>121</v>
+        <v>225</v>
+      </c>
+      <c r="M276" s="1" t="s">
+        <v>245</v>
       </c>
     </row>
     <row r="277" spans="1:13" ht="16.5" customHeight="1">
@@ -7190,19 +7193,16 @@
         <v>114</v>
       </c>
       <c r="B277" t="s">
-        <v>407</v>
+        <v>207</v>
       </c>
       <c r="C277" t="s">
         <v>9</v>
       </c>
-      <c r="D277" t="s">
-        <v>310</v>
-      </c>
-      <c r="J277" t="s">
-        <v>417</v>
+      <c r="K277" t="s">
+        <v>20</v>
       </c>
       <c r="L277" t="s">
-        <v>407</v>
+        <v>207</v>
       </c>
       <c r="M277" t="s">
         <v>121</v>
@@ -7213,19 +7213,19 @@
         <v>114</v>
       </c>
       <c r="B278" t="s">
-        <v>216</v>
+        <v>407</v>
       </c>
       <c r="C278" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
       <c r="D278" t="s">
-        <v>330</v>
+        <v>310</v>
       </c>
       <c r="J278" t="s">
-        <v>433</v>
+        <v>417</v>
       </c>
       <c r="L278" t="s">
-        <v>216</v>
+        <v>407</v>
       </c>
       <c r="M278" t="s">
         <v>121</v>
@@ -7233,19 +7233,25 @@
     </row>
     <row r="279" spans="1:13" ht="16.5" customHeight="1">
       <c r="A279" t="s">
-        <v>385</v>
+        <v>114</v>
       </c>
       <c r="B279" t="s">
-        <v>386</v>
+        <v>216</v>
       </c>
       <c r="C279" t="s">
-        <v>9</v>
+        <v>15</v>
+      </c>
+      <c r="D279" t="s">
+        <v>330</v>
+      </c>
+      <c r="J279" t="s">
+        <v>433</v>
       </c>
       <c r="L279" t="s">
-        <v>386</v>
+        <v>216</v>
       </c>
       <c r="M279" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
     </row>
     <row r="280" spans="1:13" ht="16.5" customHeight="1">
@@ -7253,22 +7259,16 @@
         <v>385</v>
       </c>
       <c r="B280" t="s">
-        <v>403</v>
+        <v>386</v>
       </c>
       <c r="C280" t="s">
         <v>9</v>
       </c>
-      <c r="D280" t="s">
-        <v>305</v>
-      </c>
-      <c r="J280" t="s">
-        <v>413</v>
-      </c>
       <c r="L280" t="s">
-        <v>403</v>
+        <v>386</v>
       </c>
       <c r="M280" t="s">
-        <v>149</v>
+        <v>120</v>
       </c>
     </row>
     <row r="281" spans="1:13" ht="16.5" customHeight="1">
@@ -7276,16 +7276,22 @@
         <v>385</v>
       </c>
       <c r="B281" t="s">
-        <v>387</v>
+        <v>403</v>
       </c>
       <c r="C281" t="s">
-        <v>15</v>
+        <v>9</v>
+      </c>
+      <c r="D281" t="s">
+        <v>305</v>
+      </c>
+      <c r="J281" t="s">
+        <v>413</v>
       </c>
       <c r="L281" t="s">
-        <v>387</v>
+        <v>403</v>
       </c>
       <c r="M281" t="s">
-        <v>122</v>
+        <v>149</v>
       </c>
     </row>
     <row r="282" spans="1:13" ht="16.5" customHeight="1">
@@ -7293,16 +7299,16 @@
         <v>385</v>
       </c>
       <c r="B282" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="C282" t="s">
-        <v>52</v>
+        <v>15</v>
       </c>
       <c r="L282" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="M282" t="s">
-        <v>127</v>
+        <v>122</v>
       </c>
     </row>
     <row r="283" spans="1:13" ht="16.5" customHeight="1">
@@ -7313,19 +7319,13 @@
         <v>388</v>
       </c>
       <c r="C283" t="s">
-        <v>15</v>
-      </c>
-      <c r="D283" t="s">
-        <v>308</v>
-      </c>
-      <c r="J283" t="s">
-        <v>439</v>
+        <v>52</v>
       </c>
       <c r="L283" t="s">
-        <v>389</v>
-      </c>
-      <c r="M283" s="1" t="s">
-        <v>245</v>
+        <v>388</v>
+      </c>
+      <c r="M283" t="s">
+        <v>127</v>
       </c>
     </row>
     <row r="284" spans="1:13" ht="16.5" customHeight="1">
@@ -7333,22 +7333,22 @@
         <v>385</v>
       </c>
       <c r="B284" t="s">
-        <v>390</v>
+        <v>388</v>
       </c>
       <c r="C284" t="s">
-        <v>9</v>
+        <v>15</v>
       </c>
       <c r="D284" t="s">
-        <v>436</v>
+        <v>308</v>
       </c>
       <c r="J284" t="s">
-        <v>434</v>
+        <v>439</v>
       </c>
       <c r="L284" t="s">
-        <v>390</v>
-      </c>
-      <c r="M284" t="s">
-        <v>121</v>
+        <v>389</v>
+      </c>
+      <c r="M284" s="1" t="s">
+        <v>245</v>
       </c>
     </row>
     <row r="285" spans="1:13" ht="16.5" customHeight="1">
@@ -7356,19 +7356,19 @@
         <v>385</v>
       </c>
       <c r="B285" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="C285" t="s">
         <v>9</v>
       </c>
       <c r="D285" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
       <c r="J285" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="L285" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="M285" t="s">
         <v>121</v>
@@ -7379,16 +7379,19 @@
         <v>385</v>
       </c>
       <c r="B286" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="C286" t="s">
         <v>9</v>
       </c>
-      <c r="K286" t="s">
-        <v>39</v>
+      <c r="D286" t="s">
+        <v>437</v>
+      </c>
+      <c r="J286" t="s">
+        <v>435</v>
       </c>
       <c r="L286" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="M286" t="s">
         <v>121</v>
@@ -7399,16 +7402,16 @@
         <v>385</v>
       </c>
       <c r="B287" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="C287" t="s">
         <v>9</v>
       </c>
-      <c r="J287" t="s">
-        <v>432</v>
+      <c r="K287" t="s">
+        <v>39</v>
       </c>
       <c r="L287" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="M287" t="s">
         <v>121</v>
@@ -7419,16 +7422,19 @@
         <v>385</v>
       </c>
       <c r="B288" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
       <c r="C288" t="s">
-        <v>15</v>
+        <v>9</v>
+      </c>
+      <c r="J288" t="s">
+        <v>432</v>
       </c>
       <c r="L288" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
       <c r="M288" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="289" spans="1:13" ht="16.5" customHeight="1">
@@ -7436,13 +7442,13 @@
         <v>385</v>
       </c>
       <c r="B289" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="C289" t="s">
         <v>15</v>
       </c>
       <c r="L289" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="M289" t="s">
         <v>122</v>
@@ -7453,19 +7459,16 @@
         <v>385</v>
       </c>
       <c r="B290" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="C290" t="s">
         <v>15</v>
       </c>
-      <c r="J290" t="s">
-        <v>438</v>
-      </c>
       <c r="L290" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="M290" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
     </row>
     <row r="291" spans="1:13" ht="16.5" customHeight="1">
@@ -7473,16 +7476,19 @@
         <v>385</v>
       </c>
       <c r="B291" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
       <c r="C291" t="s">
         <v>15</v>
       </c>
+      <c r="J291" t="s">
+        <v>438</v>
+      </c>
       <c r="L291" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
       <c r="M291" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="292" spans="1:13" ht="16.5" customHeight="1">
@@ -7490,16 +7496,16 @@
         <v>385</v>
       </c>
       <c r="B292" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
       <c r="C292" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="L292" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
       <c r="M292" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
     </row>
     <row r="293" spans="1:13" ht="16.5" customHeight="1">
@@ -7507,13 +7513,13 @@
         <v>385</v>
       </c>
       <c r="B293" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
       <c r="C293" t="s">
         <v>17</v>
       </c>
       <c r="L293" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
       <c r="M293" t="s">
         <v>121</v>
@@ -7524,13 +7530,13 @@
         <v>385</v>
       </c>
       <c r="B294" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="C294" t="s">
         <v>17</v>
       </c>
       <c r="L294" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="M294" t="s">
         <v>121</v>
@@ -7541,16 +7547,16 @@
         <v>385</v>
       </c>
       <c r="B295" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="C295" t="s">
-        <v>9</v>
+        <v>17</v>
       </c>
       <c r="L295" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="M295" t="s">
-        <v>125</v>
+        <v>121</v>
       </c>
     </row>
     <row r="296" spans="1:13" ht="16.5" customHeight="1">
@@ -7558,18 +7564,35 @@
         <v>385</v>
       </c>
       <c r="B296" t="s">
+        <v>401</v>
+      </c>
+      <c r="C296" t="s">
+        <v>9</v>
+      </c>
+      <c r="L296" t="s">
+        <v>401</v>
+      </c>
+      <c r="M296" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="297" spans="1:13" ht="16.5" customHeight="1">
+      <c r="A297" t="s">
+        <v>385</v>
+      </c>
+      <c r="B297" t="s">
         <v>402</v>
       </c>
-      <c r="C296" t="s">
-        <v>9</v>
-      </c>
-      <c r="K296" t="s">
-        <v>77</v>
-      </c>
-      <c r="L296" t="s">
+      <c r="C297" t="s">
+        <v>9</v>
+      </c>
+      <c r="K297" t="s">
+        <v>77</v>
+      </c>
+      <c r="L297" t="s">
         <v>402</v>
       </c>
-      <c r="M296" t="s">
+      <c r="M297" t="s">
         <v>121</v>
       </c>
     </row>

</xml_diff>

<commit_message>
search criteria for user.locked_untrusted
</commit_message>
<xml_diff>
--- a/criterion_property_definitions.xlsx
+++ b/criterion_property_definitions.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1787" uniqueCount="447">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1792" uniqueCount="448">
   <si>
     <t>property</t>
   </si>
@@ -1358,6 +1358,9 @@
   </si>
   <si>
     <t>trial.events.startByPeriod</t>
+  </si>
+  <si>
+    <t>user.lockedUntrusted</t>
   </si>
 </sst>
 </file>
@@ -1690,10 +1693,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:M300"/>
+  <dimension ref="A1:M301"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A77" workbookViewId="0">
-      <selection activeCell="A104" sqref="A104"/>
+    <sheetView tabSelected="1" topLeftCell="A262" workbookViewId="0">
+      <selection activeCell="A272" sqref="A272"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="15.7109375" defaultRowHeight="16.5" customHeight="1"/>
@@ -7111,19 +7114,16 @@
         <v>114</v>
       </c>
       <c r="B272" t="s">
-        <v>441</v>
+        <v>447</v>
       </c>
       <c r="C272" t="s">
-        <v>9</v>
-      </c>
-      <c r="K272" t="s">
-        <v>114</v>
+        <v>17</v>
       </c>
       <c r="L272" t="s">
-        <v>441</v>
+        <v>447</v>
       </c>
       <c r="M272" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
     </row>
     <row r="273" spans="1:13" ht="16.5" customHeight="1">
@@ -7131,16 +7131,19 @@
         <v>114</v>
       </c>
       <c r="B273" t="s">
-        <v>406</v>
+        <v>441</v>
       </c>
       <c r="C273" t="s">
-        <v>17</v>
+        <v>9</v>
+      </c>
+      <c r="K273" t="s">
+        <v>114</v>
       </c>
       <c r="L273" t="s">
-        <v>406</v>
+        <v>441</v>
       </c>
       <c r="M273" t="s">
-        <v>121</v>
+        <v>123</v>
       </c>
     </row>
     <row r="274" spans="1:13" ht="16.5" customHeight="1">
@@ -7148,13 +7151,13 @@
         <v>114</v>
       </c>
       <c r="B274" t="s">
-        <v>411</v>
+        <v>406</v>
       </c>
       <c r="C274" t="s">
         <v>17</v>
       </c>
       <c r="L274" t="s">
-        <v>411</v>
+        <v>406</v>
       </c>
       <c r="M274" t="s">
         <v>121</v>
@@ -7165,13 +7168,13 @@
         <v>114</v>
       </c>
       <c r="B275" t="s">
-        <v>268</v>
+        <v>411</v>
       </c>
       <c r="C275" t="s">
         <v>17</v>
       </c>
       <c r="L275" t="s">
-        <v>268</v>
+        <v>411</v>
       </c>
       <c r="M275" t="s">
         <v>121</v>
@@ -7182,25 +7185,13 @@
         <v>114</v>
       </c>
       <c r="B276" t="s">
-        <v>196</v>
+        <v>268</v>
       </c>
       <c r="C276" t="s">
-        <v>15</v>
-      </c>
-      <c r="D276" t="s">
-        <v>329</v>
-      </c>
-      <c r="E276" t="s">
-        <v>199</v>
-      </c>
-      <c r="F276" t="s">
-        <v>195</v>
-      </c>
-      <c r="G276" t="s">
-        <v>200</v>
+        <v>17</v>
       </c>
       <c r="L276" t="s">
-        <v>196</v>
+        <v>268</v>
       </c>
       <c r="M276" t="s">
         <v>121</v>
@@ -7211,13 +7202,25 @@
         <v>114</v>
       </c>
       <c r="B277" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="C277" t="s">
-        <v>17</v>
+        <v>15</v>
+      </c>
+      <c r="D277" t="s">
+        <v>329</v>
+      </c>
+      <c r="E277" t="s">
+        <v>199</v>
+      </c>
+      <c r="F277" t="s">
+        <v>195</v>
+      </c>
+      <c r="G277" t="s">
+        <v>200</v>
       </c>
       <c r="L277" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="M277" t="s">
         <v>121</v>
@@ -7228,16 +7231,16 @@
         <v>114</v>
       </c>
       <c r="B278" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="C278" t="s">
-        <v>52</v>
+        <v>17</v>
       </c>
       <c r="L278" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="M278" t="s">
-        <v>127</v>
+        <v>121</v>
       </c>
     </row>
     <row r="279" spans="1:13" ht="16.5" customHeight="1">
@@ -7248,19 +7251,13 @@
         <v>198</v>
       </c>
       <c r="C279" t="s">
-        <v>15</v>
-      </c>
-      <c r="D279" t="s">
-        <v>308</v>
-      </c>
-      <c r="J279" t="s">
-        <v>439</v>
+        <v>52</v>
       </c>
       <c r="L279" t="s">
-        <v>225</v>
-      </c>
-      <c r="M279" s="1" t="s">
-        <v>245</v>
+        <v>198</v>
+      </c>
+      <c r="M279" t="s">
+        <v>127</v>
       </c>
     </row>
     <row r="280" spans="1:13" ht="16.5" customHeight="1">
@@ -7268,19 +7265,22 @@
         <v>114</v>
       </c>
       <c r="B280" t="s">
-        <v>207</v>
+        <v>198</v>
       </c>
       <c r="C280" t="s">
-        <v>9</v>
-      </c>
-      <c r="K280" t="s">
-        <v>20</v>
+        <v>15</v>
+      </c>
+      <c r="D280" t="s">
+        <v>308</v>
+      </c>
+      <c r="J280" t="s">
+        <v>439</v>
       </c>
       <c r="L280" t="s">
-        <v>207</v>
-      </c>
-      <c r="M280" t="s">
-        <v>121</v>
+        <v>225</v>
+      </c>
+      <c r="M280" s="1" t="s">
+        <v>245</v>
       </c>
     </row>
     <row r="281" spans="1:13" ht="16.5" customHeight="1">
@@ -7288,19 +7288,16 @@
         <v>114</v>
       </c>
       <c r="B281" t="s">
-        <v>407</v>
+        <v>207</v>
       </c>
       <c r="C281" t="s">
         <v>9</v>
       </c>
-      <c r="D281" t="s">
-        <v>310</v>
-      </c>
-      <c r="J281" t="s">
-        <v>417</v>
+      <c r="K281" t="s">
+        <v>20</v>
       </c>
       <c r="L281" t="s">
-        <v>407</v>
+        <v>207</v>
       </c>
       <c r="M281" t="s">
         <v>121</v>
@@ -7311,19 +7308,19 @@
         <v>114</v>
       </c>
       <c r="B282" t="s">
-        <v>216</v>
+        <v>407</v>
       </c>
       <c r="C282" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
       <c r="D282" t="s">
-        <v>330</v>
+        <v>310</v>
       </c>
       <c r="J282" t="s">
-        <v>433</v>
+        <v>417</v>
       </c>
       <c r="L282" t="s">
-        <v>216</v>
+        <v>407</v>
       </c>
       <c r="M282" t="s">
         <v>121</v>
@@ -7331,19 +7328,25 @@
     </row>
     <row r="283" spans="1:13" ht="16.5" customHeight="1">
       <c r="A283" t="s">
-        <v>385</v>
+        <v>114</v>
       </c>
       <c r="B283" t="s">
-        <v>386</v>
+        <v>216</v>
       </c>
       <c r="C283" t="s">
-        <v>9</v>
+        <v>15</v>
+      </c>
+      <c r="D283" t="s">
+        <v>330</v>
+      </c>
+      <c r="J283" t="s">
+        <v>433</v>
       </c>
       <c r="L283" t="s">
-        <v>386</v>
+        <v>216</v>
       </c>
       <c r="M283" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
     </row>
     <row r="284" spans="1:13" ht="16.5" customHeight="1">
@@ -7351,22 +7354,16 @@
         <v>385</v>
       </c>
       <c r="B284" t="s">
-        <v>403</v>
+        <v>386</v>
       </c>
       <c r="C284" t="s">
         <v>9</v>
       </c>
-      <c r="D284" t="s">
-        <v>305</v>
-      </c>
-      <c r="J284" t="s">
-        <v>413</v>
-      </c>
       <c r="L284" t="s">
-        <v>403</v>
+        <v>386</v>
       </c>
       <c r="M284" t="s">
-        <v>149</v>
+        <v>120</v>
       </c>
     </row>
     <row r="285" spans="1:13" ht="16.5" customHeight="1">
@@ -7374,16 +7371,22 @@
         <v>385</v>
       </c>
       <c r="B285" t="s">
-        <v>387</v>
+        <v>403</v>
       </c>
       <c r="C285" t="s">
-        <v>15</v>
+        <v>9</v>
+      </c>
+      <c r="D285" t="s">
+        <v>305</v>
+      </c>
+      <c r="J285" t="s">
+        <v>413</v>
       </c>
       <c r="L285" t="s">
-        <v>387</v>
+        <v>403</v>
       </c>
       <c r="M285" t="s">
-        <v>122</v>
+        <v>149</v>
       </c>
     </row>
     <row r="286" spans="1:13" ht="16.5" customHeight="1">
@@ -7391,16 +7394,16 @@
         <v>385</v>
       </c>
       <c r="B286" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="C286" t="s">
-        <v>52</v>
+        <v>15</v>
       </c>
       <c r="L286" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="M286" t="s">
-        <v>127</v>
+        <v>122</v>
       </c>
     </row>
     <row r="287" spans="1:13" ht="16.5" customHeight="1">
@@ -7411,19 +7414,13 @@
         <v>388</v>
       </c>
       <c r="C287" t="s">
-        <v>15</v>
-      </c>
-      <c r="D287" t="s">
-        <v>308</v>
-      </c>
-      <c r="J287" t="s">
-        <v>439</v>
+        <v>52</v>
       </c>
       <c r="L287" t="s">
-        <v>389</v>
-      </c>
-      <c r="M287" s="1" t="s">
-        <v>245</v>
+        <v>388</v>
+      </c>
+      <c r="M287" t="s">
+        <v>127</v>
       </c>
     </row>
     <row r="288" spans="1:13" ht="16.5" customHeight="1">
@@ -7431,22 +7428,22 @@
         <v>385</v>
       </c>
       <c r="B288" t="s">
-        <v>390</v>
+        <v>388</v>
       </c>
       <c r="C288" t="s">
-        <v>9</v>
+        <v>15</v>
       </c>
       <c r="D288" t="s">
-        <v>436</v>
+        <v>308</v>
       </c>
       <c r="J288" t="s">
-        <v>434</v>
+        <v>439</v>
       </c>
       <c r="L288" t="s">
-        <v>390</v>
-      </c>
-      <c r="M288" t="s">
-        <v>121</v>
+        <v>389</v>
+      </c>
+      <c r="M288" s="1" t="s">
+        <v>245</v>
       </c>
     </row>
     <row r="289" spans="1:13" ht="16.5" customHeight="1">
@@ -7454,19 +7451,19 @@
         <v>385</v>
       </c>
       <c r="B289" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="C289" t="s">
         <v>9</v>
       </c>
       <c r="D289" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
       <c r="J289" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="L289" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="M289" t="s">
         <v>121</v>
@@ -7477,16 +7474,19 @@
         <v>385</v>
       </c>
       <c r="B290" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="C290" t="s">
         <v>9</v>
       </c>
-      <c r="K290" t="s">
-        <v>39</v>
+      <c r="D290" t="s">
+        <v>437</v>
+      </c>
+      <c r="J290" t="s">
+        <v>435</v>
       </c>
       <c r="L290" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="M290" t="s">
         <v>121</v>
@@ -7497,16 +7497,16 @@
         <v>385</v>
       </c>
       <c r="B291" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="C291" t="s">
         <v>9</v>
       </c>
-      <c r="J291" t="s">
-        <v>432</v>
+      <c r="K291" t="s">
+        <v>39</v>
       </c>
       <c r="L291" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="M291" t="s">
         <v>121</v>
@@ -7517,16 +7517,19 @@
         <v>385</v>
       </c>
       <c r="B292" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
       <c r="C292" t="s">
-        <v>15</v>
+        <v>9</v>
+      </c>
+      <c r="J292" t="s">
+        <v>432</v>
       </c>
       <c r="L292" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
       <c r="M292" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="293" spans="1:13" ht="16.5" customHeight="1">
@@ -7534,13 +7537,13 @@
         <v>385</v>
       </c>
       <c r="B293" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="C293" t="s">
         <v>15</v>
       </c>
       <c r="L293" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="M293" t="s">
         <v>122</v>
@@ -7551,19 +7554,16 @@
         <v>385</v>
       </c>
       <c r="B294" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="C294" t="s">
         <v>15</v>
       </c>
-      <c r="J294" t="s">
-        <v>438</v>
-      </c>
       <c r="L294" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="M294" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
     </row>
     <row r="295" spans="1:13" ht="16.5" customHeight="1">
@@ -7571,16 +7571,19 @@
         <v>385</v>
       </c>
       <c r="B295" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
       <c r="C295" t="s">
         <v>15</v>
       </c>
+      <c r="J295" t="s">
+        <v>438</v>
+      </c>
       <c r="L295" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
       <c r="M295" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="296" spans="1:13" ht="16.5" customHeight="1">
@@ -7588,16 +7591,16 @@
         <v>385</v>
       </c>
       <c r="B296" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
       <c r="C296" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="L296" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
       <c r="M296" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
     </row>
     <row r="297" spans="1:13" ht="16.5" customHeight="1">
@@ -7605,13 +7608,13 @@
         <v>385</v>
       </c>
       <c r="B297" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
       <c r="C297" t="s">
         <v>17</v>
       </c>
       <c r="L297" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
       <c r="M297" t="s">
         <v>121</v>
@@ -7622,13 +7625,13 @@
         <v>385</v>
       </c>
       <c r="B298" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="C298" t="s">
         <v>17</v>
       </c>
       <c r="L298" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="M298" t="s">
         <v>121</v>
@@ -7639,16 +7642,16 @@
         <v>385</v>
       </c>
       <c r="B299" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="C299" t="s">
-        <v>9</v>
+        <v>17</v>
       </c>
       <c r="L299" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="M299" t="s">
-        <v>125</v>
+        <v>121</v>
       </c>
     </row>
     <row r="300" spans="1:13" ht="16.5" customHeight="1">
@@ -7656,18 +7659,35 @@
         <v>385</v>
       </c>
       <c r="B300" t="s">
+        <v>401</v>
+      </c>
+      <c r="C300" t="s">
+        <v>9</v>
+      </c>
+      <c r="L300" t="s">
+        <v>401</v>
+      </c>
+      <c r="M300" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="301" spans="1:13" ht="16.5" customHeight="1">
+      <c r="A301" t="s">
+        <v>385</v>
+      </c>
+      <c r="B301" t="s">
         <v>402</v>
       </c>
-      <c r="C300" t="s">
-        <v>9</v>
-      </c>
-      <c r="K300" t="s">
-        <v>77</v>
-      </c>
-      <c r="L300" t="s">
+      <c r="C301" t="s">
+        <v>9</v>
+      </c>
+      <c r="K301" t="s">
+        <v>77</v>
+      </c>
+      <c r="L301" t="s">
         <v>402</v>
       </c>
-      <c r="M300" t="s">
+      <c r="M301" t="s">
         <v>121</v>
       </c>
     </row>

</xml_diff>

<commit_message>
switch department criterion from dropdown to autocomplete
</commit_message>
<xml_diff>
--- a/criterion_property_definitions.xlsx
+++ b/criterion_property_definitions.xlsx
@@ -1,10 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="24332"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\configuration\master-data\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{588537CF-6E7A-44D1-878B-534018E830B0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="75" windowWidth="28230" windowHeight="13425"/>
+    <workbookView xWindow="1560" yWindow="1560" windowWidth="26190" windowHeight="12510" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="criterion_property" sheetId="4" r:id="rId1"/>
@@ -17,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1792" uniqueCount="448">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1806" uniqueCount="449">
   <si>
     <t>property</t>
   </si>
@@ -1258,9 +1264,6 @@
     <t>jsf_converter</t>
   </si>
   <si>
-    <t>getFilterDepartments</t>
-  </si>
-  <si>
     <t>filter_items_getter_name</t>
   </si>
   <si>
@@ -1361,13 +1364,19 @@
   </si>
   <si>
     <t>user.lockedUntrusted</t>
+  </si>
+  <si>
+    <t>ctsms.Department</t>
+  </si>
+  <si>
+    <t>completeDepartment</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1405,13 +1414,21 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Larissa-Design">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office">
   <a:themeElements>
-    <a:clrScheme name="Larissa">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -1449,9 +1466,9 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Larissa">
+    <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1483,9 +1500,27 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1517,9 +1552,27 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Larissa">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -1692,14 +1745,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:M301"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A262" workbookViewId="0">
-      <selection activeCell="A272" sqref="A272"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="15.7109375" defaultRowHeight="16.5" customHeight="1"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="15.7109375" defaultRowHeight="16.5" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="15.5703125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="72.85546875" customWidth="1"/>
@@ -1713,7 +1766,7 @@
     <col min="12" max="12" width="57.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" ht="16.5" customHeight="1">
+    <row r="1" spans="1:13" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>119</v>
       </c>
@@ -1742,7 +1795,7 @@
         <v>412</v>
       </c>
       <c r="J1" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
       <c r="K1" t="s">
         <v>5</v>
@@ -1754,7 +1807,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="2" spans="1:13" ht="16.5" customHeight="1">
+    <row r="2" spans="1:13" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>7</v>
       </c>
@@ -1771,7 +1824,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="3" spans="1:13" ht="16.5" customHeight="1">
+    <row r="3" spans="1:13" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>7</v>
       </c>
@@ -1784,8 +1837,14 @@
       <c r="D3" t="s">
         <v>305</v>
       </c>
-      <c r="J3" t="s">
-        <v>413</v>
+      <c r="F3" t="s">
+        <v>11</v>
+      </c>
+      <c r="H3" t="s">
+        <v>448</v>
+      </c>
+      <c r="I3" t="s">
+        <v>447</v>
       </c>
       <c r="L3" t="s">
         <v>10</v>
@@ -1794,7 +1853,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="4" spans="1:13" ht="16.5" customHeight="1">
+    <row r="4" spans="1:13" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>7</v>
       </c>
@@ -1808,7 +1867,7 @@
         <v>306</v>
       </c>
       <c r="J4" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
       <c r="L4" t="s">
         <v>13</v>
@@ -1817,7 +1876,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="5" spans="1:13" ht="16.5" customHeight="1">
+    <row r="5" spans="1:13" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>7</v>
       </c>
@@ -1834,7 +1893,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="6" spans="1:13" ht="16.5" customHeight="1">
+    <row r="6" spans="1:13" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>7</v>
       </c>
@@ -1851,7 +1910,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="7" spans="1:13" ht="16.5" customHeight="1">
+    <row r="7" spans="1:13" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>7</v>
       </c>
@@ -1868,7 +1927,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="8" spans="1:13" ht="16.5" customHeight="1">
+    <row r="8" spans="1:13" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>7</v>
       </c>
@@ -1888,7 +1947,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="9" spans="1:13" ht="16.5" customHeight="1">
+    <row r="9" spans="1:13" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>7</v>
       </c>
@@ -1908,7 +1967,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="10" spans="1:13" ht="16.5" customHeight="1">
+    <row r="10" spans="1:13" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>7</v>
       </c>
@@ -1925,7 +1984,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="11" spans="1:13" ht="16.5" customHeight="1">
+    <row r="11" spans="1:13" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>7</v>
       </c>
@@ -1954,7 +2013,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="12" spans="1:13" ht="16.5" customHeight="1">
+    <row r="12" spans="1:13" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>7</v>
       </c>
@@ -1971,7 +2030,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="13" spans="1:13" ht="16.5" customHeight="1">
+    <row r="13" spans="1:13" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>7</v>
       </c>
@@ -1991,7 +2050,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="14" spans="1:13" ht="16.5" customHeight="1">
+    <row r="14" spans="1:13" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>7</v>
       </c>
@@ -2011,7 +2070,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="15" spans="1:13" ht="16.5" customHeight="1">
+    <row r="15" spans="1:13" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>7</v>
       </c>
@@ -2031,7 +2090,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="16" spans="1:13" ht="16.5" customHeight="1">
+    <row r="16" spans="1:13" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>7</v>
       </c>
@@ -2051,7 +2110,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="17" spans="1:13" ht="16.5" customHeight="1">
+    <row r="17" spans="1:13" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>7</v>
       </c>
@@ -2068,7 +2127,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="18" spans="1:13" ht="16.5" customHeight="1">
+    <row r="18" spans="1:13" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>7</v>
       </c>
@@ -2082,7 +2141,7 @@
         <v>308</v>
       </c>
       <c r="J18" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
       <c r="L18" t="s">
         <v>224</v>
@@ -2091,7 +2150,7 @@
         <v>245</v>
       </c>
     </row>
-    <row r="19" spans="1:13" ht="16.5" customHeight="1">
+    <row r="19" spans="1:13" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>7</v>
       </c>
@@ -2108,7 +2167,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="20" spans="1:13" ht="16.5" customHeight="1">
+    <row r="20" spans="1:13" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>7</v>
       </c>
@@ -2122,7 +2181,7 @@
         <v>308</v>
       </c>
       <c r="J20" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
       <c r="L20" t="s">
         <v>243</v>
@@ -2131,7 +2190,7 @@
         <v>245</v>
       </c>
     </row>
-    <row r="21" spans="1:13" ht="16.5" customHeight="1">
+    <row r="21" spans="1:13" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>7</v>
       </c>
@@ -2145,7 +2204,7 @@
         <v>309</v>
       </c>
       <c r="J21" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
       <c r="L21" t="s">
         <v>204</v>
@@ -2154,7 +2213,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="22" spans="1:13" ht="16.5" customHeight="1">
+    <row r="22" spans="1:13" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>7</v>
       </c>
@@ -2171,7 +2230,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="23" spans="1:13" ht="16.5" customHeight="1">
+    <row r="23" spans="1:13" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>20</v>
       </c>
@@ -2188,7 +2247,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="24" spans="1:13" ht="16.5" customHeight="1">
+    <row r="24" spans="1:13" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>20</v>
       </c>
@@ -2201,8 +2260,14 @@
       <c r="D24" t="s">
         <v>305</v>
       </c>
-      <c r="J24" t="s">
-        <v>413</v>
+      <c r="F24" t="s">
+        <v>11</v>
+      </c>
+      <c r="H24" t="s">
+        <v>448</v>
+      </c>
+      <c r="I24" t="s">
+        <v>447</v>
       </c>
       <c r="L24" t="s">
         <v>27</v>
@@ -2211,7 +2276,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="25" spans="1:13" ht="16.5" customHeight="1">
+    <row r="25" spans="1:13" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>20</v>
       </c>
@@ -2225,7 +2290,7 @@
         <v>310</v>
       </c>
       <c r="J25" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
       <c r="L25" t="s">
         <v>28</v>
@@ -2234,7 +2299,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="26" spans="1:13" ht="16.5" customHeight="1">
+    <row r="26" spans="1:13" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>20</v>
       </c>
@@ -2251,7 +2316,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="27" spans="1:13" ht="16.5" customHeight="1">
+    <row r="27" spans="1:13" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>20</v>
       </c>
@@ -2268,7 +2333,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="28" spans="1:13" ht="16.5" customHeight="1">
+    <row r="28" spans="1:13" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>20</v>
       </c>
@@ -2285,7 +2350,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="29" spans="1:13" ht="16.5" customHeight="1">
+    <row r="29" spans="1:13" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>20</v>
       </c>
@@ -2302,7 +2367,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="30" spans="1:13" ht="16.5" customHeight="1">
+    <row r="30" spans="1:13" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>20</v>
       </c>
@@ -2319,7 +2384,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="31" spans="1:13" ht="16.5" customHeight="1">
+    <row r="31" spans="1:13" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>20</v>
       </c>
@@ -2336,7 +2401,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="32" spans="1:13" ht="16.5" customHeight="1">
+    <row r="32" spans="1:13" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>20</v>
       </c>
@@ -2353,7 +2418,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="33" spans="1:13" ht="16.5" customHeight="1">
+    <row r="33" spans="1:13" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>20</v>
       </c>
@@ -2370,7 +2435,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="34" spans="1:13" ht="16.5" customHeight="1">
+    <row r="34" spans="1:13" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>20</v>
       </c>
@@ -2390,7 +2455,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="35" spans="1:13" ht="16.5" customHeight="1">
+    <row r="35" spans="1:13" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>20</v>
       </c>
@@ -2410,7 +2475,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="36" spans="1:13" ht="16.5" customHeight="1">
+    <row r="36" spans="1:13" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>20</v>
       </c>
@@ -2430,7 +2495,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="37" spans="1:13" ht="16.5" customHeight="1">
+    <row r="37" spans="1:13" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>20</v>
       </c>
@@ -2444,7 +2509,7 @@
         <v>311</v>
       </c>
       <c r="J37" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
       <c r="L37" t="s">
         <v>211</v>
@@ -2453,7 +2518,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="38" spans="1:13" ht="16.5" customHeight="1">
+    <row r="38" spans="1:13" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>20</v>
       </c>
@@ -2473,7 +2538,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="39" spans="1:13" ht="16.5" customHeight="1">
+    <row r="39" spans="1:13" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>20</v>
       </c>
@@ -2490,7 +2555,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="40" spans="1:13" ht="16.5" customHeight="1">
+    <row r="40" spans="1:13" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>20</v>
       </c>
@@ -2504,7 +2569,7 @@
         <v>308</v>
       </c>
       <c r="J40" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
       <c r="L40" t="s">
         <v>251</v>
@@ -2513,7 +2578,7 @@
         <v>244</v>
       </c>
     </row>
-    <row r="41" spans="1:13" ht="16.5" customHeight="1">
+    <row r="41" spans="1:13" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>20</v>
       </c>
@@ -2530,7 +2595,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="42" spans="1:13" ht="16.5" customHeight="1">
+    <row r="42" spans="1:13" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>20</v>
       </c>
@@ -2547,7 +2612,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="43" spans="1:13" ht="16.5" customHeight="1">
+    <row r="43" spans="1:13" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>20</v>
       </c>
@@ -2561,7 +2626,7 @@
         <v>312</v>
       </c>
       <c r="J43" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="L43" t="s">
         <v>146</v>
@@ -2570,7 +2635,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="44" spans="1:13" ht="16.5" customHeight="1">
+    <row r="44" spans="1:13" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>20</v>
       </c>
@@ -2587,7 +2652,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="45" spans="1:13" ht="16.5" customHeight="1">
+    <row r="45" spans="1:13" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>20</v>
       </c>
@@ -2616,7 +2681,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="46" spans="1:13" ht="16.5" customHeight="1">
+    <row r="46" spans="1:13" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>20</v>
       </c>
@@ -2633,7 +2698,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="47" spans="1:13" ht="16.5" customHeight="1">
+    <row r="47" spans="1:13" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>20</v>
       </c>
@@ -2650,7 +2715,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="48" spans="1:13" ht="16.5" customHeight="1">
+    <row r="48" spans="1:13" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>20</v>
       </c>
@@ -2664,7 +2729,7 @@
         <v>314</v>
       </c>
       <c r="J48" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="L48" t="s">
         <v>154</v>
@@ -2673,7 +2738,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="49" spans="1:13" ht="16.5" customHeight="1">
+    <row r="49" spans="1:13" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>20</v>
       </c>
@@ -2690,7 +2755,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="50" spans="1:13" ht="16.5" customHeight="1">
+    <row r="50" spans="1:13" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>20</v>
       </c>
@@ -2707,7 +2772,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="51" spans="1:13" ht="16.5" customHeight="1">
+    <row r="51" spans="1:13" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>20</v>
       </c>
@@ -2724,7 +2789,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="52" spans="1:13" ht="16.5" customHeight="1">
+    <row r="52" spans="1:13" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>20</v>
       </c>
@@ -2741,7 +2806,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="53" spans="1:13" ht="16.5" customHeight="1">
+    <row r="53" spans="1:13" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>20</v>
       </c>
@@ -2755,7 +2820,7 @@
         <v>308</v>
       </c>
       <c r="J53" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
       <c r="L53" t="s">
         <v>242</v>
@@ -2764,7 +2829,7 @@
         <v>245</v>
       </c>
     </row>
-    <row r="54" spans="1:13" ht="16.5" customHeight="1">
+    <row r="54" spans="1:13" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>20</v>
       </c>
@@ -2781,7 +2846,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="55" spans="1:13" ht="16.5" customHeight="1">
+    <row r="55" spans="1:13" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>20</v>
       </c>
@@ -2795,7 +2860,7 @@
         <v>308</v>
       </c>
       <c r="J55" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
       <c r="L55" t="s">
         <v>241</v>
@@ -2804,7 +2869,7 @@
         <v>245</v>
       </c>
     </row>
-    <row r="56" spans="1:13" ht="16.5" customHeight="1">
+    <row r="56" spans="1:13" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>20</v>
       </c>
@@ -2818,7 +2883,7 @@
         <v>315</v>
       </c>
       <c r="J56" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
       <c r="L56" t="s">
         <v>214</v>
@@ -2827,7 +2892,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="57" spans="1:13" ht="16.5" customHeight="1">
+    <row r="57" spans="1:13" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>20</v>
       </c>
@@ -2844,7 +2909,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="58" spans="1:13" ht="16.5" customHeight="1">
+    <row r="58" spans="1:13" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
         <v>20</v>
       </c>
@@ -2864,7 +2929,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="59" spans="1:13" ht="16.5" customHeight="1">
+    <row r="59" spans="1:13" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
         <v>20</v>
       </c>
@@ -2881,7 +2946,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="60" spans="1:13" ht="16.5" customHeight="1">
+    <row r="60" spans="1:13" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
         <v>20</v>
       </c>
@@ -2895,7 +2960,7 @@
         <v>308</v>
       </c>
       <c r="J60" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
       <c r="L60" t="s">
         <v>256</v>
@@ -2904,7 +2969,7 @@
         <v>245</v>
       </c>
     </row>
-    <row r="61" spans="1:13" ht="16.5" customHeight="1">
+    <row r="61" spans="1:13" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
         <v>20</v>
       </c>
@@ -2921,7 +2986,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="62" spans="1:13" ht="16.5" customHeight="1">
+    <row r="62" spans="1:13" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
         <v>20</v>
       </c>
@@ -2935,7 +3000,7 @@
         <v>308</v>
       </c>
       <c r="J62" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
       <c r="L62" t="s">
         <v>257</v>
@@ -2944,7 +3009,7 @@
         <v>245</v>
       </c>
     </row>
-    <row r="63" spans="1:13" ht="16.5" customHeight="1">
+    <row r="63" spans="1:13" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
         <v>41</v>
       </c>
@@ -2961,7 +3026,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="64" spans="1:13" ht="16.5" customHeight="1">
+    <row r="64" spans="1:13" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
         <v>41</v>
       </c>
@@ -2974,8 +3039,14 @@
       <c r="D64" t="s">
         <v>305</v>
       </c>
-      <c r="J64" t="s">
-        <v>413</v>
+      <c r="F64" t="s">
+        <v>11</v>
+      </c>
+      <c r="H64" t="s">
+        <v>448</v>
+      </c>
+      <c r="I64" t="s">
+        <v>447</v>
       </c>
       <c r="L64" t="s">
         <v>47</v>
@@ -2984,7 +3055,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="65" spans="1:13" ht="16.5" customHeight="1">
+    <row r="65" spans="1:13" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
         <v>41</v>
       </c>
@@ -2998,7 +3069,7 @@
         <v>311</v>
       </c>
       <c r="J65" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
       <c r="L65" t="s">
         <v>48</v>
@@ -3007,7 +3078,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="66" spans="1:13" ht="16.5" customHeight="1">
+    <row r="66" spans="1:13" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
         <v>41</v>
       </c>
@@ -3027,7 +3098,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="67" spans="1:13" ht="16.5" customHeight="1">
+    <row r="67" spans="1:13" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
         <v>41</v>
       </c>
@@ -3044,7 +3115,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="68" spans="1:13" ht="16.5" customHeight="1">
+    <row r="68" spans="1:13" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
         <v>41</v>
       </c>
@@ -3061,7 +3132,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="69" spans="1:13" ht="16.5" customHeight="1">
+    <row r="69" spans="1:13" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
         <v>41</v>
       </c>
@@ -3075,7 +3146,7 @@
         <v>308</v>
       </c>
       <c r="J69" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
       <c r="L69" t="s">
         <v>222</v>
@@ -3084,7 +3155,7 @@
         <v>244</v>
       </c>
     </row>
-    <row r="70" spans="1:13" ht="16.5" customHeight="1">
+    <row r="70" spans="1:13" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
         <v>41</v>
       </c>
@@ -3101,7 +3172,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="71" spans="1:13" ht="16.5" customHeight="1">
+    <row r="71" spans="1:13" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
         <v>41</v>
       </c>
@@ -3115,7 +3186,7 @@
         <v>308</v>
       </c>
       <c r="J71" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
       <c r="L71" t="s">
         <v>240</v>
@@ -3124,7 +3195,7 @@
         <v>245</v>
       </c>
     </row>
-    <row r="72" spans="1:13" ht="16.5" customHeight="1">
+    <row r="72" spans="1:13" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
         <v>41</v>
       </c>
@@ -3141,7 +3212,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="73" spans="1:13" ht="16.5" customHeight="1">
+    <row r="73" spans="1:13" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
         <v>41</v>
       </c>
@@ -3158,7 +3229,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="74" spans="1:13" ht="16.5" customHeight="1">
+    <row r="74" spans="1:13" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
         <v>41</v>
       </c>
@@ -3172,7 +3243,7 @@
         <v>308</v>
       </c>
       <c r="J74" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
       <c r="L74" t="s">
         <v>55</v>
@@ -3181,7 +3252,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="75" spans="1:13" ht="16.5" customHeight="1">
+    <row r="75" spans="1:13" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
         <v>41</v>
       </c>
@@ -3198,7 +3269,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="76" spans="1:13" ht="16.5" customHeight="1">
+    <row r="76" spans="1:13" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
         <v>41</v>
       </c>
@@ -3218,7 +3289,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="77" spans="1:13" ht="16.5" customHeight="1">
+    <row r="77" spans="1:13" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
         <v>41</v>
       </c>
@@ -3235,7 +3306,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="78" spans="1:13" ht="16.5" customHeight="1">
+    <row r="78" spans="1:13" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
         <v>41</v>
       </c>
@@ -3252,7 +3323,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="79" spans="1:13" ht="16.5" customHeight="1">
+    <row r="79" spans="1:13" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
         <v>41</v>
       </c>
@@ -3272,7 +3343,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="80" spans="1:13" ht="16.5" customHeight="1">
+    <row r="80" spans="1:13" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
         <v>41</v>
       </c>
@@ -3289,7 +3360,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="81" spans="1:13" ht="16.5" customHeight="1">
+    <row r="81" spans="1:13" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
         <v>41</v>
       </c>
@@ -3309,7 +3380,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="82" spans="1:13" ht="16.5" customHeight="1">
+    <row r="82" spans="1:13" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
         <v>41</v>
       </c>
@@ -3326,7 +3397,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="83" spans="1:13" ht="16.5" customHeight="1">
+    <row r="83" spans="1:13" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
         <v>39</v>
       </c>
@@ -3343,7 +3414,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="84" spans="1:13" ht="16.5" customHeight="1">
+    <row r="84" spans="1:13" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
         <v>39</v>
       </c>
@@ -3356,8 +3427,14 @@
       <c r="D84" t="s">
         <v>305</v>
       </c>
-      <c r="J84" t="s">
-        <v>413</v>
+      <c r="F84" t="s">
+        <v>11</v>
+      </c>
+      <c r="H84" t="s">
+        <v>448</v>
+      </c>
+      <c r="I84" t="s">
+        <v>447</v>
       </c>
       <c r="L84" t="s">
         <v>61</v>
@@ -3366,7 +3443,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="85" spans="1:13" ht="16.5" customHeight="1">
+    <row r="85" spans="1:13" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
         <v>39</v>
       </c>
@@ -3383,7 +3460,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="86" spans="1:13" ht="16.5" customHeight="1">
+    <row r="86" spans="1:13" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
         <v>39</v>
       </c>
@@ -3397,7 +3474,7 @@
         <v>316</v>
       </c>
       <c r="J86" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="L86" t="s">
         <v>63</v>
@@ -3406,7 +3483,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="87" spans="1:13" ht="16.5" customHeight="1">
+    <row r="87" spans="1:13" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
         <v>39</v>
       </c>
@@ -3420,7 +3497,7 @@
         <v>317</v>
       </c>
       <c r="J87" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="L87" t="s">
         <v>174</v>
@@ -3429,7 +3506,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="88" spans="1:13" ht="16.5" customHeight="1">
+    <row r="88" spans="1:13" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
         <v>39</v>
       </c>
@@ -3443,7 +3520,7 @@
         <v>318</v>
       </c>
       <c r="J88" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
       <c r="L88" t="s">
         <v>175</v>
@@ -3452,7 +3529,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="89" spans="1:13" ht="16.5" customHeight="1">
+    <row r="89" spans="1:13" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
         <v>39</v>
       </c>
@@ -3469,7 +3546,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="90" spans="1:13" ht="16.5" customHeight="1">
+    <row r="90" spans="1:13" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
         <v>39</v>
       </c>
@@ -3486,7 +3563,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="91" spans="1:13" ht="16.5" customHeight="1">
+    <row r="91" spans="1:13" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
         <v>39</v>
       </c>
@@ -3500,7 +3577,7 @@
         <v>308</v>
       </c>
       <c r="J91" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
       <c r="L91" t="s">
         <v>239</v>
@@ -3509,7 +3586,7 @@
         <v>245</v>
       </c>
     </row>
-    <row r="92" spans="1:13" ht="16.5" customHeight="1">
+    <row r="92" spans="1:13" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
         <v>39</v>
       </c>
@@ -3526,7 +3603,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="93" spans="1:13" ht="16.5" customHeight="1">
+    <row r="93" spans="1:13" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
         <v>39</v>
       </c>
@@ -3540,7 +3617,7 @@
         <v>308</v>
       </c>
       <c r="J93" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
       <c r="L93" t="s">
         <v>238</v>
@@ -3549,7 +3626,7 @@
         <v>245</v>
       </c>
     </row>
-    <row r="94" spans="1:13" ht="16.5" customHeight="1">
+    <row r="94" spans="1:13" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
         <v>39</v>
       </c>
@@ -3563,7 +3640,7 @@
         <v>409</v>
       </c>
       <c r="J94" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
       <c r="L94" t="s">
         <v>408</v>
@@ -3572,7 +3649,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="95" spans="1:13" ht="16.5" customHeight="1">
+    <row r="95" spans="1:13" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
         <v>39</v>
       </c>
@@ -3589,7 +3666,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="96" spans="1:13" ht="16.5" customHeight="1">
+    <row r="96" spans="1:13" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
         <v>39</v>
       </c>
@@ -3606,7 +3683,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="97" spans="1:13" ht="16.5" customHeight="1">
+    <row r="97" spans="1:13" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
         <v>39</v>
       </c>
@@ -3623,7 +3700,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="98" spans="1:13" ht="16.5" customHeight="1">
+    <row r="98" spans="1:13" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
         <v>39</v>
       </c>
@@ -3640,7 +3717,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="99" spans="1:13" ht="16.5" customHeight="1">
+    <row r="99" spans="1:13" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
         <v>39</v>
       </c>
@@ -3654,7 +3731,7 @@
         <v>319</v>
       </c>
       <c r="J99" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
       <c r="L99" t="s">
         <v>176</v>
@@ -3663,7 +3740,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="100" spans="1:13" ht="16.5" customHeight="1">
+    <row r="100" spans="1:13" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
         <v>39</v>
       </c>
@@ -3683,7 +3760,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="101" spans="1:13" ht="16.5" customHeight="1">
+    <row r="101" spans="1:13" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
         <v>39</v>
       </c>
@@ -3697,7 +3774,7 @@
         <v>320</v>
       </c>
       <c r="J101" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
       <c r="L101" t="s">
         <v>183</v>
@@ -3706,7 +3783,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="102" spans="1:13" ht="16.5" customHeight="1">
+    <row r="102" spans="1:13" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
         <v>39</v>
       </c>
@@ -3723,49 +3800,49 @@
         <v>125</v>
       </c>
     </row>
-    <row r="103" spans="1:13" ht="16.5" customHeight="1">
+    <row r="103" spans="1:13" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
         <v>39</v>
       </c>
       <c r="B103" t="s">
+        <v>442</v>
+      </c>
+      <c r="C103" t="s">
+        <v>9</v>
+      </c>
+      <c r="J103" t="s">
         <v>443</v>
       </c>
-      <c r="C103" t="s">
-        <v>9</v>
-      </c>
-      <c r="J103" t="s">
+      <c r="L103" t="s">
         <v>444</v>
       </c>
-      <c r="L103" t="s">
-        <v>445</v>
-      </c>
       <c r="M103" t="s">
         <v>121</v>
       </c>
     </row>
-    <row r="104" spans="1:13" ht="16.5" customHeight="1">
+    <row r="104" spans="1:13" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
         <v>39</v>
       </c>
       <c r="B104" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="C104" t="s">
         <v>52</v>
       </c>
       <c r="L104" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="M104" t="s">
         <v>246</v>
       </c>
     </row>
-    <row r="105" spans="1:13" ht="16.5" customHeight="1">
+    <row r="105" spans="1:13" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
         <v>39</v>
       </c>
       <c r="B105" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="C105" t="s">
         <v>15</v>
@@ -3774,16 +3851,16 @@
         <v>308</v>
       </c>
       <c r="J105" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
       <c r="L105" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
       <c r="M105" s="1" t="s">
         <v>245</v>
       </c>
     </row>
-    <row r="106" spans="1:13" ht="16.5" customHeight="1">
+    <row r="106" spans="1:13" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
         <v>39</v>
       </c>
@@ -3803,7 +3880,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="107" spans="1:13" ht="16.5" customHeight="1">
+    <row r="107" spans="1:13" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
         <v>39</v>
       </c>
@@ -3820,7 +3897,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="108" spans="1:13" ht="16.5" customHeight="1">
+    <row r="108" spans="1:13" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
         <v>39</v>
       </c>
@@ -3837,7 +3914,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="109" spans="1:13" ht="16.5" customHeight="1">
+    <row r="109" spans="1:13" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
         <v>39</v>
       </c>
@@ -3866,7 +3943,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="110" spans="1:13" ht="16.5" customHeight="1">
+    <row r="110" spans="1:13" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A110" t="s">
         <v>39</v>
       </c>
@@ -3883,7 +3960,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="111" spans="1:13" ht="16.5" customHeight="1">
+    <row r="111" spans="1:13" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A111" t="s">
         <v>39</v>
       </c>
@@ -3900,7 +3977,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="112" spans="1:13" ht="16.5" customHeight="1">
+    <row r="112" spans="1:13" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A112" t="s">
         <v>39</v>
       </c>
@@ -3917,7 +3994,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="113" spans="1:13" ht="16.5" customHeight="1">
+    <row r="113" spans="1:13" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A113" t="s">
         <v>71</v>
       </c>
@@ -3934,7 +4011,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="114" spans="1:13" ht="16.5" customHeight="1">
+    <row r="114" spans="1:13" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A114" t="s">
         <v>71</v>
       </c>
@@ -3951,7 +4028,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="115" spans="1:13" ht="16.5" customHeight="1">
+    <row r="115" spans="1:13" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A115" t="s">
         <v>71</v>
       </c>
@@ -3968,7 +4045,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="116" spans="1:13" ht="16.5" customHeight="1">
+    <row r="116" spans="1:13" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A116" t="s">
         <v>71</v>
       </c>
@@ -3985,7 +4062,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="117" spans="1:13" ht="16.5" customHeight="1">
+    <row r="117" spans="1:13" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A117" t="s">
         <v>71</v>
       </c>
@@ -4002,7 +4079,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="118" spans="1:13" ht="16.5" customHeight="1">
+    <row r="118" spans="1:13" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A118" t="s">
         <v>292</v>
       </c>
@@ -4019,7 +4096,7 @@
         <v>283</v>
       </c>
     </row>
-    <row r="119" spans="1:13" ht="16.5" customHeight="1">
+    <row r="119" spans="1:13" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A119" t="s">
         <v>292</v>
       </c>
@@ -4036,7 +4113,7 @@
         <v>286</v>
       </c>
     </row>
-    <row r="120" spans="1:13" ht="16.5" customHeight="1">
+    <row r="120" spans="1:13" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A120" t="s">
         <v>71</v>
       </c>
@@ -4056,7 +4133,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="121" spans="1:13" ht="16.5" customHeight="1">
+    <row r="121" spans="1:13" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A121" t="s">
         <v>71</v>
       </c>
@@ -4076,7 +4153,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="122" spans="1:13" ht="16.5" customHeight="1">
+    <row r="122" spans="1:13" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A122" t="s">
         <v>71</v>
       </c>
@@ -4096,7 +4173,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="123" spans="1:13" ht="16.5" customHeight="1">
+    <row r="123" spans="1:13" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A123" t="s">
         <v>71</v>
       </c>
@@ -4113,7 +4190,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="124" spans="1:13" ht="16.5" customHeight="1">
+    <row r="124" spans="1:13" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A124" t="s">
         <v>71</v>
       </c>
@@ -4130,7 +4207,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="125" spans="1:13" ht="16.5" customHeight="1">
+    <row r="125" spans="1:13" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A125" t="s">
         <v>71</v>
       </c>
@@ -4150,7 +4227,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="126" spans="1:13" ht="16.5" customHeight="1">
+    <row r="126" spans="1:13" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A126" t="s">
         <v>71</v>
       </c>
@@ -4164,7 +4241,7 @@
         <v>331</v>
       </c>
       <c r="J126" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
       <c r="L126" t="s">
         <v>201</v>
@@ -4173,7 +4250,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="127" spans="1:13" ht="16.5" customHeight="1">
+    <row r="127" spans="1:13" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A127" t="s">
         <v>71</v>
       </c>
@@ -4190,7 +4267,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="128" spans="1:13" ht="16.5" customHeight="1">
+    <row r="128" spans="1:13" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A128" t="s">
         <v>71</v>
       </c>
@@ -4207,7 +4284,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="129" spans="1:13" ht="16.5" customHeight="1">
+    <row r="129" spans="1:13" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A129" t="s">
         <v>77</v>
       </c>
@@ -4224,7 +4301,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="130" spans="1:13" ht="16.5" customHeight="1">
+    <row r="130" spans="1:13" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A130" t="s">
         <v>77</v>
       </c>
@@ -4237,8 +4314,14 @@
       <c r="D130" t="s">
         <v>305</v>
       </c>
-      <c r="J130" t="s">
-        <v>413</v>
+      <c r="F130" t="s">
+        <v>11</v>
+      </c>
+      <c r="H130" t="s">
+        <v>448</v>
+      </c>
+      <c r="I130" t="s">
+        <v>447</v>
       </c>
       <c r="L130" t="s">
         <v>79</v>
@@ -4247,7 +4330,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="131" spans="1:13" ht="16.5" customHeight="1">
+    <row r="131" spans="1:13" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A131" t="s">
         <v>77</v>
       </c>
@@ -4261,7 +4344,7 @@
         <v>322</v>
       </c>
       <c r="J131" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
       <c r="L131" t="s">
         <v>80</v>
@@ -4270,7 +4353,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="132" spans="1:13" ht="16.5" customHeight="1">
+    <row r="132" spans="1:13" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A132" t="s">
         <v>77</v>
       </c>
@@ -4287,7 +4370,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="133" spans="1:13" ht="16.5" customHeight="1">
+    <row r="133" spans="1:13" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A133" t="s">
         <v>77</v>
       </c>
@@ -4304,7 +4387,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="134" spans="1:13" ht="16.5" customHeight="1">
+    <row r="134" spans="1:13" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A134" t="s">
         <v>77</v>
       </c>
@@ -4321,7 +4404,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="135" spans="1:13" ht="16.5" customHeight="1">
+    <row r="135" spans="1:13" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A135" t="s">
         <v>77</v>
       </c>
@@ -4338,7 +4421,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="136" spans="1:13" ht="16.5" customHeight="1">
+    <row r="136" spans="1:13" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A136" t="s">
         <v>77</v>
       </c>
@@ -4355,7 +4438,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="137" spans="1:13" ht="16.5" customHeight="1">
+    <row r="137" spans="1:13" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A137" t="s">
         <v>77</v>
       </c>
@@ -4369,7 +4452,7 @@
         <v>323</v>
       </c>
       <c r="J137" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
       <c r="L137" t="s">
         <v>367</v>
@@ -4378,7 +4461,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="138" spans="1:13" ht="16.5" customHeight="1">
+    <row r="138" spans="1:13" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A138" t="s">
         <v>77</v>
       </c>
@@ -4395,7 +4478,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="139" spans="1:13" ht="16.5" customHeight="1">
+    <row r="139" spans="1:13" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A139" t="s">
         <v>77</v>
       </c>
@@ -4412,7 +4495,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="140" spans="1:13" ht="16.5" customHeight="1">
+    <row r="140" spans="1:13" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A140" t="s">
         <v>77</v>
       </c>
@@ -4429,7 +4512,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="141" spans="1:13" ht="16.5" customHeight="1">
+    <row r="141" spans="1:13" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A141" t="s">
         <v>77</v>
       </c>
@@ -4443,7 +4526,7 @@
         <v>323</v>
       </c>
       <c r="J141" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
       <c r="L141" t="s">
         <v>369</v>
@@ -4452,7 +4535,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="142" spans="1:13" ht="16.5" customHeight="1">
+    <row r="142" spans="1:13" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A142" t="s">
         <v>77</v>
       </c>
@@ -4469,7 +4552,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="143" spans="1:13" ht="16.5" customHeight="1">
+    <row r="143" spans="1:13" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A143" t="s">
         <v>180</v>
       </c>
@@ -4486,7 +4569,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="144" spans="1:13" ht="16.5" customHeight="1">
+    <row r="144" spans="1:13" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A144" t="s">
         <v>77</v>
       </c>
@@ -4503,7 +4586,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="145" spans="1:13" ht="16.5" customHeight="1">
+    <row r="145" spans="1:13" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A145" t="s">
         <v>77</v>
       </c>
@@ -4520,7 +4603,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="146" spans="1:13" ht="16.5" customHeight="1">
+    <row r="146" spans="1:13" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A146" t="s">
         <v>77</v>
       </c>
@@ -4540,7 +4623,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="147" spans="1:13" ht="16.5" customHeight="1">
+    <row r="147" spans="1:13" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A147" t="s">
         <v>77</v>
       </c>
@@ -4557,7 +4640,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="148" spans="1:13" ht="16.5" customHeight="1">
+    <row r="148" spans="1:13" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A148" t="s">
         <v>77</v>
       </c>
@@ -4574,7 +4657,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="149" spans="1:13" ht="16.5" customHeight="1">
+    <row r="149" spans="1:13" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A149" t="s">
         <v>180</v>
       </c>
@@ -4591,7 +4674,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="150" spans="1:13" ht="16.5" customHeight="1">
+    <row r="150" spans="1:13" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A150" t="s">
         <v>77</v>
       </c>
@@ -4605,7 +4688,7 @@
         <v>332</v>
       </c>
       <c r="J150" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
       <c r="L150" t="s">
         <v>140</v>
@@ -4614,7 +4697,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="151" spans="1:13" ht="16.5" customHeight="1">
+    <row r="151" spans="1:13" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A151" t="s">
         <v>77</v>
       </c>
@@ -4631,7 +4714,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="152" spans="1:13" ht="16.5" customHeight="1">
+    <row r="152" spans="1:13" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A152" t="s">
         <v>77</v>
       </c>
@@ -4648,7 +4731,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="153" spans="1:13" ht="16.5" customHeight="1">
+    <row r="153" spans="1:13" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A153" t="s">
         <v>77</v>
       </c>
@@ -4662,7 +4745,7 @@
         <v>308</v>
       </c>
       <c r="J153" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
       <c r="L153" t="s">
         <v>237</v>
@@ -4671,7 +4754,7 @@
         <v>244</v>
       </c>
     </row>
-    <row r="154" spans="1:13" ht="16.5" customHeight="1">
+    <row r="154" spans="1:13" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A154" t="s">
         <v>77</v>
       </c>
@@ -4691,7 +4774,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="155" spans="1:13" ht="16.5" customHeight="1">
+    <row r="155" spans="1:13" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A155" t="s">
         <v>77</v>
       </c>
@@ -4711,7 +4794,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="156" spans="1:13" ht="16.5" customHeight="1">
+    <row r="156" spans="1:13" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A156" t="s">
         <v>77</v>
       </c>
@@ -4731,7 +4814,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="157" spans="1:13" ht="16.5" customHeight="1">
+    <row r="157" spans="1:13" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A157" t="s">
         <v>77</v>
       </c>
@@ -4751,7 +4834,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="158" spans="1:13" ht="16.5" customHeight="1">
+    <row r="158" spans="1:13" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A158" t="s">
         <v>77</v>
       </c>
@@ -4768,7 +4851,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="159" spans="1:13" ht="16.5" customHeight="1">
+    <row r="159" spans="1:13" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A159" t="s">
         <v>77</v>
       </c>
@@ -4782,7 +4865,7 @@
         <v>308</v>
       </c>
       <c r="J159" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
       <c r="L159" t="s">
         <v>236</v>
@@ -4791,7 +4874,7 @@
         <v>244</v>
       </c>
     </row>
-    <row r="160" spans="1:13" ht="16.5" customHeight="1">
+    <row r="160" spans="1:13" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A160" t="s">
         <v>77</v>
       </c>
@@ -4808,7 +4891,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="161" spans="1:13" ht="16.5" customHeight="1">
+    <row r="161" spans="1:13" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A161" t="s">
         <v>77</v>
       </c>
@@ -4822,7 +4905,7 @@
         <v>308</v>
       </c>
       <c r="J161" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
       <c r="L161" t="s">
         <v>235</v>
@@ -4831,7 +4914,7 @@
         <v>244</v>
       </c>
     </row>
-    <row r="162" spans="1:13" ht="16.5" customHeight="1">
+    <row r="162" spans="1:13" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A162" t="s">
         <v>77</v>
       </c>
@@ -4848,7 +4931,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="163" spans="1:13" ht="16.5" customHeight="1">
+    <row r="163" spans="1:13" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A163" t="s">
         <v>77</v>
       </c>
@@ -4868,7 +4951,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="164" spans="1:13" ht="16.5" customHeight="1">
+    <row r="164" spans="1:13" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A164" t="s">
         <v>77</v>
       </c>
@@ -4888,7 +4971,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="165" spans="1:13" ht="16.5" customHeight="1">
+    <row r="165" spans="1:13" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A165" t="s">
         <v>77</v>
       </c>
@@ -4908,7 +4991,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="166" spans="1:13" ht="16.5" customHeight="1">
+    <row r="166" spans="1:13" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A166" t="s">
         <v>77</v>
       </c>
@@ -4925,7 +5008,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="167" spans="1:13" ht="16.5" customHeight="1">
+    <row r="167" spans="1:13" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A167" t="s">
         <v>77</v>
       </c>
@@ -4939,7 +5022,7 @@
         <v>308</v>
       </c>
       <c r="J167" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
       <c r="L167" t="s">
         <v>302</v>
@@ -4948,7 +5031,7 @@
         <v>244</v>
       </c>
     </row>
-    <row r="168" spans="1:13" ht="16.5" customHeight="1">
+    <row r="168" spans="1:13" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A168" t="s">
         <v>77</v>
       </c>
@@ -4965,7 +5048,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="169" spans="1:13" ht="16.5" customHeight="1">
+    <row r="169" spans="1:13" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A169" t="s">
         <v>77</v>
       </c>
@@ -4979,7 +5062,7 @@
         <v>308</v>
       </c>
       <c r="J169" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
       <c r="L169" t="s">
         <v>303</v>
@@ -4988,7 +5071,7 @@
         <v>244</v>
       </c>
     </row>
-    <row r="170" spans="1:13" ht="16.5" customHeight="1">
+    <row r="170" spans="1:13" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A170" t="s">
         <v>77</v>
       </c>
@@ -5005,7 +5088,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="171" spans="1:13" ht="16.5" customHeight="1">
+    <row r="171" spans="1:13" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A171" t="s">
         <v>77</v>
       </c>
@@ -5025,7 +5108,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="172" spans="1:13" ht="16.5" customHeight="1">
+    <row r="172" spans="1:13" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A172" t="s">
         <v>77</v>
       </c>
@@ -5045,7 +5128,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="173" spans="1:13" ht="16.5" customHeight="1">
+    <row r="173" spans="1:13" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A173" t="s">
         <v>77</v>
       </c>
@@ -5065,7 +5148,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="174" spans="1:13" ht="16.5" customHeight="1">
+    <row r="174" spans="1:13" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A174" t="s">
         <v>77</v>
       </c>
@@ -5085,7 +5168,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="175" spans="1:13" ht="16.5" customHeight="1">
+    <row r="175" spans="1:13" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A175" t="s">
         <v>77</v>
       </c>
@@ -5102,7 +5185,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="176" spans="1:13" ht="16.5" customHeight="1">
+    <row r="176" spans="1:13" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A176" t="s">
         <v>77</v>
       </c>
@@ -5116,7 +5199,7 @@
         <v>308</v>
       </c>
       <c r="J176" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
       <c r="L176" t="s">
         <v>234</v>
@@ -5125,7 +5208,7 @@
         <v>244</v>
       </c>
     </row>
-    <row r="177" spans="1:13" ht="16.5" customHeight="1">
+    <row r="177" spans="1:13" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A177" t="s">
         <v>77</v>
       </c>
@@ -5142,7 +5225,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="178" spans="1:13" ht="16.5" customHeight="1">
+    <row r="178" spans="1:13" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A178" t="s">
         <v>77</v>
       </c>
@@ -5156,7 +5239,7 @@
         <v>308</v>
       </c>
       <c r="J178" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
       <c r="L178" t="s">
         <v>233</v>
@@ -5165,7 +5248,7 @@
         <v>244</v>
       </c>
     </row>
-    <row r="179" spans="1:13" ht="16.5" customHeight="1">
+    <row r="179" spans="1:13" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A179" t="s">
         <v>77</v>
       </c>
@@ -5182,7 +5265,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="180" spans="1:13" ht="16.5" customHeight="1">
+    <row r="180" spans="1:13" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A180" t="s">
         <v>77</v>
       </c>
@@ -5211,7 +5294,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="181" spans="1:13" ht="16.5" customHeight="1">
+    <row r="181" spans="1:13" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A181" t="s">
         <v>77</v>
       </c>
@@ -5231,7 +5314,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="182" spans="1:13" ht="16.5" customHeight="1">
+    <row r="182" spans="1:13" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A182" t="s">
         <v>77</v>
       </c>
@@ -5251,7 +5334,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="183" spans="1:13" ht="16.5" customHeight="1">
+    <row r="183" spans="1:13" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A183" t="s">
         <v>77</v>
       </c>
@@ -5268,7 +5351,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="184" spans="1:13" ht="16.5" customHeight="1">
+    <row r="184" spans="1:13" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A184" t="s">
         <v>180</v>
       </c>
@@ -5297,7 +5380,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="185" spans="1:13" ht="16.5" customHeight="1">
+    <row r="185" spans="1:13" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A185" t="s">
         <v>77</v>
       </c>
@@ -5326,7 +5409,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="186" spans="1:13" ht="16.5" customHeight="1">
+    <row r="186" spans="1:13" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A186" t="s">
         <v>180</v>
       </c>
@@ -5355,7 +5438,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="187" spans="1:13" ht="16.5" customHeight="1">
+    <row r="187" spans="1:13" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A187" t="s">
         <v>77</v>
       </c>
@@ -5384,7 +5467,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="188" spans="1:13" ht="16.5" customHeight="1">
+    <row r="188" spans="1:13" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A188" t="s">
         <v>77</v>
       </c>
@@ -5401,7 +5484,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="189" spans="1:13" ht="16.5" customHeight="1">
+    <row r="189" spans="1:13" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A189" t="s">
         <v>77</v>
       </c>
@@ -5421,7 +5504,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="190" spans="1:13" ht="16.5" customHeight="1">
+    <row r="190" spans="1:13" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A190" t="s">
         <v>77</v>
       </c>
@@ -5438,7 +5521,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="191" spans="1:13" ht="16.5" customHeight="1">
+    <row r="191" spans="1:13" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A191" t="s">
         <v>77</v>
       </c>
@@ -5452,7 +5535,7 @@
         <v>308</v>
       </c>
       <c r="J191" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
       <c r="L191" t="s">
         <v>232</v>
@@ -5461,7 +5544,7 @@
         <v>245</v>
       </c>
     </row>
-    <row r="192" spans="1:13" ht="16.5" customHeight="1">
+    <row r="192" spans="1:13" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A192" t="s">
         <v>77</v>
       </c>
@@ -5481,7 +5564,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="193" spans="1:13" ht="16.5" customHeight="1">
+    <row r="193" spans="1:13" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A193" t="s">
         <v>77</v>
       </c>
@@ -5498,7 +5581,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="194" spans="1:13" ht="16.5" customHeight="1">
+    <row r="194" spans="1:13" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A194" t="s">
         <v>77</v>
       </c>
@@ -5515,7 +5598,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="195" spans="1:13" ht="16.5" customHeight="1">
+    <row r="195" spans="1:13" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A195" t="s">
         <v>77</v>
       </c>
@@ -5532,7 +5615,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="196" spans="1:13" ht="16.5" customHeight="1">
+    <row r="196" spans="1:13" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A196" t="s">
         <v>77</v>
       </c>
@@ -5549,7 +5632,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="197" spans="1:13" ht="16.5" customHeight="1">
+    <row r="197" spans="1:13" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A197" t="s">
         <v>77</v>
       </c>
@@ -5563,7 +5646,7 @@
         <v>308</v>
       </c>
       <c r="J197" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
       <c r="L197" t="s">
         <v>231</v>
@@ -5572,7 +5655,7 @@
         <v>244</v>
       </c>
     </row>
-    <row r="198" spans="1:13" ht="16.5" customHeight="1">
+    <row r="198" spans="1:13" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A198" t="s">
         <v>77</v>
       </c>
@@ -5589,7 +5672,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="199" spans="1:13" ht="16.5" customHeight="1">
+    <row r="199" spans="1:13" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A199" t="s">
         <v>77</v>
       </c>
@@ -5603,7 +5686,7 @@
         <v>308</v>
       </c>
       <c r="J199" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
       <c r="L199" t="s">
         <v>230</v>
@@ -5612,7 +5695,7 @@
         <v>245</v>
       </c>
     </row>
-    <row r="200" spans="1:13" ht="16.5" customHeight="1">
+    <row r="200" spans="1:13" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A200" t="s">
         <v>77</v>
       </c>
@@ -5629,7 +5712,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="201" spans="1:13" ht="16.5" customHeight="1">
+    <row r="201" spans="1:13" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A201" t="s">
         <v>77</v>
       </c>
@@ -5646,7 +5729,7 @@
         <v>289</v>
       </c>
     </row>
-    <row r="202" spans="1:13" ht="16.5" customHeight="1">
+    <row r="202" spans="1:13" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A202" t="s">
         <v>180</v>
       </c>
@@ -5675,7 +5758,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="203" spans="1:13" ht="16.5" customHeight="1">
+    <row r="203" spans="1:13" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A203" t="s">
         <v>77</v>
       </c>
@@ -5704,7 +5787,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="204" spans="1:13" ht="16.5" customHeight="1">
+    <row r="204" spans="1:13" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A204" t="s">
         <v>77</v>
       </c>
@@ -5724,7 +5807,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="205" spans="1:13" ht="16.5" customHeight="1">
+    <row r="205" spans="1:13" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A205" t="s">
         <v>77</v>
       </c>
@@ -5741,7 +5824,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="206" spans="1:13" ht="16.5" customHeight="1">
+    <row r="206" spans="1:13" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A206" t="s">
         <v>180</v>
       </c>
@@ -5770,7 +5853,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="207" spans="1:13" ht="16.5" customHeight="1">
+    <row r="207" spans="1:13" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A207" t="s">
         <v>77</v>
       </c>
@@ -5799,7 +5882,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="208" spans="1:13" ht="16.5" customHeight="1">
+    <row r="208" spans="1:13" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A208" t="s">
         <v>180</v>
       </c>
@@ -5828,7 +5911,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="209" spans="1:13" ht="16.5" customHeight="1">
+    <row r="209" spans="1:13" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A209" t="s">
         <v>77</v>
       </c>
@@ -5857,7 +5940,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="210" spans="1:13" ht="16.5" customHeight="1">
+    <row r="210" spans="1:13" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A210" t="s">
         <v>77</v>
       </c>
@@ -5874,7 +5957,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="211" spans="1:13" ht="16.5" customHeight="1">
+    <row r="211" spans="1:13" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A211" t="s">
         <v>180</v>
       </c>
@@ -5894,7 +5977,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="212" spans="1:13" ht="16.5" customHeight="1">
+    <row r="212" spans="1:13" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A212" t="s">
         <v>77</v>
       </c>
@@ -5911,7 +5994,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="213" spans="1:13" ht="16.5" customHeight="1">
+    <row r="213" spans="1:13" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A213" t="s">
         <v>77</v>
       </c>
@@ -5925,7 +6008,7 @@
         <v>308</v>
       </c>
       <c r="J213" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
       <c r="L213" t="s">
         <v>229</v>
@@ -5934,7 +6017,7 @@
         <v>245</v>
       </c>
     </row>
-    <row r="214" spans="1:13" ht="16.5" customHeight="1">
+    <row r="214" spans="1:13" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A214" t="s">
         <v>77</v>
       </c>
@@ -5954,7 +6037,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="215" spans="1:13" ht="16.5" customHeight="1">
+    <row r="215" spans="1:13" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A215" t="s">
         <v>77</v>
       </c>
@@ -5971,7 +6054,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="216" spans="1:13" ht="16.5" customHeight="1">
+    <row r="216" spans="1:13" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A216" t="s">
         <v>77</v>
       </c>
@@ -5988,7 +6071,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="217" spans="1:13" ht="16.5" customHeight="1">
+    <row r="217" spans="1:13" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A217" t="s">
         <v>77</v>
       </c>
@@ -6005,7 +6088,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="218" spans="1:13" ht="16.5" customHeight="1">
+    <row r="218" spans="1:13" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A218" t="s">
         <v>77</v>
       </c>
@@ -6022,7 +6105,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="219" spans="1:13" ht="16.5" customHeight="1">
+    <row r="219" spans="1:13" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A219" t="s">
         <v>77</v>
       </c>
@@ -6036,7 +6119,7 @@
         <v>308</v>
       </c>
       <c r="J219" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
       <c r="L219" t="s">
         <v>228</v>
@@ -6045,7 +6128,7 @@
         <v>244</v>
       </c>
     </row>
-    <row r="220" spans="1:13" ht="16.5" customHeight="1">
+    <row r="220" spans="1:13" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A220" t="s">
         <v>77</v>
       </c>
@@ -6062,7 +6145,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="221" spans="1:13" ht="16.5" customHeight="1">
+    <row r="221" spans="1:13" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A221" t="s">
         <v>77</v>
       </c>
@@ -6076,7 +6159,7 @@
         <v>308</v>
       </c>
       <c r="J221" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
       <c r="L221" t="s">
         <v>227</v>
@@ -6085,7 +6168,7 @@
         <v>245</v>
       </c>
     </row>
-    <row r="222" spans="1:13" ht="16.5" customHeight="1">
+    <row r="222" spans="1:13" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A222" t="s">
         <v>77</v>
       </c>
@@ -6102,7 +6185,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="223" spans="1:13" ht="16.5" customHeight="1">
+    <row r="223" spans="1:13" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A223" t="s">
         <v>77</v>
       </c>
@@ -6119,7 +6202,7 @@
         <v>289</v>
       </c>
     </row>
-    <row r="224" spans="1:13" ht="16.5" customHeight="1">
+    <row r="224" spans="1:13" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A224" t="s">
         <v>180</v>
       </c>
@@ -6148,7 +6231,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="225" spans="1:13" ht="16.5" customHeight="1">
+    <row r="225" spans="1:13" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A225" t="s">
         <v>77</v>
       </c>
@@ -6177,7 +6260,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="226" spans="1:13" ht="16.5" customHeight="1">
+    <row r="226" spans="1:13" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A226" t="s">
         <v>77</v>
       </c>
@@ -6197,7 +6280,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="227" spans="1:13" ht="16.5" customHeight="1">
+    <row r="227" spans="1:13" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A227" t="s">
         <v>77</v>
       </c>
@@ -6214,7 +6297,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="228" spans="1:13" ht="16.5" customHeight="1">
+    <row r="228" spans="1:13" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A228" t="s">
         <v>77</v>
       </c>
@@ -6231,7 +6314,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="229" spans="1:13" ht="16.5" customHeight="1">
+    <row r="229" spans="1:13" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A229" t="s">
         <v>77</v>
       </c>
@@ -6260,7 +6343,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="230" spans="1:13" ht="16.5" customHeight="1">
+    <row r="230" spans="1:13" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A230" t="s">
         <v>77</v>
       </c>
@@ -6277,7 +6360,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="231" spans="1:13" ht="16.5" customHeight="1">
+    <row r="231" spans="1:13" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A231" t="s">
         <v>180</v>
       </c>
@@ -6306,7 +6389,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="232" spans="1:13" ht="16.5" customHeight="1">
+    <row r="232" spans="1:13" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A232" t="s">
         <v>77</v>
       </c>
@@ -6335,7 +6418,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="233" spans="1:13" ht="16.5" customHeight="1">
+    <row r="233" spans="1:13" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A233" t="s">
         <v>180</v>
       </c>
@@ -6364,7 +6447,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="234" spans="1:13" ht="16.5" customHeight="1">
+    <row r="234" spans="1:13" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A234" t="s">
         <v>77</v>
       </c>
@@ -6393,7 +6476,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="235" spans="1:13" ht="16.5" customHeight="1">
+    <row r="235" spans="1:13" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A235" t="s">
         <v>77</v>
       </c>
@@ -6410,7 +6493,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="236" spans="1:13" ht="16.5" customHeight="1">
+    <row r="236" spans="1:13" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A236" t="s">
         <v>180</v>
       </c>
@@ -6430,7 +6513,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="237" spans="1:13" ht="16.5" customHeight="1">
+    <row r="237" spans="1:13" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A237" t="s">
         <v>77</v>
       </c>
@@ -6447,7 +6530,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="238" spans="1:13" ht="16.5" customHeight="1">
+    <row r="238" spans="1:13" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A238" t="s">
         <v>77</v>
       </c>
@@ -6461,7 +6544,7 @@
         <v>308</v>
       </c>
       <c r="J238" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
       <c r="L238" t="s">
         <v>344</v>
@@ -6470,7 +6553,7 @@
         <v>245</v>
       </c>
     </row>
-    <row r="239" spans="1:13" ht="16.5" customHeight="1">
+    <row r="239" spans="1:13" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A239" t="s">
         <v>77</v>
       </c>
@@ -6490,7 +6573,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="240" spans="1:13" ht="16.5" customHeight="1">
+    <row r="240" spans="1:13" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A240" t="s">
         <v>77</v>
       </c>
@@ -6507,7 +6590,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="241" spans="1:13" ht="16.5" customHeight="1">
+    <row r="241" spans="1:13" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A241" t="s">
         <v>77</v>
       </c>
@@ -6524,7 +6607,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="242" spans="1:13" ht="16.5" customHeight="1">
+    <row r="242" spans="1:13" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A242" t="s">
         <v>77</v>
       </c>
@@ -6541,7 +6624,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="243" spans="1:13" ht="16.5" customHeight="1">
+    <row r="243" spans="1:13" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A243" t="s">
         <v>77</v>
       </c>
@@ -6558,7 +6641,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="244" spans="1:13" ht="16.5" customHeight="1">
+    <row r="244" spans="1:13" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A244" t="s">
         <v>77</v>
       </c>
@@ -6572,7 +6655,7 @@
         <v>308</v>
       </c>
       <c r="J244" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
       <c r="L244" t="s">
         <v>350</v>
@@ -6581,7 +6664,7 @@
         <v>244</v>
       </c>
     </row>
-    <row r="245" spans="1:13" ht="16.5" customHeight="1">
+    <row r="245" spans="1:13" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A245" t="s">
         <v>77</v>
       </c>
@@ -6598,7 +6681,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="246" spans="1:13" ht="16.5" customHeight="1">
+    <row r="246" spans="1:13" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A246" t="s">
         <v>77</v>
       </c>
@@ -6612,7 +6695,7 @@
         <v>308</v>
       </c>
       <c r="J246" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
       <c r="L246" t="s">
         <v>352</v>
@@ -6621,7 +6704,7 @@
         <v>245</v>
       </c>
     </row>
-    <row r="247" spans="1:13" ht="16.5" customHeight="1">
+    <row r="247" spans="1:13" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A247" t="s">
         <v>77</v>
       </c>
@@ -6638,7 +6721,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="248" spans="1:13" ht="16.5" customHeight="1">
+    <row r="248" spans="1:13" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A248" t="s">
         <v>77</v>
       </c>
@@ -6655,7 +6738,7 @@
         <v>289</v>
       </c>
     </row>
-    <row r="249" spans="1:13" ht="16.5" customHeight="1">
+    <row r="249" spans="1:13" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A249" t="s">
         <v>180</v>
       </c>
@@ -6684,7 +6767,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="250" spans="1:13" ht="16.5" customHeight="1">
+    <row r="250" spans="1:13" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A250" t="s">
         <v>77</v>
       </c>
@@ -6713,7 +6796,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="251" spans="1:13" ht="16.5" customHeight="1">
+    <row r="251" spans="1:13" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A251" t="s">
         <v>77</v>
       </c>
@@ -6733,7 +6816,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="252" spans="1:13" ht="16.5" customHeight="1">
+    <row r="252" spans="1:13" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A252" t="s">
         <v>77</v>
       </c>
@@ -6750,7 +6833,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="253" spans="1:13" ht="16.5" customHeight="1">
+    <row r="253" spans="1:13" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A253" t="s">
         <v>77</v>
       </c>
@@ -6767,7 +6850,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="254" spans="1:13" ht="16.5" customHeight="1">
+    <row r="254" spans="1:13" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A254" t="s">
         <v>77</v>
       </c>
@@ -6781,7 +6864,7 @@
         <v>314</v>
       </c>
       <c r="J254" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="L254" t="s">
         <v>151</v>
@@ -6790,7 +6873,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="255" spans="1:13" ht="16.5" customHeight="1">
+    <row r="255" spans="1:13" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A255" t="s">
         <v>77</v>
       </c>
@@ -6807,7 +6890,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="256" spans="1:13" ht="16.5" customHeight="1">
+    <row r="256" spans="1:13" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A256" t="s">
         <v>77</v>
       </c>
@@ -6824,7 +6907,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="257" spans="1:13" ht="16.5" customHeight="1">
+    <row r="257" spans="1:13" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A257" t="s">
         <v>77</v>
       </c>
@@ -6844,7 +6927,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="258" spans="1:13" ht="16.5" customHeight="1">
+    <row r="258" spans="1:13" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A258" t="s">
         <v>77</v>
       </c>
@@ -6864,7 +6947,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="259" spans="1:13" ht="16.5" customHeight="1">
+    <row r="259" spans="1:13" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A259" t="s">
         <v>77</v>
       </c>
@@ -6875,7 +6958,7 @@
         <v>9</v>
       </c>
       <c r="J259" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
       <c r="L259" t="s">
         <v>113</v>
@@ -6884,7 +6967,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="260" spans="1:13" ht="16.5" customHeight="1">
+    <row r="260" spans="1:13" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A260" t="s">
         <v>77</v>
       </c>
@@ -6901,7 +6984,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="261" spans="1:13" ht="16.5" customHeight="1">
+    <row r="261" spans="1:13" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A261" t="s">
         <v>77</v>
       </c>
@@ -6915,7 +6998,7 @@
         <v>308</v>
       </c>
       <c r="J261" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
       <c r="L261" t="s">
         <v>226</v>
@@ -6924,7 +7007,7 @@
         <v>245</v>
       </c>
     </row>
-    <row r="262" spans="1:13" ht="16.5" customHeight="1">
+    <row r="262" spans="1:13" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A262" t="s">
         <v>77</v>
       </c>
@@ -6941,7 +7024,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="263" spans="1:13" ht="16.5" customHeight="1">
+    <row r="263" spans="1:13" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A263" t="s">
         <v>77</v>
       </c>
@@ -6958,7 +7041,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="264" spans="1:13" ht="16.5" customHeight="1">
+    <row r="264" spans="1:13" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A264" t="s">
         <v>77</v>
       </c>
@@ -6975,7 +7058,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="265" spans="1:13" ht="16.5" customHeight="1">
+    <row r="265" spans="1:13" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A265" t="s">
         <v>77</v>
       </c>
@@ -6995,7 +7078,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="266" spans="1:13" ht="16.5" customHeight="1">
+    <row r="266" spans="1:13" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A266" t="s">
         <v>77</v>
       </c>
@@ -7012,7 +7095,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="267" spans="1:13" ht="16.5" customHeight="1">
+    <row r="267" spans="1:13" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A267" t="s">
         <v>77</v>
       </c>
@@ -7026,7 +7109,7 @@
         <v>308</v>
       </c>
       <c r="J267" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
       <c r="L267" t="s">
         <v>384</v>
@@ -7035,7 +7118,7 @@
         <v>245</v>
       </c>
     </row>
-    <row r="268" spans="1:13" ht="16.5" customHeight="1">
+    <row r="268" spans="1:13" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A268" t="s">
         <v>114</v>
       </c>
@@ -7052,7 +7135,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="269" spans="1:13" ht="16.5" customHeight="1">
+    <row r="269" spans="1:13" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A269" t="s">
         <v>114</v>
       </c>
@@ -7065,8 +7148,14 @@
       <c r="D269" t="s">
         <v>305</v>
       </c>
-      <c r="J269" t="s">
-        <v>413</v>
+      <c r="F269" t="s">
+        <v>11</v>
+      </c>
+      <c r="H269" t="s">
+        <v>448</v>
+      </c>
+      <c r="I269" t="s">
+        <v>447</v>
       </c>
       <c r="L269" t="s">
         <v>116</v>
@@ -7075,7 +7164,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="270" spans="1:13" ht="16.5" customHeight="1">
+    <row r="270" spans="1:13" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A270" t="s">
         <v>114</v>
       </c>
@@ -7092,7 +7181,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="271" spans="1:13" ht="16.5" customHeight="1">
+    <row r="271" spans="1:13" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A271" t="s">
         <v>114</v>
       </c>
@@ -7109,29 +7198,29 @@
         <v>121</v>
       </c>
     </row>
-    <row r="272" spans="1:13" ht="16.5" customHeight="1">
+    <row r="272" spans="1:13" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A272" t="s">
         <v>114</v>
       </c>
       <c r="B272" t="s">
-        <v>447</v>
+        <v>446</v>
       </c>
       <c r="C272" t="s">
         <v>17</v>
       </c>
       <c r="L272" t="s">
-        <v>447</v>
+        <v>446</v>
       </c>
       <c r="M272" t="s">
         <v>121</v>
       </c>
     </row>
-    <row r="273" spans="1:13" ht="16.5" customHeight="1">
+    <row r="273" spans="1:13" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A273" t="s">
         <v>114</v>
       </c>
       <c r="B273" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
       <c r="C273" t="s">
         <v>9</v>
@@ -7140,13 +7229,13 @@
         <v>114</v>
       </c>
       <c r="L273" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
       <c r="M273" t="s">
         <v>123</v>
       </c>
     </row>
-    <row r="274" spans="1:13" ht="16.5" customHeight="1">
+    <row r="274" spans="1:13" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A274" t="s">
         <v>114</v>
       </c>
@@ -7163,7 +7252,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="275" spans="1:13" ht="16.5" customHeight="1">
+    <row r="275" spans="1:13" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A275" t="s">
         <v>114</v>
       </c>
@@ -7180,7 +7269,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="276" spans="1:13" ht="16.5" customHeight="1">
+    <row r="276" spans="1:13" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A276" t="s">
         <v>114</v>
       </c>
@@ -7197,7 +7286,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="277" spans="1:13" ht="16.5" customHeight="1">
+    <row r="277" spans="1:13" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A277" t="s">
         <v>114</v>
       </c>
@@ -7226,7 +7315,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="278" spans="1:13" ht="16.5" customHeight="1">
+    <row r="278" spans="1:13" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A278" t="s">
         <v>114</v>
       </c>
@@ -7243,7 +7332,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="279" spans="1:13" ht="16.5" customHeight="1">
+    <row r="279" spans="1:13" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A279" t="s">
         <v>114</v>
       </c>
@@ -7260,7 +7349,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="280" spans="1:13" ht="16.5" customHeight="1">
+    <row r="280" spans="1:13" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A280" t="s">
         <v>114</v>
       </c>
@@ -7274,7 +7363,7 @@
         <v>308</v>
       </c>
       <c r="J280" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
       <c r="L280" t="s">
         <v>225</v>
@@ -7283,7 +7372,7 @@
         <v>245</v>
       </c>
     </row>
-    <row r="281" spans="1:13" ht="16.5" customHeight="1">
+    <row r="281" spans="1:13" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A281" t="s">
         <v>114</v>
       </c>
@@ -7303,7 +7392,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="282" spans="1:13" ht="16.5" customHeight="1">
+    <row r="282" spans="1:13" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A282" t="s">
         <v>114</v>
       </c>
@@ -7317,7 +7406,7 @@
         <v>310</v>
       </c>
       <c r="J282" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
       <c r="L282" t="s">
         <v>407</v>
@@ -7326,7 +7415,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="283" spans="1:13" ht="16.5" customHeight="1">
+    <row r="283" spans="1:13" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A283" t="s">
         <v>114</v>
       </c>
@@ -7340,7 +7429,7 @@
         <v>330</v>
       </c>
       <c r="J283" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="L283" t="s">
         <v>216</v>
@@ -7349,7 +7438,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="284" spans="1:13" ht="16.5" customHeight="1">
+    <row r="284" spans="1:13" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A284" t="s">
         <v>385</v>
       </c>
@@ -7366,7 +7455,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="285" spans="1:13" ht="16.5" customHeight="1">
+    <row r="285" spans="1:13" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A285" t="s">
         <v>385</v>
       </c>
@@ -7379,8 +7468,14 @@
       <c r="D285" t="s">
         <v>305</v>
       </c>
-      <c r="J285" t="s">
-        <v>413</v>
+      <c r="F285" t="s">
+        <v>11</v>
+      </c>
+      <c r="H285" t="s">
+        <v>448</v>
+      </c>
+      <c r="I285" t="s">
+        <v>447</v>
       </c>
       <c r="L285" t="s">
         <v>403</v>
@@ -7389,7 +7484,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="286" spans="1:13" ht="16.5" customHeight="1">
+    <row r="286" spans="1:13" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A286" t="s">
         <v>385</v>
       </c>
@@ -7406,7 +7501,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="287" spans="1:13" ht="16.5" customHeight="1">
+    <row r="287" spans="1:13" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A287" t="s">
         <v>385</v>
       </c>
@@ -7423,7 +7518,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="288" spans="1:13" ht="16.5" customHeight="1">
+    <row r="288" spans="1:13" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A288" t="s">
         <v>385</v>
       </c>
@@ -7437,7 +7532,7 @@
         <v>308</v>
       </c>
       <c r="J288" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
       <c r="L288" t="s">
         <v>389</v>
@@ -7446,7 +7541,7 @@
         <v>245</v>
       </c>
     </row>
-    <row r="289" spans="1:13" ht="16.5" customHeight="1">
+    <row r="289" spans="1:13" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A289" t="s">
         <v>385</v>
       </c>
@@ -7457,10 +7552,10 @@
         <v>9</v>
       </c>
       <c r="D289" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="J289" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="L289" t="s">
         <v>390</v>
@@ -7469,7 +7564,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="290" spans="1:13" ht="16.5" customHeight="1">
+    <row r="290" spans="1:13" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A290" t="s">
         <v>385</v>
       </c>
@@ -7480,10 +7575,10 @@
         <v>9</v>
       </c>
       <c r="D290" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
       <c r="J290" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="L290" t="s">
         <v>391</v>
@@ -7492,7 +7587,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="291" spans="1:13" ht="16.5" customHeight="1">
+    <row r="291" spans="1:13" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A291" t="s">
         <v>385</v>
       </c>
@@ -7512,7 +7607,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="292" spans="1:13" ht="16.5" customHeight="1">
+    <row r="292" spans="1:13" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A292" t="s">
         <v>385</v>
       </c>
@@ -7523,7 +7618,7 @@
         <v>9</v>
       </c>
       <c r="J292" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
       <c r="L292" t="s">
         <v>393</v>
@@ -7532,7 +7627,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="293" spans="1:13" ht="16.5" customHeight="1">
+    <row r="293" spans="1:13" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A293" t="s">
         <v>385</v>
       </c>
@@ -7549,7 +7644,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="294" spans="1:13" ht="16.5" customHeight="1">
+    <row r="294" spans="1:13" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A294" t="s">
         <v>385</v>
       </c>
@@ -7566,7 +7661,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="295" spans="1:13" ht="16.5" customHeight="1">
+    <row r="295" spans="1:13" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A295" t="s">
         <v>385</v>
       </c>
@@ -7577,7 +7672,7 @@
         <v>15</v>
       </c>
       <c r="J295" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
       <c r="L295" t="s">
         <v>396</v>
@@ -7586,7 +7681,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="296" spans="1:13" ht="16.5" customHeight="1">
+    <row r="296" spans="1:13" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A296" t="s">
         <v>385</v>
       </c>
@@ -7603,7 +7698,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="297" spans="1:13" ht="16.5" customHeight="1">
+    <row r="297" spans="1:13" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A297" t="s">
         <v>385</v>
       </c>
@@ -7620,7 +7715,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="298" spans="1:13" ht="16.5" customHeight="1">
+    <row r="298" spans="1:13" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A298" t="s">
         <v>385</v>
       </c>
@@ -7637,7 +7732,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="299" spans="1:13" ht="16.5" customHeight="1">
+    <row r="299" spans="1:13" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A299" t="s">
         <v>385</v>
       </c>
@@ -7654,7 +7749,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="300" spans="1:13" ht="16.5" customHeight="1">
+    <row r="300" spans="1:13" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A300" t="s">
         <v>385</v>
       </c>
@@ -7671,7 +7766,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="301" spans="1:13" ht="16.5" customHeight="1">
+    <row r="301" spans="1:13" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A301" t="s">
         <v>385</v>
       </c>
@@ -7698,36 +7793,36 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>